<commit_message>
Update to biomass addition
</commit_message>
<xml_diff>
--- a/KineticModel/ecoli_test.xlsx
+++ b/KineticModel/ecoli_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="240" windowWidth="18195" windowHeight="7365" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="18195" windowHeight="7365" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ecoliT1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="88">
   <si>
     <t>Enzymes</t>
   </si>
@@ -302,6 +302,9 @@
   </si>
   <si>
     <t>dhap[e]</t>
+  </si>
+  <si>
+    <t>glc[c] + pep[c] ---&gt; g6p[c] + pyr[c]</t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1083,7 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1331,8 +1334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:P13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1428,7 +1431,7 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c r="N3" t="s">
         <v>20</v>
@@ -2382,8 +2385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update June 29 2015
</commit_message>
<xml_diff>
--- a/KineticModel/ecoli_test.xlsx
+++ b/KineticModel/ecoli_test.xlsx
@@ -4,20 +4,53 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="360" windowWidth="18195" windowHeight="7245" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="18195" windowHeight="7125" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ecoliT1" sheetId="10" r:id="rId1"/>
     <sheet name="ecoliT2" sheetId="11" r:id="rId2"/>
     <sheet name="ecoliT3" sheetId="12" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId4"/>
+    <sheet name="ecoliT4" sheetId="13" r:id="rId4"/>
+    <sheet name="ecoliT5" sheetId="16" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId6"/>
+    <sheet name="ecoliT6" sheetId="14" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="ecoliT4" localSheetId="3">ecoliT4!$A$1:$P$25</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="ecoliT4" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\ecoliT4.txt">
+      <textFields count="16">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="209">
   <si>
     <t>Enzymes</t>
   </si>
@@ -470,6 +503,201 @@
   </si>
   <si>
     <t>'h2o[e]'</t>
+  </si>
+  <si>
+    <t>[c] : g6p + atp &lt;==&gt; fdp + adp + h</t>
+  </si>
+  <si>
+    <t>pgipfk</t>
+  </si>
+  <si>
+    <t>[c] : g3p + nad + pi + adp &lt;==&gt; atp + h2o + nadh + pep</t>
+  </si>
+  <si>
+    <t>gapdeno</t>
+  </si>
+  <si>
+    <t>pyrEX</t>
+  </si>
+  <si>
+    <t>lacEX</t>
+  </si>
+  <si>
+    <t>biomassEX</t>
+  </si>
+  <si>
+    <t>h2oEX</t>
+  </si>
+  <si>
+    <t>hEX</t>
+  </si>
+  <si>
+    <t>piEX</t>
+  </si>
+  <si>
+    <t>Expyr</t>
+  </si>
+  <si>
+    <t>Exlac</t>
+  </si>
+  <si>
+    <t>Exh</t>
+  </si>
+  <si>
+    <t>Expi</t>
+  </si>
+  <si>
+    <t>pyr[e] ---&gt;</t>
+  </si>
+  <si>
+    <t>pyr[c] ---&gt; pyr[e]</t>
+  </si>
+  <si>
+    <t>lac[c] ---&gt; lac[e]</t>
+  </si>
+  <si>
+    <t>lac[e] ---&gt;</t>
+  </si>
+  <si>
+    <t>pyr[e]</t>
+  </si>
+  <si>
+    <t>lac[e]</t>
+  </si>
+  <si>
+    <t>biomass[c]</t>
+  </si>
+  <si>
+    <t>biomass[c] ---&gt;</t>
+  </si>
+  <si>
+    <t>dhap[e]</t>
+  </si>
+  <si>
+    <t>h2o[e]</t>
+  </si>
+  <si>
+    <t>h[e]</t>
+  </si>
+  <si>
+    <t>pi[e]</t>
+  </si>
+  <si>
+    <t>g6ppyr</t>
+  </si>
+  <si>
+    <t>g6p[c] + 2 adp + 2 pi ---&gt; 2 atp + pyr</t>
+  </si>
+  <si>
+    <t>1.01,1.01</t>
+  </si>
+  <si>
+    <t>0.17,0.13,0.23</t>
+  </si>
+  <si>
+    <t>0.00017,0.00013,0.00023</t>
+  </si>
+  <si>
+    <t>0.00025,0.00031,1,0.00025,0.00031</t>
+  </si>
+  <si>
+    <t>0.00033,1,0.00015,0.02,0.0029</t>
+  </si>
+  <si>
+    <t>'dhap[c]'</t>
+  </si>
+  <si>
+    <t>'nad[c]'</t>
+  </si>
+  <si>
+    <t>'nadh[c]'</t>
+  </si>
+  <si>
+    <t>'lac[c]'</t>
+  </si>
+  <si>
+    <t>'f6p[c]'</t>
+  </si>
+  <si>
+    <t>'lac[e]'</t>
+  </si>
+  <si>
+    <t>'dhap[e]'</t>
+  </si>
+  <si>
+    <t>[c] : 0.2050 g6p + 0.5191 pep + 59.81 atp + 2.8328 pyr + 59.81 h2o + 3.547 nad ---&gt; biomass + 59.81 adp + 59.81 h + 59.81 pi + 3.547 nadh</t>
+  </si>
+  <si>
+    <t>9.54E-6,1,5E-5,1,8.94E-6,6.32E-5</t>
+  </si>
+  <si>
+    <t>1,1,0.00073,1,1,1</t>
+  </si>
+  <si>
+    <t>acaldEX</t>
+  </si>
+  <si>
+    <t>etohEX</t>
+  </si>
+  <si>
+    <t>etoh[c] &lt;==&gt; etoh[e]</t>
+  </si>
+  <si>
+    <t>co2EX</t>
+  </si>
+  <si>
+    <t>co2[c] &lt;==&gt; co2[e]</t>
+  </si>
+  <si>
+    <t>Exacald</t>
+  </si>
+  <si>
+    <t>Exetoh</t>
+  </si>
+  <si>
+    <t>etoh[e] &lt;==&gt;</t>
+  </si>
+  <si>
+    <t>co2[e] &lt;==&gt;</t>
+  </si>
+  <si>
+    <t>acald[c] ---&gt; acald[e]</t>
+  </si>
+  <si>
+    <t>acald[e] ---&gt;</t>
+  </si>
+  <si>
+    <t>1,1,1,0.0106,1</t>
+  </si>
+  <si>
+    <t>acald[e]</t>
+  </si>
+  <si>
+    <t>etoh[e]</t>
+  </si>
+  <si>
+    <t>co2[e]</t>
+  </si>
+  <si>
+    <t>[c] : 0.2050 g6p + 0.5191 pep + 59.81 atp + 2.8328 pyr + 59.81 h2o + 3.547 nad + 3.7478 accoa ---&gt; biomass + 59.81 adp + 59.81 h + 59.81 pi + 3.547 nadh + 3.7478 coa</t>
+  </si>
+  <si>
+    <t>2.8E-5,1,8.3E-5,1,1,1,1.04E-2</t>
+  </si>
+  <si>
+    <t>vss (Gur = -10, O2ur = -1000)</t>
+  </si>
+  <si>
+    <t>[c] : adp + pep + h &lt;==&gt; atp + pyr</t>
+  </si>
+  <si>
+    <t>[c] : atp + h2o + pyr &lt;==&gt; amp + 2 h + pep + pi</t>
+  </si>
+  <si>
+    <t>[c] : coa + nad + pyr &lt;==&gt; accoa + co2 + nadh</t>
+  </si>
+  <si>
+    <t>[c] : amp + atp ---&gt; 2 adp</t>
   </si>
 </sst>
 </file>
@@ -559,7 +787,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -570,6 +798,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -583,6 +813,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ecoliT4" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -875,7 +1109,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,6 +1119,7 @@
     <col min="6" max="6" width="15.140625" customWidth="1"/>
     <col min="7" max="7" width="24.42578125" customWidth="1"/>
     <col min="8" max="8" width="42.5703125" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.35">
@@ -974,11 +1209,11 @@
       <c r="N3" t="s">
         <v>17</v>
       </c>
-      <c r="O3">
-        <v>1</v>
+      <c r="O3" s="10">
+        <v>8.43E-3</v>
       </c>
       <c r="P3">
-        <v>20</v>
+        <v>9.0799999999999995E-3</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1062,11 +1297,18 @@
       <c r="A7" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7">
+        <v>1.4999999999999999E-2</v>
+      </c>
       <c r="C7">
         <v>10.5</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="D7">
+        <v>0.15</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.18</v>
+      </c>
       <c r="F7" s="6">
         <v>4.2</v>
       </c>
@@ -1075,6 +1317,9 @@
       </c>
       <c r="H7" s="4" t="s">
         <v>51</v>
+      </c>
+      <c r="L7" t="s">
+        <v>173</v>
       </c>
       <c r="N7" t="s">
         <v>30</v>
@@ -1094,7 +1339,12 @@
       <c r="C8">
         <v>9000</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="D8">
+        <v>1000</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.114</v>
+      </c>
       <c r="F8" s="6">
         <v>1.4</v>
       </c>
@@ -1103,6 +1353,9 @@
       </c>
       <c r="H8" s="4" t="s">
         <v>53</v>
+      </c>
+      <c r="L8" t="s">
+        <v>172</v>
       </c>
       <c r="N8" t="s">
         <v>82</v>
@@ -1568,8 +1821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2472,15 +2725,1298 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:P30"/>
+  <sheetViews>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16:P16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="81.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.28515625" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="N2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2">
+        <v>0.1</v>
+      </c>
+      <c r="P2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6">
+        <v>-22.4</v>
+      </c>
+      <c r="G3" s="7">
+        <v>20</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="10">
+        <v>1.46E-4</v>
+      </c>
+      <c r="P3" s="10">
+        <v>2.31E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4">
+        <v>120</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="6">
+        <v>-4.5999999999999996</v>
+      </c>
+      <c r="G4" s="7">
+        <v>4.8609</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="N4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="10">
+        <v>8.43E-3</v>
+      </c>
+      <c r="P4">
+        <v>9.0799999999999995E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5">
+        <v>10.5</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="F5" s="6">
+        <v>4.2</v>
+      </c>
+      <c r="G5" s="7">
+        <v>7.47</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="N5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5" s="10">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="P5" s="10">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6">
+        <v>9000</v>
+      </c>
+      <c r="D6">
+        <v>1000</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.114</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1.4</v>
+      </c>
+      <c r="G6" s="7">
+        <v>7.47</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="L6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" s="10">
+        <v>4.37E-4</v>
+      </c>
+      <c r="P6" s="10">
+        <v>7.0399999999999998E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="F7" s="6">
+        <v>-3.8</v>
+      </c>
+      <c r="G7" s="7">
+        <v>15.08</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="N7" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" s="10">
+        <v>8.1300000000000001E-3</v>
+      </c>
+      <c r="P7" s="10">
+        <v>1.14E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8">
+        <v>232</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6">
+        <v>-5.3</v>
+      </c>
+      <c r="G8" s="7">
+        <v>1.7582</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="L8" t="s">
+        <v>175</v>
+      </c>
+      <c r="N8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O8" s="10">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9">
+        <v>-1.2</v>
+      </c>
+      <c r="G9" s="7">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="N9" t="s">
+        <v>23</v>
+      </c>
+      <c r="O9">
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="P9">
+        <v>1.6400000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10">
+        <v>166</v>
+      </c>
+      <c r="F10" s="6">
+        <v>-6.4</v>
+      </c>
+      <c r="G10" s="7">
+        <v>1.75</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L10" t="s">
+        <v>176</v>
+      </c>
+      <c r="N10" t="s">
+        <v>52</v>
+      </c>
+      <c r="O10">
+        <v>3.3700000000000001E-4</v>
+      </c>
+      <c r="P10">
+        <v>4.26E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="F11">
+        <v>-0.1</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="N11" t="s">
+        <v>25</v>
+      </c>
+      <c r="O11" s="10">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="P11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="N12" t="s">
+        <v>57</v>
+      </c>
+      <c r="O12" s="10">
+        <v>2.32E-3</v>
+      </c>
+      <c r="P12" s="10">
+        <v>2.8E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="N13" t="s">
+        <v>30</v>
+      </c>
+      <c r="O13" s="10">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="N14" t="s">
+        <v>58</v>
+      </c>
+      <c r="O14" s="10">
+        <v>5.4500000000000003E-5</v>
+      </c>
+      <c r="P14" s="10">
+        <v>1.27E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>150</v>
+      </c>
+      <c r="H15" t="s">
+        <v>165</v>
+      </c>
+      <c r="N15" t="s">
+        <v>78</v>
+      </c>
+      <c r="O15" s="10">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="N16" t="s">
+        <v>82</v>
+      </c>
+      <c r="O16" s="10">
+        <v>2.32E-4</v>
+      </c>
+      <c r="P16" s="10">
+        <v>3.4099999999999999E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N17" t="s">
+        <v>63</v>
+      </c>
+      <c r="O17" s="10">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="P17" s="10">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N18" t="s">
+        <v>164</v>
+      </c>
+      <c r="O18" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="P18" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="N19" t="s">
+        <v>163</v>
+      </c>
+      <c r="O19" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="P19" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="N20" t="s">
+        <v>162</v>
+      </c>
+      <c r="O20" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="P20" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="N21" t="s">
+        <v>166</v>
+      </c>
+      <c r="O21">
+        <v>0.1</v>
+      </c>
+      <c r="P21">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N22" t="s">
+        <v>167</v>
+      </c>
+      <c r="O22">
+        <v>0.1</v>
+      </c>
+      <c r="P22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="N23" t="s">
+        <v>168</v>
+      </c>
+      <c r="O23">
+        <v>0.1</v>
+      </c>
+      <c r="P23">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="N24" t="s">
+        <v>169</v>
+      </c>
+      <c r="O24">
+        <v>0.1</v>
+      </c>
+      <c r="P24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="H30" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="66.28515625" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="N2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2">
+        <v>0.1</v>
+      </c>
+      <c r="P2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="D3" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6">
+        <v>-22.38</v>
+      </c>
+      <c r="G3" s="7">
+        <v>20</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="10">
+        <v>1.46E-4</v>
+      </c>
+      <c r="P3" s="10">
+        <v>2.31E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4">
+        <v>120</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="6">
+        <v>-4.5999999999999996</v>
+      </c>
+      <c r="G4" s="7">
+        <v>4.8609</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="N4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="10">
+        <v>8.43E-3</v>
+      </c>
+      <c r="P4">
+        <v>9.0799999999999995E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5">
+        <v>10.5</v>
+      </c>
+      <c r="D5" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="F5" s="6">
+        <v>4.2</v>
+      </c>
+      <c r="G5" s="7">
+        <v>7.47</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="N5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5" s="10">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="P5" s="10">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6">
+        <v>9000</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.114</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1.4</v>
+      </c>
+      <c r="G6" s="7">
+        <v>7.47</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="L6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" s="10">
+        <v>4.37E-4</v>
+      </c>
+      <c r="P6" s="10">
+        <v>7.0399999999999998E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="D7" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="F7" s="6">
+        <v>-3.8</v>
+      </c>
+      <c r="G7" s="7">
+        <v>15.08</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="N7" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" s="10">
+        <v>8.1300000000000001E-3</v>
+      </c>
+      <c r="P7" s="10">
+        <v>1.14E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8">
+        <v>232</v>
+      </c>
+      <c r="D8" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6">
+        <v>-5.3</v>
+      </c>
+      <c r="G8" s="7">
+        <v>1.7582</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="L8" t="s">
+        <v>175</v>
+      </c>
+      <c r="N8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O8" s="10">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="F9">
+        <v>-1.2</v>
+      </c>
+      <c r="G9" s="7">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="L9" t="s">
+        <v>203</v>
+      </c>
+      <c r="N9" t="s">
+        <v>23</v>
+      </c>
+      <c r="O9">
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="P9">
+        <v>1.6400000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="D10" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="F10">
+        <v>-8.3000000000000007</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="L10" t="s">
+        <v>186</v>
+      </c>
+      <c r="N10" t="s">
+        <v>52</v>
+      </c>
+      <c r="O10">
+        <v>3.3700000000000001E-4</v>
+      </c>
+      <c r="P10">
+        <v>4.26E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="F11">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="L11" t="s">
+        <v>185</v>
+      </c>
+      <c r="N11" t="s">
+        <v>25</v>
+      </c>
+      <c r="O11" s="10">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="P11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="F12">
+        <v>-6</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="L12" t="s">
+        <v>198</v>
+      </c>
+      <c r="N12" t="s">
+        <v>57</v>
+      </c>
+      <c r="O12" s="10">
+        <v>2.32E-3</v>
+      </c>
+      <c r="P12" s="10">
+        <v>2.8E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="D13" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="F13">
+        <v>-0.1</v>
+      </c>
+      <c r="G13" s="7">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="N13" t="s">
+        <v>30</v>
+      </c>
+      <c r="O13" s="10">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="H14" t="s">
+        <v>202</v>
+      </c>
+      <c r="N14" t="s">
+        <v>58</v>
+      </c>
+      <c r="O14" s="10">
+        <v>5.4500000000000003E-5</v>
+      </c>
+      <c r="P14" s="10">
+        <v>1.27E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="H15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N15" t="s">
+        <v>78</v>
+      </c>
+      <c r="O15" s="10">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="N16" t="s">
+        <v>82</v>
+      </c>
+      <c r="O16" s="10">
+        <v>2.32E-4</v>
+      </c>
+      <c r="P16" s="10">
+        <v>3.4099999999999999E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="N17" t="s">
+        <v>89</v>
+      </c>
+      <c r="O17" s="10">
+        <v>8.8300000000000005E-5</v>
+      </c>
+      <c r="P17" s="10">
+        <v>2.12E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N18" t="s">
+        <v>88</v>
+      </c>
+      <c r="O18" s="10">
+        <v>5.2899999999999996E-4</v>
+      </c>
+      <c r="P18" s="10">
+        <v>6.9399999999999996E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N19" t="s">
+        <v>125</v>
+      </c>
+      <c r="O19" s="10">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="P19" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="N20" t="s">
+        <v>97</v>
+      </c>
+      <c r="O20" s="10">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="P20" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="N21" t="s">
+        <v>164</v>
+      </c>
+      <c r="O21">
+        <v>0.1</v>
+      </c>
+      <c r="P21">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="N22" t="s">
+        <v>162</v>
+      </c>
+      <c r="O22">
+        <v>0.1</v>
+      </c>
+      <c r="P22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N23" t="s">
+        <v>167</v>
+      </c>
+      <c r="O23">
+        <v>0.1</v>
+      </c>
+      <c r="P23">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="N24" t="s">
+        <v>168</v>
+      </c>
+      <c r="O24">
+        <v>0.1</v>
+      </c>
+      <c r="P24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N25" t="s">
+        <v>169</v>
+      </c>
+      <c r="O25">
+        <v>0.1</v>
+      </c>
+      <c r="P25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="N26" t="s">
+        <v>199</v>
+      </c>
+      <c r="O26">
+        <v>0.1</v>
+      </c>
+      <c r="P26">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="N27" t="s">
+        <v>200</v>
+      </c>
+      <c r="O27">
+        <v>0.1</v>
+      </c>
+      <c r="P27">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="N28" t="s">
+        <v>201</v>
+      </c>
+      <c r="O28">
+        <v>0.1</v>
+      </c>
+      <c r="P28">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="N29" t="s">
+        <v>118</v>
+      </c>
+      <c r="O29" s="10">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="P29" s="10">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19:F19"/>
+      <selection activeCell="H1" sqref="H1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -2496,8 +4032,14 @@
       <c r="F1">
         <v>25.638618721437901</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1">
+        <v>1.46711607655114E-4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -2513,8 +4055,14 @@
       <c r="F2">
         <v>5.3163126811608601</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2">
+        <v>8.6285423391734804E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -2530,8 +4078,14 @@
       <c r="F3">
         <v>0.78557553733909802</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="10">
+        <v>4.9368759497838799E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2547,8 +4101,14 @@
       <c r="F4">
         <v>21.457869626851199</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4">
+        <v>9.32289101793384E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -2564,8 +4124,14 @@
       <c r="F5">
         <v>19.836793984803499</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5">
+        <v>1.5483521235014E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -2581,8 +4147,14 @@
       <c r="F6">
         <v>3.7474811869904001</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6">
+        <v>5.4352434550192198E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -2598,8 +4170,14 @@
       <c r="F7">
         <v>24.874390430792602</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7">
+        <v>0.87535153401658305</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -2615,8 +4193,14 @@
       <c r="F8">
         <v>7.3070607871037101</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>177</v>
+      </c>
+      <c r="I8">
+        <v>3.6065856671560899E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -2626,8 +4210,14 @@
       <c r="D9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9">
+        <v>6.9964888408613</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>141</v>
       </c>
@@ -2637,8 +4227,14 @@
       <c r="D10" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>178</v>
+      </c>
+      <c r="I10">
+        <v>2.4640131284932101E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>142</v>
       </c>
@@ -2654,8 +4250,14 @@
       <c r="F11">
         <v>2.6879925817396901</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11">
+        <v>0.27829481169186299</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -2665,8 +4267,14 @@
       <c r="D12" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>141</v>
+      </c>
+      <c r="I12">
+        <v>2.2545346919701998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -2682,8 +4290,14 @@
       <c r="F13">
         <v>20.723261978467001</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>179</v>
+      </c>
+      <c r="I13">
+        <v>1.12488536843141E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -2693,8 +4307,14 @@
       <c r="D14" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>142</v>
+      </c>
+      <c r="I14">
+        <v>3.0895093372903398E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -2704,8 +4324,14 @@
       <c r="D15" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>180</v>
+      </c>
+      <c r="I15" s="10">
+        <v>2.1744747175046701E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -2715,8 +4341,14 @@
       <c r="D16" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>181</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -2726,14 +4358,26 @@
       <c r="D17" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>44</v>
+      </c>
+      <c r="I17">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="D18" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>45</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="D19" t="s">
         <v>21</v>
@@ -2744,21 +4388,164 @@
       <c r="F19">
         <v>19.593225065036101</v>
       </c>
-      <c r="H19" s="8"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>182</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>183</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>23</v>
       </c>
       <c r="G21" s="7"/>
+      <c r="H21" t="s">
+        <v>143</v>
+      </c>
+      <c r="I21">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I22">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>50</v>
+      </c>
+      <c r="I23">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>47</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="36.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="E3" s="5">
+        <v>4581156.7432856048</v>
+      </c>
+      <c r="F3" s="6">
+        <v>-22.38</v>
+      </c>
+      <c r="G3" s="7">
+        <v>20</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>170</v>
+      </c>
+      <c r="H4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
August 28 - Home
</commit_message>
<xml_diff>
--- a/KineticModel/ecoli_test.xlsx
+++ b/KineticModel/ecoli_test.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="540" windowWidth="18195" windowHeight="7065" activeTab="9"/>
   </bookViews>
@@ -20,7 +25,7 @@
     <sheet name="ecoliN2" sheetId="10" r:id="rId11"/>
     <sheet name="Sheet3" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -2720,7 +2725,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2755,7 +2760,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3350,7 +3355,7 @@
   <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="H35" sqref="H35:H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Start from scratch - September 24
</commit_message>
<xml_diff>
--- a/KineticModel/ecoli_test.xlsx
+++ b/KineticModel/ecoli_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="600" windowWidth="18195" windowHeight="7005" activeTab="9"/>
+    <workbookView xWindow="480" yWindow="660" windowWidth="18195" windowHeight="6945" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="ecoliT1" sheetId="1" r:id="rId1"/>
@@ -17,16 +17,19 @@
     <sheet name="ecoliT6" sheetId="7" r:id="rId8"/>
     <sheet name="Sheet2" sheetId="5" r:id="rId9"/>
     <sheet name="ecoliN1" sheetId="11" r:id="rId10"/>
-    <sheet name="ecoliN2" sheetId="10" r:id="rId11"/>
-    <sheet name="Sheet3" sheetId="12" r:id="rId12"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId11"/>
+    <sheet name="ecoliN2" sheetId="10" r:id="rId12"/>
+    <sheet name="Sheet3" sheetId="12" r:id="rId13"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId14"/>
+  </externalReferences>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1732" uniqueCount="813">
   <si>
     <t>Enzymes</t>
   </si>
@@ -2489,6 +2492,24 @@
   </si>
   <si>
     <t>[c] : h + nadh + oaa &lt;==&gt; mal + nad</t>
+  </si>
+  <si>
+    <t>EC</t>
+  </si>
+  <si>
+    <t>1.2.1.51</t>
+  </si>
+  <si>
+    <t>2.3.3.16</t>
+  </si>
+  <si>
+    <t>1.8.1.4</t>
+  </si>
+  <si>
+    <t>2.3.1.54</t>
+  </si>
+  <si>
+    <t>1.10.3.12</t>
   </si>
 </sst>
 </file>
@@ -2676,6 +2697,1511 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Ecoli_core_S"/>
+      <sheetName val="reactions"/>
+      <sheetName val="rxn max and min"/>
+      <sheetName val="metabolites"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>abbreviation</v>
+          </cell>
+          <cell r="B1" t="str">
+            <v xml:space="preserve"> officialName</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v xml:space="preserve"> equation</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v xml:space="preserve"> subSystem</v>
+          </cell>
+          <cell r="E1" t="str">
+            <v xml:space="preserve"> proteinClass</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>ACALD</v>
+          </cell>
+          <cell r="B2" t="str">
+            <v>acetaldehyde dehydrogenase (acetylating)</v>
+          </cell>
+          <cell r="C2" t="str">
+            <v>[c] : acald + coa + nad &lt;==&gt; accoa + h + nadh</v>
+          </cell>
+          <cell r="D2" t="str">
+            <v>Pyruvate Metabolism</v>
+          </cell>
+          <cell r="E2" t="str">
+            <v>1.2.1.10</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>ACALDt</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>acetaldehyde reversible transport</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>acald[e] &lt;==&gt; acald[c]</v>
+          </cell>
+          <cell r="D3" t="str">
+            <v>Transport, Extracellular</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>ACKr</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>acetate kinase</v>
+          </cell>
+          <cell r="C4" t="str">
+            <v>[c] : ac + atp &lt;==&gt; actp + adp</v>
+          </cell>
+          <cell r="D4" t="str">
+            <v>Pyruvate Metabolism</v>
+          </cell>
+          <cell r="E4" t="str">
+            <v>2.7.2.1</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>ACONTa</v>
+          </cell>
+          <cell r="B5" t="str">
+            <v>aconitase (half-reaction A, Citrate hydro-lyase)</v>
+          </cell>
+          <cell r="C5" t="str">
+            <v>[c] : cit &lt;==&gt; acon-C + h2o</v>
+          </cell>
+          <cell r="D5" t="str">
+            <v>Citric Acid Cycle</v>
+          </cell>
+          <cell r="E5" t="str">
+            <v>4.2.1.3</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>ACONTb</v>
+          </cell>
+          <cell r="B6" t="str">
+            <v>aconitase (half-reaction B, Isocitrate hydro-lyase)</v>
+          </cell>
+          <cell r="C6" t="str">
+            <v>[c] : acon-C + h2o &lt;==&gt; icit</v>
+          </cell>
+          <cell r="D6" t="str">
+            <v>Citric Acid Cycle</v>
+          </cell>
+          <cell r="E6" t="str">
+            <v>4.2.1.3</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>ACt2r</v>
+          </cell>
+          <cell r="B7" t="str">
+            <v>acetate reversible transport via proton symport</v>
+          </cell>
+          <cell r="C7" t="str">
+            <v>ac[e] + h[e] &lt;==&gt; ac[c] + h[c]</v>
+          </cell>
+          <cell r="D7" t="str">
+            <v>Transport, Extracellular</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>ADK1</v>
+          </cell>
+          <cell r="B8" t="str">
+            <v>adenylate kinase</v>
+          </cell>
+          <cell r="C8" t="str">
+            <v>[c] : amp + atp &lt;==&gt; (2) adp</v>
+          </cell>
+          <cell r="D8" t="str">
+            <v>Oxidative Phosphorylation</v>
+          </cell>
+          <cell r="E8" t="str">
+            <v>2.7.4.3</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>AKGDH</v>
+          </cell>
+          <cell r="B9" t="str">
+            <v>2-Oxogluterate dehydrogenase</v>
+          </cell>
+          <cell r="C9" t="str">
+            <v>[c] : akg + coa + nad --&gt; co2 + nadh + succoa</v>
+          </cell>
+          <cell r="D9" t="str">
+            <v>Citric Acid Cycle</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>AKGt2r</v>
+          </cell>
+          <cell r="B10" t="str">
+            <v>2-oxoglutarate reversible transport via symport</v>
+          </cell>
+          <cell r="C10" t="str">
+            <v>akg[e] + h[e] &lt;==&gt; akg[c] + h[c]</v>
+          </cell>
+          <cell r="D10" t="str">
+            <v>Transport, Extracellular</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>ALCD2x</v>
+          </cell>
+          <cell r="B11" t="str">
+            <v>alcohol dehydrogenase (ethanol)</v>
+          </cell>
+          <cell r="C11" t="str">
+            <v>[c] : etoh + nad &lt;==&gt; acald + h + nadh</v>
+          </cell>
+          <cell r="D11" t="str">
+            <v>Pyruvate Metabolism</v>
+          </cell>
+          <cell r="E11" t="str">
+            <v>1.1.1.1</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>ATPM</v>
+          </cell>
+          <cell r="B12" t="str">
+            <v>ATP maintenance requirement</v>
+          </cell>
+          <cell r="C12" t="str">
+            <v>[c] : atp + h2o --&gt; adp + h + pi</v>
+          </cell>
+          <cell r="D12" t="str">
+            <v>Oxidative Phosphorylation</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>ATPS4r</v>
+          </cell>
+          <cell r="B13" t="str">
+            <v>ATP synthase (four protons for one ATP)</v>
+          </cell>
+          <cell r="C13" t="str">
+            <v>adp[c] + (4) h[e] + pi[c] &lt;==&gt; atp[c] + (3) h[c] + h2o[c]</v>
+          </cell>
+          <cell r="D13" t="str">
+            <v>Oxidative Phosphorylation</v>
+          </cell>
+          <cell r="E13" t="str">
+            <v>3.6.3.14</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>Biomass_Ecoli_core_w/GAM</v>
+          </cell>
+          <cell r="B14" t="str">
+            <v>Biomass Objective Function with GAM</v>
+          </cell>
+          <cell r="C14" t="str">
+            <v>[c] : (1.496) 3pg + (3.7478) accoa + (59.8100) atp + (0.3610) e4p + (0.0709) f6p + (0.1290) g3p + (0.2050) g6p + (0.2557) gln-L + (4.9414) glu-L + (59.8100) h2o + (3.5470) nad + (13.0279) nadph + (1.7867) oaa + (0.5191) pep + (2.8328) pyr + (0.8977) r5p --&gt; (59.8100) adp + (4.1182) akg + (3.7478) coa + (59.8100) h + (3.5470) nadh + (13.0279) nadp + (59.8100) pi</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>CO2t</v>
+          </cell>
+          <cell r="B15" t="str">
+            <v>CO2 transporter via diffusion</v>
+          </cell>
+          <cell r="C15" t="str">
+            <v>co2[e] &lt;==&gt; co2[c]</v>
+          </cell>
+          <cell r="D15" t="str">
+            <v>Transport, Extracellular</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>CS</v>
+          </cell>
+          <cell r="B16" t="str">
+            <v>citrate synthase</v>
+          </cell>
+          <cell r="C16" t="str">
+            <v>[c] : accoa + h2o + oaa --&gt; cit + coa + h</v>
+          </cell>
+          <cell r="D16" t="str">
+            <v>Citric Acid Cycle</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>CYTBD</v>
+          </cell>
+          <cell r="B17" t="str">
+            <v>cytochrome oxidase bd (ubiquinol-8: 2 protons)</v>
+          </cell>
+          <cell r="C17" t="str">
+            <v>(2) h[c] + (0.5) o2[c] + q8h2[c] --&gt; (2) h[e] + h2o[c] + q8[c]</v>
+          </cell>
+          <cell r="D17" t="str">
+            <v>Oxidative Phosphorylation</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>D_LACt2</v>
+          </cell>
+          <cell r="B18" t="str">
+            <v>D-lactate transport via proton symport</v>
+          </cell>
+          <cell r="C18" t="str">
+            <v>h[e] + lac-D[e] &lt;==&gt; h[c] + lac-D[c]</v>
+          </cell>
+          <cell r="D18" t="str">
+            <v>Transport, Extracellular</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>ENO</v>
+          </cell>
+          <cell r="B19" t="str">
+            <v>enolase</v>
+          </cell>
+          <cell r="C19" t="str">
+            <v>[c] : 2pg &lt;==&gt; h2o + pep</v>
+          </cell>
+          <cell r="D19" t="str">
+            <v>Glycolysis/Gluconeogenesis</v>
+          </cell>
+          <cell r="E19" t="str">
+            <v>4.2.1.11</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>ETOHt2r</v>
+          </cell>
+          <cell r="B20" t="str">
+            <v>ethanol reversible transport via proton symport</v>
+          </cell>
+          <cell r="C20" t="str">
+            <v>etoh[e] + h[e] &lt;==&gt; etoh[c] + h[c]</v>
+          </cell>
+          <cell r="D20" t="str">
+            <v>Transport, Extracellular</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21" t="str">
+            <v>EX_ac(e)</v>
+          </cell>
+          <cell r="B21" t="str">
+            <v>Acetate exchange</v>
+          </cell>
+          <cell r="C21" t="str">
+            <v>[e] : ac &lt;==&gt;</v>
+          </cell>
+          <cell r="D21" t="str">
+            <v>Exchange</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22" t="str">
+            <v>EX_acald(e)</v>
+          </cell>
+          <cell r="B22" t="str">
+            <v>Acetaldehyde exchange</v>
+          </cell>
+          <cell r="C22" t="str">
+            <v>[e] : acald &lt;==&gt;</v>
+          </cell>
+          <cell r="D22" t="str">
+            <v>Exchange</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23" t="str">
+            <v>EX_akg(e)</v>
+          </cell>
+          <cell r="B23" t="str">
+            <v>2-Oxoglutarate exchange</v>
+          </cell>
+          <cell r="C23" t="str">
+            <v>[e] : akg &lt;==&gt;</v>
+          </cell>
+          <cell r="D23" t="str">
+            <v>Exchange</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24" t="str">
+            <v>EX_co2(e)</v>
+          </cell>
+          <cell r="B24" t="str">
+            <v>CO2 exchange</v>
+          </cell>
+          <cell r="C24" t="str">
+            <v>[e] : co2 &lt;==&gt;</v>
+          </cell>
+          <cell r="D24" t="str">
+            <v>Exchange</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25" t="str">
+            <v>EX_etoh(e)</v>
+          </cell>
+          <cell r="B25" t="str">
+            <v>Ethanol exchange</v>
+          </cell>
+          <cell r="C25" t="str">
+            <v>[e] : etoh &lt;==&gt;</v>
+          </cell>
+          <cell r="D25" t="str">
+            <v>Exchange</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26" t="str">
+            <v>EX_for(e)</v>
+          </cell>
+          <cell r="B26" t="str">
+            <v>Formate exchange</v>
+          </cell>
+          <cell r="C26" t="str">
+            <v>[e] : for &lt;==&gt;</v>
+          </cell>
+          <cell r="D26" t="str">
+            <v>Exchange</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27" t="str">
+            <v>EX_fru(e)</v>
+          </cell>
+          <cell r="B27" t="str">
+            <v>D-Fructose exchange</v>
+          </cell>
+          <cell r="C27" t="str">
+            <v>[e] : fru &lt;==&gt;</v>
+          </cell>
+          <cell r="D27" t="str">
+            <v>Exchange</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28" t="str">
+            <v>EX_fum(e)</v>
+          </cell>
+          <cell r="B28" t="str">
+            <v>Fumarate exchange</v>
+          </cell>
+          <cell r="C28" t="str">
+            <v>[e] : fum &lt;==&gt;</v>
+          </cell>
+          <cell r="D28" t="str">
+            <v>Exchange</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29" t="str">
+            <v>EX_glc(e)</v>
+          </cell>
+          <cell r="B29" t="str">
+            <v>D-Glucose exchange</v>
+          </cell>
+          <cell r="C29" t="str">
+            <v>[e] : glc-D &lt;==&gt;</v>
+          </cell>
+          <cell r="D29" t="str">
+            <v>Exchange</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30" t="str">
+            <v>EX_gln_L(e)</v>
+          </cell>
+          <cell r="B30" t="str">
+            <v>L-Glutamine exchange</v>
+          </cell>
+          <cell r="C30" t="str">
+            <v>[e] : gln-L &lt;==&gt;</v>
+          </cell>
+          <cell r="D30" t="str">
+            <v>Exchange</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31" t="str">
+            <v>EX_glu_L(e)</v>
+          </cell>
+          <cell r="B31" t="str">
+            <v>L-Glutamate exchange</v>
+          </cell>
+          <cell r="C31" t="str">
+            <v>[e] : glu-L &lt;==&gt;</v>
+          </cell>
+          <cell r="D31" t="str">
+            <v>Exchange</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32" t="str">
+            <v>EX_h(e)</v>
+          </cell>
+          <cell r="B32" t="str">
+            <v>H+ exchange</v>
+          </cell>
+          <cell r="C32" t="str">
+            <v>[e] : h &lt;==&gt;</v>
+          </cell>
+          <cell r="D32" t="str">
+            <v>Exchange</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33" t="str">
+            <v>EX_h2o(e)</v>
+          </cell>
+          <cell r="B33" t="str">
+            <v>H2O exchange</v>
+          </cell>
+          <cell r="C33" t="str">
+            <v>[e] : h2o &lt;==&gt;</v>
+          </cell>
+          <cell r="D33" t="str">
+            <v>Exchange</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34" t="str">
+            <v>EX_lac_D(e)</v>
+          </cell>
+          <cell r="B34" t="str">
+            <v>D-Lactate exchange</v>
+          </cell>
+          <cell r="C34" t="str">
+            <v>[e] : lac-D &lt;==&gt;</v>
+          </cell>
+          <cell r="D34" t="str">
+            <v>Exchange</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35" t="str">
+            <v>EX_mal_L(e)</v>
+          </cell>
+          <cell r="B35" t="str">
+            <v>L-Malate exchange</v>
+          </cell>
+          <cell r="C35" t="str">
+            <v>[e] : mal-L &lt;==&gt;</v>
+          </cell>
+          <cell r="D35" t="str">
+            <v>Exchange</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36" t="str">
+            <v>EX_nh4(e)</v>
+          </cell>
+          <cell r="B36" t="str">
+            <v>Ammonium exchange</v>
+          </cell>
+          <cell r="C36" t="str">
+            <v>[e] : nh4 &lt;==&gt;</v>
+          </cell>
+          <cell r="D36" t="str">
+            <v>Exchange</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37" t="str">
+            <v>EX_o2(e)</v>
+          </cell>
+          <cell r="B37" t="str">
+            <v>O2 exchange</v>
+          </cell>
+          <cell r="C37" t="str">
+            <v>[e] : o2 &lt;==&gt;</v>
+          </cell>
+          <cell r="D37" t="str">
+            <v>Exchange</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38" t="str">
+            <v>EX_pi(e)</v>
+          </cell>
+          <cell r="B38" t="str">
+            <v>Phosphate exchange</v>
+          </cell>
+          <cell r="C38" t="str">
+            <v>[e] : pi &lt;==&gt;</v>
+          </cell>
+          <cell r="D38" t="str">
+            <v>Exchange</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39" t="str">
+            <v>EX_pyr(e)</v>
+          </cell>
+          <cell r="B39" t="str">
+            <v>Pyruvate exchange</v>
+          </cell>
+          <cell r="C39" t="str">
+            <v>[e] : pyr &lt;==&gt;</v>
+          </cell>
+          <cell r="D39" t="str">
+            <v>Exchange</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40" t="str">
+            <v>EX_succ(e)</v>
+          </cell>
+          <cell r="B40" t="str">
+            <v>Succinate exchange</v>
+          </cell>
+          <cell r="C40" t="str">
+            <v>[e] : succ &lt;==&gt;</v>
+          </cell>
+          <cell r="D40" t="str">
+            <v>Exchange</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41" t="str">
+            <v>FBA</v>
+          </cell>
+          <cell r="B41" t="str">
+            <v>fructose-bisphosphate aldolase</v>
+          </cell>
+          <cell r="C41" t="str">
+            <v>[c] : fdp &lt;==&gt; dhap + g3p</v>
+          </cell>
+          <cell r="D41" t="str">
+            <v>Glycolysis/Gluconeogenesis</v>
+          </cell>
+          <cell r="E41" t="str">
+            <v>4.1.2.13</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42" t="str">
+            <v>FBP</v>
+          </cell>
+          <cell r="B42" t="str">
+            <v>fructose-bisphosphatase</v>
+          </cell>
+          <cell r="C42" t="str">
+            <v>[c] : fdp + h2o --&gt; f6p + pi</v>
+          </cell>
+          <cell r="D42" t="str">
+            <v>Glycolysis/Gluconeogenesis</v>
+          </cell>
+          <cell r="E42" t="str">
+            <v>3.1.3.11</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43" t="str">
+            <v>FORt2</v>
+          </cell>
+          <cell r="B43" t="str">
+            <v>formate transport via proton symport (uptake only)</v>
+          </cell>
+          <cell r="C43" t="str">
+            <v>for[e] + h[e] --&gt; for[c] + h[c]</v>
+          </cell>
+          <cell r="D43" t="str">
+            <v>Transport, Extracellular</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44" t="str">
+            <v>FORti</v>
+          </cell>
+          <cell r="B44" t="str">
+            <v>formate transport via diffusion</v>
+          </cell>
+          <cell r="C44" t="str">
+            <v>for[c] --&gt; for[e]</v>
+          </cell>
+          <cell r="D44" t="str">
+            <v>Transport, Extracellular</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45" t="str">
+            <v>FRD7</v>
+          </cell>
+          <cell r="B45" t="str">
+            <v>fumarate reductase</v>
+          </cell>
+          <cell r="C45" t="str">
+            <v>[c] : fum + q8h2 --&gt; q8 + succ</v>
+          </cell>
+          <cell r="D45" t="str">
+            <v>Oxidative Phosphorylation</v>
+          </cell>
+          <cell r="E45" t="str">
+            <v>1.3.99.1</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46" t="str">
+            <v>FRUpts2</v>
+          </cell>
+          <cell r="B46" t="str">
+            <v>Fructose transport via PEP:Pyr PTS (f6p generating)</v>
+          </cell>
+          <cell r="C46" t="str">
+            <v>fru[e] + pep[c] --&gt; f6p[c] + pyr[c]</v>
+          </cell>
+          <cell r="D46" t="str">
+            <v>Transport, Extracellular</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47" t="str">
+            <v>FUM</v>
+          </cell>
+          <cell r="B47" t="str">
+            <v>fumarase</v>
+          </cell>
+          <cell r="C47" t="str">
+            <v>[c] : fum + h2o &lt;==&gt; mal-L</v>
+          </cell>
+          <cell r="D47" t="str">
+            <v>Citric Acid Cycle</v>
+          </cell>
+          <cell r="E47" t="str">
+            <v>4.2.1.2</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48" t="str">
+            <v>FUMt2_2</v>
+          </cell>
+          <cell r="B48" t="str">
+            <v>Fumarate transport via proton symport (2 H)</v>
+          </cell>
+          <cell r="C48" t="str">
+            <v>fum[e] + (2) h[e] --&gt; fum[c] + (2) h[c]</v>
+          </cell>
+          <cell r="D48" t="str">
+            <v>Transport, Extracellular</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49" t="str">
+            <v>G6PDH2r</v>
+          </cell>
+          <cell r="B49" t="str">
+            <v>glucose 6-phosphate dehydrogenase</v>
+          </cell>
+          <cell r="C49" t="str">
+            <v>[c] : g6p + nadp &lt;==&gt; 6pgl + h + nadph</v>
+          </cell>
+          <cell r="D49" t="str">
+            <v>Pentose Phosphate Pathway</v>
+          </cell>
+          <cell r="E49" t="str">
+            <v>1.1.1.49</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50" t="str">
+            <v>GAPD</v>
+          </cell>
+          <cell r="B50" t="str">
+            <v>glyceraldehyde-3-phosphate dehydrogenase</v>
+          </cell>
+          <cell r="C50" t="str">
+            <v>[c] : g3p + nad + pi &lt;==&gt; 13dpg + h + nadh</v>
+          </cell>
+          <cell r="D50" t="str">
+            <v>Glycolysis/Gluconeogenesis</v>
+          </cell>
+          <cell r="E50" t="str">
+            <v>1.2.1.12</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51" t="str">
+            <v>GLCpts</v>
+          </cell>
+          <cell r="B51" t="str">
+            <v>D-glucose transport via PEP:Pyr PTS</v>
+          </cell>
+          <cell r="C51" t="str">
+            <v>glc-D[e] + pep[c] --&gt; g6p[c] + pyr[c]</v>
+          </cell>
+          <cell r="D51" t="str">
+            <v>Transport, Extracellular</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="A52" t="str">
+            <v>GLNS</v>
+          </cell>
+          <cell r="B52" t="str">
+            <v>glutamine synthetase</v>
+          </cell>
+          <cell r="C52" t="str">
+            <v>[c] : atp + glu-L + nh4 --&gt; adp + gln-L + h + pi</v>
+          </cell>
+          <cell r="D52" t="str">
+            <v>Glutamate Metabolism</v>
+          </cell>
+          <cell r="E52" t="str">
+            <v>6.3.1.2</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="A53" t="str">
+            <v>GLNabc</v>
+          </cell>
+          <cell r="B53" t="str">
+            <v>L-glutamine transport via ABC system</v>
+          </cell>
+          <cell r="C53" t="str">
+            <v>atp[c] + gln-L[e] + h2o[c] --&gt; adp[c] + gln-L[c] + h[c] + pi[c]</v>
+          </cell>
+          <cell r="D53" t="str">
+            <v>Transport, Extracellular</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="A54" t="str">
+            <v>GLUDy</v>
+          </cell>
+          <cell r="B54" t="str">
+            <v>glutamate dehydrogenase (NADP)</v>
+          </cell>
+          <cell r="C54" t="str">
+            <v>[c] : glu-L + h2o + nadp &lt;==&gt; akg + h + nadph + nh4</v>
+          </cell>
+          <cell r="D54" t="str">
+            <v>Glutamate Metabolism</v>
+          </cell>
+          <cell r="E54" t="str">
+            <v>1.4.1.4</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="A55" t="str">
+            <v>GLUN</v>
+          </cell>
+          <cell r="B55" t="str">
+            <v>glutaminase</v>
+          </cell>
+          <cell r="C55" t="str">
+            <v>[c] : gln-L + h2o --&gt; glu-L + nh4</v>
+          </cell>
+          <cell r="D55" t="str">
+            <v>Glutamate Metabolism</v>
+          </cell>
+          <cell r="E55" t="str">
+            <v>3.5.1.2</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="A56" t="str">
+            <v>GLUSy</v>
+          </cell>
+          <cell r="B56" t="str">
+            <v>glutamate synthase (NADPH)</v>
+          </cell>
+          <cell r="C56" t="str">
+            <v>[c] : akg + gln-L + h + nadph --&gt; (2) glu-L + nadp</v>
+          </cell>
+          <cell r="D56" t="str">
+            <v>Glutamate Metabolism</v>
+          </cell>
+          <cell r="E56" t="str">
+            <v>1.4.1.13</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="A57" t="str">
+            <v>GLUt2r</v>
+          </cell>
+          <cell r="B57" t="str">
+            <v>L-glutamate transport via proton symport, reversible (periplasm)</v>
+          </cell>
+          <cell r="C57" t="str">
+            <v>glu-L[e] + h[e] &lt;==&gt; glu-L[c] + h[c]</v>
+          </cell>
+          <cell r="D57" t="str">
+            <v>Transport, Extracellular</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="A58" t="str">
+            <v>GND</v>
+          </cell>
+          <cell r="B58" t="str">
+            <v>phosphogluconate dehydrogenase</v>
+          </cell>
+          <cell r="C58" t="str">
+            <v>[c] : 6pgc + nadp --&gt; co2 + nadph + ru5p-D</v>
+          </cell>
+          <cell r="D58" t="str">
+            <v>Pentose Phosphate Pathway</v>
+          </cell>
+          <cell r="E58" t="str">
+            <v>1.1.1.44</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="A59" t="str">
+            <v>H2Ot</v>
+          </cell>
+          <cell r="B59" t="str">
+            <v>H2O transport via diffusion</v>
+          </cell>
+          <cell r="C59" t="str">
+            <v>h2o[e] &lt;==&gt; h2o[c]</v>
+          </cell>
+          <cell r="D59" t="str">
+            <v>Transport, Extracellular</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="A60" t="str">
+            <v>ICDHyr</v>
+          </cell>
+          <cell r="B60" t="str">
+            <v>isocitrate dehydrogenase (NADP)</v>
+          </cell>
+          <cell r="C60" t="str">
+            <v>[c] : icit + nadp &lt;==&gt; akg + co2 + nadph</v>
+          </cell>
+          <cell r="D60" t="str">
+            <v>Citric Acid Cycle</v>
+          </cell>
+          <cell r="E60" t="str">
+            <v>1.1.1.42</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="A61" t="str">
+            <v>ICL</v>
+          </cell>
+          <cell r="B61" t="str">
+            <v>Isocitrate lyase</v>
+          </cell>
+          <cell r="C61" t="str">
+            <v>[c] : icit --&gt; glx + succ</v>
+          </cell>
+          <cell r="D61" t="str">
+            <v>Anaplerotic reactions</v>
+          </cell>
+          <cell r="E61" t="str">
+            <v>4.1.3.1</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="A62" t="str">
+            <v>LDH_D</v>
+          </cell>
+          <cell r="B62" t="str">
+            <v>D-lactate dehydrogenase</v>
+          </cell>
+          <cell r="C62" t="str">
+            <v>[c] : lac-D + nad &lt;==&gt; h + nadh + pyr</v>
+          </cell>
+          <cell r="D62" t="str">
+            <v>Pyruvate Metabolism</v>
+          </cell>
+          <cell r="E62" t="str">
+            <v>1.1.1.28</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="A63" t="str">
+            <v>MALS</v>
+          </cell>
+          <cell r="B63" t="str">
+            <v>malate synthase</v>
+          </cell>
+          <cell r="C63" t="str">
+            <v>[c] : accoa + glx + h2o --&gt; coa + h + mal-L</v>
+          </cell>
+          <cell r="D63" t="str">
+            <v>Anaplerotic reactions</v>
+          </cell>
+          <cell r="E63" t="str">
+            <v>4.1.3.2</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="A64" t="str">
+            <v>MALt2_2</v>
+          </cell>
+          <cell r="B64" t="str">
+            <v>Malate transport via proton symport (2 H)</v>
+          </cell>
+          <cell r="C64" t="str">
+            <v>(2) h[e] + mal-L[e] --&gt; (2) h[c] + mal-L[c]</v>
+          </cell>
+          <cell r="D64" t="str">
+            <v>Transport, Extracellular</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="A65" t="str">
+            <v>MDH</v>
+          </cell>
+          <cell r="B65" t="str">
+            <v>malate dehydrogenase</v>
+          </cell>
+          <cell r="C65" t="str">
+            <v>[c] : mal-L + nad &lt;==&gt; h + nadh + oaa</v>
+          </cell>
+          <cell r="D65" t="str">
+            <v>Citric Acid Cycle</v>
+          </cell>
+          <cell r="E65" t="str">
+            <v>1.1.1.37</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="A66" t="str">
+            <v>ME1</v>
+          </cell>
+          <cell r="B66" t="str">
+            <v>malic enzyme (NAD)</v>
+          </cell>
+          <cell r="C66" t="str">
+            <v>[c] : mal-L + nad --&gt; co2 + nadh + pyr</v>
+          </cell>
+          <cell r="D66" t="str">
+            <v>Anaplerotic reactions</v>
+          </cell>
+          <cell r="E66" t="str">
+            <v>1.1.1.38</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="A67" t="str">
+            <v>ME2</v>
+          </cell>
+          <cell r="B67" t="str">
+            <v>malic enzyme (NADP)</v>
+          </cell>
+          <cell r="C67" t="str">
+            <v>[c] : mal-L + nadp --&gt; co2 + nadph + pyr</v>
+          </cell>
+          <cell r="D67" t="str">
+            <v>Anaplerotic reactions</v>
+          </cell>
+          <cell r="E67" t="str">
+            <v>1.1.1.40</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="A68" t="str">
+            <v>NADH16</v>
+          </cell>
+          <cell r="B68" t="str">
+            <v>NADH dehydrogenase (ubiquinone-8 &amp; 3 protons)</v>
+          </cell>
+          <cell r="C68" t="str">
+            <v>(4) h[c] + nadh[c] + q8[c] --&gt; (3) h[e] + nad[c] + q8h2[c]</v>
+          </cell>
+          <cell r="D68" t="str">
+            <v>Oxidative Phosphorylation</v>
+          </cell>
+          <cell r="E68" t="str">
+            <v>1.6.5.3</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="A69" t="str">
+            <v>NADTRHD</v>
+          </cell>
+          <cell r="B69" t="str">
+            <v>NAD transhydrogenase</v>
+          </cell>
+          <cell r="C69" t="str">
+            <v>[c] : nad + nadph --&gt; nadh + nadp</v>
+          </cell>
+          <cell r="D69" t="str">
+            <v>Oxidative Phosphorylation</v>
+          </cell>
+          <cell r="E69" t="str">
+            <v>1.6.1.2</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="A70" t="str">
+            <v>NH4t</v>
+          </cell>
+          <cell r="B70" t="str">
+            <v>ammonia reversible transport</v>
+          </cell>
+          <cell r="C70" t="str">
+            <v>nh4[e] &lt;==&gt; nh4[c]</v>
+          </cell>
+          <cell r="D70" t="str">
+            <v>Inorganic Ion Transport and Metabolism</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="A71" t="str">
+            <v>O2t</v>
+          </cell>
+          <cell r="B71" t="str">
+            <v>o2 transport via diffusion</v>
+          </cell>
+          <cell r="C71" t="str">
+            <v>o2[e] &lt;==&gt; o2[c]</v>
+          </cell>
+          <cell r="D71" t="str">
+            <v>Transport, Extracellular</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="A72" t="str">
+            <v>PDH</v>
+          </cell>
+          <cell r="B72" t="str">
+            <v>pyruvate dehydrogenase</v>
+          </cell>
+          <cell r="C72" t="str">
+            <v>[c] : coa + nad + pyr --&gt; accoa + co2 + nadh</v>
+          </cell>
+          <cell r="D72" t="str">
+            <v>Glycolysis/Gluconeogenesis</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="A73" t="str">
+            <v>PFK</v>
+          </cell>
+          <cell r="B73" t="str">
+            <v>phosphofructokinase</v>
+          </cell>
+          <cell r="C73" t="str">
+            <v>[c] : atp + f6p --&gt; adp + fdp + h</v>
+          </cell>
+          <cell r="D73" t="str">
+            <v>Glycolysis/Gluconeogenesis</v>
+          </cell>
+          <cell r="E73" t="str">
+            <v>2.7.1.11</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="A74" t="str">
+            <v>PFL</v>
+          </cell>
+          <cell r="B74" t="str">
+            <v>pyruvate formate lyase</v>
+          </cell>
+          <cell r="C74" t="str">
+            <v>[c] : coa + pyr --&gt; accoa + for</v>
+          </cell>
+          <cell r="D74" t="str">
+            <v>Pyruvate Metabolism</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="A75" t="str">
+            <v>PGI</v>
+          </cell>
+          <cell r="B75" t="str">
+            <v>glucose-6-phosphate isomerase</v>
+          </cell>
+          <cell r="C75" t="str">
+            <v>[c] : g6p &lt;==&gt; f6p</v>
+          </cell>
+          <cell r="D75" t="str">
+            <v>Glycolysis/Gluconeogenesis</v>
+          </cell>
+          <cell r="E75" t="str">
+            <v>5.3.1.9</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="A76" t="str">
+            <v>PGK</v>
+          </cell>
+          <cell r="B76" t="str">
+            <v>phosphoglycerate kinase</v>
+          </cell>
+          <cell r="C76" t="str">
+            <v>[c] : 3pg + atp &lt;==&gt; 13dpg + adp</v>
+          </cell>
+          <cell r="D76" t="str">
+            <v>Glycolysis/Gluconeogenesis</v>
+          </cell>
+          <cell r="E76" t="str">
+            <v>2.7.2.3</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="A77" t="str">
+            <v>PGL</v>
+          </cell>
+          <cell r="B77" t="str">
+            <v>6-phosphogluconolactonase</v>
+          </cell>
+          <cell r="C77" t="str">
+            <v>[c] : 6pgl + h2o --&gt; 6pgc + h</v>
+          </cell>
+          <cell r="D77" t="str">
+            <v>Pentose Phosphate Pathway</v>
+          </cell>
+          <cell r="E77" t="str">
+            <v>3.1.1.31</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="A78" t="str">
+            <v>PGM</v>
+          </cell>
+          <cell r="B78" t="str">
+            <v>phosphoglycerate mutase</v>
+          </cell>
+          <cell r="C78" t="str">
+            <v>[c] : 2pg &lt;==&gt; 3pg</v>
+          </cell>
+          <cell r="D78" t="str">
+            <v>Glycolysis/Gluconeogenesis</v>
+          </cell>
+          <cell r="E78" t="str">
+            <v>5.4.2.1</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="A79" t="str">
+            <v>PIt2r</v>
+          </cell>
+          <cell r="B79" t="str">
+            <v>phosphate reversible transport via proton symport</v>
+          </cell>
+          <cell r="C79" t="str">
+            <v>h[e] + pi[e] &lt;==&gt; h[c] + pi[c]</v>
+          </cell>
+          <cell r="D79" t="str">
+            <v>Inorganic Ion Transport and Metabolism</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="A80" t="str">
+            <v>PPC</v>
+          </cell>
+          <cell r="B80" t="str">
+            <v>phosphoenolpyruvate carboxylase</v>
+          </cell>
+          <cell r="C80" t="str">
+            <v>[c] : co2 + h2o + pep --&gt; h + oaa + pi</v>
+          </cell>
+          <cell r="D80" t="str">
+            <v>Anaplerotic reactions</v>
+          </cell>
+          <cell r="E80" t="str">
+            <v>4.1.1.31</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="A81" t="str">
+            <v>PPCK</v>
+          </cell>
+          <cell r="B81" t="str">
+            <v>phosphoenolpyruvate carboxykinase</v>
+          </cell>
+          <cell r="C81" t="str">
+            <v>[c] : atp + oaa --&gt; adp + co2 + pep</v>
+          </cell>
+          <cell r="D81" t="str">
+            <v>Anaplerotic reactions</v>
+          </cell>
+          <cell r="E81" t="str">
+            <v>4.1.1.49</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="A82" t="str">
+            <v>PPS</v>
+          </cell>
+          <cell r="B82" t="str">
+            <v>phosphoenolpyruvate synthase</v>
+          </cell>
+          <cell r="C82" t="str">
+            <v>[c] : atp + h2o + pyr --&gt; amp + (2) h + pep + pi</v>
+          </cell>
+          <cell r="D82" t="str">
+            <v>Glycolysis/Gluconeogenesis</v>
+          </cell>
+          <cell r="E82" t="str">
+            <v>2.7.9.2</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="A83" t="str">
+            <v>PTAr</v>
+          </cell>
+          <cell r="B83" t="str">
+            <v>phosphotransacetylase</v>
+          </cell>
+          <cell r="C83" t="str">
+            <v>[c] : accoa + pi &lt;==&gt; actp + coa</v>
+          </cell>
+          <cell r="D83" t="str">
+            <v>Pyruvate Metabolism</v>
+          </cell>
+          <cell r="E83" t="str">
+            <v>2.3.1.8</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="A84" t="str">
+            <v>PYK</v>
+          </cell>
+          <cell r="B84" t="str">
+            <v>pyruvate kinase</v>
+          </cell>
+          <cell r="C84" t="str">
+            <v>[c] : adp + h + pep --&gt; atp + pyr</v>
+          </cell>
+          <cell r="D84" t="str">
+            <v>Glycolysis/Gluconeogenesis</v>
+          </cell>
+          <cell r="E84" t="str">
+            <v>2.7.1.40</v>
+          </cell>
+        </row>
+        <row r="85">
+          <cell r="A85" t="str">
+            <v>PYRt2r</v>
+          </cell>
+          <cell r="B85" t="str">
+            <v>pyruvate reversible transport via proton symport</v>
+          </cell>
+          <cell r="C85" t="str">
+            <v>h[e] + pyr[e] &lt;==&gt; h[c] + pyr[c]</v>
+          </cell>
+          <cell r="D85" t="str">
+            <v>Transport, Extracellular</v>
+          </cell>
+        </row>
+        <row r="86">
+          <cell r="A86" t="str">
+            <v>RPE</v>
+          </cell>
+          <cell r="B86" t="str">
+            <v>ribulose 5-phosphate 3-epimerase</v>
+          </cell>
+          <cell r="C86" t="str">
+            <v>[c] : ru5p-D &lt;==&gt; xu5p-D</v>
+          </cell>
+          <cell r="D86" t="str">
+            <v>Pentose Phosphate Pathway</v>
+          </cell>
+          <cell r="E86" t="str">
+            <v>5.1.3.1</v>
+          </cell>
+        </row>
+        <row r="87">
+          <cell r="A87" t="str">
+            <v>RPI</v>
+          </cell>
+          <cell r="B87" t="str">
+            <v>ribose-5-phosphate isomerase</v>
+          </cell>
+          <cell r="C87" t="str">
+            <v>[c] : r5p &lt;==&gt; ru5p-D</v>
+          </cell>
+          <cell r="D87" t="str">
+            <v>Pentose Phosphate Pathway</v>
+          </cell>
+          <cell r="E87" t="str">
+            <v>5.3.1.6</v>
+          </cell>
+        </row>
+        <row r="88">
+          <cell r="A88" t="str">
+            <v>SUCCt2_2</v>
+          </cell>
+          <cell r="B88" t="str">
+            <v>succinate transport via proton symport (2 H)</v>
+          </cell>
+          <cell r="C88" t="str">
+            <v>(2) h[e] + succ[e] --&gt; (2) h[c] + succ[c]</v>
+          </cell>
+          <cell r="D88" t="str">
+            <v>Transport, Extracellular</v>
+          </cell>
+        </row>
+        <row r="89">
+          <cell r="A89" t="str">
+            <v>SUCCt3</v>
+          </cell>
+          <cell r="B89" t="str">
+            <v>succinate transport out via proton antiport</v>
+          </cell>
+          <cell r="C89" t="str">
+            <v>h[e] + succ[c] --&gt; h[c] + succ[e]</v>
+          </cell>
+          <cell r="D89" t="str">
+            <v>Transport, Extracellular</v>
+          </cell>
+        </row>
+        <row r="90">
+          <cell r="A90" t="str">
+            <v>SUCDi</v>
+          </cell>
+          <cell r="B90" t="str">
+            <v>succinate dehydrogenase (irreversible)</v>
+          </cell>
+          <cell r="C90" t="str">
+            <v>[c] : q8 + succ --&gt; fum + q8h2</v>
+          </cell>
+          <cell r="D90" t="str">
+            <v>Oxidative Phosphorylation</v>
+          </cell>
+          <cell r="E90" t="str">
+            <v>1.3.99.1</v>
+          </cell>
+        </row>
+        <row r="91">
+          <cell r="A91" t="str">
+            <v>SUCOAS</v>
+          </cell>
+          <cell r="B91" t="str">
+            <v>succinyl-CoA synthetase (ADP-forming)</v>
+          </cell>
+          <cell r="C91" t="str">
+            <v>[c] : atp + coa + succ &lt;==&gt; adp + pi + succoa</v>
+          </cell>
+          <cell r="D91" t="str">
+            <v>Citric Acid Cycle</v>
+          </cell>
+          <cell r="E91" t="str">
+            <v>6.2.1.5</v>
+          </cell>
+        </row>
+        <row r="92">
+          <cell r="A92" t="str">
+            <v>TALA</v>
+          </cell>
+          <cell r="B92" t="str">
+            <v>transaldolase</v>
+          </cell>
+          <cell r="C92" t="str">
+            <v>[c] : g3p + s7p &lt;==&gt; e4p + f6p</v>
+          </cell>
+          <cell r="D92" t="str">
+            <v>Pentose Phosphate Pathway</v>
+          </cell>
+          <cell r="E92" t="str">
+            <v>2.2.1.2</v>
+          </cell>
+        </row>
+        <row r="93">
+          <cell r="A93" t="str">
+            <v>THD2</v>
+          </cell>
+          <cell r="B93" t="str">
+            <v>NAD(P) transhydrogenase</v>
+          </cell>
+          <cell r="C93" t="str">
+            <v>(2) h[e] + nadh[c] + nadp[c] --&gt; (2) h[c] + nad[c] + nadph[c]</v>
+          </cell>
+          <cell r="D93" t="str">
+            <v>Oxidative Phosphorylation</v>
+          </cell>
+          <cell r="E93" t="str">
+            <v>1.6.1.1</v>
+          </cell>
+        </row>
+        <row r="94">
+          <cell r="A94" t="str">
+            <v>TKT1</v>
+          </cell>
+          <cell r="B94" t="str">
+            <v>transketolase</v>
+          </cell>
+          <cell r="C94" t="str">
+            <v>[c] : r5p + xu5p-D &lt;==&gt; g3p + s7p</v>
+          </cell>
+          <cell r="D94" t="str">
+            <v>Pentose Phosphate Pathway</v>
+          </cell>
+          <cell r="E94" t="str">
+            <v>2.2.1.1</v>
+          </cell>
+        </row>
+        <row r="95">
+          <cell r="A95" t="str">
+            <v>TKT2</v>
+          </cell>
+          <cell r="B95" t="str">
+            <v>transketolase</v>
+          </cell>
+          <cell r="C95" t="str">
+            <v>[c] : e4p + xu5p-D &lt;==&gt; f6p + g3p</v>
+          </cell>
+          <cell r="D95" t="str">
+            <v>Pentose Phosphate Pathway</v>
+          </cell>
+          <cell r="E95" t="str">
+            <v>2.2.1.1</v>
+          </cell>
+        </row>
+        <row r="96">
+          <cell r="A96" t="str">
+            <v>TPI</v>
+          </cell>
+          <cell r="B96" t="str">
+            <v>triose-phosphate isomerase</v>
+          </cell>
+          <cell r="C96" t="str">
+            <v>[c] : dhap &lt;==&gt; g3p</v>
+          </cell>
+          <cell r="D96" t="str">
+            <v>Glycolysis/Gluconeogenesis</v>
+          </cell>
+          <cell r="E96" t="str">
+            <v>5.3.1.1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3350,8 +4876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5208,6 +6734,2674 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P83"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="6.5703125" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="41.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="73" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="73" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="79" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="73" t="s">
+        <v>807</v>
+      </c>
+      <c r="J1" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="73" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="73" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="73" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="73" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="77" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="73"/>
+      <c r="C2" s="11">
+        <v>250</v>
+      </c>
+      <c r="D2" s="73">
+        <v>1</v>
+      </c>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73">
+        <f>VLOOKUP(A2,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-9.1</v>
+      </c>
+      <c r="G2" s="73">
+        <v>20</v>
+      </c>
+      <c r="H2" s="77" t="s">
+        <v>303</v>
+      </c>
+      <c r="I2" s="77">
+        <f>VLOOKUP(A2,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="73">
+        <v>5.5599999999999997E-2</v>
+      </c>
+      <c r="P2" s="73">
+        <v>5.5599999999999997E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="77" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73">
+        <v>11.09</v>
+      </c>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73">
+        <f>VLOOKUP(A3,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-0.8</v>
+      </c>
+      <c r="G3" s="73">
+        <v>19.801039425479001</v>
+      </c>
+      <c r="H3" s="77" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="77" t="str">
+        <f>VLOOKUP(A3,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.3.1.9</v>
+      </c>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="73">
+        <v>3.48</v>
+      </c>
+      <c r="P3" s="73">
+        <v>3.48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="77" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73">
+        <v>49</v>
+      </c>
+      <c r="D4" s="73">
+        <v>2.7690000000000001</v>
+      </c>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73">
+        <f>VLOOKUP(A4,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-3.8</v>
+      </c>
+      <c r="G4" s="73">
+        <v>19.0346044708484</v>
+      </c>
+      <c r="H4" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="77" t="str">
+        <f>VLOOKUP(A4,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.1.11</v>
+      </c>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" s="73">
+        <v>0.6</v>
+      </c>
+      <c r="P4" s="73">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="77" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73">
+        <v>22</v>
+      </c>
+      <c r="D5" s="73">
+        <v>0</v>
+      </c>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73">
+        <f>VLOOKUP(A5,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-2.8</v>
+      </c>
+      <c r="G5" s="73">
+        <v>0</v>
+      </c>
+      <c r="H5" s="77" t="s">
+        <v>293</v>
+      </c>
+      <c r="I5" s="77" t="str">
+        <f>VLOOKUP(A5,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>3.1.3.11</v>
+      </c>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="73" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" s="73">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="P5" s="73">
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="77" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73">
+        <v>8.5</v>
+      </c>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73">
+        <f>VLOOKUP(A6,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>4.2</v>
+      </c>
+      <c r="G6" s="73">
+        <v>19.0346044708484</v>
+      </c>
+      <c r="H6" s="77" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6" s="77" t="str">
+        <f>VLOOKUP(A6,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.1.2.13</v>
+      </c>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
+      <c r="L6" s="73"/>
+      <c r="M6" s="73"/>
+      <c r="N6" s="73" t="s">
+        <v>796</v>
+      </c>
+      <c r="O6" s="73">
+        <v>0.218</v>
+      </c>
+      <c r="P6" s="73">
+        <v>0.218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="77" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73">
+        <v>56.87</v>
+      </c>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73">
+        <v>1.4</v>
+      </c>
+      <c r="G7" s="78">
+        <v>19.0346044708484</v>
+      </c>
+      <c r="H7" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="I7" s="77" t="str">
+        <f>VLOOKUP(A7,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.3.1.1</v>
+      </c>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="O7" s="73">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="P7" s="73">
+        <v>0.16700000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="77" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73">
+        <v>671.72</v>
+      </c>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73">
+        <f>VLOOKUP(A8,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="G8" s="73">
+        <v>37.420015145125497</v>
+      </c>
+      <c r="H8" s="77" t="s">
+        <v>297</v>
+      </c>
+      <c r="I8" s="77" t="str">
+        <f>VLOOKUP(A8,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.2.1.12</v>
+      </c>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
+      <c r="M8" s="73"/>
+      <c r="N8" s="73" t="s">
+        <v>187</v>
+      </c>
+      <c r="O8" s="73">
+        <v>2.13</v>
+      </c>
+      <c r="P8" s="73">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="77" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73">
+        <v>2225</v>
+      </c>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73">
+        <v>-2.8</v>
+      </c>
+      <c r="G9" s="73">
+        <v>37.420015145125497</v>
+      </c>
+      <c r="H9" s="77" t="s">
+        <v>795</v>
+      </c>
+      <c r="I9" s="77" t="str">
+        <f>VLOOKUP(A9,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.2.3</v>
+      </c>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="73"/>
+      <c r="N9" s="73" t="s">
+        <v>194</v>
+      </c>
+      <c r="O9" s="73">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="P9" s="73">
+        <v>0.39900000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="77" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73">
+        <v>90.55</v>
+      </c>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73">
+        <f>VLOOKUP(A10,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="73">
+        <v>35.968088220815801</v>
+      </c>
+      <c r="H10" s="77" t="s">
+        <v>131</v>
+      </c>
+      <c r="I10" s="77" t="str">
+        <f>VLOOKUP(A10,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.4.2.1</v>
+      </c>
+      <c r="J10" s="73"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="73"/>
+      <c r="N10" s="73" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="73">
+        <v>2.67</v>
+      </c>
+      <c r="P10" s="73">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="77" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" s="73"/>
+      <c r="C11" s="73">
+        <v>355.79</v>
+      </c>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73">
+        <f>VLOOKUP(A11,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-0.9</v>
+      </c>
+      <c r="G11" s="73">
+        <v>35.968088220815801</v>
+      </c>
+      <c r="H11" s="77" t="s">
+        <v>302</v>
+      </c>
+      <c r="I11" s="77" t="str">
+        <f>VLOOKUP(A11,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.2.1.11</v>
+      </c>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
+      <c r="M11" s="73"/>
+      <c r="N11" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="O11" s="73">
+        <v>2.67</v>
+      </c>
+      <c r="P11" s="73">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73">
+        <v>10.17</v>
+      </c>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="73">
+        <f>VLOOKUP(A12,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-5.3</v>
+      </c>
+      <c r="G12" s="73">
+        <v>15.464281224553</v>
+      </c>
+      <c r="H12" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="77" t="str">
+        <f>VLOOKUP(A12,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.1.40</v>
+      </c>
+      <c r="J12" s="73"/>
+      <c r="K12" s="73"/>
+      <c r="L12" s="73"/>
+      <c r="M12" s="73"/>
+      <c r="N12" s="73" t="s">
+        <v>797</v>
+      </c>
+      <c r="O12" s="73">
+        <v>0.111</v>
+      </c>
+      <c r="P12" s="73">
+        <v>0.111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="77" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73">
+        <v>0</v>
+      </c>
+      <c r="D13" s="73">
+        <v>0</v>
+      </c>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73">
+        <f>VLOOKUP(A13,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-1.2</v>
+      </c>
+      <c r="G13" s="73">
+        <v>0</v>
+      </c>
+      <c r="H13" s="77" t="s">
+        <v>135</v>
+      </c>
+      <c r="I13" s="77" t="str">
+        <f>VLOOKUP(A13,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.9.2</v>
+      </c>
+      <c r="J13" s="73"/>
+      <c r="K13" s="73"/>
+      <c r="L13" s="73"/>
+      <c r="M13" s="73"/>
+      <c r="N13" s="73" t="s">
+        <v>798</v>
+      </c>
+      <c r="O13" s="73">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="P13" s="73">
+        <v>0.13800000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="77" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" s="73"/>
+      <c r="C14" s="73">
+        <v>6.32</v>
+      </c>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73">
+        <f>VLOOKUP(A14,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-8.3000000000000007</v>
+      </c>
+      <c r="G14" s="73">
+        <v>0</v>
+      </c>
+      <c r="H14" s="77" t="s">
+        <v>139</v>
+      </c>
+      <c r="I14" s="77" t="s">
+        <v>808</v>
+      </c>
+      <c r="J14" s="73"/>
+      <c r="K14" s="73"/>
+      <c r="L14" s="73"/>
+      <c r="M14" s="73"/>
+      <c r="N14" s="73" t="s">
+        <v>799</v>
+      </c>
+      <c r="O14" s="73">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="P14" s="73">
+        <v>0.27600000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="77" t="s">
+        <v>239</v>
+      </c>
+      <c r="B15" s="73"/>
+      <c r="C15" s="73">
+        <v>81</v>
+      </c>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73">
+        <f>VLOOKUP(A15,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-8.6</v>
+      </c>
+      <c r="G15" s="73">
+        <v>0</v>
+      </c>
+      <c r="H15" s="77" t="s">
+        <v>238</v>
+      </c>
+      <c r="I15" s="77" t="s">
+        <v>809</v>
+      </c>
+      <c r="J15" s="73"/>
+      <c r="K15" s="73"/>
+      <c r="L15" s="73"/>
+      <c r="M15" s="73"/>
+      <c r="N15" s="73" t="s">
+        <v>800</v>
+      </c>
+      <c r="O15" s="73">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="P15" s="73">
+        <v>0.39800000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="78" t="s">
+        <v>317</v>
+      </c>
+      <c r="B16" s="73"/>
+      <c r="C16" s="73">
+        <v>5.3</v>
+      </c>
+      <c r="D16" s="73"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="73">
+        <f>VLOOKUP(A16,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>1.5</v>
+      </c>
+      <c r="G16" s="73">
+        <v>0</v>
+      </c>
+      <c r="H16" s="78" t="s">
+        <v>240</v>
+      </c>
+      <c r="I16" s="77" t="str">
+        <f>VLOOKUP(A16,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.2.1.3</v>
+      </c>
+      <c r="J16" s="73"/>
+      <c r="K16" s="73"/>
+      <c r="L16" s="73"/>
+      <c r="M16" s="73"/>
+      <c r="N16" s="73" t="s">
+        <v>801</v>
+      </c>
+      <c r="O16" s="73">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="P16" s="73">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="77" t="s">
+        <v>323</v>
+      </c>
+      <c r="B17" s="73"/>
+      <c r="C17" s="73">
+        <v>106.4</v>
+      </c>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73">
+        <f>VLOOKUP(A17,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>3.4</v>
+      </c>
+      <c r="G17" s="73">
+        <v>0</v>
+      </c>
+      <c r="H17" s="77" t="s">
+        <v>242</v>
+      </c>
+      <c r="I17" s="77" t="str">
+        <f>VLOOKUP(A17,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.1.1.42</v>
+      </c>
+      <c r="J17" s="73"/>
+      <c r="K17" s="73"/>
+      <c r="L17" s="73"/>
+      <c r="M17" s="73"/>
+      <c r="N17" s="73" t="s">
+        <v>195</v>
+      </c>
+      <c r="O17" s="73">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="P17" s="73">
+        <v>0.95499999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="77" t="s">
+        <v>325</v>
+      </c>
+      <c r="B18" s="73"/>
+      <c r="C18" s="73">
+        <v>5.2</v>
+      </c>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73">
+        <f>VLOOKUP(A18,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G18" s="73">
+        <v>0</v>
+      </c>
+      <c r="H18" s="77" t="s">
+        <v>327</v>
+      </c>
+      <c r="I18" s="77" t="str">
+        <f>VLOOKUP(A18,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.1.3.1</v>
+      </c>
+      <c r="J18" s="73"/>
+      <c r="K18" s="73"/>
+      <c r="L18" s="73"/>
+      <c r="M18" s="73"/>
+      <c r="N18" s="73" t="s">
+        <v>38</v>
+      </c>
+      <c r="O18" s="73">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="P18" s="73">
+        <v>0.59499999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="77" t="s">
+        <v>328</v>
+      </c>
+      <c r="B19" s="73"/>
+      <c r="C19" s="73">
+        <v>48.1</v>
+      </c>
+      <c r="D19" s="73"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73">
+        <f>VLOOKUP(A19,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-8.6999999999999993</v>
+      </c>
+      <c r="G19" s="73">
+        <v>0</v>
+      </c>
+      <c r="H19" s="77" t="s">
+        <v>340</v>
+      </c>
+      <c r="I19" s="77" t="str">
+        <f>VLOOKUP(A19,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.1.3.2</v>
+      </c>
+      <c r="J19" s="73"/>
+      <c r="K19" s="73"/>
+      <c r="L19" s="73"/>
+      <c r="M19" s="73"/>
+      <c r="N19" s="73" t="s">
+        <v>41</v>
+      </c>
+      <c r="O19" s="73">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="P19" s="73">
+        <v>4.2699999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="77" t="s">
+        <v>245</v>
+      </c>
+      <c r="B20" s="73"/>
+      <c r="C20" s="73">
+        <v>49</v>
+      </c>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73">
+        <f>VLOOKUP(A20,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-8.3000000000000007</v>
+      </c>
+      <c r="G20" s="73">
+        <v>3.9968753072807401</v>
+      </c>
+      <c r="H20" s="77" t="s">
+        <v>244</v>
+      </c>
+      <c r="I20" s="77" t="s">
+        <v>810</v>
+      </c>
+      <c r="J20" s="73"/>
+      <c r="K20" s="73"/>
+      <c r="L20" s="73"/>
+      <c r="M20" s="73"/>
+      <c r="N20" s="73" t="s">
+        <v>802</v>
+      </c>
+      <c r="O20" s="73">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="P20" s="73">
+        <v>0.19500000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="77" t="s">
+        <v>332</v>
+      </c>
+      <c r="B21" s="73"/>
+      <c r="C21" s="73">
+        <v>44.73</v>
+      </c>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="73">
+        <v>-1</v>
+      </c>
+      <c r="G21" s="73">
+        <v>-3.9968753072807401</v>
+      </c>
+      <c r="H21" s="77" t="s">
+        <v>246</v>
+      </c>
+      <c r="I21" s="77" t="str">
+        <f>VLOOKUP(A21,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>6.2.1.5</v>
+      </c>
+      <c r="J21" s="73"/>
+      <c r="K21" s="73"/>
+      <c r="L21" s="73"/>
+      <c r="M21" s="73"/>
+      <c r="N21" s="73" t="s">
+        <v>803</v>
+      </c>
+      <c r="O21" s="73">
+        <v>6.2E-2</v>
+      </c>
+      <c r="P21" s="73">
+        <v>6.2E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="78" t="s">
+        <v>334</v>
+      </c>
+      <c r="B22" s="73"/>
+      <c r="C22" s="73">
+        <v>24</v>
+      </c>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73">
+        <v>-2.1</v>
+      </c>
+      <c r="G22" s="73">
+        <v>3.9968753072807401</v>
+      </c>
+      <c r="H22" s="78" t="s">
+        <v>248</v>
+      </c>
+      <c r="I22" s="77" t="str">
+        <f>VLOOKUP(A22,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.3.99.1</v>
+      </c>
+      <c r="J22" s="73"/>
+      <c r="K22" s="73"/>
+      <c r="L22" s="73"/>
+      <c r="M22" s="73"/>
+      <c r="N22" s="73" t="s">
+        <v>100</v>
+      </c>
+      <c r="O22" s="73">
+        <v>1.47</v>
+      </c>
+      <c r="P22" s="73">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="78" t="s">
+        <v>251</v>
+      </c>
+      <c r="B23" s="73"/>
+      <c r="C23" s="73">
+        <v>3.4</v>
+      </c>
+      <c r="D23" s="73">
+        <v>0</v>
+      </c>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73">
+        <f>VLOOKUP(A23,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>5.9</v>
+      </c>
+      <c r="G23" s="73">
+        <v>0</v>
+      </c>
+      <c r="H23" s="78" t="s">
+        <v>250</v>
+      </c>
+      <c r="I23" s="77" t="str">
+        <f>VLOOKUP(A23,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.3.99.1</v>
+      </c>
+      <c r="J23" s="73"/>
+      <c r="K23" s="73"/>
+      <c r="L23" s="73"/>
+      <c r="M23" s="73"/>
+      <c r="N23" s="73" t="s">
+        <v>101</v>
+      </c>
+      <c r="O23" s="73">
+        <v>0.1</v>
+      </c>
+      <c r="P23" s="73">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="77" t="s">
+        <v>252</v>
+      </c>
+      <c r="B24" s="73"/>
+      <c r="C24" s="73">
+        <v>51.7</v>
+      </c>
+      <c r="D24" s="73"/>
+      <c r="E24" s="73"/>
+      <c r="F24" s="73">
+        <f>VLOOKUP(A24,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-0.6</v>
+      </c>
+      <c r="G24" s="73">
+        <v>3.9968753072807401</v>
+      </c>
+      <c r="H24" s="77" t="s">
+        <v>263</v>
+      </c>
+      <c r="I24" s="77" t="str">
+        <f>VLOOKUP(A24,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.2.1.2</v>
+      </c>
+      <c r="J24" s="73"/>
+      <c r="K24" s="73"/>
+      <c r="L24" s="73"/>
+      <c r="M24" s="73"/>
+      <c r="N24" s="73" t="s">
+        <v>804</v>
+      </c>
+      <c r="O24" s="73">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="P24" s="73">
+        <v>0.80800000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="77" t="s">
+        <v>253</v>
+      </c>
+      <c r="B25" s="73"/>
+      <c r="C25" s="73">
+        <v>1</v>
+      </c>
+      <c r="D25" s="73">
+        <v>50</v>
+      </c>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73">
+        <v>-6.4</v>
+      </c>
+      <c r="G25" s="73">
+        <v>-1.73406272437436</v>
+      </c>
+      <c r="H25" s="77" t="s">
+        <v>806</v>
+      </c>
+      <c r="I25" s="77" t="str">
+        <f>VLOOKUP(A25,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.1.1.37</v>
+      </c>
+      <c r="J25" s="73"/>
+      <c r="K25" s="73"/>
+      <c r="L25" s="73"/>
+      <c r="M25" s="73"/>
+      <c r="N25" s="73"/>
+      <c r="O25" s="73"/>
+      <c r="P25" s="73"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="77" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26" s="73"/>
+      <c r="C26" s="73">
+        <v>12.8</v>
+      </c>
+      <c r="D26" s="73"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73">
+        <f>VLOOKUP(A26,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="G26" s="73">
+        <v>34.977749829395002</v>
+      </c>
+      <c r="H26" s="77" t="s">
+        <v>142</v>
+      </c>
+      <c r="I26" s="77" t="s">
+        <v>811</v>
+      </c>
+      <c r="J26" s="73"/>
+      <c r="K26" s="73"/>
+      <c r="L26" s="73"/>
+      <c r="M26" s="73"/>
+      <c r="N26" s="73"/>
+      <c r="O26" s="73"/>
+      <c r="P26" s="73"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="77" t="s">
+        <v>305</v>
+      </c>
+      <c r="B27" s="73"/>
+      <c r="C27" s="73">
+        <v>320</v>
+      </c>
+      <c r="D27" s="73">
+        <v>0</v>
+      </c>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73">
+        <v>-6.4</v>
+      </c>
+      <c r="G27" s="73">
+        <v>0</v>
+      </c>
+      <c r="H27" s="77" t="s">
+        <v>805</v>
+      </c>
+      <c r="I27" s="77" t="str">
+        <f>VLOOKUP(A27,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.1.1.28</v>
+      </c>
+      <c r="J27" s="73"/>
+      <c r="K27" s="73"/>
+      <c r="L27" s="73"/>
+      <c r="M27" s="73"/>
+      <c r="N27" s="73"/>
+      <c r="O27" s="73"/>
+      <c r="P27" s="73"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="77" t="s">
+        <v>212</v>
+      </c>
+      <c r="B28" s="73"/>
+      <c r="C28" s="73">
+        <v>120</v>
+      </c>
+      <c r="D28" s="73">
+        <v>0</v>
+      </c>
+      <c r="E28" s="73"/>
+      <c r="F28" s="73">
+        <f>VLOOKUP(A28,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>3.8</v>
+      </c>
+      <c r="G28" s="78">
+        <v>21.2358352193176</v>
+      </c>
+      <c r="H28" s="77" t="s">
+        <v>211</v>
+      </c>
+      <c r="I28" s="77" t="str">
+        <f>VLOOKUP(A28,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.3.1.8</v>
+      </c>
+      <c r="J28" s="73"/>
+      <c r="K28" s="73"/>
+      <c r="L28" s="73"/>
+      <c r="M28" s="73"/>
+      <c r="N28" s="73"/>
+      <c r="O28" s="73"/>
+      <c r="P28" s="73"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="77" t="s">
+        <v>214</v>
+      </c>
+      <c r="B29" s="73"/>
+      <c r="C29" s="73">
+        <v>280</v>
+      </c>
+      <c r="D29" s="73">
+        <v>0</v>
+      </c>
+      <c r="E29" s="73"/>
+      <c r="F29" s="73">
+        <f>VLOOKUP(A29,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>4.3</v>
+      </c>
+      <c r="G29" s="73">
+        <v>-21.2358352193176</v>
+      </c>
+      <c r="H29" s="77" t="s">
+        <v>213</v>
+      </c>
+      <c r="I29" s="77" t="str">
+        <f>VLOOKUP(A29,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.2.1</v>
+      </c>
+      <c r="J29" s="73"/>
+      <c r="K29" s="73"/>
+      <c r="L29" s="73"/>
+      <c r="M29" s="73"/>
+      <c r="N29" s="73"/>
+      <c r="O29" s="73"/>
+      <c r="P29" s="73"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="B30" s="73"/>
+      <c r="C30" s="73">
+        <v>15.7</v>
+      </c>
+      <c r="D30" s="73">
+        <v>0</v>
+      </c>
+      <c r="E30" s="73"/>
+      <c r="F30" s="73">
+        <f>VLOOKUP(A30,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-4.4000000000000004</v>
+      </c>
+      <c r="G30" s="73">
+        <v>-10.1045270920776</v>
+      </c>
+      <c r="H30" s="78" t="s">
+        <v>143</v>
+      </c>
+      <c r="I30" s="77" t="str">
+        <f>VLOOKUP(A30,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.2.1.10</v>
+      </c>
+      <c r="J30" s="73"/>
+      <c r="K30" s="73"/>
+      <c r="L30" s="73"/>
+      <c r="M30" s="73"/>
+      <c r="N30" s="73"/>
+      <c r="O30" s="73"/>
+      <c r="P30" s="73"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="78" t="s">
+        <v>145</v>
+      </c>
+      <c r="B31" s="73"/>
+      <c r="C31" s="73">
+        <v>150.19999999999999</v>
+      </c>
+      <c r="D31" s="73">
+        <v>0</v>
+      </c>
+      <c r="E31" s="73"/>
+      <c r="F31" s="73">
+        <v>-6</v>
+      </c>
+      <c r="G31" s="73">
+        <v>10.1045270920776</v>
+      </c>
+      <c r="H31" s="78" t="s">
+        <v>146</v>
+      </c>
+      <c r="I31" s="77" t="str">
+        <f>VLOOKUP(A31,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.1.1.1</v>
+      </c>
+      <c r="J31" s="73"/>
+      <c r="K31" s="73"/>
+      <c r="L31" s="73"/>
+      <c r="M31" s="73"/>
+      <c r="N31" s="73"/>
+      <c r="O31" s="73"/>
+      <c r="P31" s="73"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="77" t="s">
+        <v>415</v>
+      </c>
+      <c r="B32" s="73"/>
+      <c r="C32" s="73">
+        <v>174</v>
+      </c>
+      <c r="D32" s="73">
+        <v>0.63</v>
+      </c>
+      <c r="E32" s="73"/>
+      <c r="F32" s="73">
+        <f>VLOOKUP(A32,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-1.6</v>
+      </c>
+      <c r="G32" s="73">
+        <v>0</v>
+      </c>
+      <c r="H32" s="77" t="s">
+        <v>417</v>
+      </c>
+      <c r="I32" s="77" t="str">
+        <f>VLOOKUP(A32,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.1.1.49</v>
+      </c>
+      <c r="J32" s="73"/>
+      <c r="K32" s="73"/>
+      <c r="L32" s="73"/>
+      <c r="M32" s="73"/>
+      <c r="N32" s="73"/>
+      <c r="O32" s="73"/>
+      <c r="P32" s="73"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="77" t="s">
+        <v>419</v>
+      </c>
+      <c r="B33" s="73"/>
+      <c r="C33" s="73">
+        <v>0</v>
+      </c>
+      <c r="D33" s="73"/>
+      <c r="E33" s="73"/>
+      <c r="F33" s="73">
+        <f>VLOOKUP(A33,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="G33" s="73">
+        <v>0</v>
+      </c>
+      <c r="H33" s="77" t="s">
+        <v>421</v>
+      </c>
+      <c r="I33" s="77" t="str">
+        <f>VLOOKUP(A33,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>3.1.1.31</v>
+      </c>
+      <c r="J33" s="73"/>
+      <c r="K33" s="73"/>
+      <c r="L33" s="73"/>
+      <c r="M33" s="73"/>
+      <c r="N33" s="73"/>
+      <c r="O33" s="73"/>
+      <c r="P33" s="73"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="77" t="s">
+        <v>422</v>
+      </c>
+      <c r="B34" s="73"/>
+      <c r="C34" s="73">
+        <v>75.650000000000006</v>
+      </c>
+      <c r="D34" s="73"/>
+      <c r="E34" s="73"/>
+      <c r="F34" s="73">
+        <f>VLOOKUP(A34,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0.9</v>
+      </c>
+      <c r="G34" s="73">
+        <v>0</v>
+      </c>
+      <c r="H34" s="77" t="s">
+        <v>424</v>
+      </c>
+      <c r="I34" s="77" t="str">
+        <f>VLOOKUP(A34,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.1.1.44</v>
+      </c>
+      <c r="J34" s="73"/>
+      <c r="K34" s="73"/>
+      <c r="L34" s="73"/>
+      <c r="M34" s="73"/>
+      <c r="N34" s="73"/>
+      <c r="O34" s="73"/>
+      <c r="P34" s="73"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="77" t="s">
+        <v>425</v>
+      </c>
+      <c r="B35" s="73"/>
+      <c r="C35" s="73">
+        <v>21.05</v>
+      </c>
+      <c r="D35" s="73"/>
+      <c r="E35" s="73"/>
+      <c r="F35" s="73">
+        <v>0</v>
+      </c>
+      <c r="G35" s="78">
+        <v>-0.69762371202792395</v>
+      </c>
+      <c r="H35" s="77" t="s">
+        <v>427</v>
+      </c>
+      <c r="I35" s="77" t="str">
+        <f>VLOOKUP(A35,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.1.3.1</v>
+      </c>
+      <c r="J35" s="73"/>
+      <c r="K35" s="73"/>
+      <c r="L35" s="73"/>
+      <c r="M35" s="73"/>
+      <c r="N35" s="73"/>
+      <c r="O35" s="73"/>
+      <c r="P35" s="73"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="77" t="s">
+        <v>428</v>
+      </c>
+      <c r="B36" s="73"/>
+      <c r="C36" s="73">
+        <v>2100</v>
+      </c>
+      <c r="D36" s="73"/>
+      <c r="E36" s="73"/>
+      <c r="F36" s="73">
+        <v>0.5</v>
+      </c>
+      <c r="G36" s="78">
+        <v>-0.69762371202792395</v>
+      </c>
+      <c r="H36" s="77" t="s">
+        <v>430</v>
+      </c>
+      <c r="I36" s="77" t="str">
+        <f>VLOOKUP(A36,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.3.1.6</v>
+      </c>
+      <c r="J36" s="73"/>
+      <c r="K36" s="73"/>
+      <c r="L36" s="73"/>
+      <c r="M36" s="73"/>
+      <c r="N36" s="73"/>
+      <c r="O36" s="73"/>
+      <c r="P36" s="73"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="77" t="s">
+        <v>431</v>
+      </c>
+      <c r="B37" s="73"/>
+      <c r="C37" s="73">
+        <v>55.57</v>
+      </c>
+      <c r="D37" s="73"/>
+      <c r="E37" s="73"/>
+      <c r="F37" s="73">
+        <v>1.9</v>
+      </c>
+      <c r="G37" s="73">
+        <v>-0.17362949649665499</v>
+      </c>
+      <c r="H37" s="77" t="s">
+        <v>433</v>
+      </c>
+      <c r="I37" s="77" t="str">
+        <f>VLOOKUP(A37,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.2.1.1</v>
+      </c>
+      <c r="J37" s="73"/>
+      <c r="K37" s="73"/>
+      <c r="L37" s="73"/>
+      <c r="M37" s="73"/>
+      <c r="N37" s="73"/>
+      <c r="O37" s="73"/>
+      <c r="P37" s="73"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="77" t="s">
+        <v>436</v>
+      </c>
+      <c r="B38" s="73"/>
+      <c r="C38" s="73">
+        <v>16.57</v>
+      </c>
+      <c r="D38" s="73"/>
+      <c r="E38" s="73"/>
+      <c r="F38" s="73">
+        <v>-1.7</v>
+      </c>
+      <c r="G38" s="73">
+        <v>-0.17362949649665499</v>
+      </c>
+      <c r="H38" s="77" t="s">
+        <v>438</v>
+      </c>
+      <c r="I38" s="77" t="str">
+        <f>VLOOKUP(A38,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.2.1.2</v>
+      </c>
+      <c r="J38" s="73"/>
+      <c r="K38" s="73"/>
+      <c r="L38" s="73"/>
+      <c r="M38" s="73"/>
+      <c r="N38" s="73"/>
+      <c r="O38" s="73"/>
+      <c r="P38" s="73"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="77" t="s">
+        <v>434</v>
+      </c>
+      <c r="B39" s="73"/>
+      <c r="C39" s="73">
+        <v>15.45</v>
+      </c>
+      <c r="D39" s="73"/>
+      <c r="E39" s="73"/>
+      <c r="F39" s="73">
+        <v>-1.7</v>
+      </c>
+      <c r="G39" s="73">
+        <v>-0.52399421553126901</v>
+      </c>
+      <c r="H39" s="77" t="s">
+        <v>435</v>
+      </c>
+      <c r="I39" s="77" t="str">
+        <f>VLOOKUP(A39,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.2.1.1</v>
+      </c>
+      <c r="J39" s="73"/>
+      <c r="K39" s="73"/>
+      <c r="L39" s="73"/>
+      <c r="M39" s="73"/>
+      <c r="N39" s="73"/>
+      <c r="O39" s="73"/>
+      <c r="P39" s="73"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="78" t="s">
+        <v>169</v>
+      </c>
+      <c r="B40" s="73"/>
+      <c r="C40" s="73">
+        <v>0</v>
+      </c>
+      <c r="D40" s="73"/>
+      <c r="E40" s="73"/>
+      <c r="F40" s="73">
+        <f>VLOOKUP(A40,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-17.399999999999999</v>
+      </c>
+      <c r="G40" s="73">
+        <v>16.0031246927193</v>
+      </c>
+      <c r="H40" s="78" t="s">
+        <v>170</v>
+      </c>
+      <c r="I40" s="77" t="str">
+        <f>VLOOKUP(A40,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.6.5.3</v>
+      </c>
+      <c r="J40" s="73"/>
+      <c r="K40" s="73"/>
+      <c r="L40" s="73"/>
+      <c r="M40" s="73"/>
+      <c r="N40" s="73"/>
+      <c r="O40" s="73"/>
+      <c r="P40" s="73"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" s="77" t="s">
+        <v>441</v>
+      </c>
+      <c r="B41" s="73"/>
+      <c r="C41" s="73">
+        <v>0</v>
+      </c>
+      <c r="D41" s="73"/>
+      <c r="E41" s="73"/>
+      <c r="F41" s="73">
+        <f>VLOOKUP(A41,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-0.3</v>
+      </c>
+      <c r="G41" s="73">
+        <v>0</v>
+      </c>
+      <c r="H41" s="77" t="s">
+        <v>443</v>
+      </c>
+      <c r="I41" s="77" t="str">
+        <f>VLOOKUP(A41,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.6.1.2</v>
+      </c>
+      <c r="J41" s="73"/>
+      <c r="K41" s="73"/>
+      <c r="L41" s="73"/>
+      <c r="M41" s="73"/>
+      <c r="N41" s="73"/>
+      <c r="O41" s="73"/>
+      <c r="P41" s="73"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" s="77" t="s">
+        <v>444</v>
+      </c>
+      <c r="B42" s="73"/>
+      <c r="C42" s="73">
+        <v>0</v>
+      </c>
+      <c r="D42" s="73"/>
+      <c r="E42" s="73"/>
+      <c r="F42" s="73">
+        <v>0.3</v>
+      </c>
+      <c r="G42" s="73">
+        <v>10.381277508814</v>
+      </c>
+      <c r="H42" s="77" t="s">
+        <v>447</v>
+      </c>
+      <c r="I42" s="77" t="str">
+        <f>VLOOKUP(A42,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.6.1.1</v>
+      </c>
+      <c r="J42" s="73"/>
+      <c r="K42" s="73"/>
+      <c r="L42" s="73"/>
+      <c r="M42" s="73"/>
+      <c r="N42" s="73"/>
+      <c r="O42" s="73"/>
+      <c r="P42" s="73"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" s="77" t="s">
+        <v>178</v>
+      </c>
+      <c r="B43" s="73"/>
+      <c r="C43" s="73">
+        <v>0</v>
+      </c>
+      <c r="D43" s="73"/>
+      <c r="E43" s="73"/>
+      <c r="F43" s="73">
+        <f>VLOOKUP(A43,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="G43" s="73">
+        <v>0</v>
+      </c>
+      <c r="H43" s="77" t="s">
+        <v>177</v>
+      </c>
+      <c r="I43" s="77" t="str">
+        <f>VLOOKUP(A43,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.4.3</v>
+      </c>
+      <c r="J43" s="73"/>
+      <c r="K43" s="73"/>
+      <c r="L43" s="73"/>
+      <c r="M43" s="73"/>
+      <c r="N43" s="73"/>
+      <c r="O43" s="73"/>
+      <c r="P43" s="73"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" s="77" t="s">
+        <v>171</v>
+      </c>
+      <c r="B44" s="73"/>
+      <c r="C44" s="73">
+        <v>0</v>
+      </c>
+      <c r="D44" s="73"/>
+      <c r="E44" s="73"/>
+      <c r="F44" s="73">
+        <f>VLOOKUP(A44,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-6.6</v>
+      </c>
+      <c r="G44" s="73">
+        <v>8.39</v>
+      </c>
+      <c r="H44" s="77" t="s">
+        <v>172</v>
+      </c>
+      <c r="I44" s="77">
+        <f>VLOOKUP(A44,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J44" s="73"/>
+      <c r="K44" s="73"/>
+      <c r="L44" s="73"/>
+      <c r="M44" s="73"/>
+      <c r="N44" s="73"/>
+      <c r="O44" s="73"/>
+      <c r="P44" s="73"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" s="77" t="s">
+        <v>173</v>
+      </c>
+      <c r="B45" s="73"/>
+      <c r="C45" s="73">
+        <v>0</v>
+      </c>
+      <c r="D45" s="73"/>
+      <c r="E45" s="73"/>
+      <c r="F45" s="73">
+        <f>VLOOKUP(A45,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>6.6</v>
+      </c>
+      <c r="G45" s="73">
+        <v>7.35555836532013</v>
+      </c>
+      <c r="H45" s="77" t="s">
+        <v>453</v>
+      </c>
+      <c r="I45" s="77" t="str">
+        <f>VLOOKUP(A45,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>3.6.3.14</v>
+      </c>
+      <c r="J45" s="73"/>
+      <c r="K45" s="73"/>
+      <c r="L45" s="73"/>
+      <c r="M45" s="73"/>
+      <c r="N45" s="73"/>
+      <c r="O45" s="73"/>
+      <c r="P45" s="73"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" s="77" t="s">
+        <v>167</v>
+      </c>
+      <c r="B46" s="73"/>
+      <c r="C46" s="73">
+        <v>0</v>
+      </c>
+      <c r="D46" s="73"/>
+      <c r="E46" s="73"/>
+      <c r="F46" s="73">
+        <f>VLOOKUP(A46,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-37.200000000000003</v>
+      </c>
+      <c r="G46" s="73">
+        <v>20</v>
+      </c>
+      <c r="H46" s="77" t="s">
+        <v>168</v>
+      </c>
+      <c r="I46" s="77" t="s">
+        <v>812</v>
+      </c>
+      <c r="J46" s="73"/>
+      <c r="K46" s="73"/>
+      <c r="L46" s="73"/>
+      <c r="M46" s="73"/>
+      <c r="N46" s="73"/>
+      <c r="O46" s="73"/>
+      <c r="P46" s="73"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" s="77" t="s">
+        <v>234</v>
+      </c>
+      <c r="B47" s="73"/>
+      <c r="C47" s="73">
+        <v>13.74</v>
+      </c>
+      <c r="D47" s="73">
+        <v>18.2</v>
+      </c>
+      <c r="E47" s="73"/>
+      <c r="F47" s="73">
+        <f>VLOOKUP(A47,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-6.8</v>
+      </c>
+      <c r="G47" s="73">
+        <v>0</v>
+      </c>
+      <c r="H47" s="77" t="s">
+        <v>235</v>
+      </c>
+      <c r="I47" s="77" t="str">
+        <f>VLOOKUP(A47,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.1.1.31</v>
+      </c>
+      <c r="J47" s="73"/>
+      <c r="K47" s="73"/>
+      <c r="L47" s="73"/>
+      <c r="M47" s="73"/>
+      <c r="N47" s="73"/>
+      <c r="O47" s="73"/>
+      <c r="P47" s="73"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="77" t="s">
+        <v>237</v>
+      </c>
+      <c r="B48" s="73"/>
+      <c r="C48" s="73">
+        <v>0</v>
+      </c>
+      <c r="D48" s="73">
+        <v>0</v>
+      </c>
+      <c r="E48" s="73"/>
+      <c r="F48" s="73">
+        <f>VLOOKUP(A48,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0.2</v>
+      </c>
+      <c r="G48" s="73">
+        <v>0</v>
+      </c>
+      <c r="H48" s="77" t="s">
+        <v>236</v>
+      </c>
+      <c r="I48" s="77" t="str">
+        <f>VLOOKUP(A48,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.1.1.49</v>
+      </c>
+      <c r="J48" s="73"/>
+      <c r="K48" s="73"/>
+      <c r="L48" s="73"/>
+      <c r="M48" s="73"/>
+      <c r="N48" s="73"/>
+      <c r="O48" s="73"/>
+      <c r="P48" s="73"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" s="77" t="s">
+        <v>254</v>
+      </c>
+      <c r="B49" s="73"/>
+      <c r="C49" s="73">
+        <v>0</v>
+      </c>
+      <c r="D49" s="73">
+        <v>0</v>
+      </c>
+      <c r="E49" s="73"/>
+      <c r="F49" s="73">
+        <f>VLOOKUP(A49,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>1.3</v>
+      </c>
+      <c r="G49" s="73">
+        <v>0</v>
+      </c>
+      <c r="H49" s="77" t="s">
+        <v>262</v>
+      </c>
+      <c r="I49" s="77" t="str">
+        <f>VLOOKUP(A49,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.1.1.38</v>
+      </c>
+      <c r="J49" s="73"/>
+      <c r="K49" s="73"/>
+      <c r="L49" s="73"/>
+      <c r="M49" s="73"/>
+      <c r="N49" s="73"/>
+      <c r="O49" s="73"/>
+      <c r="P49" s="73"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" s="77" t="s">
+        <v>364</v>
+      </c>
+      <c r="B50" s="73"/>
+      <c r="C50" s="73">
+        <v>0</v>
+      </c>
+      <c r="D50" s="73">
+        <v>0</v>
+      </c>
+      <c r="E50" s="73"/>
+      <c r="F50" s="73">
+        <f>VLOOKUP(A50,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>1.6</v>
+      </c>
+      <c r="G50" s="73">
+        <v>2.2628125829063799</v>
+      </c>
+      <c r="H50" s="77" t="s">
+        <v>367</v>
+      </c>
+      <c r="I50" s="77" t="str">
+        <f>VLOOKUP(A50,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.1.1.40</v>
+      </c>
+      <c r="J50" s="73"/>
+      <c r="K50" s="73"/>
+      <c r="L50" s="73"/>
+      <c r="M50" s="73"/>
+      <c r="N50" s="73"/>
+      <c r="O50" s="73"/>
+      <c r="P50" s="73"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" s="77" t="s">
+        <v>663</v>
+      </c>
+      <c r="B51" s="73"/>
+      <c r="C51" s="73"/>
+      <c r="D51" s="73"/>
+      <c r="E51" s="73"/>
+      <c r="F51" s="73">
+        <f>VLOOKUP(A51,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G51" s="73">
+        <v>7.11118951189348</v>
+      </c>
+      <c r="H51" s="77" t="s">
+        <v>665</v>
+      </c>
+      <c r="I51" s="77"/>
+      <c r="J51" s="73"/>
+      <c r="K51" s="73"/>
+      <c r="L51" s="73"/>
+      <c r="M51" s="73"/>
+      <c r="N51" s="73"/>
+      <c r="O51" s="73"/>
+      <c r="P51" s="73"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" s="77" t="s">
+        <v>463</v>
+      </c>
+      <c r="B52" s="73"/>
+      <c r="C52" s="11">
+        <v>1.6670000000000001E-2</v>
+      </c>
+      <c r="D52" s="73"/>
+      <c r="E52" s="73"/>
+      <c r="F52" s="73">
+        <f>VLOOKUP(A52,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G52" s="73">
+        <v>10</v>
+      </c>
+      <c r="H52" s="77" t="s">
+        <v>166</v>
+      </c>
+      <c r="I52" s="77"/>
+      <c r="J52" s="73"/>
+      <c r="K52" s="73"/>
+      <c r="L52" s="73"/>
+      <c r="M52" s="73"/>
+      <c r="N52" s="73"/>
+      <c r="O52" s="73"/>
+      <c r="P52" s="73"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" s="77" t="s">
+        <v>456</v>
+      </c>
+      <c r="B53" s="73"/>
+      <c r="C53" s="73"/>
+      <c r="D53" s="73"/>
+      <c r="E53" s="73"/>
+      <c r="F53" s="73">
+        <f>VLOOKUP(A53,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G53" s="73">
+        <v>3.5703232462952501</v>
+      </c>
+      <c r="H53" s="77" t="s">
+        <v>458</v>
+      </c>
+      <c r="I53" s="77"/>
+      <c r="J53" s="73"/>
+      <c r="K53" s="73"/>
+      <c r="L53" s="73"/>
+      <c r="M53" s="73"/>
+      <c r="N53" s="73"/>
+      <c r="O53" s="73"/>
+      <c r="P53" s="73"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" s="77" t="s">
+        <v>397</v>
+      </c>
+      <c r="B54" s="73"/>
+      <c r="C54" s="73"/>
+      <c r="D54" s="73"/>
+      <c r="E54" s="73"/>
+      <c r="F54" s="73">
+        <f>VLOOKUP(A54,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G54" s="73">
+        <v>-6.25968789018712</v>
+      </c>
+      <c r="H54" s="77" t="s">
+        <v>399</v>
+      </c>
+      <c r="I54" s="77"/>
+      <c r="J54" s="73"/>
+      <c r="K54" s="73"/>
+      <c r="L54" s="73"/>
+      <c r="M54" s="73"/>
+      <c r="N54" s="73"/>
+      <c r="O54" s="73"/>
+      <c r="P54" s="73"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" s="77" t="s">
+        <v>343</v>
+      </c>
+      <c r="B55" s="73"/>
+      <c r="C55" s="73"/>
+      <c r="D55" s="73"/>
+      <c r="E55" s="73"/>
+      <c r="F55" s="73">
+        <v>0</v>
+      </c>
+      <c r="G55" s="73">
+        <v>0</v>
+      </c>
+      <c r="H55" s="77" t="s">
+        <v>345</v>
+      </c>
+      <c r="I55" s="77"/>
+      <c r="J55" s="73"/>
+      <c r="K55" s="73"/>
+      <c r="L55" s="73"/>
+      <c r="M55" s="73"/>
+      <c r="N55" s="73"/>
+      <c r="O55" s="73"/>
+      <c r="P55" s="73"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56" s="77" t="s">
+        <v>346</v>
+      </c>
+      <c r="B56" s="73"/>
+      <c r="C56" s="73"/>
+      <c r="D56" s="73"/>
+      <c r="E56" s="73"/>
+      <c r="F56" s="73">
+        <v>0</v>
+      </c>
+      <c r="G56" s="73">
+        <v>0</v>
+      </c>
+      <c r="H56" s="77" t="s">
+        <v>352</v>
+      </c>
+      <c r="I56" s="77"/>
+      <c r="J56" s="73"/>
+      <c r="K56" s="73"/>
+      <c r="L56" s="73"/>
+      <c r="M56" s="73"/>
+      <c r="N56" s="73"/>
+      <c r="O56" s="73"/>
+      <c r="P56" s="73"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" s="77" t="s">
+        <v>349</v>
+      </c>
+      <c r="B57" s="73"/>
+      <c r="C57" s="73"/>
+      <c r="D57" s="73"/>
+      <c r="E57" s="73"/>
+      <c r="F57" s="73">
+        <v>0</v>
+      </c>
+      <c r="G57" s="73">
+        <v>0</v>
+      </c>
+      <c r="H57" s="77" t="s">
+        <v>351</v>
+      </c>
+      <c r="I57" s="77"/>
+      <c r="J57" s="73"/>
+      <c r="K57" s="73"/>
+      <c r="L57" s="73"/>
+      <c r="M57" s="73"/>
+      <c r="N57" s="73"/>
+      <c r="O57" s="73"/>
+      <c r="P57" s="73"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58" s="77" t="s">
+        <v>353</v>
+      </c>
+      <c r="B58" s="73"/>
+      <c r="C58" s="73"/>
+      <c r="D58" s="73"/>
+      <c r="E58" s="73"/>
+      <c r="F58" s="73">
+        <f>VLOOKUP(A58,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G58" s="73">
+        <v>0</v>
+      </c>
+      <c r="H58" s="77" t="s">
+        <v>355</v>
+      </c>
+      <c r="I58" s="77"/>
+      <c r="J58" s="73"/>
+      <c r="K58" s="73"/>
+      <c r="L58" s="73"/>
+      <c r="M58" s="73"/>
+      <c r="N58" s="73"/>
+      <c r="O58" s="73"/>
+      <c r="P58" s="73"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" s="77" t="s">
+        <v>356</v>
+      </c>
+      <c r="B59" s="73"/>
+      <c r="C59" s="73"/>
+      <c r="D59" s="73"/>
+      <c r="E59" s="73"/>
+      <c r="F59" s="73">
+        <f>VLOOKUP(A59,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G59" s="73">
+        <v>0</v>
+      </c>
+      <c r="H59" s="77" t="s">
+        <v>359</v>
+      </c>
+      <c r="I59" s="77"/>
+      <c r="J59" s="73"/>
+      <c r="K59" s="73"/>
+      <c r="L59" s="73"/>
+      <c r="M59" s="73"/>
+      <c r="N59" s="73"/>
+      <c r="O59" s="73"/>
+      <c r="P59" s="73"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" s="78" t="s">
+        <v>360</v>
+      </c>
+      <c r="B60" s="73"/>
+      <c r="C60" s="73"/>
+      <c r="D60" s="73"/>
+      <c r="E60" s="73"/>
+      <c r="F60" s="73">
+        <f>VLOOKUP(A60,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G60" s="73">
+        <v>0</v>
+      </c>
+      <c r="H60" s="78" t="s">
+        <v>363</v>
+      </c>
+      <c r="I60" s="77"/>
+      <c r="J60" s="73"/>
+      <c r="K60" s="73"/>
+      <c r="L60" s="73"/>
+      <c r="M60" s="73"/>
+      <c r="N60" s="73"/>
+      <c r="O60" s="73"/>
+      <c r="P60" s="73"/>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A61" s="77" t="s">
+        <v>368</v>
+      </c>
+      <c r="B61" s="73"/>
+      <c r="C61" s="73"/>
+      <c r="D61" s="73"/>
+      <c r="E61" s="73"/>
+      <c r="F61" s="73">
+        <f>VLOOKUP(A61,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G61" s="73">
+        <v>0</v>
+      </c>
+      <c r="H61" s="77" t="s">
+        <v>371</v>
+      </c>
+      <c r="I61" s="77"/>
+      <c r="J61" s="73"/>
+      <c r="K61" s="73"/>
+      <c r="L61" s="73"/>
+      <c r="M61" s="73"/>
+      <c r="N61" s="73"/>
+      <c r="O61" s="73"/>
+      <c r="P61" s="73"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A62" s="78" t="s">
+        <v>378</v>
+      </c>
+      <c r="B62" s="73"/>
+      <c r="C62" s="73"/>
+      <c r="D62" s="73"/>
+      <c r="E62" s="73"/>
+      <c r="F62" s="73">
+        <f>VLOOKUP(A62,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G62" s="73">
+        <v>0</v>
+      </c>
+      <c r="H62" s="78" t="s">
+        <v>380</v>
+      </c>
+      <c r="I62" s="77"/>
+      <c r="J62" s="73"/>
+      <c r="K62" s="73"/>
+      <c r="L62" s="73"/>
+      <c r="M62" s="73"/>
+      <c r="N62" s="73"/>
+      <c r="O62" s="73"/>
+      <c r="P62" s="73"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A63" s="78" t="s">
+        <v>381</v>
+      </c>
+      <c r="B63" s="73"/>
+      <c r="C63" s="73"/>
+      <c r="D63" s="73"/>
+      <c r="E63" s="73"/>
+      <c r="F63" s="73">
+        <f>VLOOKUP(A63,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G63" s="73">
+        <v>34.977749829395002</v>
+      </c>
+      <c r="H63" s="78" t="s">
+        <v>383</v>
+      </c>
+      <c r="I63" s="77"/>
+      <c r="J63" s="73"/>
+      <c r="K63" s="73"/>
+      <c r="L63" s="73"/>
+      <c r="M63" s="73"/>
+      <c r="N63" s="73"/>
+      <c r="O63" s="73"/>
+      <c r="P63" s="73"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64" s="77" t="s">
+        <v>384</v>
+      </c>
+      <c r="B64" s="73"/>
+      <c r="C64" s="73"/>
+      <c r="D64" s="73"/>
+      <c r="E64" s="73"/>
+      <c r="F64" s="73">
+        <f>VLOOKUP(A64,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G64" s="73">
+        <v>-10.1045270920776</v>
+      </c>
+      <c r="H64" s="77" t="s">
+        <v>386</v>
+      </c>
+      <c r="I64" s="77"/>
+      <c r="J64" s="73"/>
+      <c r="K64" s="73"/>
+      <c r="L64" s="73"/>
+      <c r="M64" s="73"/>
+      <c r="N64" s="73"/>
+      <c r="O64" s="73"/>
+      <c r="P64" s="73"/>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A65" s="77" t="s">
+        <v>387</v>
+      </c>
+      <c r="B65" s="73"/>
+      <c r="C65" s="73"/>
+      <c r="D65" s="73"/>
+      <c r="E65" s="73"/>
+      <c r="F65" s="73">
+        <f>VLOOKUP(A65,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G65" s="73">
+        <v>-21.2358352193176</v>
+      </c>
+      <c r="H65" s="77" t="s">
+        <v>389</v>
+      </c>
+      <c r="I65" s="77"/>
+      <c r="J65" s="73"/>
+      <c r="K65" s="73"/>
+      <c r="L65" s="73"/>
+      <c r="M65" s="73"/>
+      <c r="N65" s="73"/>
+      <c r="O65" s="73"/>
+      <c r="P65" s="73"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A66" s="78" t="s">
+        <v>390</v>
+      </c>
+      <c r="B66" s="73"/>
+      <c r="C66" s="73"/>
+      <c r="D66" s="73"/>
+      <c r="E66" s="73"/>
+      <c r="F66" s="73">
+        <f>VLOOKUP(A66,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G66" s="73">
+        <v>0</v>
+      </c>
+      <c r="H66" s="78" t="s">
+        <v>392</v>
+      </c>
+      <c r="I66" s="77"/>
+      <c r="J66" s="73"/>
+      <c r="K66" s="73"/>
+      <c r="L66" s="73"/>
+      <c r="M66" s="73"/>
+      <c r="N66" s="73"/>
+      <c r="O66" s="73"/>
+      <c r="P66" s="73"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A67" s="77" t="s">
+        <v>401</v>
+      </c>
+      <c r="B67" s="73"/>
+      <c r="C67" s="73"/>
+      <c r="D67" s="73"/>
+      <c r="E67" s="73"/>
+      <c r="F67" s="73">
+        <v>0</v>
+      </c>
+      <c r="G67" s="73">
+        <v>0</v>
+      </c>
+      <c r="H67" s="77" t="s">
+        <v>149</v>
+      </c>
+      <c r="I67" s="77"/>
+      <c r="J67" s="73"/>
+      <c r="K67" s="73"/>
+      <c r="L67" s="73"/>
+      <c r="M67" s="73"/>
+      <c r="N67" s="73"/>
+      <c r="O67" s="73"/>
+      <c r="P67" s="73"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68" s="77" t="s">
+        <v>402</v>
+      </c>
+      <c r="B68" s="73"/>
+      <c r="C68" s="73"/>
+      <c r="D68" s="73"/>
+      <c r="E68" s="73"/>
+      <c r="F68" s="73">
+        <v>0</v>
+      </c>
+      <c r="G68" s="73">
+        <v>0</v>
+      </c>
+      <c r="H68" s="77" t="s">
+        <v>258</v>
+      </c>
+      <c r="I68" s="77"/>
+      <c r="J68" s="73"/>
+      <c r="K68" s="73"/>
+      <c r="L68" s="73"/>
+      <c r="M68" s="73"/>
+      <c r="N68" s="73"/>
+      <c r="O68" s="73"/>
+      <c r="P68" s="73"/>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A69" s="77" t="s">
+        <v>403</v>
+      </c>
+      <c r="B69" s="73"/>
+      <c r="C69" s="73"/>
+      <c r="D69" s="73"/>
+      <c r="E69" s="73"/>
+      <c r="F69" s="73">
+        <v>0</v>
+      </c>
+      <c r="G69" s="73">
+        <v>0</v>
+      </c>
+      <c r="H69" s="77" t="s">
+        <v>256</v>
+      </c>
+      <c r="I69" s="77"/>
+      <c r="J69" s="73"/>
+      <c r="K69" s="73"/>
+      <c r="L69" s="73"/>
+      <c r="M69" s="73"/>
+      <c r="N69" s="73"/>
+      <c r="O69" s="73"/>
+      <c r="P69" s="73"/>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A70" s="77" t="s">
+        <v>404</v>
+      </c>
+      <c r="B70" s="73"/>
+      <c r="C70" s="73"/>
+      <c r="D70" s="73"/>
+      <c r="E70" s="73"/>
+      <c r="F70" s="73">
+        <v>0</v>
+      </c>
+      <c r="G70" s="73">
+        <v>0</v>
+      </c>
+      <c r="H70" s="77" t="s">
+        <v>260</v>
+      </c>
+      <c r="I70" s="77"/>
+      <c r="J70" s="73"/>
+      <c r="K70" s="73"/>
+      <c r="L70" s="73"/>
+      <c r="M70" s="73"/>
+      <c r="N70" s="73"/>
+      <c r="O70" s="73"/>
+      <c r="P70" s="73"/>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A71" s="77" t="s">
+        <v>405</v>
+      </c>
+      <c r="B71" s="73"/>
+      <c r="C71" s="73"/>
+      <c r="D71" s="73"/>
+      <c r="E71" s="73"/>
+      <c r="F71" s="73">
+        <v>0</v>
+      </c>
+      <c r="G71" s="73">
+        <v>0</v>
+      </c>
+      <c r="H71" s="77" t="s">
+        <v>265</v>
+      </c>
+      <c r="I71" s="77"/>
+      <c r="J71" s="73"/>
+      <c r="K71" s="73"/>
+      <c r="L71" s="73"/>
+      <c r="M71" s="73"/>
+      <c r="N71" s="73"/>
+      <c r="O71" s="73"/>
+      <c r="P71" s="73"/>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A72" s="77" t="s">
+        <v>406</v>
+      </c>
+      <c r="B72" s="73"/>
+      <c r="C72" s="73"/>
+      <c r="D72" s="73"/>
+      <c r="E72" s="73"/>
+      <c r="F72" s="73">
+        <v>0</v>
+      </c>
+      <c r="G72" s="73">
+        <v>0</v>
+      </c>
+      <c r="H72" s="77" t="s">
+        <v>152</v>
+      </c>
+      <c r="I72" s="77"/>
+      <c r="J72" s="73"/>
+      <c r="K72" s="73"/>
+      <c r="L72" s="73"/>
+      <c r="M72" s="73"/>
+      <c r="N72" s="73"/>
+      <c r="O72" s="73"/>
+      <c r="P72" s="73"/>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A73" s="77" t="s">
+        <v>407</v>
+      </c>
+      <c r="B73" s="73"/>
+      <c r="C73" s="73"/>
+      <c r="D73" s="73"/>
+      <c r="E73" s="73"/>
+      <c r="F73" s="73">
+        <v>0</v>
+      </c>
+      <c r="G73" s="73">
+        <v>34.977749829395002</v>
+      </c>
+      <c r="H73" s="77" t="s">
+        <v>285</v>
+      </c>
+      <c r="I73" s="77"/>
+      <c r="J73" s="73"/>
+      <c r="K73" s="73"/>
+      <c r="L73" s="73"/>
+      <c r="M73" s="73"/>
+      <c r="N73" s="73"/>
+      <c r="O73" s="73"/>
+      <c r="P73" s="73"/>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A74" s="77" t="s">
+        <v>408</v>
+      </c>
+      <c r="B74" s="73"/>
+      <c r="C74" s="73"/>
+      <c r="D74" s="73"/>
+      <c r="E74" s="73"/>
+      <c r="F74" s="73">
+        <v>0</v>
+      </c>
+      <c r="G74" s="73">
+        <v>10.1045270920776</v>
+      </c>
+      <c r="H74" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="I74" s="77"/>
+      <c r="J74" s="73"/>
+      <c r="K74" s="73"/>
+      <c r="L74" s="73"/>
+      <c r="M74" s="73"/>
+      <c r="N74" s="73"/>
+      <c r="O74" s="73"/>
+      <c r="P74" s="73"/>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A75" s="77" t="s">
+        <v>409</v>
+      </c>
+      <c r="B75" s="73"/>
+      <c r="C75" s="73"/>
+      <c r="D75" s="73"/>
+      <c r="E75" s="73"/>
+      <c r="F75" s="73">
+        <v>0</v>
+      </c>
+      <c r="G75" s="73">
+        <v>21.2358352193176</v>
+      </c>
+      <c r="H75" s="77" t="s">
+        <v>216</v>
+      </c>
+      <c r="I75" s="77"/>
+      <c r="J75" s="73"/>
+      <c r="K75" s="73"/>
+      <c r="L75" s="73"/>
+      <c r="M75" s="73"/>
+      <c r="N75" s="73"/>
+      <c r="O75" s="73"/>
+      <c r="P75" s="73"/>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A76" s="77" t="s">
+        <v>410</v>
+      </c>
+      <c r="B76" s="73"/>
+      <c r="C76" s="73"/>
+      <c r="D76" s="73"/>
+      <c r="E76" s="73"/>
+      <c r="F76" s="73">
+        <v>0</v>
+      </c>
+      <c r="G76" s="73">
+        <v>0</v>
+      </c>
+      <c r="H76" s="77" t="s">
+        <v>157</v>
+      </c>
+      <c r="I76" s="77"/>
+      <c r="J76" s="73"/>
+      <c r="K76" s="73"/>
+      <c r="L76" s="73"/>
+      <c r="M76" s="73"/>
+      <c r="N76" s="73"/>
+      <c r="O76" s="73"/>
+      <c r="P76" s="73"/>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A77" s="77" t="s">
+        <v>411</v>
+      </c>
+      <c r="B77" s="73"/>
+      <c r="C77" s="73"/>
+      <c r="D77" s="73"/>
+      <c r="E77" s="73"/>
+      <c r="F77" s="73">
+        <v>0</v>
+      </c>
+      <c r="G77" s="73">
+        <v>-20</v>
+      </c>
+      <c r="H77" s="77" t="s">
+        <v>794</v>
+      </c>
+      <c r="I77" s="77"/>
+      <c r="J77" s="73"/>
+      <c r="K77" s="73"/>
+      <c r="L77" s="73"/>
+      <c r="M77" s="73"/>
+      <c r="N77" s="73"/>
+      <c r="O77" s="73"/>
+      <c r="P77" s="73"/>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A78" s="77" t="s">
+        <v>412</v>
+      </c>
+      <c r="B78" s="73"/>
+      <c r="C78" s="73"/>
+      <c r="D78" s="73"/>
+      <c r="E78" s="73"/>
+      <c r="F78" s="73">
+        <v>0</v>
+      </c>
+      <c r="G78" s="73">
+        <v>6.25968789018712</v>
+      </c>
+      <c r="H78" s="77" t="s">
+        <v>400</v>
+      </c>
+      <c r="I78" s="77"/>
+      <c r="J78" s="73"/>
+      <c r="K78" s="73"/>
+      <c r="L78" s="73"/>
+      <c r="M78" s="73"/>
+      <c r="N78" s="73"/>
+      <c r="O78" s="73"/>
+      <c r="P78" s="73"/>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A79" s="77" t="s">
+        <v>413</v>
+      </c>
+      <c r="B79" s="73"/>
+      <c r="C79" s="73"/>
+      <c r="D79" s="73"/>
+      <c r="E79" s="73"/>
+      <c r="F79" s="73">
+        <v>0</v>
+      </c>
+      <c r="G79" s="73">
+        <v>65.594624664349297</v>
+      </c>
+      <c r="H79" s="77" t="s">
+        <v>205</v>
+      </c>
+      <c r="I79" s="77"/>
+      <c r="J79" s="73"/>
+      <c r="K79" s="73"/>
+      <c r="L79" s="73"/>
+      <c r="M79" s="73"/>
+      <c r="N79" s="73"/>
+      <c r="O79" s="73"/>
+      <c r="P79" s="73"/>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A80" s="77" t="s">
+        <v>414</v>
+      </c>
+      <c r="B80" s="73"/>
+      <c r="C80" s="73"/>
+      <c r="D80" s="73"/>
+      <c r="E80" s="73"/>
+      <c r="F80" s="73">
+        <v>0</v>
+      </c>
+      <c r="G80" s="73">
+        <v>-7.11118951189348</v>
+      </c>
+      <c r="H80" s="77" t="s">
+        <v>206</v>
+      </c>
+      <c r="I80" s="77"/>
+      <c r="J80" s="73"/>
+      <c r="K80" s="73"/>
+      <c r="L80" s="73"/>
+      <c r="M80" s="73"/>
+      <c r="N80" s="73"/>
+      <c r="O80" s="73"/>
+      <c r="P80" s="73"/>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A81" s="77" t="s">
+        <v>460</v>
+      </c>
+      <c r="B81" s="73"/>
+      <c r="C81" s="73"/>
+      <c r="D81" s="73"/>
+      <c r="E81" s="73"/>
+      <c r="F81" s="73">
+        <v>0</v>
+      </c>
+      <c r="G81" s="73">
+        <v>-3.5703232462952501</v>
+      </c>
+      <c r="H81" s="77" t="s">
+        <v>209</v>
+      </c>
+      <c r="I81" s="77"/>
+      <c r="J81" s="73"/>
+      <c r="K81" s="73"/>
+      <c r="L81" s="73"/>
+      <c r="M81" s="73"/>
+      <c r="N81" s="73"/>
+      <c r="O81" s="73"/>
+      <c r="P81" s="73"/>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A82" s="77" t="s">
+        <v>461</v>
+      </c>
+      <c r="B82" s="73"/>
+      <c r="C82" s="73"/>
+      <c r="D82" s="73"/>
+      <c r="E82" s="73"/>
+      <c r="F82" s="73">
+        <v>0</v>
+      </c>
+      <c r="G82" s="73">
+        <v>-10</v>
+      </c>
+      <c r="H82" s="77" t="s">
+        <v>462</v>
+      </c>
+      <c r="I82" s="77"/>
+      <c r="J82" s="73"/>
+      <c r="K82" s="73"/>
+      <c r="L82" s="73"/>
+      <c r="M82" s="73"/>
+      <c r="N82" s="73"/>
+      <c r="O82" s="73"/>
+      <c r="P82" s="73"/>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A83" s="78" t="s">
+        <v>179</v>
+      </c>
+      <c r="B83" s="73"/>
+      <c r="C83" s="73"/>
+      <c r="D83" s="73"/>
+      <c r="E83" s="73"/>
+      <c r="F83" s="73">
+        <v>0</v>
+      </c>
+      <c r="G83" s="73">
+        <v>0.97053938790751804</v>
+      </c>
+      <c r="H83" s="78" t="s">
+        <v>793</v>
+      </c>
+      <c r="I83" s="73"/>
+      <c r="J83" s="73"/>
+      <c r="K83" s="73"/>
+      <c r="L83" s="73"/>
+      <c r="M83" s="73"/>
+      <c r="N83" s="73"/>
+      <c r="O83" s="73"/>
+      <c r="P83" s="73"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6522,7 +10716,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L96"/>
   <sheetViews>

</xml_diff>

<commit_message>
Sept 29 - Home
</commit_message>
<xml_diff>
--- a/KineticModel/ecoli_test.xlsx
+++ b/KineticModel/ecoli_test.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="720" windowWidth="18195" windowHeight="6885" activeTab="10"/>
+    <workbookView xWindow="480" yWindow="720" windowWidth="18195" windowHeight="6885" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="ecoliT1" sheetId="1" r:id="rId1"/>
@@ -24,12 +29,12 @@
   <externalReferences>
     <externalReference r:id="rId14"/>
   </externalReferences>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1733" uniqueCount="814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1736" uniqueCount="817">
   <si>
     <t>Enzymes</t>
   </si>
@@ -2513,6 +2518,15 @@
   </si>
   <si>
     <t>2.3.3.9</t>
+  </si>
+  <si>
+    <t>Enzyme Name</t>
+  </si>
+  <si>
+    <t>delGlb</t>
+  </si>
+  <si>
+    <t>delGub</t>
   </si>
 </sst>
 </file>
@@ -2698,6 +2712,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -4250,7 +4267,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4285,7 +4302,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4880,7 +4897,7 @@
   <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:P83"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6737,2663 +6754,2508 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P83"/>
+  <dimension ref="A1:S83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="6.5703125" customWidth="1"/>
-    <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="8" width="41.5703125" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" customWidth="1"/>
+    <col min="13" max="13" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73" t="s">
+      <c r="B1" t="s">
+        <v>814</v>
+      </c>
+      <c r="C1" s="79" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>815</v>
+      </c>
+      <c r="F1" t="s">
+        <v>816</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="73" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="73" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="73" t="s">
+      <c r="J1" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="76" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="74" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="79" t="s">
+      <c r="K1" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="79" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="73" t="s">
+      <c r="L1" s="73" t="s">
         <v>807</v>
       </c>
-      <c r="J1" s="73" t="s">
+      <c r="M1" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="73" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="73" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="73" t="s">
+      <c r="P1" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="73" t="s">
+      <c r="Q1" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="73" t="s">
+      <c r="R1" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="73" t="s">
+      <c r="S1" s="73" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="11">
-        <v>250</v>
+      <c r="C2" s="77" t="s">
+        <v>303</v>
       </c>
       <c r="D2" s="73">
-        <v>1</v>
-      </c>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73">
         <f>VLOOKUP(A2,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>-9.1</v>
       </c>
-      <c r="G2" s="73">
+      <c r="H2" s="11">
+        <v>250</v>
+      </c>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73">
+        <v>1</v>
+      </c>
+      <c r="K2" s="73">
         <v>20</v>
       </c>
-      <c r="H2" s="77" t="s">
-        <v>303</v>
-      </c>
-      <c r="I2" s="77">
+      <c r="L2" s="77">
         <f>VLOOKUP(A2,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
       <c r="M2" s="73"/>
-      <c r="N2" s="73" t="s">
+      <c r="N2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="73">
+      <c r="R2" s="73">
         <v>5.5599999999999997E-2</v>
       </c>
-      <c r="P2" s="73">
+      <c r="S2" s="73">
         <v>5.5599999999999997E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73">
-        <v>11.09</v>
-      </c>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73">
+      <c r="C3" s="77" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="73">
         <f>VLOOKUP(A3,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>-0.8</v>
       </c>
-      <c r="G3" s="73">
+      <c r="H3" s="73">
+        <v>11.09</v>
+      </c>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73">
         <v>19.801039425479001</v>
       </c>
-      <c r="H3" s="77" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="77" t="str">
+      <c r="L3" s="77" t="str">
         <f>VLOOKUP(A3,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>5.3.1.9</v>
       </c>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
       <c r="M3" s="73"/>
-      <c r="N3" s="73" t="s">
+      <c r="N3" s="73"/>
+      <c r="P3" s="73"/>
+      <c r="Q3" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="73">
+      <c r="R3" s="73">
         <v>3.48</v>
       </c>
-      <c r="P3" s="73">
+      <c r="S3" s="73">
         <v>3.48</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73">
-        <v>49</v>
+      <c r="C4" s="77" t="s">
+        <v>25</v>
       </c>
       <c r="D4" s="73">
-        <v>2.7690000000000001</v>
-      </c>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73">
         <f>VLOOKUP(A4,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>-3.8</v>
       </c>
-      <c r="G4" s="73">
+      <c r="H4" s="73">
+        <v>49</v>
+      </c>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73">
+        <v>2.7690000000000001</v>
+      </c>
+      <c r="K4" s="73">
         <v>19.0346044708484</v>
       </c>
-      <c r="H4" s="77" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="77" t="str">
+      <c r="L4" s="77" t="str">
         <f>VLOOKUP(A4,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>2.7.1.11</v>
       </c>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
       <c r="M4" s="73"/>
-      <c r="N4" s="73" t="s">
+      <c r="N4" s="73"/>
+      <c r="P4" s="73"/>
+      <c r="Q4" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="O4" s="73">
+      <c r="R4" s="73">
         <v>0.6</v>
       </c>
-      <c r="P4" s="73">
+      <c r="S4" s="73">
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>124</v>
       </c>
-      <c r="B5" s="73"/>
-      <c r="C5" s="73">
-        <v>22</v>
+      <c r="C5" s="77" t="s">
+        <v>293</v>
       </c>
       <c r="D5" s="73">
-        <v>0</v>
-      </c>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73">
         <f>VLOOKUP(A5,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>-2.8</v>
       </c>
-      <c r="G5" s="73">
-        <v>0</v>
-      </c>
-      <c r="H5" s="77" t="s">
-        <v>293</v>
-      </c>
-      <c r="I5" s="77" t="str">
+      <c r="H5" s="73">
+        <v>22</v>
+      </c>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73">
+        <v>0</v>
+      </c>
+      <c r="K5" s="73">
+        <v>0</v>
+      </c>
+      <c r="L5" s="77" t="str">
         <f>VLOOKUP(A5,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>3.1.3.11</v>
       </c>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="73"/>
       <c r="M5" s="73"/>
-      <c r="N5" s="73" t="s">
+      <c r="N5" s="73"/>
+      <c r="P5" s="73"/>
+      <c r="Q5" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="O5" s="73">
+      <c r="R5" s="73">
         <v>0.27200000000000002</v>
       </c>
-      <c r="P5" s="73">
+      <c r="S5" s="73">
         <v>0.27200000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73">
-        <v>8.5</v>
-      </c>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73">
+      <c r="C6" s="77" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="73">
         <f>VLOOKUP(A6,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>4.2</v>
       </c>
-      <c r="G6" s="73">
+      <c r="H6" s="73">
+        <v>8.5</v>
+      </c>
+      <c r="I6" s="73"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73">
         <v>19.0346044708484</v>
       </c>
-      <c r="H6" s="77" t="s">
-        <v>80</v>
-      </c>
-      <c r="I6" s="77" t="str">
+      <c r="L6" s="77" t="str">
         <f>VLOOKUP(A6,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>4.1.2.13</v>
       </c>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="73"/>
       <c r="M6" s="73"/>
-      <c r="N6" s="73" t="s">
+      <c r="N6" s="73"/>
+      <c r="P6" s="73"/>
+      <c r="Q6" s="73" t="s">
         <v>796</v>
       </c>
-      <c r="O6" s="73">
+      <c r="R6" s="73">
         <v>0.218</v>
       </c>
-      <c r="P6" s="73">
+      <c r="S6" s="73">
         <v>0.218</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="s">
         <v>125</v>
       </c>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73">
+      <c r="C7" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="73">
+        <v>1.4</v>
+      </c>
+      <c r="H7" s="73">
         <v>56.87</v>
       </c>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73">
-        <v>1.4</v>
-      </c>
-      <c r="G7" s="78">
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="78">
         <v>19.0346044708484</v>
       </c>
-      <c r="H7" s="77" t="s">
-        <v>88</v>
-      </c>
-      <c r="I7" s="77" t="str">
+      <c r="L7" s="77" t="str">
         <f>VLOOKUP(A7,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>5.3.1.1</v>
       </c>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
-      <c r="L7" s="73"/>
       <c r="M7" s="73"/>
-      <c r="N7" s="73" t="s">
+      <c r="N7" s="73"/>
+      <c r="P7" s="73"/>
+      <c r="Q7" s="73" t="s">
         <v>83</v>
       </c>
-      <c r="O7" s="73">
+      <c r="R7" s="73">
         <v>0.16700000000000001</v>
       </c>
-      <c r="P7" s="73">
+      <c r="S7" s="73">
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73">
-        <v>671.72</v>
-      </c>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73">
+      <c r="C8" s="77" t="s">
+        <v>297</v>
+      </c>
+      <c r="D8" s="73">
         <f>VLOOKUP(A8,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>-0.1</v>
       </c>
-      <c r="G8" s="73">
+      <c r="H8" s="73">
+        <v>671.72</v>
+      </c>
+      <c r="I8" s="73"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73">
         <v>37.420015145125497</v>
       </c>
-      <c r="H8" s="77" t="s">
-        <v>297</v>
-      </c>
-      <c r="I8" s="77" t="str">
+      <c r="L8" s="77" t="str">
         <f>VLOOKUP(A8,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>1.2.1.12</v>
       </c>
-      <c r="J8" s="73"/>
-      <c r="K8" s="73"/>
-      <c r="L8" s="73"/>
       <c r="M8" s="73"/>
-      <c r="N8" s="73" t="s">
+      <c r="N8" s="73"/>
+      <c r="P8" s="73"/>
+      <c r="Q8" s="73" t="s">
         <v>187</v>
       </c>
-      <c r="O8" s="73">
+      <c r="R8" s="73">
         <v>2.13</v>
       </c>
-      <c r="P8" s="73">
+      <c r="S8" s="73">
         <v>2.13</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="77" t="s">
         <v>129</v>
       </c>
-      <c r="B9" s="73"/>
-      <c r="C9" s="73">
+      <c r="C9" s="77" t="s">
+        <v>795</v>
+      </c>
+      <c r="D9" s="73">
+        <v>-2.8</v>
+      </c>
+      <c r="H9" s="73">
         <v>2225</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73">
-        <v>-2.8</v>
-      </c>
-      <c r="G9" s="73">
+      <c r="I9" s="73"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73">
         <v>37.420015145125497</v>
       </c>
-      <c r="H9" s="77" t="s">
-        <v>795</v>
-      </c>
-      <c r="I9" s="77" t="str">
+      <c r="L9" s="77" t="str">
         <f>VLOOKUP(A9,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>2.7.2.3</v>
       </c>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="73"/>
       <c r="M9" s="73"/>
-      <c r="N9" s="73" t="s">
+      <c r="N9" s="73"/>
+      <c r="P9" s="73"/>
+      <c r="Q9" s="73" t="s">
         <v>194</v>
       </c>
-      <c r="O9" s="73">
+      <c r="R9" s="73">
         <v>0.39900000000000002</v>
       </c>
-      <c r="P9" s="73">
+      <c r="S9" s="73">
         <v>0.39900000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73">
+      <c r="C10" s="77" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" s="73">
+        <v>4.2</v>
+      </c>
+      <c r="H10" s="73">
         <v>90.55</v>
       </c>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73">
-        <v>4.2</v>
-      </c>
-      <c r="G10" s="73">
+      <c r="I10" s="73"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="73">
         <v>35.968088220815801</v>
       </c>
-      <c r="H10" s="77" t="s">
-        <v>131</v>
-      </c>
-      <c r="I10" s="77" t="str">
+      <c r="L10" s="77" t="str">
         <f>VLOOKUP(A10,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>5.4.2.1</v>
       </c>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
       <c r="M10" s="73"/>
-      <c r="N10" s="73" t="s">
+      <c r="N10" s="73"/>
+      <c r="P10" s="73"/>
+      <c r="Q10" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="O10" s="73">
+      <c r="R10" s="73">
         <v>2.67</v>
       </c>
-      <c r="P10" s="73">
+      <c r="S10" s="73">
         <v>2.67</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="77" t="s">
         <v>134</v>
       </c>
-      <c r="B11" s="73"/>
-      <c r="C11" s="73">
-        <v>355.79</v>
-      </c>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73">
+      <c r="C11" s="77" t="s">
+        <v>302</v>
+      </c>
+      <c r="D11" s="73">
         <f>VLOOKUP(A11,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>-0.9</v>
       </c>
-      <c r="G11" s="73">
+      <c r="H11" s="73">
+        <v>355.79</v>
+      </c>
+      <c r="I11" s="73"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73">
         <v>35.968088220815801</v>
       </c>
-      <c r="H11" s="77" t="s">
-        <v>302</v>
-      </c>
-      <c r="I11" s="77" t="str">
+      <c r="L11" s="77" t="str">
         <f>VLOOKUP(A11,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>4.2.1.11</v>
       </c>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
       <c r="M11" s="73"/>
-      <c r="N11" s="73" t="s">
+      <c r="N11" s="73"/>
+      <c r="P11" s="73"/>
+      <c r="Q11" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="O11" s="73">
+      <c r="R11" s="73">
         <v>2.67</v>
       </c>
-      <c r="P11" s="73">
+      <c r="S11" s="73">
         <v>2.67</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="73"/>
-      <c r="C12" s="73">
-        <v>10.17</v>
-      </c>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73">
+      <c r="C12" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="73">
         <f>VLOOKUP(A12,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>-5.3</v>
       </c>
-      <c r="G12" s="73">
+      <c r="H12" s="73">
+        <v>10.17</v>
+      </c>
+      <c r="I12" s="73"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="73">
         <v>15.464281224553</v>
       </c>
-      <c r="H12" s="77" t="s">
-        <v>34</v>
-      </c>
-      <c r="I12" s="77" t="str">
+      <c r="L12" s="77" t="str">
         <f>VLOOKUP(A12,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>2.7.1.40</v>
       </c>
-      <c r="J12" s="73"/>
-      <c r="K12" s="73"/>
-      <c r="L12" s="73"/>
       <c r="M12" s="73"/>
-      <c r="N12" s="73" t="s">
+      <c r="N12" s="73"/>
+      <c r="P12" s="73"/>
+      <c r="Q12" s="73" t="s">
         <v>797</v>
       </c>
-      <c r="O12" s="73">
+      <c r="R12" s="73">
         <v>0.111</v>
       </c>
-      <c r="P12" s="73">
+      <c r="S12" s="73">
         <v>0.111</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="77" t="s">
         <v>136</v>
       </c>
-      <c r="B13" s="73"/>
-      <c r="C13" s="73">
-        <v>0</v>
+      <c r="C13" s="77" t="s">
+        <v>135</v>
       </c>
       <c r="D13" s="73">
-        <v>0</v>
-      </c>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73">
         <f>VLOOKUP(A13,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>-1.2</v>
       </c>
-      <c r="G13" s="73">
-        <v>0</v>
-      </c>
-      <c r="H13" s="77" t="s">
-        <v>135</v>
-      </c>
-      <c r="I13" s="77" t="str">
+      <c r="H13" s="73">
+        <v>0</v>
+      </c>
+      <c r="I13" s="73"/>
+      <c r="J13" s="73">
+        <v>0</v>
+      </c>
+      <c r="K13" s="73">
+        <v>0</v>
+      </c>
+      <c r="L13" s="77" t="str">
         <f>VLOOKUP(A13,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>2.7.9.2</v>
       </c>
-      <c r="J13" s="73"/>
-      <c r="K13" s="73"/>
-      <c r="L13" s="73"/>
       <c r="M13" s="73"/>
-      <c r="N13" s="73" t="s">
+      <c r="N13" s="73"/>
+      <c r="P13" s="73"/>
+      <c r="Q13" s="73" t="s">
         <v>798</v>
       </c>
-      <c r="O13" s="73">
+      <c r="R13" s="73">
         <v>0.13800000000000001</v>
       </c>
-      <c r="P13" s="73">
+      <c r="S13" s="73">
         <v>0.13800000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="77" t="s">
         <v>140</v>
       </c>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73">
-        <v>6.32</v>
-      </c>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73">
+      <c r="C14" s="77" t="s">
+        <v>139</v>
+      </c>
+      <c r="D14" s="73">
         <f>VLOOKUP(A14,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>-8.3000000000000007</v>
       </c>
-      <c r="G14" s="73">
-        <v>0</v>
-      </c>
-      <c r="H14" s="77" t="s">
-        <v>139</v>
-      </c>
-      <c r="I14" s="77" t="s">
+      <c r="H14" s="73">
+        <v>6.32</v>
+      </c>
+      <c r="I14" s="73"/>
+      <c r="J14" s="73"/>
+      <c r="K14" s="73">
+        <v>0</v>
+      </c>
+      <c r="L14" s="77" t="s">
         <v>808</v>
       </c>
-      <c r="J14" s="73"/>
-      <c r="K14" s="73"/>
-      <c r="L14" s="73"/>
       <c r="M14" s="73"/>
-      <c r="N14" s="73" t="s">
+      <c r="N14" s="73"/>
+      <c r="P14" s="73"/>
+      <c r="Q14" s="73" t="s">
         <v>799</v>
       </c>
-      <c r="O14" s="73">
+      <c r="R14" s="73">
         <v>0.27600000000000002</v>
       </c>
-      <c r="P14" s="73">
+      <c r="S14" s="73">
         <v>0.27600000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="77" t="s">
         <v>239</v>
       </c>
-      <c r="B15" s="73"/>
-      <c r="C15" s="73">
-        <v>81</v>
-      </c>
-      <c r="D15" s="73"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="73">
+      <c r="C15" s="77" t="s">
+        <v>238</v>
+      </c>
+      <c r="D15" s="73">
         <f>VLOOKUP(A15,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>-8.6</v>
       </c>
-      <c r="G15" s="73">
-        <v>0</v>
-      </c>
-      <c r="H15" s="77" t="s">
-        <v>238</v>
-      </c>
-      <c r="I15" s="77" t="s">
+      <c r="H15" s="73">
+        <v>81</v>
+      </c>
+      <c r="I15" s="73"/>
+      <c r="J15" s="73"/>
+      <c r="K15" s="73">
+        <v>0</v>
+      </c>
+      <c r="L15" s="77" t="s">
         <v>812</v>
       </c>
-      <c r="J15" s="73"/>
-      <c r="K15" s="73"/>
-      <c r="L15" s="73"/>
       <c r="M15" s="73"/>
-      <c r="N15" s="73" t="s">
+      <c r="N15" s="73"/>
+      <c r="P15" s="73"/>
+      <c r="Q15" s="73" t="s">
         <v>800</v>
       </c>
-      <c r="O15" s="73">
+      <c r="R15" s="73">
         <v>0.39800000000000002</v>
       </c>
-      <c r="P15" s="73">
+      <c r="S15" s="73">
         <v>0.39800000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="78" t="s">
         <v>317</v>
       </c>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73">
-        <v>5.3</v>
-      </c>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73">
+      <c r="C16" s="78" t="s">
+        <v>240</v>
+      </c>
+      <c r="D16" s="73">
         <f>VLOOKUP(A16,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>1.5</v>
       </c>
-      <c r="G16" s="73">
-        <v>0</v>
-      </c>
-      <c r="H16" s="78" t="s">
-        <v>240</v>
-      </c>
-      <c r="I16" s="77" t="str">
+      <c r="H16" s="73">
+        <v>5.3</v>
+      </c>
+      <c r="I16" s="73"/>
+      <c r="J16" s="73"/>
+      <c r="K16" s="73">
+        <v>0</v>
+      </c>
+      <c r="L16" s="77" t="str">
         <f>VLOOKUP(A16,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>4.2.1.3</v>
       </c>
-      <c r="J16" s="73"/>
-      <c r="K16" s="73"/>
-      <c r="L16" s="73"/>
       <c r="M16" s="73"/>
-      <c r="N16" s="73" t="s">
+      <c r="N16" s="73"/>
+      <c r="P16" s="73"/>
+      <c r="Q16" s="73" t="s">
         <v>801</v>
       </c>
-      <c r="O16" s="73">
+      <c r="R16" s="73">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="P16" s="73">
+      <c r="S16" s="73">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="77" t="s">
         <v>323</v>
       </c>
-      <c r="B17" s="73"/>
-      <c r="C17" s="73">
-        <v>106.4</v>
-      </c>
-      <c r="D17" s="73"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="73">
+      <c r="C17" s="77" t="s">
+        <v>242</v>
+      </c>
+      <c r="D17" s="73">
         <f>VLOOKUP(A17,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>3.4</v>
       </c>
-      <c r="G17" s="73">
-        <v>0</v>
-      </c>
-      <c r="H17" s="77" t="s">
-        <v>242</v>
-      </c>
-      <c r="I17" s="77" t="str">
+      <c r="H17" s="73">
+        <v>106.4</v>
+      </c>
+      <c r="I17" s="73"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="73">
+        <v>0</v>
+      </c>
+      <c r="L17" s="77" t="str">
         <f>VLOOKUP(A17,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>1.1.1.42</v>
       </c>
-      <c r="J17" s="73"/>
-      <c r="K17" s="73"/>
-      <c r="L17" s="73"/>
       <c r="M17" s="73"/>
-      <c r="N17" s="73" t="s">
+      <c r="N17" s="73"/>
+      <c r="P17" s="73"/>
+      <c r="Q17" s="73" t="s">
         <v>195</v>
       </c>
-      <c r="O17" s="73">
+      <c r="R17" s="73">
         <v>0.95499999999999996</v>
       </c>
-      <c r="P17" s="73">
+      <c r="S17" s="73">
         <v>0.95499999999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="77" t="s">
         <v>325</v>
       </c>
-      <c r="B18" s="73"/>
-      <c r="C18" s="73">
-        <v>5.2</v>
-      </c>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73">
+      <c r="C18" s="77" t="s">
+        <v>327</v>
+      </c>
+      <c r="D18" s="73">
         <f>VLOOKUP(A18,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="G18" s="73">
-        <v>0</v>
-      </c>
-      <c r="H18" s="77" t="s">
-        <v>327</v>
-      </c>
-      <c r="I18" s="77" t="str">
+      <c r="H18" s="73">
+        <v>5.2</v>
+      </c>
+      <c r="I18" s="73"/>
+      <c r="J18" s="73"/>
+      <c r="K18" s="73">
+        <v>0</v>
+      </c>
+      <c r="L18" s="77" t="str">
         <f>VLOOKUP(A18,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>4.1.3.1</v>
       </c>
-      <c r="J18" s="73"/>
-      <c r="K18" s="73"/>
-      <c r="L18" s="73"/>
       <c r="M18" s="73"/>
-      <c r="N18" s="73" t="s">
+      <c r="N18" s="73"/>
+      <c r="P18" s="73"/>
+      <c r="Q18" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="O18" s="73">
+      <c r="R18" s="73">
         <v>0.59499999999999997</v>
       </c>
-      <c r="P18" s="73">
+      <c r="S18" s="73">
         <v>0.59499999999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="77" t="s">
         <v>328</v>
       </c>
-      <c r="B19" s="73"/>
-      <c r="C19" s="73">
-        <v>48.1</v>
-      </c>
-      <c r="D19" s="73"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="73">
+      <c r="C19" s="77" t="s">
+        <v>340</v>
+      </c>
+      <c r="D19" s="73">
         <f>VLOOKUP(A19,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>-8.6999999999999993</v>
       </c>
-      <c r="G19" s="73">
-        <v>0</v>
-      </c>
-      <c r="H19" s="77" t="s">
-        <v>340</v>
-      </c>
-      <c r="I19" s="77" t="s">
+      <c r="H19" s="73">
+        <v>48.1</v>
+      </c>
+      <c r="I19" s="73"/>
+      <c r="J19" s="73"/>
+      <c r="K19" s="73">
+        <v>0</v>
+      </c>
+      <c r="L19" s="77" t="s">
         <v>813</v>
       </c>
-      <c r="J19" s="73"/>
-      <c r="K19" s="73"/>
-      <c r="L19" s="73"/>
       <c r="M19" s="73"/>
-      <c r="N19" s="73" t="s">
+      <c r="N19" s="73"/>
+      <c r="P19" s="73"/>
+      <c r="Q19" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="O19" s="73">
+      <c r="R19" s="73">
         <v>4.2699999999999996</v>
       </c>
-      <c r="P19" s="73">
+      <c r="S19" s="73">
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="77" t="s">
         <v>245</v>
       </c>
-      <c r="B20" s="73"/>
-      <c r="C20" s="73">
-        <v>49</v>
-      </c>
-      <c r="D20" s="73"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="73">
+      <c r="C20" s="77" t="s">
+        <v>244</v>
+      </c>
+      <c r="D20" s="73">
         <f>VLOOKUP(A20,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>-8.3000000000000007</v>
       </c>
-      <c r="G20" s="73">
+      <c r="H20" s="73">
+        <v>49</v>
+      </c>
+      <c r="I20" s="73"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="73">
         <v>3.9968753072807401</v>
       </c>
-      <c r="H20" s="77" t="s">
-        <v>244</v>
-      </c>
-      <c r="I20" s="77" t="s">
+      <c r="L20" s="77" t="s">
         <v>809</v>
       </c>
-      <c r="J20" s="73"/>
-      <c r="K20" s="73"/>
-      <c r="L20" s="73"/>
       <c r="M20" s="73"/>
-      <c r="N20" s="73" t="s">
+      <c r="N20" s="73"/>
+      <c r="P20" s="73"/>
+      <c r="Q20" s="73" t="s">
         <v>802</v>
       </c>
-      <c r="O20" s="73">
+      <c r="R20" s="73">
         <v>0.19500000000000001</v>
       </c>
-      <c r="P20" s="73">
+      <c r="S20" s="73">
         <v>0.19500000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="77" t="s">
         <v>332</v>
       </c>
-      <c r="B21" s="73"/>
-      <c r="C21" s="73">
+      <c r="C21" s="77" t="s">
+        <v>246</v>
+      </c>
+      <c r="D21" s="73">
+        <v>-1</v>
+      </c>
+      <c r="H21" s="73">
         <v>44.73</v>
       </c>
-      <c r="D21" s="73"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="73">
-        <v>-1</v>
-      </c>
-      <c r="G21" s="73">
+      <c r="I21" s="73"/>
+      <c r="J21" s="73"/>
+      <c r="K21" s="73">
         <v>-3.9968753072807401</v>
       </c>
-      <c r="H21" s="77" t="s">
-        <v>246</v>
-      </c>
-      <c r="I21" s="77" t="str">
+      <c r="L21" s="77" t="str">
         <f>VLOOKUP(A21,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>6.2.1.5</v>
       </c>
-      <c r="J21" s="73"/>
-      <c r="K21" s="73"/>
-      <c r="L21" s="73"/>
       <c r="M21" s="73"/>
-      <c r="N21" s="73" t="s">
+      <c r="N21" s="73"/>
+      <c r="P21" s="73"/>
+      <c r="Q21" s="73" t="s">
         <v>803</v>
       </c>
-      <c r="O21" s="73">
+      <c r="R21" s="73">
         <v>6.2E-2</v>
       </c>
-      <c r="P21" s="73">
+      <c r="S21" s="73">
         <v>6.2E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="78" t="s">
         <v>334</v>
       </c>
-      <c r="B22" s="73"/>
-      <c r="C22" s="73">
+      <c r="C22" s="78" t="s">
+        <v>248</v>
+      </c>
+      <c r="D22" s="73">
+        <v>-2.1</v>
+      </c>
+      <c r="H22" s="73">
         <v>24</v>
       </c>
-      <c r="D22" s="73"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="73">
-        <v>-2.1</v>
-      </c>
-      <c r="G22" s="73">
+      <c r="I22" s="73"/>
+      <c r="J22" s="73"/>
+      <c r="K22" s="73">
         <v>3.9968753072807401</v>
       </c>
-      <c r="H22" s="78" t="s">
-        <v>248</v>
-      </c>
-      <c r="I22" s="77" t="str">
+      <c r="L22" s="77" t="str">
         <f>VLOOKUP(A22,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>1.3.99.1</v>
       </c>
-      <c r="J22" s="73"/>
-      <c r="K22" s="73"/>
-      <c r="L22" s="73"/>
       <c r="M22" s="73"/>
-      <c r="N22" s="73" t="s">
+      <c r="N22" s="73"/>
+      <c r="P22" s="73"/>
+      <c r="Q22" s="73" t="s">
         <v>100</v>
       </c>
-      <c r="O22" s="73">
+      <c r="R22" s="73">
         <v>1.47</v>
       </c>
-      <c r="P22" s="73">
+      <c r="S22" s="73">
         <v>1.47</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="78" t="s">
         <v>251</v>
       </c>
-      <c r="B23" s="73"/>
-      <c r="C23" s="73">
-        <v>3.4</v>
+      <c r="C23" s="78" t="s">
+        <v>250</v>
       </c>
       <c r="D23" s="73">
-        <v>0</v>
-      </c>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73">
         <f>VLOOKUP(A23,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>5.9</v>
       </c>
-      <c r="G23" s="73">
-        <v>0</v>
-      </c>
-      <c r="H23" s="78" t="s">
-        <v>250</v>
-      </c>
-      <c r="I23" s="77" t="str">
+      <c r="H23" s="73">
+        <v>3.4</v>
+      </c>
+      <c r="I23" s="73"/>
+      <c r="J23" s="73">
+        <v>0</v>
+      </c>
+      <c r="K23" s="73">
+        <v>0</v>
+      </c>
+      <c r="L23" s="77" t="str">
         <f>VLOOKUP(A23,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>1.3.99.1</v>
       </c>
-      <c r="J23" s="73"/>
-      <c r="K23" s="73"/>
-      <c r="L23" s="73"/>
       <c r="M23" s="73"/>
-      <c r="N23" s="73" t="s">
+      <c r="N23" s="73"/>
+      <c r="P23" s="73"/>
+      <c r="Q23" s="73" t="s">
         <v>101</v>
       </c>
-      <c r="O23" s="73">
+      <c r="R23" s="73">
         <v>0.1</v>
       </c>
-      <c r="P23" s="73">
+      <c r="S23" s="73">
         <v>0.1</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="77" t="s">
         <v>252</v>
       </c>
-      <c r="B24" s="73"/>
-      <c r="C24" s="73">
-        <v>51.7</v>
-      </c>
-      <c r="D24" s="73"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="73">
+      <c r="C24" s="77" t="s">
+        <v>263</v>
+      </c>
+      <c r="D24" s="73">
         <f>VLOOKUP(A24,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>-0.6</v>
       </c>
-      <c r="G24" s="73">
+      <c r="H24" s="73">
+        <v>51.7</v>
+      </c>
+      <c r="I24" s="73"/>
+      <c r="J24" s="73"/>
+      <c r="K24" s="73">
         <v>3.9968753072807401</v>
       </c>
-      <c r="H24" s="77" t="s">
-        <v>263</v>
-      </c>
-      <c r="I24" s="77" t="str">
+      <c r="L24" s="77" t="str">
         <f>VLOOKUP(A24,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>4.2.1.2</v>
       </c>
-      <c r="J24" s="73"/>
-      <c r="K24" s="73"/>
-      <c r="L24" s="73"/>
       <c r="M24" s="73"/>
-      <c r="N24" s="73" t="s">
+      <c r="N24" s="73"/>
+      <c r="P24" s="73"/>
+      <c r="Q24" s="73" t="s">
         <v>804</v>
       </c>
-      <c r="O24" s="73">
+      <c r="R24" s="73">
         <v>0.80800000000000005</v>
       </c>
-      <c r="P24" s="73">
+      <c r="S24" s="73">
         <v>0.80800000000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="77" t="s">
         <v>253</v>
       </c>
-      <c r="B25" s="73"/>
-      <c r="C25" s="73">
+      <c r="C25" s="77" t="s">
+        <v>806</v>
+      </c>
+      <c r="D25" s="73">
+        <v>-6.4</v>
+      </c>
+      <c r="H25" s="73">
         <v>1</v>
       </c>
-      <c r="D25" s="73">
+      <c r="I25" s="73"/>
+      <c r="J25" s="73">
         <v>50</v>
       </c>
-      <c r="E25" s="73"/>
-      <c r="F25" s="73">
-        <v>-6.4</v>
-      </c>
-      <c r="G25" s="73">
+      <c r="K25" s="73">
         <v>-1.73406272437436</v>
       </c>
-      <c r="H25" s="77" t="s">
-        <v>806</v>
-      </c>
-      <c r="I25" s="77" t="str">
+      <c r="L25" s="77" t="str">
         <f>VLOOKUP(A25,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>1.1.1.37</v>
       </c>
-      <c r="J25" s="73"/>
-      <c r="K25" s="73"/>
-      <c r="L25" s="73"/>
       <c r="M25" s="73"/>
       <c r="N25" s="73"/>
-      <c r="O25" s="73"/>
       <c r="P25" s="73"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q25" s="73"/>
+      <c r="R25" s="73"/>
+      <c r="S25" s="73"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="77" t="s">
         <v>141</v>
       </c>
-      <c r="B26" s="73"/>
-      <c r="C26" s="73">
-        <v>12.8</v>
-      </c>
-      <c r="D26" s="73"/>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73">
+      <c r="C26" s="77" t="s">
+        <v>142</v>
+      </c>
+      <c r="D26" s="73">
         <f>VLOOKUP(A26,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>-5.0999999999999996</v>
       </c>
-      <c r="G26" s="73">
+      <c r="H26" s="73">
+        <v>12.8</v>
+      </c>
+      <c r="I26" s="73"/>
+      <c r="J26" s="73"/>
+      <c r="K26" s="73">
         <v>34.977749829395002</v>
       </c>
-      <c r="H26" s="77" t="s">
-        <v>142</v>
-      </c>
-      <c r="I26" s="77" t="s">
+      <c r="L26" s="77" t="s">
         <v>810</v>
       </c>
-      <c r="J26" s="73"/>
-      <c r="K26" s="73"/>
-      <c r="L26" s="73"/>
       <c r="M26" s="73"/>
       <c r="N26" s="73"/>
-      <c r="O26" s="73"/>
       <c r="P26" s="73"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q26" s="73"/>
+      <c r="R26" s="73"/>
+      <c r="S26" s="73"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="77" t="s">
         <v>305</v>
       </c>
-      <c r="B27" s="73"/>
-      <c r="C27" s="73">
+      <c r="C27" s="77" t="s">
+        <v>805</v>
+      </c>
+      <c r="D27" s="73">
+        <v>-6.4</v>
+      </c>
+      <c r="H27" s="73">
         <v>320</v>
       </c>
-      <c r="D27" s="73">
-        <v>0</v>
-      </c>
-      <c r="E27" s="73"/>
-      <c r="F27" s="73">
-        <v>-6.4</v>
-      </c>
-      <c r="G27" s="73">
-        <v>0</v>
-      </c>
-      <c r="H27" s="77" t="s">
-        <v>805</v>
-      </c>
-      <c r="I27" s="77" t="str">
+      <c r="I27" s="73"/>
+      <c r="J27" s="73">
+        <v>0</v>
+      </c>
+      <c r="K27" s="73">
+        <v>0</v>
+      </c>
+      <c r="L27" s="77" t="str">
         <f>VLOOKUP(A27,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>1.1.1.28</v>
       </c>
-      <c r="J27" s="73"/>
-      <c r="K27" s="73"/>
-      <c r="L27" s="73"/>
       <c r="M27" s="73"/>
       <c r="N27" s="73"/>
-      <c r="O27" s="73"/>
       <c r="P27" s="73"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q27" s="73"/>
+      <c r="R27" s="73"/>
+      <c r="S27" s="73"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="77" t="s">
         <v>212</v>
       </c>
-      <c r="B28" s="73"/>
-      <c r="C28" s="73">
-        <v>120</v>
+      <c r="C28" s="77" t="s">
+        <v>211</v>
       </c>
       <c r="D28" s="73">
-        <v>0</v>
-      </c>
-      <c r="E28" s="73"/>
-      <c r="F28" s="73">
         <f>VLOOKUP(A28,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>3.8</v>
       </c>
-      <c r="G28" s="78">
+      <c r="H28" s="73">
+        <v>120</v>
+      </c>
+      <c r="I28" s="73"/>
+      <c r="J28" s="73">
+        <v>0</v>
+      </c>
+      <c r="K28" s="78">
         <v>21.2358352193176</v>
       </c>
-      <c r="H28" s="77" t="s">
-        <v>211</v>
-      </c>
-      <c r="I28" s="77" t="str">
+      <c r="L28" s="77" t="str">
         <f>VLOOKUP(A28,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>2.3.1.8</v>
       </c>
-      <c r="J28" s="73"/>
-      <c r="K28" s="73"/>
-      <c r="L28" s="73"/>
       <c r="M28" s="73"/>
       <c r="N28" s="73"/>
-      <c r="O28" s="73"/>
       <c r="P28" s="73"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q28" s="73"/>
+      <c r="R28" s="73"/>
+      <c r="S28" s="73"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="77" t="s">
         <v>214</v>
       </c>
-      <c r="B29" s="73"/>
-      <c r="C29" s="73">
-        <v>280</v>
+      <c r="C29" s="77" t="s">
+        <v>213</v>
       </c>
       <c r="D29" s="73">
-        <v>0</v>
-      </c>
-      <c r="E29" s="73"/>
-      <c r="F29" s="73">
         <f>VLOOKUP(A29,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>4.3</v>
       </c>
-      <c r="G29" s="73">
+      <c r="H29" s="73">
+        <v>280</v>
+      </c>
+      <c r="I29" s="73"/>
+      <c r="J29" s="73">
+        <v>0</v>
+      </c>
+      <c r="K29" s="73">
         <v>-21.2358352193176</v>
       </c>
-      <c r="H29" s="77" t="s">
-        <v>213</v>
-      </c>
-      <c r="I29" s="77" t="str">
+      <c r="L29" s="77" t="str">
         <f>VLOOKUP(A29,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>2.7.2.1</v>
       </c>
-      <c r="J29" s="73"/>
-      <c r="K29" s="73"/>
-      <c r="L29" s="73"/>
       <c r="M29" s="73"/>
       <c r="N29" s="73"/>
-      <c r="O29" s="73"/>
       <c r="P29" s="73"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q29" s="73"/>
+      <c r="R29" s="73"/>
+      <c r="S29" s="73"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="78" t="s">
         <v>144</v>
       </c>
-      <c r="B30" s="73"/>
-      <c r="C30" s="73">
-        <v>15.7</v>
+      <c r="C30" s="78" t="s">
+        <v>143</v>
       </c>
       <c r="D30" s="73">
-        <v>0</v>
-      </c>
-      <c r="E30" s="73"/>
-      <c r="F30" s="73">
         <f>VLOOKUP(A30,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>-4.4000000000000004</v>
       </c>
-      <c r="G30" s="73">
+      <c r="H30" s="73">
+        <v>15.7</v>
+      </c>
+      <c r="I30" s="73"/>
+      <c r="J30" s="73">
+        <v>0</v>
+      </c>
+      <c r="K30" s="73">
         <v>-10.1045270920776</v>
       </c>
-      <c r="H30" s="78" t="s">
-        <v>143</v>
-      </c>
-      <c r="I30" s="77" t="str">
+      <c r="L30" s="77" t="str">
         <f>VLOOKUP(A30,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>1.2.1.10</v>
       </c>
-      <c r="J30" s="73"/>
-      <c r="K30" s="73"/>
-      <c r="L30" s="73"/>
       <c r="M30" s="73"/>
       <c r="N30" s="73"/>
-      <c r="O30" s="73"/>
       <c r="P30" s="73"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q30" s="73"/>
+      <c r="R30" s="73"/>
+      <c r="S30" s="73"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="78" t="s">
         <v>145</v>
       </c>
-      <c r="B31" s="73"/>
-      <c r="C31" s="73">
+      <c r="C31" s="78" t="s">
+        <v>146</v>
+      </c>
+      <c r="D31" s="73">
+        <v>-6</v>
+      </c>
+      <c r="H31" s="73">
         <v>150.19999999999999</v>
       </c>
-      <c r="D31" s="73">
-        <v>0</v>
-      </c>
-      <c r="E31" s="73"/>
-      <c r="F31" s="73">
-        <v>-6</v>
-      </c>
-      <c r="G31" s="73">
+      <c r="I31" s="73"/>
+      <c r="J31" s="73">
+        <v>0</v>
+      </c>
+      <c r="K31" s="73">
         <v>10.1045270920776</v>
       </c>
-      <c r="H31" s="78" t="s">
-        <v>146</v>
-      </c>
-      <c r="I31" s="77" t="str">
+      <c r="L31" s="77" t="str">
         <f>VLOOKUP(A31,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>1.1.1.1</v>
       </c>
-      <c r="J31" s="73"/>
-      <c r="K31" s="73"/>
-      <c r="L31" s="73"/>
       <c r="M31" s="73"/>
       <c r="N31" s="73"/>
-      <c r="O31" s="73"/>
       <c r="P31" s="73"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q31" s="73"/>
+      <c r="R31" s="73"/>
+      <c r="S31" s="73"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="77" t="s">
         <v>415</v>
       </c>
-      <c r="B32" s="73"/>
-      <c r="C32" s="73">
-        <v>174</v>
+      <c r="C32" s="77" t="s">
+        <v>417</v>
       </c>
       <c r="D32" s="73">
-        <v>0.63</v>
-      </c>
-      <c r="E32" s="73"/>
-      <c r="F32" s="73">
         <f>VLOOKUP(A32,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>-1.6</v>
       </c>
-      <c r="G32" s="73">
-        <v>0</v>
-      </c>
-      <c r="H32" s="77" t="s">
-        <v>417</v>
-      </c>
-      <c r="I32" s="77" t="str">
+      <c r="H32" s="73">
+        <v>174</v>
+      </c>
+      <c r="I32" s="73"/>
+      <c r="J32" s="73">
+        <v>0.63</v>
+      </c>
+      <c r="K32" s="73">
+        <v>0</v>
+      </c>
+      <c r="L32" s="77" t="str">
         <f>VLOOKUP(A32,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>1.1.1.49</v>
       </c>
-      <c r="J32" s="73"/>
-      <c r="K32" s="73"/>
-      <c r="L32" s="73"/>
       <c r="M32" s="73"/>
       <c r="N32" s="73"/>
-      <c r="O32" s="73"/>
       <c r="P32" s="73"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q32" s="73"/>
+      <c r="R32" s="73"/>
+      <c r="S32" s="73"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="77" t="s">
         <v>419</v>
       </c>
-      <c r="B33" s="73"/>
-      <c r="C33" s="73">
-        <v>0</v>
-      </c>
-      <c r="D33" s="73"/>
-      <c r="E33" s="73"/>
-      <c r="F33" s="73">
+      <c r="C33" s="77" t="s">
+        <v>421</v>
+      </c>
+      <c r="D33" s="73">
         <f>VLOOKUP(A33,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>-5.0999999999999996</v>
       </c>
-      <c r="G33" s="73">
-        <v>0</v>
-      </c>
-      <c r="H33" s="77" t="s">
-        <v>421</v>
-      </c>
-      <c r="I33" s="77" t="str">
+      <c r="H33" s="73">
+        <v>0</v>
+      </c>
+      <c r="I33" s="73"/>
+      <c r="J33" s="73"/>
+      <c r="K33" s="73">
+        <v>0</v>
+      </c>
+      <c r="L33" s="77" t="str">
         <f>VLOOKUP(A33,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>3.1.1.31</v>
       </c>
-      <c r="J33" s="73"/>
-      <c r="K33" s="73"/>
-      <c r="L33" s="73"/>
       <c r="M33" s="73"/>
       <c r="N33" s="73"/>
-      <c r="O33" s="73"/>
       <c r="P33" s="73"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q33" s="73"/>
+      <c r="R33" s="73"/>
+      <c r="S33" s="73"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="77" t="s">
         <v>422</v>
       </c>
-      <c r="B34" s="73"/>
-      <c r="C34" s="73">
-        <v>75.650000000000006</v>
-      </c>
-      <c r="D34" s="73"/>
-      <c r="E34" s="73"/>
-      <c r="F34" s="73">
+      <c r="C34" s="77" t="s">
+        <v>424</v>
+      </c>
+      <c r="D34" s="73">
         <f>VLOOKUP(A34,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>0.9</v>
       </c>
-      <c r="G34" s="73">
-        <v>0</v>
-      </c>
-      <c r="H34" s="77" t="s">
-        <v>424</v>
-      </c>
-      <c r="I34" s="77" t="str">
+      <c r="H34" s="73">
+        <v>75.650000000000006</v>
+      </c>
+      <c r="I34" s="73"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="73">
+        <v>0</v>
+      </c>
+      <c r="L34" s="77" t="str">
         <f>VLOOKUP(A34,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>1.1.1.44</v>
       </c>
-      <c r="J34" s="73"/>
-      <c r="K34" s="73"/>
-      <c r="L34" s="73"/>
       <c r="M34" s="73"/>
       <c r="N34" s="73"/>
-      <c r="O34" s="73"/>
       <c r="P34" s="73"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q34" s="73"/>
+      <c r="R34" s="73"/>
+      <c r="S34" s="73"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="77" t="s">
         <v>425</v>
       </c>
-      <c r="B35" s="73"/>
-      <c r="C35" s="73">
+      <c r="C35" s="77" t="s">
+        <v>427</v>
+      </c>
+      <c r="D35" s="73">
+        <v>0</v>
+      </c>
+      <c r="H35" s="73">
         <v>21.05</v>
       </c>
-      <c r="D35" s="73"/>
-      <c r="E35" s="73"/>
-      <c r="F35" s="73">
-        <v>0</v>
-      </c>
-      <c r="G35" s="78">
+      <c r="I35" s="73"/>
+      <c r="J35" s="73"/>
+      <c r="K35" s="78">
         <v>-0.69762371202792395</v>
       </c>
-      <c r="H35" s="77" t="s">
-        <v>427</v>
-      </c>
-      <c r="I35" s="77" t="str">
+      <c r="L35" s="77" t="str">
         <f>VLOOKUP(A35,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>5.1.3.1</v>
       </c>
-      <c r="J35" s="73"/>
-      <c r="K35" s="73"/>
-      <c r="L35" s="73"/>
       <c r="M35" s="73"/>
       <c r="N35" s="73"/>
-      <c r="O35" s="73"/>
       <c r="P35" s="73"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q35" s="73"/>
+      <c r="R35" s="73"/>
+      <c r="S35" s="73"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="77" t="s">
         <v>428</v>
       </c>
-      <c r="B36" s="73"/>
-      <c r="C36" s="73">
+      <c r="C36" s="77" t="s">
+        <v>430</v>
+      </c>
+      <c r="D36" s="73">
+        <v>0.5</v>
+      </c>
+      <c r="H36" s="73">
         <v>2100</v>
       </c>
-      <c r="D36" s="73"/>
-      <c r="E36" s="73"/>
-      <c r="F36" s="73">
-        <v>0.5</v>
-      </c>
-      <c r="G36" s="78">
+      <c r="I36" s="73"/>
+      <c r="J36" s="73"/>
+      <c r="K36" s="78">
         <v>-0.69762371202792395</v>
       </c>
-      <c r="H36" s="77" t="s">
-        <v>430</v>
-      </c>
-      <c r="I36" s="77" t="str">
+      <c r="L36" s="77" t="str">
         <f>VLOOKUP(A36,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>5.3.1.6</v>
       </c>
-      <c r="J36" s="73"/>
-      <c r="K36" s="73"/>
-      <c r="L36" s="73"/>
       <c r="M36" s="73"/>
       <c r="N36" s="73"/>
-      <c r="O36" s="73"/>
       <c r="P36" s="73"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q36" s="73"/>
+      <c r="R36" s="73"/>
+      <c r="S36" s="73"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="77" t="s">
         <v>431</v>
       </c>
-      <c r="B37" s="73"/>
-      <c r="C37" s="73">
+      <c r="C37" s="77" t="s">
+        <v>433</v>
+      </c>
+      <c r="D37" s="73">
+        <v>1.9</v>
+      </c>
+      <c r="H37" s="73">
         <v>55.57</v>
       </c>
-      <c r="D37" s="73"/>
-      <c r="E37" s="73"/>
-      <c r="F37" s="73">
-        <v>1.9</v>
-      </c>
-      <c r="G37" s="73">
+      <c r="I37" s="73"/>
+      <c r="J37" s="73"/>
+      <c r="K37" s="73">
         <v>-0.17362949649665499</v>
       </c>
-      <c r="H37" s="77" t="s">
-        <v>433</v>
-      </c>
-      <c r="I37" s="77" t="str">
+      <c r="L37" s="77" t="str">
         <f>VLOOKUP(A37,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>2.2.1.1</v>
       </c>
-      <c r="J37" s="73"/>
-      <c r="K37" s="73"/>
-      <c r="L37" s="73"/>
       <c r="M37" s="73"/>
       <c r="N37" s="73"/>
-      <c r="O37" s="73"/>
       <c r="P37" s="73"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q37" s="73"/>
+      <c r="R37" s="73"/>
+      <c r="S37" s="73"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="77" t="s">
         <v>436</v>
       </c>
-      <c r="B38" s="73"/>
-      <c r="C38" s="73">
+      <c r="C38" s="77" t="s">
+        <v>438</v>
+      </c>
+      <c r="D38" s="73">
+        <v>-1.7</v>
+      </c>
+      <c r="H38" s="73">
         <v>16.57</v>
       </c>
-      <c r="D38" s="73"/>
-      <c r="E38" s="73"/>
-      <c r="F38" s="73">
-        <v>-1.7</v>
-      </c>
-      <c r="G38" s="73">
+      <c r="I38" s="73"/>
+      <c r="J38" s="73"/>
+      <c r="K38" s="73">
         <v>-0.17362949649665499</v>
       </c>
-      <c r="H38" s="77" t="s">
-        <v>438</v>
-      </c>
-      <c r="I38" s="77" t="str">
+      <c r="L38" s="77" t="str">
         <f>VLOOKUP(A38,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>2.2.1.2</v>
       </c>
-      <c r="J38" s="73"/>
-      <c r="K38" s="73"/>
-      <c r="L38" s="73"/>
       <c r="M38" s="73"/>
       <c r="N38" s="73"/>
-      <c r="O38" s="73"/>
       <c r="P38" s="73"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q38" s="73"/>
+      <c r="R38" s="73"/>
+      <c r="S38" s="73"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="77" t="s">
         <v>434</v>
       </c>
-      <c r="B39" s="73"/>
-      <c r="C39" s="73">
+      <c r="C39" s="77" t="s">
+        <v>435</v>
+      </c>
+      <c r="D39" s="73">
+        <v>-1.7</v>
+      </c>
+      <c r="H39" s="73">
         <v>15.45</v>
       </c>
-      <c r="D39" s="73"/>
-      <c r="E39" s="73"/>
-      <c r="F39" s="73">
-        <v>-1.7</v>
-      </c>
-      <c r="G39" s="73">
+      <c r="I39" s="73"/>
+      <c r="J39" s="73"/>
+      <c r="K39" s="73">
         <v>-0.52399421553126901</v>
       </c>
-      <c r="H39" s="77" t="s">
-        <v>435</v>
-      </c>
-      <c r="I39" s="77" t="str">
+      <c r="L39" s="77" t="str">
         <f>VLOOKUP(A39,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>2.2.1.1</v>
       </c>
-      <c r="J39" s="73"/>
-      <c r="K39" s="73"/>
-      <c r="L39" s="73"/>
       <c r="M39" s="73"/>
       <c r="N39" s="73"/>
-      <c r="O39" s="73"/>
       <c r="P39" s="73"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q39" s="73"/>
+      <c r="R39" s="73"/>
+      <c r="S39" s="73"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="78" t="s">
         <v>169</v>
       </c>
-      <c r="B40" s="73"/>
-      <c r="C40" s="73">
-        <v>0</v>
-      </c>
-      <c r="D40" s="73"/>
-      <c r="E40" s="73"/>
-      <c r="F40" s="73">
+      <c r="C40" s="78" t="s">
+        <v>170</v>
+      </c>
+      <c r="D40" s="73">
         <f>VLOOKUP(A40,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>-17.399999999999999</v>
       </c>
-      <c r="G40" s="73">
+      <c r="H40" s="73">
+        <v>0</v>
+      </c>
+      <c r="I40" s="73"/>
+      <c r="J40" s="73"/>
+      <c r="K40" s="73">
         <v>16.0031246927193</v>
       </c>
-      <c r="H40" s="78" t="s">
-        <v>170</v>
-      </c>
-      <c r="I40" s="77" t="str">
+      <c r="L40" s="77" t="str">
         <f>VLOOKUP(A40,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>1.6.5.3</v>
       </c>
-      <c r="J40" s="73"/>
-      <c r="K40" s="73"/>
-      <c r="L40" s="73"/>
       <c r="M40" s="73"/>
       <c r="N40" s="73"/>
-      <c r="O40" s="73"/>
       <c r="P40" s="73"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q40" s="73"/>
+      <c r="R40" s="73"/>
+      <c r="S40" s="73"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="77" t="s">
         <v>441</v>
       </c>
-      <c r="B41" s="73"/>
-      <c r="C41" s="73">
-        <v>0</v>
-      </c>
-      <c r="D41" s="73"/>
-      <c r="E41" s="73"/>
-      <c r="F41" s="73">
+      <c r="C41" s="77" t="s">
+        <v>443</v>
+      </c>
+      <c r="D41" s="73">
         <f>VLOOKUP(A41,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>-0.3</v>
       </c>
-      <c r="G41" s="73">
-        <v>0</v>
-      </c>
-      <c r="H41" s="77" t="s">
-        <v>443</v>
-      </c>
-      <c r="I41" s="77" t="str">
+      <c r="H41" s="73">
+        <v>0</v>
+      </c>
+      <c r="I41" s="73"/>
+      <c r="J41" s="73"/>
+      <c r="K41" s="73">
+        <v>0</v>
+      </c>
+      <c r="L41" s="77" t="str">
         <f>VLOOKUP(A41,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>1.6.1.2</v>
       </c>
-      <c r="J41" s="73"/>
-      <c r="K41" s="73"/>
-      <c r="L41" s="73"/>
       <c r="M41" s="73"/>
       <c r="N41" s="73"/>
-      <c r="O41" s="73"/>
       <c r="P41" s="73"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q41" s="73"/>
+      <c r="R41" s="73"/>
+      <c r="S41" s="73"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="77" t="s">
         <v>444</v>
       </c>
-      <c r="B42" s="73"/>
-      <c r="C42" s="73">
-        <v>0</v>
-      </c>
-      <c r="D42" s="73"/>
-      <c r="E42" s="73"/>
-      <c r="F42" s="73">
+      <c r="C42" s="77" t="s">
+        <v>447</v>
+      </c>
+      <c r="D42" s="73">
         <v>0.3</v>
       </c>
-      <c r="G42" s="73">
+      <c r="H42" s="73">
+        <v>0</v>
+      </c>
+      <c r="I42" s="73"/>
+      <c r="J42" s="73"/>
+      <c r="K42" s="73">
         <v>10.381277508814</v>
       </c>
-      <c r="H42" s="77" t="s">
-        <v>447</v>
-      </c>
-      <c r="I42" s="77" t="str">
+      <c r="L42" s="77" t="str">
         <f>VLOOKUP(A42,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>1.6.1.1</v>
       </c>
-      <c r="J42" s="73"/>
-      <c r="K42" s="73"/>
-      <c r="L42" s="73"/>
       <c r="M42" s="73"/>
       <c r="N42" s="73"/>
-      <c r="O42" s="73"/>
       <c r="P42" s="73"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q42" s="73"/>
+      <c r="R42" s="73"/>
+      <c r="S42" s="73"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="77" t="s">
         <v>178</v>
       </c>
-      <c r="B43" s="73"/>
-      <c r="C43" s="73">
-        <v>0</v>
-      </c>
-      <c r="D43" s="73"/>
-      <c r="E43" s="73"/>
-      <c r="F43" s="73">
+      <c r="C43" s="77" t="s">
+        <v>177</v>
+      </c>
+      <c r="D43" s="73">
         <f>VLOOKUP(A43,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>-0.1</v>
       </c>
-      <c r="G43" s="73">
-        <v>0</v>
-      </c>
-      <c r="H43" s="77" t="s">
-        <v>177</v>
-      </c>
-      <c r="I43" s="77" t="str">
+      <c r="H43" s="73">
+        <v>0</v>
+      </c>
+      <c r="I43" s="73"/>
+      <c r="J43" s="73"/>
+      <c r="K43" s="73">
+        <v>0</v>
+      </c>
+      <c r="L43" s="77" t="str">
         <f>VLOOKUP(A43,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>2.7.4.3</v>
       </c>
-      <c r="J43" s="73"/>
-      <c r="K43" s="73"/>
-      <c r="L43" s="73"/>
       <c r="M43" s="73"/>
       <c r="N43" s="73"/>
-      <c r="O43" s="73"/>
       <c r="P43" s="73"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q43" s="73"/>
+      <c r="R43" s="73"/>
+      <c r="S43" s="73"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="77" t="s">
         <v>171</v>
       </c>
-      <c r="B44" s="73"/>
-      <c r="C44" s="73">
-        <v>0</v>
-      </c>
-      <c r="D44" s="73"/>
-      <c r="E44" s="73"/>
-      <c r="F44" s="73">
+      <c r="C44" s="77" t="s">
+        <v>172</v>
+      </c>
+      <c r="D44" s="73">
         <f>VLOOKUP(A44,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>-6.6</v>
       </c>
-      <c r="G44" s="73">
+      <c r="H44" s="73">
+        <v>0</v>
+      </c>
+      <c r="I44" s="73"/>
+      <c r="J44" s="73"/>
+      <c r="K44" s="73">
         <v>8.39</v>
       </c>
-      <c r="H44" s="77" t="s">
-        <v>172</v>
-      </c>
-      <c r="I44" s="77">
+      <c r="L44" s="77">
         <f>VLOOKUP(A44,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="J44" s="73"/>
-      <c r="K44" s="73"/>
-      <c r="L44" s="73"/>
       <c r="M44" s="73"/>
       <c r="N44" s="73"/>
-      <c r="O44" s="73"/>
       <c r="P44" s="73"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q44" s="73"/>
+      <c r="R44" s="73"/>
+      <c r="S44" s="73"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="77" t="s">
         <v>173</v>
       </c>
-      <c r="B45" s="73"/>
-      <c r="C45" s="73">
-        <v>0</v>
-      </c>
-      <c r="D45" s="73"/>
-      <c r="E45" s="73"/>
-      <c r="F45" s="73">
+      <c r="C45" s="77" t="s">
+        <v>453</v>
+      </c>
+      <c r="D45" s="73">
         <f>VLOOKUP(A45,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>6.6</v>
       </c>
-      <c r="G45" s="73">
+      <c r="H45" s="73">
+        <v>0</v>
+      </c>
+      <c r="I45" s="73"/>
+      <c r="J45" s="73"/>
+      <c r="K45" s="73">
         <v>7.35555836532013</v>
       </c>
-      <c r="H45" s="77" t="s">
-        <v>453</v>
-      </c>
-      <c r="I45" s="77" t="str">
+      <c r="L45" s="77" t="str">
         <f>VLOOKUP(A45,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>3.6.3.14</v>
       </c>
-      <c r="J45" s="73"/>
-      <c r="K45" s="73"/>
-      <c r="L45" s="73"/>
       <c r="M45" s="73"/>
       <c r="N45" s="73"/>
-      <c r="O45" s="73"/>
       <c r="P45" s="73"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q45" s="73"/>
+      <c r="R45" s="73"/>
+      <c r="S45" s="73"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="77" t="s">
         <v>167</v>
       </c>
-      <c r="B46" s="73"/>
-      <c r="C46" s="73">
-        <v>0</v>
-      </c>
-      <c r="D46" s="73"/>
-      <c r="E46" s="73"/>
-      <c r="F46" s="73">
+      <c r="C46" s="77" t="s">
+        <v>168</v>
+      </c>
+      <c r="D46" s="73">
         <f>VLOOKUP(A46,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>-37.200000000000003</v>
       </c>
-      <c r="G46" s="73">
+      <c r="H46" s="73">
+        <v>0</v>
+      </c>
+      <c r="I46" s="73"/>
+      <c r="J46" s="73"/>
+      <c r="K46" s="73">
         <v>20</v>
       </c>
-      <c r="H46" s="77" t="s">
-        <v>168</v>
-      </c>
-      <c r="I46" s="77" t="s">
+      <c r="L46" s="77" t="s">
         <v>811</v>
       </c>
-      <c r="J46" s="73"/>
-      <c r="K46" s="73"/>
-      <c r="L46" s="73"/>
       <c r="M46" s="73"/>
       <c r="N46" s="73"/>
-      <c r="O46" s="73"/>
       <c r="P46" s="73"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q46" s="73"/>
+      <c r="R46" s="73"/>
+      <c r="S46" s="73"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="77" t="s">
         <v>234</v>
       </c>
-      <c r="B47" s="73"/>
-      <c r="C47" s="73">
-        <v>13.74</v>
+      <c r="C47" s="77" t="s">
+        <v>235</v>
       </c>
       <c r="D47" s="73">
-        <v>18.2</v>
-      </c>
-      <c r="E47" s="73"/>
-      <c r="F47" s="73">
         <f>VLOOKUP(A47,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>-6.8</v>
       </c>
-      <c r="G47" s="73">
-        <v>0</v>
-      </c>
-      <c r="H47" s="77" t="s">
-        <v>235</v>
-      </c>
-      <c r="I47" s="77" t="str">
+      <c r="H47" s="73">
+        <v>13.74</v>
+      </c>
+      <c r="I47" s="73"/>
+      <c r="J47" s="73">
+        <v>18.2</v>
+      </c>
+      <c r="K47" s="73">
+        <v>0</v>
+      </c>
+      <c r="L47" s="77" t="str">
         <f>VLOOKUP(A47,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>4.1.1.31</v>
       </c>
-      <c r="J47" s="73"/>
-      <c r="K47" s="73"/>
-      <c r="L47" s="73"/>
       <c r="M47" s="73"/>
       <c r="N47" s="73"/>
-      <c r="O47" s="73"/>
       <c r="P47" s="73"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q47" s="73"/>
+      <c r="R47" s="73"/>
+      <c r="S47" s="73"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="77" t="s">
         <v>237</v>
       </c>
-      <c r="B48" s="73"/>
-      <c r="C48" s="73">
-        <v>0</v>
+      <c r="C48" s="77" t="s">
+        <v>236</v>
       </c>
       <c r="D48" s="73">
-        <v>0</v>
-      </c>
-      <c r="E48" s="73"/>
-      <c r="F48" s="73">
         <f>VLOOKUP(A48,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>0.2</v>
       </c>
-      <c r="G48" s="73">
-        <v>0</v>
-      </c>
-      <c r="H48" s="77" t="s">
-        <v>236</v>
-      </c>
-      <c r="I48" s="77" t="str">
+      <c r="H48" s="73">
+        <v>0</v>
+      </c>
+      <c r="I48" s="73"/>
+      <c r="J48" s="73">
+        <v>0</v>
+      </c>
+      <c r="K48" s="73">
+        <v>0</v>
+      </c>
+      <c r="L48" s="77" t="str">
         <f>VLOOKUP(A48,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>4.1.1.49</v>
       </c>
-      <c r="J48" s="73"/>
-      <c r="K48" s="73"/>
-      <c r="L48" s="73"/>
       <c r="M48" s="73"/>
       <c r="N48" s="73"/>
-      <c r="O48" s="73"/>
       <c r="P48" s="73"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q48" s="73"/>
+      <c r="R48" s="73"/>
+      <c r="S48" s="73"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="77" t="s">
         <v>254</v>
       </c>
-      <c r="B49" s="73"/>
-      <c r="C49" s="73">
-        <v>0</v>
+      <c r="C49" s="77" t="s">
+        <v>262</v>
       </c>
       <c r="D49" s="73">
-        <v>0</v>
-      </c>
-      <c r="E49" s="73"/>
-      <c r="F49" s="73">
         <f>VLOOKUP(A49,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>1.3</v>
       </c>
-      <c r="G49" s="73">
-        <v>0</v>
-      </c>
-      <c r="H49" s="77" t="s">
-        <v>262</v>
-      </c>
-      <c r="I49" s="77" t="str">
+      <c r="H49" s="73">
+        <v>0</v>
+      </c>
+      <c r="I49" s="73"/>
+      <c r="J49" s="73">
+        <v>0</v>
+      </c>
+      <c r="K49" s="73">
+        <v>0</v>
+      </c>
+      <c r="L49" s="77" t="str">
         <f>VLOOKUP(A49,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>1.1.1.38</v>
       </c>
-      <c r="J49" s="73"/>
-      <c r="K49" s="73"/>
-      <c r="L49" s="73"/>
       <c r="M49" s="73"/>
       <c r="N49" s="73"/>
-      <c r="O49" s="73"/>
       <c r="P49" s="73"/>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q49" s="73"/>
+      <c r="R49" s="73"/>
+      <c r="S49" s="73"/>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="77" t="s">
         <v>364</v>
       </c>
-      <c r="B50" s="73"/>
-      <c r="C50" s="73">
-        <v>0</v>
+      <c r="C50" s="77" t="s">
+        <v>367</v>
       </c>
       <c r="D50" s="73">
-        <v>0</v>
-      </c>
-      <c r="E50" s="73"/>
-      <c r="F50" s="73">
         <f>VLOOKUP(A50,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>1.6</v>
       </c>
-      <c r="G50" s="73">
+      <c r="H50" s="73">
+        <v>0</v>
+      </c>
+      <c r="I50" s="73"/>
+      <c r="J50" s="73">
+        <v>0</v>
+      </c>
+      <c r="K50" s="73">
         <v>2.2628125829063799</v>
       </c>
-      <c r="H50" s="77" t="s">
-        <v>367</v>
-      </c>
-      <c r="I50" s="77" t="str">
+      <c r="L50" s="77" t="str">
         <f>VLOOKUP(A50,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>1.1.1.40</v>
       </c>
-      <c r="J50" s="73"/>
-      <c r="K50" s="73"/>
-      <c r="L50" s="73"/>
       <c r="M50" s="73"/>
       <c r="N50" s="73"/>
-      <c r="O50" s="73"/>
       <c r="P50" s="73"/>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q50" s="73"/>
+      <c r="R50" s="73"/>
+      <c r="S50" s="73"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="77" t="s">
         <v>663</v>
       </c>
-      <c r="B51" s="73"/>
-      <c r="C51" s="73"/>
-      <c r="D51" s="73"/>
-      <c r="E51" s="73"/>
-      <c r="F51" s="73">
+      <c r="C51" s="77" t="s">
+        <v>665</v>
+      </c>
+      <c r="D51" s="73">
         <f>VLOOKUP(A51,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G51" s="73">
+      <c r="H51" s="73"/>
+      <c r="I51" s="73"/>
+      <c r="J51" s="73"/>
+      <c r="K51" s="73">
         <v>7.11118951189348</v>
       </c>
-      <c r="H51" s="77" t="s">
-        <v>665</v>
-      </c>
-      <c r="I51" s="77"/>
-      <c r="J51" s="73"/>
-      <c r="K51" s="73"/>
-      <c r="L51" s="73"/>
+      <c r="L51" s="77"/>
       <c r="M51" s="73"/>
       <c r="N51" s="73"/>
-      <c r="O51" s="73"/>
       <c r="P51" s="73"/>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q51" s="73"/>
+      <c r="R51" s="73"/>
+      <c r="S51" s="73"/>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="77" t="s">
         <v>463</v>
       </c>
-      <c r="B52" s="73"/>
-      <c r="C52" s="11">
+      <c r="C52" s="77" t="s">
+        <v>166</v>
+      </c>
+      <c r="D52" s="73">
+        <f>VLOOKUP(A52,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H52" s="11">
         <v>1.6670000000000001E-2</v>
       </c>
-      <c r="D52" s="73"/>
-      <c r="E52" s="73"/>
-      <c r="F52" s="73">
-        <f>VLOOKUP(A52,Sheet3!$A$2:$I$84,6,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="G52" s="73">
+      <c r="I52" s="73"/>
+      <c r="J52" s="73"/>
+      <c r="K52" s="73">
         <v>10</v>
       </c>
-      <c r="H52" s="77" t="s">
-        <v>166</v>
-      </c>
-      <c r="I52" s="77"/>
-      <c r="J52" s="73"/>
-      <c r="K52" s="73"/>
-      <c r="L52" s="73"/>
+      <c r="L52" s="77"/>
       <c r="M52" s="73"/>
       <c r="N52" s="73"/>
-      <c r="O52" s="73"/>
       <c r="P52" s="73"/>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q52" s="73"/>
+      <c r="R52" s="73"/>
+      <c r="S52" s="73"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="77" t="s">
         <v>456</v>
       </c>
-      <c r="B53" s="73"/>
-      <c r="C53" s="73"/>
-      <c r="D53" s="73"/>
-      <c r="E53" s="73"/>
-      <c r="F53" s="73">
+      <c r="C53" s="77" t="s">
+        <v>458</v>
+      </c>
+      <c r="D53" s="73">
         <f>VLOOKUP(A53,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G53" s="73">
+      <c r="H53" s="73"/>
+      <c r="I53" s="73"/>
+      <c r="J53" s="73"/>
+      <c r="K53" s="73">
         <v>3.5703232462952501</v>
       </c>
-      <c r="H53" s="77" t="s">
-        <v>458</v>
-      </c>
-      <c r="I53" s="77"/>
-      <c r="J53" s="73"/>
-      <c r="K53" s="73"/>
-      <c r="L53" s="73"/>
+      <c r="L53" s="77"/>
       <c r="M53" s="73"/>
       <c r="N53" s="73"/>
-      <c r="O53" s="73"/>
       <c r="P53" s="73"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q53" s="73"/>
+      <c r="R53" s="73"/>
+      <c r="S53" s="73"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="77" t="s">
         <v>397</v>
       </c>
-      <c r="B54" s="73"/>
-      <c r="C54" s="73"/>
-      <c r="D54" s="73"/>
-      <c r="E54" s="73"/>
-      <c r="F54" s="73">
+      <c r="C54" s="77" t="s">
+        <v>399</v>
+      </c>
+      <c r="D54" s="73">
         <f>VLOOKUP(A54,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G54" s="73">
+      <c r="H54" s="73"/>
+      <c r="I54" s="73"/>
+      <c r="J54" s="73"/>
+      <c r="K54" s="73">
         <v>-6.25968789018712</v>
       </c>
-      <c r="H54" s="77" t="s">
-        <v>399</v>
-      </c>
-      <c r="I54" s="77"/>
-      <c r="J54" s="73"/>
-      <c r="K54" s="73"/>
-      <c r="L54" s="73"/>
+      <c r="L54" s="77"/>
       <c r="M54" s="73"/>
       <c r="N54" s="73"/>
-      <c r="O54" s="73"/>
       <c r="P54" s="73"/>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q54" s="73"/>
+      <c r="R54" s="73"/>
+      <c r="S54" s="73"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="77" t="s">
         <v>343</v>
       </c>
-      <c r="B55" s="73"/>
-      <c r="C55" s="73"/>
-      <c r="D55" s="73"/>
-      <c r="E55" s="73"/>
-      <c r="F55" s="73">
-        <v>0</v>
-      </c>
-      <c r="G55" s="73">
-        <v>0</v>
-      </c>
-      <c r="H55" s="77" t="s">
+      <c r="C55" s="77" t="s">
         <v>345</v>
       </c>
-      <c r="I55" s="77"/>
+      <c r="D55" s="73">
+        <v>0</v>
+      </c>
+      <c r="H55" s="73"/>
+      <c r="I55" s="73"/>
       <c r="J55" s="73"/>
-      <c r="K55" s="73"/>
-      <c r="L55" s="73"/>
+      <c r="K55" s="73">
+        <v>0</v>
+      </c>
+      <c r="L55" s="77"/>
       <c r="M55" s="73"/>
       <c r="N55" s="73"/>
-      <c r="O55" s="73"/>
       <c r="P55" s="73"/>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q55" s="73"/>
+      <c r="R55" s="73"/>
+      <c r="S55" s="73"/>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="77" t="s">
         <v>346</v>
       </c>
-      <c r="B56" s="73"/>
-      <c r="C56" s="73"/>
-      <c r="D56" s="73"/>
-      <c r="E56" s="73"/>
-      <c r="F56" s="73">
-        <v>0</v>
-      </c>
-      <c r="G56" s="73">
-        <v>0</v>
-      </c>
-      <c r="H56" s="77" t="s">
+      <c r="C56" s="77" t="s">
         <v>352</v>
       </c>
-      <c r="I56" s="77"/>
+      <c r="D56" s="73">
+        <v>0</v>
+      </c>
+      <c r="H56" s="73"/>
+      <c r="I56" s="73"/>
       <c r="J56" s="73"/>
-      <c r="K56" s="73"/>
-      <c r="L56" s="73"/>
+      <c r="K56" s="73">
+        <v>0</v>
+      </c>
+      <c r="L56" s="77"/>
       <c r="M56" s="73"/>
       <c r="N56" s="73"/>
-      <c r="O56" s="73"/>
       <c r="P56" s="73"/>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q56" s="73"/>
+      <c r="R56" s="73"/>
+      <c r="S56" s="73"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="77" t="s">
         <v>349</v>
       </c>
-      <c r="B57" s="73"/>
-      <c r="C57" s="73"/>
-      <c r="D57" s="73"/>
-      <c r="E57" s="73"/>
-      <c r="F57" s="73">
-        <v>0</v>
-      </c>
-      <c r="G57" s="73">
-        <v>0</v>
-      </c>
-      <c r="H57" s="77" t="s">
+      <c r="C57" s="77" t="s">
         <v>351</v>
       </c>
-      <c r="I57" s="77"/>
+      <c r="D57" s="73">
+        <v>0</v>
+      </c>
+      <c r="H57" s="73"/>
+      <c r="I57" s="73"/>
       <c r="J57" s="73"/>
-      <c r="K57" s="73"/>
-      <c r="L57" s="73"/>
+      <c r="K57" s="73">
+        <v>0</v>
+      </c>
+      <c r="L57" s="77"/>
       <c r="M57" s="73"/>
       <c r="N57" s="73"/>
-      <c r="O57" s="73"/>
       <c r="P57" s="73"/>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q57" s="73"/>
+      <c r="R57" s="73"/>
+      <c r="S57" s="73"/>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="77" t="s">
         <v>353</v>
       </c>
-      <c r="B58" s="73"/>
-      <c r="C58" s="73"/>
-      <c r="D58" s="73"/>
-      <c r="E58" s="73"/>
-      <c r="F58" s="73">
+      <c r="C58" s="77" t="s">
+        <v>355</v>
+      </c>
+      <c r="D58" s="73">
         <f>VLOOKUP(A58,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G58" s="73">
-        <v>0</v>
-      </c>
-      <c r="H58" s="77" t="s">
-        <v>355</v>
-      </c>
-      <c r="I58" s="77"/>
+      <c r="H58" s="73"/>
+      <c r="I58" s="73"/>
       <c r="J58" s="73"/>
-      <c r="K58" s="73"/>
-      <c r="L58" s="73"/>
+      <c r="K58" s="73">
+        <v>0</v>
+      </c>
+      <c r="L58" s="77"/>
       <c r="M58" s="73"/>
       <c r="N58" s="73"/>
-      <c r="O58" s="73"/>
       <c r="P58" s="73"/>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q58" s="73"/>
+      <c r="R58" s="73"/>
+      <c r="S58" s="73"/>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="77" t="s">
         <v>356</v>
       </c>
-      <c r="B59" s="73"/>
-      <c r="C59" s="73"/>
-      <c r="D59" s="73"/>
-      <c r="E59" s="73"/>
-      <c r="F59" s="73">
+      <c r="C59" s="77" t="s">
+        <v>359</v>
+      </c>
+      <c r="D59" s="73">
         <f>VLOOKUP(A59,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G59" s="73">
-        <v>0</v>
-      </c>
-      <c r="H59" s="77" t="s">
-        <v>359</v>
-      </c>
-      <c r="I59" s="77"/>
+      <c r="H59" s="73"/>
+      <c r="I59" s="73"/>
       <c r="J59" s="73"/>
-      <c r="K59" s="73"/>
-      <c r="L59" s="73"/>
+      <c r="K59" s="73">
+        <v>0</v>
+      </c>
+      <c r="L59" s="77"/>
       <c r="M59" s="73"/>
       <c r="N59" s="73"/>
-      <c r="O59" s="73"/>
       <c r="P59" s="73"/>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q59" s="73"/>
+      <c r="R59" s="73"/>
+      <c r="S59" s="73"/>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="78" t="s">
         <v>360</v>
       </c>
-      <c r="B60" s="73"/>
-      <c r="C60" s="73"/>
-      <c r="D60" s="73"/>
-      <c r="E60" s="73"/>
-      <c r="F60" s="73">
+      <c r="C60" s="78" t="s">
+        <v>363</v>
+      </c>
+      <c r="D60" s="73">
         <f>VLOOKUP(A60,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G60" s="73">
-        <v>0</v>
-      </c>
-      <c r="H60" s="78" t="s">
-        <v>363</v>
-      </c>
-      <c r="I60" s="77"/>
+      <c r="H60" s="73"/>
+      <c r="I60" s="73"/>
       <c r="J60" s="73"/>
-      <c r="K60" s="73"/>
-      <c r="L60" s="73"/>
+      <c r="K60" s="73">
+        <v>0</v>
+      </c>
+      <c r="L60" s="77"/>
       <c r="M60" s="73"/>
       <c r="N60" s="73"/>
-      <c r="O60" s="73"/>
       <c r="P60" s="73"/>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q60" s="73"/>
+      <c r="R60" s="73"/>
+      <c r="S60" s="73"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="77" t="s">
         <v>368</v>
       </c>
-      <c r="B61" s="73"/>
-      <c r="C61" s="73"/>
-      <c r="D61" s="73"/>
-      <c r="E61" s="73"/>
-      <c r="F61" s="73">
+      <c r="C61" s="77" t="s">
+        <v>371</v>
+      </c>
+      <c r="D61" s="73">
         <f>VLOOKUP(A61,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G61" s="73">
-        <v>0</v>
-      </c>
-      <c r="H61" s="77" t="s">
-        <v>371</v>
-      </c>
-      <c r="I61" s="77"/>
+      <c r="H61" s="73"/>
+      <c r="I61" s="73"/>
       <c r="J61" s="73"/>
-      <c r="K61" s="73"/>
-      <c r="L61" s="73"/>
+      <c r="K61" s="73">
+        <v>0</v>
+      </c>
+      <c r="L61" s="77"/>
       <c r="M61" s="73"/>
       <c r="N61" s="73"/>
-      <c r="O61" s="73"/>
       <c r="P61" s="73"/>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q61" s="73"/>
+      <c r="R61" s="73"/>
+      <c r="S61" s="73"/>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="78" t="s">
         <v>378</v>
       </c>
-      <c r="B62" s="73"/>
-      <c r="C62" s="73"/>
-      <c r="D62" s="73"/>
-      <c r="E62" s="73"/>
-      <c r="F62" s="73">
+      <c r="C62" s="78" t="s">
+        <v>380</v>
+      </c>
+      <c r="D62" s="73">
         <f>VLOOKUP(A62,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G62" s="73">
-        <v>0</v>
-      </c>
-      <c r="H62" s="78" t="s">
-        <v>380</v>
-      </c>
-      <c r="I62" s="77"/>
+      <c r="H62" s="73"/>
+      <c r="I62" s="73"/>
       <c r="J62" s="73"/>
-      <c r="K62" s="73"/>
-      <c r="L62" s="73"/>
+      <c r="K62" s="73">
+        <v>0</v>
+      </c>
+      <c r="L62" s="77"/>
       <c r="M62" s="73"/>
       <c r="N62" s="73"/>
-      <c r="O62" s="73"/>
       <c r="P62" s="73"/>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q62" s="73"/>
+      <c r="R62" s="73"/>
+      <c r="S62" s="73"/>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="78" t="s">
         <v>381</v>
       </c>
-      <c r="B63" s="73"/>
-      <c r="C63" s="73"/>
-      <c r="D63" s="73"/>
-      <c r="E63" s="73"/>
-      <c r="F63" s="73">
+      <c r="C63" s="78" t="s">
+        <v>383</v>
+      </c>
+      <c r="D63" s="73">
         <f>VLOOKUP(A63,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G63" s="73">
+      <c r="H63" s="73"/>
+      <c r="I63" s="73"/>
+      <c r="J63" s="73"/>
+      <c r="K63" s="73">
         <v>34.977749829395002</v>
       </c>
-      <c r="H63" s="78" t="s">
-        <v>383</v>
-      </c>
-      <c r="I63" s="77"/>
-      <c r="J63" s="73"/>
-      <c r="K63" s="73"/>
-      <c r="L63" s="73"/>
+      <c r="L63" s="77"/>
       <c r="M63" s="73"/>
       <c r="N63" s="73"/>
-      <c r="O63" s="73"/>
       <c r="P63" s="73"/>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q63" s="73"/>
+      <c r="R63" s="73"/>
+      <c r="S63" s="73"/>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="77" t="s">
         <v>384</v>
       </c>
-      <c r="B64" s="73"/>
-      <c r="C64" s="73"/>
-      <c r="D64" s="73"/>
-      <c r="E64" s="73"/>
-      <c r="F64" s="73">
+      <c r="C64" s="77" t="s">
+        <v>386</v>
+      </c>
+      <c r="D64" s="73">
         <f>VLOOKUP(A64,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G64" s="73">
+      <c r="H64" s="73"/>
+      <c r="I64" s="73"/>
+      <c r="J64" s="73"/>
+      <c r="K64" s="73">
         <v>-10.1045270920776</v>
       </c>
-      <c r="H64" s="77" t="s">
-        <v>386</v>
-      </c>
-      <c r="I64" s="77"/>
-      <c r="J64" s="73"/>
-      <c r="K64" s="73"/>
-      <c r="L64" s="73"/>
+      <c r="L64" s="77"/>
       <c r="M64" s="73"/>
       <c r="N64" s="73"/>
-      <c r="O64" s="73"/>
       <c r="P64" s="73"/>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q64" s="73"/>
+      <c r="R64" s="73"/>
+      <c r="S64" s="73"/>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="77" t="s">
         <v>387</v>
       </c>
-      <c r="B65" s="73"/>
-      <c r="C65" s="73"/>
-      <c r="D65" s="73"/>
-      <c r="E65" s="73"/>
-      <c r="F65" s="73">
+      <c r="C65" s="77" t="s">
+        <v>389</v>
+      </c>
+      <c r="D65" s="73">
         <f>VLOOKUP(A65,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G65" s="73">
+      <c r="H65" s="73"/>
+      <c r="I65" s="73"/>
+      <c r="J65" s="73"/>
+      <c r="K65" s="73">
         <v>-21.2358352193176</v>
       </c>
-      <c r="H65" s="77" t="s">
-        <v>389</v>
-      </c>
-      <c r="I65" s="77"/>
-      <c r="J65" s="73"/>
-      <c r="K65" s="73"/>
-      <c r="L65" s="73"/>
+      <c r="L65" s="77"/>
       <c r="M65" s="73"/>
       <c r="N65" s="73"/>
-      <c r="O65" s="73"/>
       <c r="P65" s="73"/>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q65" s="73"/>
+      <c r="R65" s="73"/>
+      <c r="S65" s="73"/>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="78" t="s">
         <v>390</v>
       </c>
-      <c r="B66" s="73"/>
-      <c r="C66" s="73"/>
-      <c r="D66" s="73"/>
-      <c r="E66" s="73"/>
-      <c r="F66" s="73">
+      <c r="C66" s="78" t="s">
+        <v>392</v>
+      </c>
+      <c r="D66" s="73">
         <f>VLOOKUP(A66,Sheet3!$A$2:$I$84,6,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G66" s="73">
-        <v>0</v>
-      </c>
-      <c r="H66" s="78" t="s">
-        <v>392</v>
-      </c>
-      <c r="I66" s="77"/>
+      <c r="H66" s="73"/>
+      <c r="I66" s="73"/>
       <c r="J66" s="73"/>
-      <c r="K66" s="73"/>
-      <c r="L66" s="73"/>
+      <c r="K66" s="73">
+        <v>0</v>
+      </c>
+      <c r="L66" s="77"/>
       <c r="M66" s="73"/>
       <c r="N66" s="73"/>
-      <c r="O66" s="73"/>
       <c r="P66" s="73"/>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q66" s="73"/>
+      <c r="R66" s="73"/>
+      <c r="S66" s="73"/>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="77" t="s">
         <v>401</v>
       </c>
-      <c r="B67" s="73"/>
-      <c r="C67" s="73"/>
-      <c r="D67" s="73"/>
-      <c r="E67" s="73"/>
-      <c r="F67" s="73">
-        <v>0</v>
-      </c>
-      <c r="G67" s="73">
-        <v>0</v>
-      </c>
-      <c r="H67" s="77" t="s">
+      <c r="C67" s="77" t="s">
         <v>149</v>
       </c>
-      <c r="I67" s="77"/>
+      <c r="D67" s="73">
+        <v>0</v>
+      </c>
+      <c r="H67" s="73"/>
+      <c r="I67" s="73"/>
       <c r="J67" s="73"/>
-      <c r="K67" s="73"/>
-      <c r="L67" s="73"/>
+      <c r="K67" s="73">
+        <v>0</v>
+      </c>
+      <c r="L67" s="77"/>
       <c r="M67" s="73"/>
       <c r="N67" s="73"/>
-      <c r="O67" s="73"/>
       <c r="P67" s="73"/>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q67" s="73"/>
+      <c r="R67" s="73"/>
+      <c r="S67" s="73"/>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="77" t="s">
         <v>402</v>
       </c>
-      <c r="B68" s="73"/>
-      <c r="C68" s="73"/>
-      <c r="D68" s="73"/>
-      <c r="E68" s="73"/>
-      <c r="F68" s="73">
-        <v>0</v>
-      </c>
-      <c r="G68" s="73">
-        <v>0</v>
-      </c>
-      <c r="H68" s="77" t="s">
+      <c r="C68" s="77" t="s">
         <v>258</v>
       </c>
-      <c r="I68" s="77"/>
+      <c r="D68" s="73">
+        <v>0</v>
+      </c>
+      <c r="H68" s="73"/>
+      <c r="I68" s="73"/>
       <c r="J68" s="73"/>
-      <c r="K68" s="73"/>
-      <c r="L68" s="73"/>
+      <c r="K68" s="73">
+        <v>0</v>
+      </c>
+      <c r="L68" s="77"/>
       <c r="M68" s="73"/>
       <c r="N68" s="73"/>
-      <c r="O68" s="73"/>
       <c r="P68" s="73"/>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q68" s="73"/>
+      <c r="R68" s="73"/>
+      <c r="S68" s="73"/>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="77" t="s">
         <v>403</v>
       </c>
-      <c r="B69" s="73"/>
-      <c r="C69" s="73"/>
-      <c r="D69" s="73"/>
-      <c r="E69" s="73"/>
-      <c r="F69" s="73">
-        <v>0</v>
-      </c>
-      <c r="G69" s="73">
-        <v>0</v>
-      </c>
-      <c r="H69" s="77" t="s">
+      <c r="C69" s="77" t="s">
         <v>256</v>
       </c>
-      <c r="I69" s="77"/>
+      <c r="D69" s="73">
+        <v>0</v>
+      </c>
+      <c r="H69" s="73"/>
+      <c r="I69" s="73"/>
       <c r="J69" s="73"/>
-      <c r="K69" s="73"/>
-      <c r="L69" s="73"/>
+      <c r="K69" s="73">
+        <v>0</v>
+      </c>
+      <c r="L69" s="77"/>
       <c r="M69" s="73"/>
       <c r="N69" s="73"/>
-      <c r="O69" s="73"/>
       <c r="P69" s="73"/>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q69" s="73"/>
+      <c r="R69" s="73"/>
+      <c r="S69" s="73"/>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="77" t="s">
         <v>404</v>
       </c>
-      <c r="B70" s="73"/>
-      <c r="C70" s="73"/>
-      <c r="D70" s="73"/>
-      <c r="E70" s="73"/>
-      <c r="F70" s="73">
-        <v>0</v>
-      </c>
-      <c r="G70" s="73">
-        <v>0</v>
-      </c>
-      <c r="H70" s="77" t="s">
+      <c r="C70" s="77" t="s">
         <v>260</v>
       </c>
-      <c r="I70" s="77"/>
+      <c r="D70" s="73">
+        <v>0</v>
+      </c>
+      <c r="H70" s="73"/>
+      <c r="I70" s="73"/>
       <c r="J70" s="73"/>
-      <c r="K70" s="73"/>
-      <c r="L70" s="73"/>
+      <c r="K70" s="73">
+        <v>0</v>
+      </c>
+      <c r="L70" s="77"/>
       <c r="M70" s="73"/>
       <c r="N70" s="73"/>
-      <c r="O70" s="73"/>
       <c r="P70" s="73"/>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q70" s="73"/>
+      <c r="R70" s="73"/>
+      <c r="S70" s="73"/>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="77" t="s">
         <v>405</v>
       </c>
-      <c r="B71" s="73"/>
-      <c r="C71" s="73"/>
-      <c r="D71" s="73"/>
-      <c r="E71" s="73"/>
-      <c r="F71" s="73">
-        <v>0</v>
-      </c>
-      <c r="G71" s="73">
-        <v>0</v>
-      </c>
-      <c r="H71" s="77" t="s">
+      <c r="C71" s="77" t="s">
         <v>265</v>
       </c>
-      <c r="I71" s="77"/>
+      <c r="D71" s="73">
+        <v>0</v>
+      </c>
+      <c r="H71" s="73"/>
+      <c r="I71" s="73"/>
       <c r="J71" s="73"/>
-      <c r="K71" s="73"/>
-      <c r="L71" s="73"/>
+      <c r="K71" s="73">
+        <v>0</v>
+      </c>
+      <c r="L71" s="77"/>
       <c r="M71" s="73"/>
       <c r="N71" s="73"/>
-      <c r="O71" s="73"/>
       <c r="P71" s="73"/>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q71" s="73"/>
+      <c r="R71" s="73"/>
+      <c r="S71" s="73"/>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="77" t="s">
         <v>406</v>
       </c>
-      <c r="B72" s="73"/>
-      <c r="C72" s="73"/>
-      <c r="D72" s="73"/>
-      <c r="E72" s="73"/>
-      <c r="F72" s="73">
-        <v>0</v>
-      </c>
-      <c r="G72" s="73">
-        <v>0</v>
-      </c>
-      <c r="H72" s="77" t="s">
+      <c r="C72" s="77" t="s">
         <v>152</v>
       </c>
-      <c r="I72" s="77"/>
+      <c r="D72" s="73">
+        <v>0</v>
+      </c>
+      <c r="H72" s="73"/>
+      <c r="I72" s="73"/>
       <c r="J72" s="73"/>
-      <c r="K72" s="73"/>
-      <c r="L72" s="73"/>
+      <c r="K72" s="73">
+        <v>0</v>
+      </c>
+      <c r="L72" s="77"/>
       <c r="M72" s="73"/>
       <c r="N72" s="73"/>
-      <c r="O72" s="73"/>
       <c r="P72" s="73"/>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q72" s="73"/>
+      <c r="R72" s="73"/>
+      <c r="S72" s="73"/>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="77" t="s">
         <v>407</v>
       </c>
-      <c r="B73" s="73"/>
-      <c r="C73" s="73"/>
-      <c r="D73" s="73"/>
-      <c r="E73" s="73"/>
-      <c r="F73" s="73">
-        <v>0</v>
-      </c>
-      <c r="G73" s="73">
+      <c r="C73" s="77" t="s">
+        <v>285</v>
+      </c>
+      <c r="D73" s="73">
+        <v>0</v>
+      </c>
+      <c r="H73" s="73"/>
+      <c r="I73" s="73"/>
+      <c r="J73" s="73"/>
+      <c r="K73" s="73">
         <v>34.977749829395002</v>
       </c>
-      <c r="H73" s="77" t="s">
-        <v>285</v>
-      </c>
-      <c r="I73" s="77"/>
-      <c r="J73" s="73"/>
-      <c r="K73" s="73"/>
-      <c r="L73" s="73"/>
+      <c r="L73" s="77"/>
       <c r="M73" s="73"/>
       <c r="N73" s="73"/>
-      <c r="O73" s="73"/>
       <c r="P73" s="73"/>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q73" s="73"/>
+      <c r="R73" s="73"/>
+      <c r="S73" s="73"/>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="77" t="s">
         <v>408</v>
       </c>
-      <c r="B74" s="73"/>
-      <c r="C74" s="73"/>
-      <c r="D74" s="73"/>
-      <c r="E74" s="73"/>
-      <c r="F74" s="73">
-        <v>0</v>
-      </c>
-      <c r="G74" s="73">
+      <c r="C74" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="D74" s="73">
+        <v>0</v>
+      </c>
+      <c r="H74" s="73"/>
+      <c r="I74" s="73"/>
+      <c r="J74" s="73"/>
+      <c r="K74" s="73">
         <v>10.1045270920776</v>
       </c>
-      <c r="H74" s="77" t="s">
-        <v>161</v>
-      </c>
-      <c r="I74" s="77"/>
-      <c r="J74" s="73"/>
-      <c r="K74" s="73"/>
-      <c r="L74" s="73"/>
+      <c r="L74" s="77"/>
       <c r="M74" s="73"/>
       <c r="N74" s="73"/>
-      <c r="O74" s="73"/>
       <c r="P74" s="73"/>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q74" s="73"/>
+      <c r="R74" s="73"/>
+      <c r="S74" s="73"/>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="77" t="s">
         <v>409</v>
       </c>
-      <c r="B75" s="73"/>
-      <c r="C75" s="73"/>
-      <c r="D75" s="73"/>
-      <c r="E75" s="73"/>
-      <c r="F75" s="73">
-        <v>0</v>
-      </c>
-      <c r="G75" s="73">
+      <c r="C75" s="77" t="s">
+        <v>216</v>
+      </c>
+      <c r="D75" s="73">
+        <v>0</v>
+      </c>
+      <c r="H75" s="73"/>
+      <c r="I75" s="73"/>
+      <c r="J75" s="73"/>
+      <c r="K75" s="73">
         <v>21.2358352193176</v>
       </c>
-      <c r="H75" s="77" t="s">
-        <v>216</v>
-      </c>
-      <c r="I75" s="77"/>
-      <c r="J75" s="73"/>
-      <c r="K75" s="73"/>
-      <c r="L75" s="73"/>
+      <c r="L75" s="77"/>
       <c r="M75" s="73"/>
       <c r="N75" s="73"/>
-      <c r="O75" s="73"/>
       <c r="P75" s="73"/>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q75" s="73"/>
+      <c r="R75" s="73"/>
+      <c r="S75" s="73"/>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="77" t="s">
         <v>410</v>
       </c>
-      <c r="B76" s="73"/>
-      <c r="C76" s="73"/>
-      <c r="D76" s="73"/>
-      <c r="E76" s="73"/>
-      <c r="F76" s="73">
-        <v>0</v>
-      </c>
-      <c r="G76" s="73">
-        <v>0</v>
-      </c>
-      <c r="H76" s="77" t="s">
+      <c r="C76" s="77" t="s">
         <v>157</v>
       </c>
-      <c r="I76" s="77"/>
+      <c r="D76" s="73">
+        <v>0</v>
+      </c>
+      <c r="H76" s="73"/>
+      <c r="I76" s="73"/>
       <c r="J76" s="73"/>
-      <c r="K76" s="73"/>
-      <c r="L76" s="73"/>
+      <c r="K76" s="73">
+        <v>0</v>
+      </c>
+      <c r="L76" s="77"/>
       <c r="M76" s="73"/>
       <c r="N76" s="73"/>
-      <c r="O76" s="73"/>
       <c r="P76" s="73"/>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q76" s="73"/>
+      <c r="R76" s="73"/>
+      <c r="S76" s="73"/>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="77" t="s">
         <v>411</v>
       </c>
-      <c r="B77" s="73"/>
-      <c r="C77" s="73"/>
-      <c r="D77" s="73"/>
-      <c r="E77" s="73"/>
-      <c r="F77" s="73">
-        <v>0</v>
-      </c>
-      <c r="G77" s="73">
+      <c r="C77" s="77" t="s">
+        <v>794</v>
+      </c>
+      <c r="D77" s="73">
+        <v>0</v>
+      </c>
+      <c r="H77" s="73"/>
+      <c r="I77" s="73"/>
+      <c r="J77" s="73"/>
+      <c r="K77" s="73">
         <v>-20</v>
       </c>
-      <c r="H77" s="77" t="s">
-        <v>794</v>
-      </c>
-      <c r="I77" s="77"/>
-      <c r="J77" s="73"/>
-      <c r="K77" s="73"/>
-      <c r="L77" s="73"/>
+      <c r="L77" s="77"/>
       <c r="M77" s="73"/>
       <c r="N77" s="73"/>
-      <c r="O77" s="73"/>
       <c r="P77" s="73"/>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q77" s="73"/>
+      <c r="R77" s="73"/>
+      <c r="S77" s="73"/>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="77" t="s">
         <v>412</v>
       </c>
-      <c r="B78" s="73"/>
-      <c r="C78" s="73"/>
-      <c r="D78" s="73"/>
-      <c r="E78" s="73"/>
-      <c r="F78" s="73">
-        <v>0</v>
-      </c>
-      <c r="G78" s="73">
+      <c r="C78" s="77" t="s">
+        <v>400</v>
+      </c>
+      <c r="D78" s="73">
+        <v>0</v>
+      </c>
+      <c r="H78" s="73"/>
+      <c r="I78" s="73"/>
+      <c r="J78" s="73"/>
+      <c r="K78" s="73">
         <v>6.25968789018712</v>
       </c>
-      <c r="H78" s="77" t="s">
-        <v>400</v>
-      </c>
-      <c r="I78" s="77"/>
-      <c r="J78" s="73"/>
-      <c r="K78" s="73"/>
-      <c r="L78" s="73"/>
+      <c r="L78" s="77"/>
       <c r="M78" s="73"/>
       <c r="N78" s="73"/>
-      <c r="O78" s="73"/>
       <c r="P78" s="73"/>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q78" s="73"/>
+      <c r="R78" s="73"/>
+      <c r="S78" s="73"/>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="77" t="s">
         <v>413</v>
       </c>
-      <c r="B79" s="73"/>
-      <c r="C79" s="73"/>
-      <c r="D79" s="73"/>
-      <c r="E79" s="73"/>
-      <c r="F79" s="73">
-        <v>0</v>
-      </c>
-      <c r="G79" s="73">
+      <c r="C79" s="77" t="s">
+        <v>205</v>
+      </c>
+      <c r="D79" s="73">
+        <v>0</v>
+      </c>
+      <c r="H79" s="73"/>
+      <c r="I79" s="73"/>
+      <c r="J79" s="73"/>
+      <c r="K79" s="73">
         <v>65.594624664349297</v>
       </c>
-      <c r="H79" s="77" t="s">
-        <v>205</v>
-      </c>
-      <c r="I79" s="77"/>
-      <c r="J79" s="73"/>
-      <c r="K79" s="73"/>
-      <c r="L79" s="73"/>
+      <c r="L79" s="77"/>
       <c r="M79" s="73"/>
       <c r="N79" s="73"/>
-      <c r="O79" s="73"/>
       <c r="P79" s="73"/>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q79" s="73"/>
+      <c r="R79" s="73"/>
+      <c r="S79" s="73"/>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="77" t="s">
         <v>414</v>
       </c>
-      <c r="B80" s="73"/>
-      <c r="C80" s="73"/>
-      <c r="D80" s="73"/>
-      <c r="E80" s="73"/>
-      <c r="F80" s="73">
-        <v>0</v>
-      </c>
-      <c r="G80" s="73">
+      <c r="C80" s="77" t="s">
+        <v>206</v>
+      </c>
+      <c r="D80" s="73">
+        <v>0</v>
+      </c>
+      <c r="H80" s="73"/>
+      <c r="I80" s="73"/>
+      <c r="J80" s="73"/>
+      <c r="K80" s="73">
         <v>-7.11118951189348</v>
       </c>
-      <c r="H80" s="77" t="s">
-        <v>206</v>
-      </c>
-      <c r="I80" s="77"/>
-      <c r="J80" s="73"/>
-      <c r="K80" s="73"/>
-      <c r="L80" s="73"/>
+      <c r="L80" s="77"/>
       <c r="M80" s="73"/>
       <c r="N80" s="73"/>
-      <c r="O80" s="73"/>
       <c r="P80" s="73"/>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q80" s="73"/>
+      <c r="R80" s="73"/>
+      <c r="S80" s="73"/>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" s="77" t="s">
         <v>460</v>
       </c>
-      <c r="B81" s="73"/>
-      <c r="C81" s="73"/>
-      <c r="D81" s="73"/>
-      <c r="E81" s="73"/>
-      <c r="F81" s="73">
-        <v>0</v>
-      </c>
-      <c r="G81" s="73">
+      <c r="C81" s="77" t="s">
+        <v>209</v>
+      </c>
+      <c r="D81" s="73">
+        <v>0</v>
+      </c>
+      <c r="H81" s="73"/>
+      <c r="I81" s="73"/>
+      <c r="J81" s="73"/>
+      <c r="K81" s="73">
         <v>-3.5703232462952501</v>
       </c>
-      <c r="H81" s="77" t="s">
-        <v>209</v>
-      </c>
-      <c r="I81" s="77"/>
-      <c r="J81" s="73"/>
-      <c r="K81" s="73"/>
-      <c r="L81" s="73"/>
+      <c r="L81" s="77"/>
       <c r="M81" s="73"/>
       <c r="N81" s="73"/>
-      <c r="O81" s="73"/>
       <c r="P81" s="73"/>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q81" s="73"/>
+      <c r="R81" s="73"/>
+      <c r="S81" s="73"/>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" s="77" t="s">
         <v>461</v>
       </c>
-      <c r="B82" s="73"/>
-      <c r="C82" s="73"/>
-      <c r="D82" s="73"/>
-      <c r="E82" s="73"/>
-      <c r="F82" s="73">
-        <v>0</v>
-      </c>
-      <c r="G82" s="73">
+      <c r="C82" s="77" t="s">
+        <v>462</v>
+      </c>
+      <c r="D82" s="73">
+        <v>0</v>
+      </c>
+      <c r="H82" s="73"/>
+      <c r="I82" s="73"/>
+      <c r="J82" s="73"/>
+      <c r="K82" s="73">
         <v>-10</v>
       </c>
-      <c r="H82" s="77" t="s">
-        <v>462</v>
-      </c>
-      <c r="I82" s="77"/>
-      <c r="J82" s="73"/>
-      <c r="K82" s="73"/>
-      <c r="L82" s="73"/>
+      <c r="L82" s="77"/>
       <c r="M82" s="73"/>
       <c r="N82" s="73"/>
-      <c r="O82" s="73"/>
       <c r="P82" s="73"/>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q82" s="73"/>
+      <c r="R82" s="73"/>
+      <c r="S82" s="73"/>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" s="78" t="s">
         <v>179</v>
       </c>
-      <c r="B83" s="73"/>
-      <c r="C83" s="73"/>
-      <c r="D83" s="73"/>
-      <c r="E83" s="73"/>
-      <c r="F83" s="73">
-        <v>0</v>
-      </c>
-      <c r="G83" s="73">
-        <v>0.97053938790751804</v>
-      </c>
-      <c r="H83" s="78" t="s">
+      <c r="C83" s="78" t="s">
         <v>793</v>
       </c>
+      <c r="D83" s="73">
+        <v>0</v>
+      </c>
+      <c r="H83" s="73"/>
       <c r="I83" s="73"/>
       <c r="J83" s="73"/>
-      <c r="K83" s="73"/>
+      <c r="K83" s="73">
+        <v>0.97053938790751804</v>
+      </c>
       <c r="L83" s="73"/>
       <c r="M83" s="73"/>
       <c r="N83" s="73"/>
-      <c r="O83" s="73"/>
       <c r="P83" s="73"/>
+      <c r="Q83" s="73"/>
+      <c r="R83" s="73"/>
+      <c r="S83" s="73"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Working version w/o Vmax estimation
</commit_message>
<xml_diff>
--- a/KineticModel/ecoli_test.xlsx
+++ b/KineticModel/ecoli_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="780" windowWidth="18195" windowHeight="6825" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="480" yWindow="840" windowWidth="18195" windowHeight="6765" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="ecoliT1" sheetId="1" r:id="rId1"/>
@@ -20,16 +20,17 @@
     <sheet name="Sheet1" sheetId="13" r:id="rId11"/>
     <sheet name="ecoliN2" sheetId="10" r:id="rId12"/>
     <sheet name="Sheet3" sheetId="12" r:id="rId13"/>
+    <sheet name="Sheet4" sheetId="14" r:id="rId14"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId14"/>
+    <externalReference r:id="rId15"/>
   </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1737" uniqueCount="833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="834">
   <si>
     <t>Enzymes</t>
   </si>
@@ -2570,6 +2571,9 @@
   </si>
   <si>
     <t>[c] : h + oaa + pi &lt;==&gt; co2 + h2o + pep</t>
+  </si>
+  <si>
+    <t>0.28,0.147</t>
   </si>
 </sst>
 </file>
@@ -2775,7 +2779,7 @@
       <sheetName val="metabolites"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="1">
           <cell r="A1" t="str">
@@ -4263,8 +4267,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4942,7 +4946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
@@ -6803,8 +6807,8 @@
   <dimension ref="A1:T83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6907,9 +6911,7 @@
         <v>250</v>
       </c>
       <c r="J2" s="73"/>
-      <c r="K2" s="73">
-        <v>1</v>
-      </c>
+      <c r="K2" s="73"/>
       <c r="L2" s="84">
         <v>20</v>
       </c>
@@ -6953,13 +6955,15 @@
       <c r="J3" s="73"/>
       <c r="K3" s="73"/>
       <c r="L3" s="84">
-        <v>19.801039425479001</v>
+        <v>19.641084088999801</v>
       </c>
       <c r="M3" s="77" t="str">
         <f>VLOOKUP(A3,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>5.3.1.9</v>
       </c>
-      <c r="N3" s="73"/>
+      <c r="N3" s="73" t="s">
+        <v>833</v>
+      </c>
       <c r="O3" s="73"/>
       <c r="Q3" s="73"/>
       <c r="R3" s="73" t="s">
@@ -6993,11 +6997,9 @@
         <v>49</v>
       </c>
       <c r="J4" s="73"/>
-      <c r="K4" s="73">
-        <v>2.7690000000000001</v>
-      </c>
+      <c r="K4" s="73"/>
       <c r="L4" s="84">
-        <v>19.0346044708484</v>
+        <v>18.2584699674542</v>
       </c>
       <c r="M4" s="77" t="str">
         <f>VLOOKUP(A4,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -7037,9 +7039,7 @@
         <v>22</v>
       </c>
       <c r="J5" s="73"/>
-      <c r="K5" s="73">
-        <v>0</v>
-      </c>
+      <c r="K5" s="73"/>
       <c r="L5" s="84">
         <v>0</v>
       </c>
@@ -7084,7 +7084,7 @@
       <c r="J6" s="73"/>
       <c r="K6" s="73"/>
       <c r="L6" s="84">
-        <v>19.0346044708484</v>
+        <v>18.2584699674542</v>
       </c>
       <c r="M6" s="77" t="str">
         <f>VLOOKUP(A6,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -7129,7 +7129,7 @@
       <c r="J7" s="73"/>
       <c r="K7" s="73"/>
       <c r="L7" s="85">
-        <v>-19.0346044708484</v>
+        <v>-18.2584699674542</v>
       </c>
       <c r="M7" s="77" t="str">
         <f>VLOOKUP(A7,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -7171,7 +7171,7 @@
       <c r="J8" s="73"/>
       <c r="K8" s="73"/>
       <c r="L8" s="84">
-        <v>37.420015145125497</v>
+        <v>35.345823579454603</v>
       </c>
       <c r="M8" s="77" t="str">
         <f>VLOOKUP(A8,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -7213,7 +7213,7 @@
       <c r="J9" s="73"/>
       <c r="K9" s="73"/>
       <c r="L9" s="84">
-        <v>-37.420015145125497</v>
+        <v>-35.345823579454603</v>
       </c>
       <c r="M9" s="77" t="str">
         <f>VLOOKUP(A9,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -7255,7 +7255,7 @@
       <c r="J10" s="73"/>
       <c r="K10" s="73"/>
       <c r="L10" s="84">
-        <v>-35.968088220815801</v>
+        <v>-32.726612833814102</v>
       </c>
       <c r="M10" s="77" t="str">
         <f>VLOOKUP(A10,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -7297,7 +7297,7 @@
       <c r="J11" s="73"/>
       <c r="K11" s="73"/>
       <c r="L11" s="84">
-        <v>35.968088220815801</v>
+        <v>32.726612833814102</v>
       </c>
       <c r="M11" s="77" t="str">
         <f>VLOOKUP(A11,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -7337,9 +7337,11 @@
         <v>10.17</v>
       </c>
       <c r="J12" s="73"/>
-      <c r="K12" s="73"/>
+      <c r="K12" s="73">
+        <v>0.97</v>
+      </c>
       <c r="L12" s="84">
-        <v>-15.464281224553</v>
+        <v>-15.8997796489202</v>
       </c>
       <c r="M12" s="77" t="str">
         <f>VLOOKUP(A12,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -7379,9 +7381,7 @@
         <v>1</v>
       </c>
       <c r="J13" s="73"/>
-      <c r="K13" s="73">
-        <v>0</v>
-      </c>
+      <c r="K13" s="73"/>
       <c r="L13" s="84">
         <v>0</v>
       </c>
@@ -7425,7 +7425,7 @@
       <c r="J14" s="73"/>
       <c r="K14" s="73"/>
       <c r="L14" s="84">
-        <v>0</v>
+        <v>8.4636074707051101</v>
       </c>
       <c r="M14" s="77" t="s">
         <v>820</v>
@@ -7465,7 +7465,7 @@
       <c r="J15" s="73"/>
       <c r="K15" s="73"/>
       <c r="L15" s="84">
-        <v>0</v>
+        <v>7.2101829496634</v>
       </c>
       <c r="M15" s="77" t="s">
         <v>811</v>
@@ -7506,7 +7506,7 @@
       <c r="J16" s="73"/>
       <c r="K16" s="73"/>
       <c r="L16" s="84">
-        <v>0</v>
+        <v>-7.2101829496634</v>
       </c>
       <c r="M16" s="77" t="str">
         <f>VLOOKUP(A16,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -7548,7 +7548,7 @@
       <c r="J17" s="73"/>
       <c r="K17" s="73"/>
       <c r="L17" s="84">
-        <v>0</v>
+        <v>-7.2101829496634</v>
       </c>
       <c r="M17" s="77" t="str">
         <f>VLOOKUP(A17,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -7672,7 +7672,7 @@
       <c r="J20" s="73"/>
       <c r="K20" s="73"/>
       <c r="L20" s="84">
-        <v>3.9968753072807401</v>
+        <v>0</v>
       </c>
       <c r="M20" s="77" t="s">
         <v>808</v>
@@ -7713,7 +7713,7 @@
       <c r="J21" s="73"/>
       <c r="K21" s="73"/>
       <c r="L21" s="84">
-        <v>-3.9968753072807401</v>
+        <v>0</v>
       </c>
       <c r="M21" s="77" t="str">
         <f>VLOOKUP(A21,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -7754,7 +7754,7 @@
       <c r="J22" s="73"/>
       <c r="K22" s="73"/>
       <c r="L22" s="84">
-        <v>3.9968753072807401</v>
+        <v>100</v>
       </c>
       <c r="M22" s="77" t="str">
         <f>VLOOKUP(A22,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -7792,15 +7792,10 @@
       <c r="H23" s="73">
         <v>250</v>
       </c>
-      <c r="I23">
-        <v>110</v>
-      </c>
       <c r="J23" s="73"/>
-      <c r="K23" s="73">
-        <v>0</v>
-      </c>
+      <c r="K23" s="73"/>
       <c r="L23" s="84">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="M23" s="77" t="str">
         <f>VLOOKUP(A23,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -7838,13 +7833,10 @@
       <c r="H24" s="73">
         <v>51.7</v>
       </c>
-      <c r="I24">
-        <v>11.2</v>
-      </c>
       <c r="J24" s="73"/>
       <c r="K24" s="73"/>
       <c r="L24" s="84">
-        <v>-3.9968753072807401</v>
+        <v>0</v>
       </c>
       <c r="M24" s="77" t="str">
         <f>VLOOKUP(A24,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -7887,7 +7879,7 @@
         <v>50</v>
       </c>
       <c r="L25" s="84">
-        <v>1.73406272437436</v>
+        <v>0</v>
       </c>
       <c r="M25" s="77" t="str">
         <f>VLOOKUP(A25,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -7919,13 +7911,12 @@
       <c r="H26" s="73">
         <v>12.8</v>
       </c>
-      <c r="I26">
-        <v>4</v>
-      </c>
       <c r="J26" s="73"/>
-      <c r="K26" s="73"/>
+      <c r="K26" s="73">
+        <v>0.125</v>
+      </c>
       <c r="L26" s="84">
-        <v>-34.977749829395002</v>
+        <v>-22.476479530989</v>
       </c>
       <c r="M26" s="77" t="s">
         <v>809</v>
@@ -7958,9 +7949,7 @@
       </c>
       <c r="I27" s="73"/>
       <c r="J27" s="73"/>
-      <c r="K27" s="73">
-        <v>0</v>
-      </c>
+      <c r="K27" s="73"/>
       <c r="L27" s="84">
         <v>0</v>
       </c>
@@ -7996,11 +7985,9 @@
         <v>120</v>
       </c>
       <c r="J28" s="73"/>
-      <c r="K28" s="73">
-        <v>0</v>
-      </c>
+      <c r="K28" s="73"/>
       <c r="L28" s="85">
-        <v>21.2358352193176</v>
+        <v>31.588586774545199</v>
       </c>
       <c r="M28" s="77" t="str">
         <f>VLOOKUP(A28,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -8034,11 +8021,9 @@
         <v>280</v>
       </c>
       <c r="J29" s="73"/>
-      <c r="K29" s="73">
-        <v>0</v>
-      </c>
+      <c r="K29" s="73"/>
       <c r="L29" s="84">
-        <v>-21.2358352193176</v>
+        <v>-31.588586774545199</v>
       </c>
       <c r="M29" s="77" t="str">
         <f>VLOOKUP(A29,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -8072,11 +8057,9 @@
         <v>15.7</v>
       </c>
       <c r="J30" s="73"/>
-      <c r="K30" s="73">
-        <v>0</v>
-      </c>
+      <c r="K30" s="73"/>
       <c r="L30" s="84">
-        <v>-10.1045270920776</v>
+        <v>0</v>
       </c>
       <c r="M30" s="77" t="str">
         <f>VLOOKUP(A30,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -8110,11 +8093,9 @@
         <v>150.19999999999999</v>
       </c>
       <c r="J31" s="73"/>
-      <c r="K31" s="73">
-        <v>0</v>
-      </c>
+      <c r="K31" s="73"/>
       <c r="L31" s="84">
-        <v>-10.1045270920776</v>
+        <v>0</v>
       </c>
       <c r="M31" s="77" t="str">
         <f>VLOOKUP(A31,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -8260,7 +8241,7 @@
       <c r="J35" s="73"/>
       <c r="K35" s="73"/>
       <c r="L35" s="85">
-        <v>-0.69762371202792395</v>
+        <v>-1.2584817406192199</v>
       </c>
       <c r="M35" s="77" t="str">
         <f>VLOOKUP(A35,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -8295,7 +8276,7 @@
       <c r="J36" s="73"/>
       <c r="K36" s="73"/>
       <c r="L36" s="85">
-        <v>-0.69762371202792395</v>
+        <v>-1.2584817406192199</v>
       </c>
       <c r="M36" s="77" t="str">
         <f>VLOOKUP(A36,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -8331,7 +8312,7 @@
       <c r="J37" s="73"/>
       <c r="K37" s="73"/>
       <c r="L37" s="84">
-        <v>0.17362949649665499</v>
+        <v>0.31321978769724201</v>
       </c>
       <c r="M37" s="77" t="str">
         <f>VLOOKUP(A37,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -8366,7 +8347,7 @@
       <c r="J38" s="73"/>
       <c r="K38" s="73"/>
       <c r="L38" s="84">
-        <v>-0.17362949649665499</v>
+        <v>-0.31321978769724201</v>
       </c>
       <c r="M38" s="77" t="str">
         <f>VLOOKUP(A38,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -8404,7 +8385,7 @@
       <c r="J39" s="73"/>
       <c r="K39" s="73"/>
       <c r="L39" s="84">
-        <v>0.52399421553126901</v>
+        <v>0.94526195292197401</v>
       </c>
       <c r="M39" s="77" t="str">
         <f>VLOOKUP(A39,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -8440,7 +8421,7 @@
       <c r="J40" s="73"/>
       <c r="K40" s="73"/>
       <c r="L40" s="84">
-        <v>-16.0031246927193</v>
+        <v>-20</v>
       </c>
       <c r="M40" s="77" t="str">
         <f>VLOOKUP(A40,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -8477,7 +8458,7 @@
       <c r="J41" s="73"/>
       <c r="K41" s="73"/>
       <c r="L41" s="84">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="M41" s="77" t="str">
         <f>VLOOKUP(A41,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -8513,7 +8494,7 @@
       <c r="J42" s="73"/>
       <c r="K42" s="73"/>
       <c r="L42" s="84">
-        <v>-10.381277508814</v>
+        <v>69.980448284876005</v>
       </c>
       <c r="M42" s="77" t="str">
         <f>VLOOKUP(A42,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -8584,10 +8565,7 @@
       <c r="L44" s="84">
         <v>8.39</v>
       </c>
-      <c r="M44" s="77">
-        <f>VLOOKUP(A44,[1]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>0</v>
-      </c>
+      <c r="M44" s="77"/>
       <c r="N44" s="73"/>
       <c r="O44" s="73"/>
       <c r="Q44" s="73"/>
@@ -8612,16 +8590,14 @@
       <c r="G45" s="11">
         <v>42000</v>
       </c>
-      <c r="H45" s="73">
-        <v>3800</v>
-      </c>
+      <c r="H45" s="73"/>
       <c r="I45">
         <v>2200</v>
       </c>
       <c r="J45" s="73"/>
       <c r="K45" s="73"/>
       <c r="L45" s="84">
-        <v>-7.35555836532013</v>
+        <v>-48.530185510493098</v>
       </c>
       <c r="M45" s="77" t="str">
         <f>VLOOKUP(A45,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -8682,9 +8658,6 @@
       <c r="F47">
         <v>55.6</v>
       </c>
-      <c r="H47">
-        <v>13.74</v>
-      </c>
       <c r="I47" s="73">
         <v>540</v>
       </c>
@@ -8693,7 +8666,7 @@
         <v>18.2</v>
       </c>
       <c r="L47" s="84">
-        <v>0</v>
+        <v>4.0820119341314696</v>
       </c>
       <c r="M47" s="77" t="str">
         <f>VLOOKUP(A47,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -8727,9 +8700,7 @@
         <v>1</v>
       </c>
       <c r="J48" s="73"/>
-      <c r="K48" s="73">
-        <v>0</v>
-      </c>
+      <c r="K48" s="73"/>
       <c r="L48" s="84">
         <v>0</v>
       </c>
@@ -8765,9 +8736,7 @@
         <v>1</v>
       </c>
       <c r="J49" s="73"/>
-      <c r="K49" s="73">
-        <v>0</v>
-      </c>
+      <c r="K49" s="73"/>
       <c r="L49" s="84">
         <v>0</v>
       </c>
@@ -8803,11 +8772,9 @@
         <v>1</v>
       </c>
       <c r="J50" s="73"/>
-      <c r="K50" s="73">
-        <v>0</v>
-      </c>
+      <c r="K50" s="73"/>
       <c r="L50" s="84">
-        <v>2.2628125829063799</v>
+        <v>0</v>
       </c>
       <c r="M50" s="77" t="str">
         <f>VLOOKUP(A50,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -8840,7 +8807,7 @@
       <c r="J51" s="73"/>
       <c r="K51" s="73"/>
       <c r="L51" s="84">
-        <v>7.11118951189348</v>
+        <v>0.55691231785686302</v>
       </c>
       <c r="M51" s="77"/>
       <c r="N51" s="73"/>
@@ -8900,7 +8867,7 @@
       <c r="J53" s="73"/>
       <c r="K53" s="73"/>
       <c r="L53" s="84">
-        <v>3.5703232462952501</v>
+        <v>6.4407022526654396</v>
       </c>
       <c r="M53" s="77"/>
       <c r="N53" s="73"/>
@@ -8930,7 +8897,7 @@
       <c r="J54" s="73"/>
       <c r="K54" s="73"/>
       <c r="L54" s="84">
-        <v>-6.25968789018712</v>
+        <v>-5.3354364551731797</v>
       </c>
       <c r="M54" s="77"/>
       <c r="N54" s="73"/>
@@ -9197,7 +9164,7 @@
       <c r="J63" s="73"/>
       <c r="K63" s="73"/>
       <c r="L63" s="84">
-        <v>34.977749829395002</v>
+        <v>22.476479530989</v>
       </c>
       <c r="M63" s="77"/>
       <c r="N63" s="73"/>
@@ -9227,7 +9194,7 @@
       <c r="J64" s="73"/>
       <c r="K64" s="73"/>
       <c r="L64" s="84">
-        <v>-10.1045270920776</v>
+        <v>0</v>
       </c>
       <c r="M64" s="77"/>
       <c r="N64" s="73"/>
@@ -9257,7 +9224,7 @@
       <c r="J65" s="73"/>
       <c r="K65" s="73"/>
       <c r="L65" s="84">
-        <v>-21.2358352193176</v>
+        <v>-31.588586774545199</v>
       </c>
       <c r="M65" s="77"/>
       <c r="N65" s="73"/>
@@ -9455,7 +9422,7 @@
       <c r="J73" s="73"/>
       <c r="K73" s="73"/>
       <c r="L73" s="84">
-        <v>34.977749829395002</v>
+        <v>22.476479530989</v>
       </c>
       <c r="M73" s="77"/>
       <c r="N73" s="73"/>
@@ -9479,7 +9446,7 @@
       <c r="J74" s="73"/>
       <c r="K74" s="73"/>
       <c r="L74" s="84">
-        <v>10.1045270920776</v>
+        <v>0</v>
       </c>
       <c r="M74" s="77"/>
       <c r="N74" s="73"/>
@@ -9503,7 +9470,7 @@
       <c r="J75" s="73"/>
       <c r="K75" s="73"/>
       <c r="L75" s="84">
-        <v>21.2358352193176</v>
+        <v>31.588586774545199</v>
       </c>
       <c r="M75" s="77"/>
       <c r="N75" s="73"/>
@@ -9575,7 +9542,7 @@
       <c r="J78" s="73"/>
       <c r="K78" s="73"/>
       <c r="L78" s="84">
-        <v>6.25968789018712</v>
+        <v>5.3354364551731797</v>
       </c>
       <c r="M78" s="77"/>
       <c r="N78" s="73"/>
@@ -9599,7 +9566,7 @@
       <c r="J79" s="73"/>
       <c r="K79" s="73"/>
       <c r="L79" s="84">
-        <v>65.594624664349297</v>
+        <v>70.988039049659307</v>
       </c>
       <c r="M79" s="77"/>
       <c r="N79" s="73"/>
@@ -9623,7 +9590,7 @@
       <c r="J80" s="73"/>
       <c r="K80" s="73"/>
       <c r="L80" s="84">
-        <v>-7.11118951189348</v>
+        <v>-0.55691231785686302</v>
       </c>
       <c r="M80" s="77"/>
       <c r="N80" s="73"/>
@@ -9647,7 +9614,7 @@
       <c r="J81" s="73"/>
       <c r="K81" s="73"/>
       <c r="L81" s="84">
-        <v>-3.5703232462952501</v>
+        <v>-6.4407022526654396</v>
       </c>
       <c r="M81" s="77"/>
       <c r="N81" s="73"/>
@@ -9695,7 +9662,7 @@
       <c r="J83" s="73"/>
       <c r="K83" s="73"/>
       <c r="L83" s="84">
-        <v>0.97053938790751804</v>
+        <v>1.7508093219521601</v>
       </c>
       <c r="M83" s="73"/>
       <c r="N83" s="73"/>
@@ -11031,7 +10998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L96"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="I83" sqref="I83"/>
     </sheetView>
   </sheetViews>
@@ -14356,6 +14323,3261 @@
   <sortState ref="A2:L85">
     <sortCondition ref="D2:D85"/>
   </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T83"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection sqref="A1:T83"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="73" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="73" t="s">
+        <v>813</v>
+      </c>
+      <c r="C1" s="79" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="73" t="s">
+        <v>814</v>
+      </c>
+      <c r="F1" s="73" t="s">
+        <v>815</v>
+      </c>
+      <c r="G1" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="73" t="s">
+        <v>816</v>
+      </c>
+      <c r="I1" s="73" t="s">
+        <v>817</v>
+      </c>
+      <c r="J1" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="73" t="s">
+        <v>807</v>
+      </c>
+      <c r="N1" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="73" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="73" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="73" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="73" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="73" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="77" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="73"/>
+      <c r="C2" s="77" t="s">
+        <v>303</v>
+      </c>
+      <c r="D2" s="73">
+        <f>VLOOKUP(A2,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-9.1</v>
+      </c>
+      <c r="E2" s="73">
+        <v>-50.4</v>
+      </c>
+      <c r="F2" s="73">
+        <v>0.9</v>
+      </c>
+      <c r="G2" s="73"/>
+      <c r="H2" s="86">
+        <v>250</v>
+      </c>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73">
+        <v>1</v>
+      </c>
+      <c r="L2" s="84">
+        <v>20</v>
+      </c>
+      <c r="M2" s="77">
+        <f>VLOOKUP(A2,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="73"/>
+      <c r="R2" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="73">
+        <v>5.5599999999999997E-2</v>
+      </c>
+      <c r="T2" s="73">
+        <v>5.5599999999999997E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="77" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="73"/>
+      <c r="C3" s="77" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="73">
+        <f>VLOOKUP(A3,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-0.8</v>
+      </c>
+      <c r="E3" s="73">
+        <v>-17.100000000000001</v>
+      </c>
+      <c r="F3" s="73">
+        <v>20.6</v>
+      </c>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73">
+        <v>11.09</v>
+      </c>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="84">
+        <v>19.801039425479001</v>
+      </c>
+      <c r="M3" s="77" t="str">
+        <f>VLOOKUP(A3,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.3.1.9</v>
+      </c>
+      <c r="N3" s="73" t="s">
+        <v>833</v>
+      </c>
+      <c r="O3" s="73"/>
+      <c r="P3" s="73"/>
+      <c r="Q3" s="73"/>
+      <c r="R3" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="S3" s="73">
+        <v>3.48</v>
+      </c>
+      <c r="T3" s="73">
+        <v>3.48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="77" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="73"/>
+      <c r="C4" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="73">
+        <f>VLOOKUP(A4,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-3.8</v>
+      </c>
+      <c r="E4" s="73">
+        <v>-53.9</v>
+      </c>
+      <c r="F4" s="73">
+        <v>21.4</v>
+      </c>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73">
+        <v>49</v>
+      </c>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73">
+        <v>2.7690000000000001</v>
+      </c>
+      <c r="L4" s="84">
+        <v>19.0346044708484</v>
+      </c>
+      <c r="M4" s="77" t="str">
+        <f>VLOOKUP(A4,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.1.11</v>
+      </c>
+      <c r="N4" s="73"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="73"/>
+      <c r="Q4" s="73"/>
+      <c r="R4" s="73" t="s">
+        <v>29</v>
+      </c>
+      <c r="S4" s="73">
+        <v>0.6</v>
+      </c>
+      <c r="T4" s="73">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="77" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="73"/>
+      <c r="C5" s="77" t="s">
+        <v>293</v>
+      </c>
+      <c r="D5" s="73">
+        <f>VLOOKUP(A5,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-2.8</v>
+      </c>
+      <c r="E5" s="73">
+        <v>-48.8</v>
+      </c>
+      <c r="F5" s="73">
+        <v>-9.6999999999999993</v>
+      </c>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73">
+        <v>22</v>
+      </c>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73">
+        <v>0</v>
+      </c>
+      <c r="L5" s="84">
+        <v>0</v>
+      </c>
+      <c r="M5" s="77" t="str">
+        <f>VLOOKUP(A5,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>3.1.3.11</v>
+      </c>
+      <c r="N5" s="73"/>
+      <c r="O5" s="73"/>
+      <c r="P5" s="73"/>
+      <c r="Q5" s="73"/>
+      <c r="R5" s="73" t="s">
+        <v>32</v>
+      </c>
+      <c r="S5" s="73">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="T5" s="73">
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="77" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="73"/>
+      <c r="C6" s="77" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="73">
+        <f>VLOOKUP(A6,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>4.2</v>
+      </c>
+      <c r="E6" s="73">
+        <v>-29.4</v>
+      </c>
+      <c r="F6" s="73">
+        <v>27.1</v>
+      </c>
+      <c r="G6" s="11"/>
+      <c r="H6" s="73">
+        <v>8.5</v>
+      </c>
+      <c r="I6" s="73"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
+      <c r="L6" s="84">
+        <v>19.0346044708484</v>
+      </c>
+      <c r="M6" s="77" t="str">
+        <f>VLOOKUP(A6,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.1.2.13</v>
+      </c>
+      <c r="N6" s="73"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="73"/>
+      <c r="Q6" s="73"/>
+      <c r="R6" s="73" t="s">
+        <v>796</v>
+      </c>
+      <c r="S6" s="73">
+        <v>0.218</v>
+      </c>
+      <c r="T6" s="73">
+        <v>0.218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="77" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="73"/>
+      <c r="C7" s="77" t="s">
+        <v>818</v>
+      </c>
+      <c r="D7" s="73">
+        <v>-1.4</v>
+      </c>
+      <c r="E7" s="73">
+        <v>-24.3</v>
+      </c>
+      <c r="F7" s="73">
+        <v>13.4</v>
+      </c>
+      <c r="G7" s="73">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73">
+        <v>9000</v>
+      </c>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="85">
+        <v>-19.0346044708484</v>
+      </c>
+      <c r="M7" s="77" t="str">
+        <f>VLOOKUP(A7,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.3.1.1</v>
+      </c>
+      <c r="N7" s="73"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="73"/>
+      <c r="Q7" s="73"/>
+      <c r="R7" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="S7" s="73">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="T7" s="73">
+        <v>0.16700000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="77" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="73"/>
+      <c r="C8" s="77" t="s">
+        <v>297</v>
+      </c>
+      <c r="D8" s="73">
+        <f>VLOOKUP(A8,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="E8" s="73">
+        <v>-12.8</v>
+      </c>
+      <c r="F8" s="73">
+        <v>62.6</v>
+      </c>
+      <c r="G8" s="73"/>
+      <c r="H8" s="73">
+        <v>671.72</v>
+      </c>
+      <c r="I8" s="73"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="84">
+        <v>37.420015145125497</v>
+      </c>
+      <c r="M8" s="77" t="str">
+        <f>VLOOKUP(A8,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.2.1.12</v>
+      </c>
+      <c r="N8" s="73"/>
+      <c r="O8" s="73"/>
+      <c r="P8" s="73"/>
+      <c r="Q8" s="73"/>
+      <c r="R8" s="73" t="s">
+        <v>187</v>
+      </c>
+      <c r="S8" s="73">
+        <v>2.13</v>
+      </c>
+      <c r="T8" s="73">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="77" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="73"/>
+      <c r="C9" s="77" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" s="73">
+        <v>2.8</v>
+      </c>
+      <c r="E9" s="73">
+        <v>-19.2</v>
+      </c>
+      <c r="F9" s="73">
+        <v>56.1</v>
+      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73">
+        <v>2225</v>
+      </c>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="84">
+        <v>-37.420015145125497</v>
+      </c>
+      <c r="M9" s="77" t="str">
+        <f>VLOOKUP(A9,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.2.3</v>
+      </c>
+      <c r="N9" s="73"/>
+      <c r="O9" s="73"/>
+      <c r="P9" s="73"/>
+      <c r="Q9" s="73"/>
+      <c r="R9" s="73" t="s">
+        <v>194</v>
+      </c>
+      <c r="S9" s="73">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="T9" s="73">
+        <v>0.39900000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="77" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" s="73"/>
+      <c r="C10" s="77" t="s">
+        <v>300</v>
+      </c>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73">
+        <v>-23.1</v>
+      </c>
+      <c r="F10" s="73">
+        <v>14.6</v>
+      </c>
+      <c r="G10" s="73">
+        <v>5.49</v>
+      </c>
+      <c r="H10" s="73"/>
+      <c r="I10" s="73">
+        <v>90.55</v>
+      </c>
+      <c r="J10" s="73"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="84">
+        <v>-35.968088220815801</v>
+      </c>
+      <c r="M10" s="77" t="str">
+        <f>VLOOKUP(A10,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.4.2.1</v>
+      </c>
+      <c r="N10" s="73"/>
+      <c r="O10" s="73"/>
+      <c r="P10" s="73"/>
+      <c r="Q10" s="73"/>
+      <c r="R10" s="73" t="s">
+        <v>23</v>
+      </c>
+      <c r="S10" s="73">
+        <v>2.67</v>
+      </c>
+      <c r="T10" s="73">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="77" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" s="73"/>
+      <c r="C11" s="77" t="s">
+        <v>302</v>
+      </c>
+      <c r="D11" s="73">
+        <f>VLOOKUP(A11,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-0.9</v>
+      </c>
+      <c r="E11" s="73">
+        <v>-22.9</v>
+      </c>
+      <c r="F11" s="73">
+        <v>14.7</v>
+      </c>
+      <c r="G11" s="73"/>
+      <c r="H11" s="73">
+        <v>355.79</v>
+      </c>
+      <c r="I11" s="73"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="84">
+        <v>35.968088220815801</v>
+      </c>
+      <c r="M11" s="77" t="str">
+        <f>VLOOKUP(A11,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.2.1.11</v>
+      </c>
+      <c r="N11" s="73"/>
+      <c r="O11" s="73"/>
+      <c r="P11" s="73"/>
+      <c r="Q11" s="73"/>
+      <c r="R11" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="S11" s="73">
+        <v>2.67</v>
+      </c>
+      <c r="T11" s="73">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="73"/>
+      <c r="C12" s="77" t="s">
+        <v>819</v>
+      </c>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73">
+        <v>-10.8</v>
+      </c>
+      <c r="F12" s="73">
+        <v>65.3</v>
+      </c>
+      <c r="G12" s="11">
+        <v>1.4E-5</v>
+      </c>
+      <c r="H12" s="73"/>
+      <c r="I12" s="73">
+        <v>10.17</v>
+      </c>
+      <c r="J12" s="73"/>
+      <c r="K12" s="73"/>
+      <c r="L12" s="84">
+        <v>-15.464281224553</v>
+      </c>
+      <c r="M12" s="77" t="str">
+        <f>VLOOKUP(A12,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.1.40</v>
+      </c>
+      <c r="N12" s="73"/>
+      <c r="O12" s="73"/>
+      <c r="P12" s="73"/>
+      <c r="Q12" s="73"/>
+      <c r="R12" s="73" t="s">
+        <v>797</v>
+      </c>
+      <c r="S12" s="73">
+        <v>0.111</v>
+      </c>
+      <c r="T12" s="73">
+        <v>0.111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="77" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" s="73"/>
+      <c r="C13" s="77" t="s">
+        <v>135</v>
+      </c>
+      <c r="D13" s="73">
+        <f>VLOOKUP(A13,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-1.2</v>
+      </c>
+      <c r="E13" s="73">
+        <v>-50.9</v>
+      </c>
+      <c r="F13" s="73">
+        <v>24.4</v>
+      </c>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73">
+        <v>1</v>
+      </c>
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="73">
+        <v>0</v>
+      </c>
+      <c r="L13" s="84">
+        <v>0</v>
+      </c>
+      <c r="M13" s="77" t="str">
+        <f>VLOOKUP(A13,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.9.2</v>
+      </c>
+      <c r="N13" s="73"/>
+      <c r="O13" s="73"/>
+      <c r="P13" s="73"/>
+      <c r="Q13" s="73"/>
+      <c r="R13" s="73" t="s">
+        <v>798</v>
+      </c>
+      <c r="S13" s="73">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="T13" s="73">
+        <v>0.13800000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="77" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" s="73"/>
+      <c r="C14" s="77" t="s">
+        <v>139</v>
+      </c>
+      <c r="D14" s="73">
+        <f>VLOOKUP(A14,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-8.3000000000000007</v>
+      </c>
+      <c r="E14" s="73">
+        <v>-73</v>
+      </c>
+      <c r="F14" s="73">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G14" s="73"/>
+      <c r="H14" s="73">
+        <v>6.32</v>
+      </c>
+      <c r="I14" s="73"/>
+      <c r="J14" s="73"/>
+      <c r="K14" s="73"/>
+      <c r="L14" s="84">
+        <v>0</v>
+      </c>
+      <c r="M14" s="77" t="s">
+        <v>820</v>
+      </c>
+      <c r="N14" s="73"/>
+      <c r="O14" s="73"/>
+      <c r="P14" s="73"/>
+      <c r="Q14" s="73"/>
+      <c r="R14" s="73" t="s">
+        <v>799</v>
+      </c>
+      <c r="S14" s="73">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="T14" s="73">
+        <v>0.27600000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="77" t="s">
+        <v>239</v>
+      </c>
+      <c r="B15" s="73"/>
+      <c r="C15" s="77" t="s">
+        <v>821</v>
+      </c>
+      <c r="D15" s="73">
+        <v>8.6</v>
+      </c>
+      <c r="E15" s="73">
+        <v>-4</v>
+      </c>
+      <c r="F15" s="73">
+        <v>60.9</v>
+      </c>
+      <c r="G15" s="73"/>
+      <c r="H15" s="73"/>
+      <c r="I15" s="73">
+        <v>81</v>
+      </c>
+      <c r="J15" s="73"/>
+      <c r="K15" s="73"/>
+      <c r="L15" s="84">
+        <v>0</v>
+      </c>
+      <c r="M15" s="77" t="s">
+        <v>811</v>
+      </c>
+      <c r="N15" s="73"/>
+      <c r="O15" s="73"/>
+      <c r="P15" s="73"/>
+      <c r="Q15" s="73"/>
+      <c r="R15" s="73" t="s">
+        <v>800</v>
+      </c>
+      <c r="S15" s="73">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="T15" s="73">
+        <v>0.39800000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="78" t="s">
+        <v>317</v>
+      </c>
+      <c r="B16" s="73"/>
+      <c r="C16" s="78" t="s">
+        <v>240</v>
+      </c>
+      <c r="D16" s="73">
+        <f>VLOOKUP(A16,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>1.5</v>
+      </c>
+      <c r="E16" s="73">
+        <v>-11.2</v>
+      </c>
+      <c r="F16" s="73">
+        <v>26.5</v>
+      </c>
+      <c r="G16" s="73"/>
+      <c r="H16" s="73">
+        <v>5.3</v>
+      </c>
+      <c r="I16" s="73"/>
+      <c r="J16" s="73"/>
+      <c r="K16" s="73"/>
+      <c r="L16" s="84">
+        <v>0</v>
+      </c>
+      <c r="M16" s="77" t="str">
+        <f>VLOOKUP(A16,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.2.1.3</v>
+      </c>
+      <c r="N16" s="73"/>
+      <c r="O16" s="73"/>
+      <c r="P16" s="73"/>
+      <c r="Q16" s="73"/>
+      <c r="R16" s="73" t="s">
+        <v>801</v>
+      </c>
+      <c r="S16" s="73">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="T16" s="73">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="77" t="s">
+        <v>323</v>
+      </c>
+      <c r="B17" s="73"/>
+      <c r="C17" s="77" t="s">
+        <v>242</v>
+      </c>
+      <c r="D17" s="73">
+        <f>VLOOKUP(A17,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>3.4</v>
+      </c>
+      <c r="E17" s="73">
+        <v>-48.4</v>
+      </c>
+      <c r="F17" s="73">
+        <v>26.9</v>
+      </c>
+      <c r="G17" s="73"/>
+      <c r="H17" s="73">
+        <v>106.4</v>
+      </c>
+      <c r="I17" s="73"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="73"/>
+      <c r="L17" s="84">
+        <v>0</v>
+      </c>
+      <c r="M17" s="77" t="str">
+        <f>VLOOKUP(A17,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.1.1.42</v>
+      </c>
+      <c r="N17" s="73"/>
+      <c r="O17" s="73"/>
+      <c r="P17" s="73"/>
+      <c r="Q17" s="73"/>
+      <c r="R17" s="73" t="s">
+        <v>195</v>
+      </c>
+      <c r="S17" s="73">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="T17" s="73">
+        <v>0.95499999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="77" t="s">
+        <v>325</v>
+      </c>
+      <c r="B18" s="73"/>
+      <c r="C18" s="77" t="s">
+        <v>327</v>
+      </c>
+      <c r="D18" s="73">
+        <f>VLOOKUP(A18,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E18" s="73">
+        <v>-38.700000000000003</v>
+      </c>
+      <c r="F18" s="73">
+        <v>17.8</v>
+      </c>
+      <c r="G18" s="73"/>
+      <c r="H18" s="73">
+        <v>5.2</v>
+      </c>
+      <c r="I18" s="73"/>
+      <c r="J18" s="73"/>
+      <c r="K18" s="73"/>
+      <c r="L18" s="84">
+        <v>0</v>
+      </c>
+      <c r="M18" s="77" t="str">
+        <f>VLOOKUP(A18,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.1.3.1</v>
+      </c>
+      <c r="N18" s="73"/>
+      <c r="O18" s="73"/>
+      <c r="P18" s="73"/>
+      <c r="Q18" s="73"/>
+      <c r="R18" s="73" t="s">
+        <v>38</v>
+      </c>
+      <c r="S18" s="73">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="T18" s="73">
+        <v>0.59499999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="77" t="s">
+        <v>328</v>
+      </c>
+      <c r="B19" s="73"/>
+      <c r="C19" s="77" t="s">
+        <v>822</v>
+      </c>
+      <c r="D19" s="73">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E19" s="73">
+        <v>-9.1</v>
+      </c>
+      <c r="F19" s="73">
+        <v>63.1</v>
+      </c>
+      <c r="G19" s="73"/>
+      <c r="H19" s="73"/>
+      <c r="I19" s="73">
+        <v>48.1</v>
+      </c>
+      <c r="J19" s="73"/>
+      <c r="K19" s="73"/>
+      <c r="L19" s="84">
+        <v>0</v>
+      </c>
+      <c r="M19" s="77" t="s">
+        <v>812</v>
+      </c>
+      <c r="N19" s="73"/>
+      <c r="O19" s="73"/>
+      <c r="P19" s="73"/>
+      <c r="Q19" s="73"/>
+      <c r="R19" s="73" t="s">
+        <v>41</v>
+      </c>
+      <c r="S19" s="73">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="T19" s="73">
+        <v>4.2699999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="77" t="s">
+        <v>245</v>
+      </c>
+      <c r="B20" s="73"/>
+      <c r="C20" s="77" t="s">
+        <v>244</v>
+      </c>
+      <c r="D20" s="73">
+        <f>VLOOKUP(A20,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-8.3000000000000007</v>
+      </c>
+      <c r="E20" s="73">
+        <v>-72.3</v>
+      </c>
+      <c r="F20" s="73">
+        <v>20.3</v>
+      </c>
+      <c r="G20" s="73"/>
+      <c r="H20" s="73">
+        <v>49</v>
+      </c>
+      <c r="I20" s="73"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="73"/>
+      <c r="L20" s="84">
+        <v>3.9968753072807401</v>
+      </c>
+      <c r="M20" s="77" t="s">
+        <v>808</v>
+      </c>
+      <c r="N20" s="73"/>
+      <c r="O20" s="73"/>
+      <c r="P20" s="73"/>
+      <c r="Q20" s="73"/>
+      <c r="R20" s="73" t="s">
+        <v>802</v>
+      </c>
+      <c r="S20" s="73">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="T20" s="73">
+        <v>0.19500000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="77" t="s">
+        <v>332</v>
+      </c>
+      <c r="B21" s="73"/>
+      <c r="C21" s="77" t="s">
+        <v>246</v>
+      </c>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73">
+        <v>-39.5</v>
+      </c>
+      <c r="F21" s="73">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="G21" s="73">
+        <v>2.12</v>
+      </c>
+      <c r="H21" s="73">
+        <v>44.73</v>
+      </c>
+      <c r="I21" s="73"/>
+      <c r="J21" s="73"/>
+      <c r="K21" s="73"/>
+      <c r="L21" s="84">
+        <v>-3.9968753072807401</v>
+      </c>
+      <c r="M21" s="77" t="str">
+        <f>VLOOKUP(A21,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>6.2.1.5</v>
+      </c>
+      <c r="N21" s="73"/>
+      <c r="O21" s="73"/>
+      <c r="P21" s="73"/>
+      <c r="Q21" s="73"/>
+      <c r="R21" s="73" t="s">
+        <v>803</v>
+      </c>
+      <c r="S21" s="73">
+        <v>6.2E-2</v>
+      </c>
+      <c r="T21" s="73">
+        <v>6.2E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="78" t="s">
+        <v>334</v>
+      </c>
+      <c r="B22" s="73"/>
+      <c r="C22" s="78" t="s">
+        <v>248</v>
+      </c>
+      <c r="D22" s="73">
+        <v>-2.1</v>
+      </c>
+      <c r="E22" s="73">
+        <v>-40.4</v>
+      </c>
+      <c r="F22" s="73">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="G22" s="73"/>
+      <c r="H22" s="73">
+        <v>24</v>
+      </c>
+      <c r="I22" s="73"/>
+      <c r="J22" s="73"/>
+      <c r="K22" s="73"/>
+      <c r="L22" s="84">
+        <v>3.9968753072807401</v>
+      </c>
+      <c r="M22" s="77" t="str">
+        <f>VLOOKUP(A22,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.3.99.1</v>
+      </c>
+      <c r="N22" s="73"/>
+      <c r="O22" s="73"/>
+      <c r="P22" s="73"/>
+      <c r="Q22" s="73"/>
+      <c r="R22" s="73" t="s">
+        <v>100</v>
+      </c>
+      <c r="S22" s="73">
+        <v>1.47</v>
+      </c>
+      <c r="T22" s="73">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="78" t="s">
+        <v>251</v>
+      </c>
+      <c r="B23" s="73"/>
+      <c r="C23" s="78" t="s">
+        <v>823</v>
+      </c>
+      <c r="D23" s="73">
+        <v>-5.9</v>
+      </c>
+      <c r="E23" s="73">
+        <v>-40.4</v>
+      </c>
+      <c r="F23" s="73">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="G23" s="73"/>
+      <c r="H23" s="73">
+        <v>250</v>
+      </c>
+      <c r="I23" s="73">
+        <v>110</v>
+      </c>
+      <c r="J23" s="73"/>
+      <c r="K23" s="73">
+        <v>0</v>
+      </c>
+      <c r="L23" s="84">
+        <v>0</v>
+      </c>
+      <c r="M23" s="77" t="str">
+        <f>VLOOKUP(A23,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.3.99.1</v>
+      </c>
+      <c r="N23" s="73"/>
+      <c r="O23" s="73"/>
+      <c r="P23" s="73"/>
+      <c r="Q23" s="73"/>
+      <c r="R23" s="73" t="s">
+        <v>101</v>
+      </c>
+      <c r="S23" s="73">
+        <v>0.1</v>
+      </c>
+      <c r="T23" s="73">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="77" t="s">
+        <v>252</v>
+      </c>
+      <c r="B24" s="73"/>
+      <c r="C24" s="77" t="s">
+        <v>824</v>
+      </c>
+      <c r="D24" s="73">
+        <v>0.6</v>
+      </c>
+      <c r="E24" s="73">
+        <v>-15.4</v>
+      </c>
+      <c r="F24" s="73">
+        <v>22.3</v>
+      </c>
+      <c r="G24" s="73"/>
+      <c r="H24" s="73">
+        <v>51.7</v>
+      </c>
+      <c r="I24" s="73">
+        <v>11.2</v>
+      </c>
+      <c r="J24" s="73"/>
+      <c r="K24" s="73"/>
+      <c r="L24" s="84">
+        <v>-3.9968753072807401</v>
+      </c>
+      <c r="M24" s="77" t="str">
+        <f>VLOOKUP(A24,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.2.1.2</v>
+      </c>
+      <c r="N24" s="73"/>
+      <c r="O24" s="73"/>
+      <c r="P24" s="73"/>
+      <c r="Q24" s="73"/>
+      <c r="R24" s="73" t="s">
+        <v>804</v>
+      </c>
+      <c r="S24" s="73">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="T24" s="73">
+        <v>0.80800000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="77" t="s">
+        <v>253</v>
+      </c>
+      <c r="B25" s="73"/>
+      <c r="C25" s="77" t="s">
+        <v>261</v>
+      </c>
+      <c r="D25" s="73">
+        <v>6.4</v>
+      </c>
+      <c r="E25" s="73">
+        <v>-7.3</v>
+      </c>
+      <c r="F25" s="73">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="G25" s="73"/>
+      <c r="H25" s="73">
+        <v>931</v>
+      </c>
+      <c r="I25" s="73"/>
+      <c r="J25" s="73"/>
+      <c r="K25" s="73">
+        <v>50</v>
+      </c>
+      <c r="L25" s="84">
+        <v>1.73406272437436</v>
+      </c>
+      <c r="M25" s="77" t="str">
+        <f>VLOOKUP(A25,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.1.1.37</v>
+      </c>
+      <c r="N25" s="73"/>
+      <c r="O25" s="73"/>
+      <c r="P25" s="73"/>
+      <c r="Q25" s="73"/>
+      <c r="R25" s="73"/>
+      <c r="S25" s="73"/>
+      <c r="T25" s="73"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="77" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26" s="73"/>
+      <c r="C26" s="77" t="s">
+        <v>825</v>
+      </c>
+      <c r="D26" s="73">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E26" s="73">
+        <v>-16.399999999999999</v>
+      </c>
+      <c r="F26" s="73">
+        <v>51.5</v>
+      </c>
+      <c r="G26" s="73"/>
+      <c r="H26" s="73">
+        <v>12.8</v>
+      </c>
+      <c r="I26" s="73">
+        <v>4</v>
+      </c>
+      <c r="J26" s="73"/>
+      <c r="K26" s="73"/>
+      <c r="L26" s="84">
+        <v>-34.977749829395002</v>
+      </c>
+      <c r="M26" s="77" t="s">
+        <v>809</v>
+      </c>
+      <c r="N26" s="73"/>
+      <c r="O26" s="73"/>
+      <c r="P26" s="73"/>
+      <c r="Q26" s="73"/>
+      <c r="R26" s="73"/>
+      <c r="S26" s="73"/>
+      <c r="T26" s="73"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="77" t="s">
+        <v>305</v>
+      </c>
+      <c r="B27" s="73"/>
+      <c r="C27" s="77" t="s">
+        <v>826</v>
+      </c>
+      <c r="D27" s="73">
+        <v>6.4</v>
+      </c>
+      <c r="E27" s="73">
+        <v>-13.2</v>
+      </c>
+      <c r="F27" s="73">
+        <v>62.1</v>
+      </c>
+      <c r="G27" s="73"/>
+      <c r="H27" s="73">
+        <v>320</v>
+      </c>
+      <c r="I27" s="73"/>
+      <c r="J27" s="73"/>
+      <c r="K27" s="73">
+        <v>0</v>
+      </c>
+      <c r="L27" s="84">
+        <v>0</v>
+      </c>
+      <c r="M27" s="77" t="str">
+        <f>VLOOKUP(A27,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.1.1.28</v>
+      </c>
+      <c r="N27" s="73"/>
+      <c r="O27" s="73"/>
+      <c r="P27" s="73"/>
+      <c r="Q27" s="73"/>
+      <c r="R27" s="73"/>
+      <c r="S27" s="73"/>
+      <c r="T27" s="73"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="77" t="s">
+        <v>212</v>
+      </c>
+      <c r="B28" s="73"/>
+      <c r="C28" s="77" t="s">
+        <v>211</v>
+      </c>
+      <c r="D28" s="73">
+        <f>VLOOKUP(A28,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>3.8</v>
+      </c>
+      <c r="E28" s="73">
+        <v>-20.399999999999999</v>
+      </c>
+      <c r="F28" s="73">
+        <v>28.7</v>
+      </c>
+      <c r="G28" s="73"/>
+      <c r="H28" s="73">
+        <v>120</v>
+      </c>
+      <c r="I28" s="73"/>
+      <c r="J28" s="73"/>
+      <c r="K28" s="73">
+        <v>0</v>
+      </c>
+      <c r="L28" s="85">
+        <v>21.2358352193176</v>
+      </c>
+      <c r="M28" s="77" t="str">
+        <f>VLOOKUP(A28,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.3.1.8</v>
+      </c>
+      <c r="N28" s="73"/>
+      <c r="O28" s="73"/>
+      <c r="P28" s="73"/>
+      <c r="Q28" s="73"/>
+      <c r="R28" s="73"/>
+      <c r="S28" s="73"/>
+      <c r="T28" s="73"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="77" t="s">
+        <v>214</v>
+      </c>
+      <c r="B29" s="73"/>
+      <c r="C29" s="77" t="s">
+        <v>213</v>
+      </c>
+      <c r="D29" s="73">
+        <f>VLOOKUP(A29,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>4.3</v>
+      </c>
+      <c r="E29" s="73">
+        <v>-24.3</v>
+      </c>
+      <c r="F29" s="73">
+        <v>52.1</v>
+      </c>
+      <c r="G29" s="73"/>
+      <c r="H29" s="73">
+        <v>280</v>
+      </c>
+      <c r="I29" s="73"/>
+      <c r="J29" s="73"/>
+      <c r="K29" s="73">
+        <v>0</v>
+      </c>
+      <c r="L29" s="84">
+        <v>-21.2358352193176</v>
+      </c>
+      <c r="M29" s="77" t="str">
+        <f>VLOOKUP(A29,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.2.1</v>
+      </c>
+      <c r="N29" s="73"/>
+      <c r="O29" s="73"/>
+      <c r="P29" s="73"/>
+      <c r="Q29" s="73"/>
+      <c r="R29" s="73"/>
+      <c r="S29" s="73"/>
+      <c r="T29" s="73"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="B30" s="73"/>
+      <c r="C30" s="78" t="s">
+        <v>143</v>
+      </c>
+      <c r="D30" s="73">
+        <f>VLOOKUP(A30,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-4.4000000000000004</v>
+      </c>
+      <c r="E30" s="73">
+        <v>-47.4</v>
+      </c>
+      <c r="F30" s="73">
+        <v>49.2</v>
+      </c>
+      <c r="G30" s="73"/>
+      <c r="H30" s="73">
+        <v>15.7</v>
+      </c>
+      <c r="I30" s="73"/>
+      <c r="J30" s="73"/>
+      <c r="K30" s="73">
+        <v>0</v>
+      </c>
+      <c r="L30" s="84">
+        <v>-10.1045270920776</v>
+      </c>
+      <c r="M30" s="77" t="str">
+        <f>VLOOKUP(A30,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.2.1.10</v>
+      </c>
+      <c r="N30" s="73"/>
+      <c r="O30" s="73"/>
+      <c r="P30" s="73"/>
+      <c r="Q30" s="73"/>
+      <c r="R30" s="73"/>
+      <c r="S30" s="73"/>
+      <c r="T30" s="73"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="78" t="s">
+        <v>145</v>
+      </c>
+      <c r="B31" s="73"/>
+      <c r="C31" s="78" t="s">
+        <v>377</v>
+      </c>
+      <c r="D31" s="73"/>
+      <c r="E31" s="73">
+        <v>-16.600000000000001</v>
+      </c>
+      <c r="F31" s="73">
+        <v>59.3</v>
+      </c>
+      <c r="G31" s="11">
+        <v>1.6000000000000001E-4</v>
+      </c>
+      <c r="H31" s="73">
+        <v>150.19999999999999</v>
+      </c>
+      <c r="I31" s="73"/>
+      <c r="J31" s="73"/>
+      <c r="K31" s="73">
+        <v>0</v>
+      </c>
+      <c r="L31" s="84">
+        <v>-10.1045270920776</v>
+      </c>
+      <c r="M31" s="77" t="str">
+        <f>VLOOKUP(A31,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.1.1.1</v>
+      </c>
+      <c r="N31" s="73"/>
+      <c r="O31" s="73"/>
+      <c r="P31" s="73"/>
+      <c r="Q31" s="73"/>
+      <c r="R31" s="73"/>
+      <c r="S31" s="73"/>
+      <c r="T31" s="73"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="77" t="s">
+        <v>415</v>
+      </c>
+      <c r="B32" s="73"/>
+      <c r="C32" s="77" t="s">
+        <v>417</v>
+      </c>
+      <c r="D32" s="73">
+        <f>VLOOKUP(A32,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-1.6</v>
+      </c>
+      <c r="E32" s="73">
+        <v>-42.6</v>
+      </c>
+      <c r="F32" s="73">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="G32" s="73"/>
+      <c r="H32" s="73">
+        <v>174</v>
+      </c>
+      <c r="I32" s="73"/>
+      <c r="J32" s="73"/>
+      <c r="K32" s="73">
+        <v>0.63</v>
+      </c>
+      <c r="L32" s="84">
+        <v>0</v>
+      </c>
+      <c r="M32" s="77" t="str">
+        <f>VLOOKUP(A32,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.1.1.49</v>
+      </c>
+      <c r="N32" s="73"/>
+      <c r="O32" s="73"/>
+      <c r="P32" s="73"/>
+      <c r="Q32" s="73"/>
+      <c r="R32" s="73"/>
+      <c r="S32" s="73"/>
+      <c r="T32" s="73"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" s="77" t="s">
+        <v>419</v>
+      </c>
+      <c r="B33" s="73"/>
+      <c r="C33" s="77" t="s">
+        <v>421</v>
+      </c>
+      <c r="D33" s="73">
+        <f>VLOOKUP(A33,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="E33" s="73">
+        <v>-39.799999999999997</v>
+      </c>
+      <c r="F33" s="73">
+        <v>-2.1</v>
+      </c>
+      <c r="G33" s="73"/>
+      <c r="H33" s="73">
+        <v>25</v>
+      </c>
+      <c r="I33" s="73"/>
+      <c r="J33" s="73"/>
+      <c r="K33" s="73"/>
+      <c r="L33" s="84">
+        <v>0</v>
+      </c>
+      <c r="M33" s="77" t="str">
+        <f>VLOOKUP(A33,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>3.1.1.31</v>
+      </c>
+      <c r="N33" s="73"/>
+      <c r="O33" s="73"/>
+      <c r="P33" s="73"/>
+      <c r="Q33" s="73"/>
+      <c r="R33" s="73"/>
+      <c r="S33" s="73"/>
+      <c r="T33" s="73"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" s="77" t="s">
+        <v>422</v>
+      </c>
+      <c r="B34" s="73"/>
+      <c r="C34" s="77" t="s">
+        <v>424</v>
+      </c>
+      <c r="D34" s="73">
+        <f>VLOOKUP(A34,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0.9</v>
+      </c>
+      <c r="E34" s="73">
+        <v>-43.6</v>
+      </c>
+      <c r="F34" s="73">
+        <v>31.7</v>
+      </c>
+      <c r="G34" s="73"/>
+      <c r="H34" s="73">
+        <v>75.650000000000006</v>
+      </c>
+      <c r="I34" s="73"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="73"/>
+      <c r="L34" s="84">
+        <v>0</v>
+      </c>
+      <c r="M34" s="77" t="str">
+        <f>VLOOKUP(A34,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.1.1.44</v>
+      </c>
+      <c r="N34" s="73"/>
+      <c r="O34" s="73"/>
+      <c r="P34" s="73"/>
+      <c r="Q34" s="73"/>
+      <c r="R34" s="73"/>
+      <c r="S34" s="73"/>
+      <c r="T34" s="73"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" s="77" t="s">
+        <v>425</v>
+      </c>
+      <c r="B35" s="73"/>
+      <c r="C35" s="77" t="s">
+        <v>427</v>
+      </c>
+      <c r="D35" s="73"/>
+      <c r="E35" s="73">
+        <v>-22.2</v>
+      </c>
+      <c r="F35" s="73">
+        <v>15.5</v>
+      </c>
+      <c r="G35" s="73">
+        <v>3.91</v>
+      </c>
+      <c r="H35" s="73">
+        <v>21.05</v>
+      </c>
+      <c r="I35" s="73"/>
+      <c r="J35" s="73"/>
+      <c r="K35" s="73"/>
+      <c r="L35" s="85">
+        <v>-0.69762371202792395</v>
+      </c>
+      <c r="M35" s="77" t="str">
+        <f>VLOOKUP(A35,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.1.3.1</v>
+      </c>
+      <c r="N35" s="73"/>
+      <c r="O35" s="73"/>
+      <c r="P35" s="73"/>
+      <c r="Q35" s="73"/>
+      <c r="R35" s="73"/>
+      <c r="S35" s="73"/>
+      <c r="T35" s="73"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" s="77" t="s">
+        <v>428</v>
+      </c>
+      <c r="B36" s="73"/>
+      <c r="C36" s="77" t="s">
+        <v>430</v>
+      </c>
+      <c r="D36" s="73">
+        <v>0.5</v>
+      </c>
+      <c r="E36" s="73">
+        <v>-16.899999999999999</v>
+      </c>
+      <c r="F36" s="73">
+        <v>20.8</v>
+      </c>
+      <c r="G36" s="73"/>
+      <c r="H36" s="73">
+        <v>2100</v>
+      </c>
+      <c r="I36" s="73"/>
+      <c r="J36" s="73"/>
+      <c r="K36" s="73"/>
+      <c r="L36" s="85">
+        <v>-0.69762371202792395</v>
+      </c>
+      <c r="M36" s="77" t="str">
+        <f>VLOOKUP(A36,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.3.1.6</v>
+      </c>
+      <c r="N36" s="73"/>
+      <c r="O36" s="73"/>
+      <c r="P36" s="73"/>
+      <c r="Q36" s="73"/>
+      <c r="R36" s="73"/>
+      <c r="S36" s="73"/>
+      <c r="T36" s="73"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" s="77" t="s">
+        <v>431</v>
+      </c>
+      <c r="B37" s="73"/>
+      <c r="C37" s="77" t="s">
+        <v>827</v>
+      </c>
+      <c r="D37" s="73"/>
+      <c r="E37" s="73">
+        <v>-33.9</v>
+      </c>
+      <c r="F37" s="73">
+        <v>41.5</v>
+      </c>
+      <c r="G37" s="73">
+        <v>0.216</v>
+      </c>
+      <c r="H37" s="73"/>
+      <c r="I37" s="73">
+        <v>55.57</v>
+      </c>
+      <c r="J37" s="73"/>
+      <c r="K37" s="73"/>
+      <c r="L37" s="84">
+        <v>0.17362949649665499</v>
+      </c>
+      <c r="M37" s="77" t="str">
+        <f>VLOOKUP(A37,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.2.1.1</v>
+      </c>
+      <c r="N37" s="73"/>
+      <c r="O37" s="73"/>
+      <c r="P37" s="73"/>
+      <c r="Q37" s="73"/>
+      <c r="R37" s="73"/>
+      <c r="S37" s="73"/>
+      <c r="T37" s="73"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" s="77" t="s">
+        <v>436</v>
+      </c>
+      <c r="B38" s="73"/>
+      <c r="C38" s="77" t="s">
+        <v>438</v>
+      </c>
+      <c r="D38" s="73">
+        <v>-1.7</v>
+      </c>
+      <c r="E38" s="73">
+        <v>-38.4</v>
+      </c>
+      <c r="F38" s="73">
+        <v>36.9</v>
+      </c>
+      <c r="G38" s="73"/>
+      <c r="H38" s="73">
+        <v>16.57</v>
+      </c>
+      <c r="I38" s="73"/>
+      <c r="J38" s="73"/>
+      <c r="K38" s="73"/>
+      <c r="L38" s="84">
+        <v>-0.17362949649665499</v>
+      </c>
+      <c r="M38" s="77" t="str">
+        <f>VLOOKUP(A38,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.2.1.2</v>
+      </c>
+      <c r="N38" s="73"/>
+      <c r="O38" s="73"/>
+      <c r="P38" s="73"/>
+      <c r="Q38" s="73"/>
+      <c r="R38" s="73"/>
+      <c r="S38" s="73"/>
+      <c r="T38" s="73"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" s="77" t="s">
+        <v>434</v>
+      </c>
+      <c r="B39" s="73"/>
+      <c r="C39" s="77" t="s">
+        <v>828</v>
+      </c>
+      <c r="D39" s="73">
+        <v>1.7</v>
+      </c>
+      <c r="E39" s="73">
+        <v>-27.7</v>
+      </c>
+      <c r="F39" s="73">
+        <v>47.7</v>
+      </c>
+      <c r="G39" s="73">
+        <v>1.77E-2</v>
+      </c>
+      <c r="H39" s="73"/>
+      <c r="I39" s="73">
+        <v>15.45</v>
+      </c>
+      <c r="J39" s="73"/>
+      <c r="K39" s="73"/>
+      <c r="L39" s="84">
+        <v>0.52399421553126901</v>
+      </c>
+      <c r="M39" s="77" t="str">
+        <f>VLOOKUP(A39,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.2.1.1</v>
+      </c>
+      <c r="N39" s="73"/>
+      <c r="O39" s="73"/>
+      <c r="P39" s="73"/>
+      <c r="Q39" s="73"/>
+      <c r="R39" s="73"/>
+      <c r="S39" s="73"/>
+      <c r="T39" s="73"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" s="78" t="s">
+        <v>169</v>
+      </c>
+      <c r="B40" s="73"/>
+      <c r="C40" s="78" t="s">
+        <v>829</v>
+      </c>
+      <c r="D40" s="73">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="E40" s="73">
+        <v>24.2</v>
+      </c>
+      <c r="F40" s="73">
+        <v>122.4</v>
+      </c>
+      <c r="G40" s="73"/>
+      <c r="H40" s="73"/>
+      <c r="I40" s="73">
+        <v>26</v>
+      </c>
+      <c r="J40" s="73"/>
+      <c r="K40" s="73"/>
+      <c r="L40" s="84">
+        <v>-16.0031246927193</v>
+      </c>
+      <c r="M40" s="77" t="str">
+        <f>VLOOKUP(A40,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.6.5.3</v>
+      </c>
+      <c r="N40" s="73"/>
+      <c r="O40" s="73"/>
+      <c r="P40" s="73"/>
+      <c r="Q40" s="73"/>
+      <c r="R40" s="73"/>
+      <c r="S40" s="73"/>
+      <c r="T40" s="73"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" s="77" t="s">
+        <v>441</v>
+      </c>
+      <c r="B41" s="73"/>
+      <c r="C41" s="77" t="s">
+        <v>830</v>
+      </c>
+      <c r="D41" s="73"/>
+      <c r="E41" s="73">
+        <v>-38.6</v>
+      </c>
+      <c r="F41" s="73">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="G41" s="73">
+        <v>1.48</v>
+      </c>
+      <c r="H41" s="73"/>
+      <c r="I41" s="73">
+        <v>6.6699999999999995E-2</v>
+      </c>
+      <c r="J41" s="73"/>
+      <c r="K41" s="73"/>
+      <c r="L41" s="84">
+        <v>0</v>
+      </c>
+      <c r="M41" s="77" t="str">
+        <f>VLOOKUP(A41,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.6.1.2</v>
+      </c>
+      <c r="N41" s="73"/>
+      <c r="O41" s="73"/>
+      <c r="P41" s="73"/>
+      <c r="Q41" s="73"/>
+      <c r="R41" s="73"/>
+      <c r="S41" s="73"/>
+      <c r="T41" s="73"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" s="77" t="s">
+        <v>444</v>
+      </c>
+      <c r="B42" s="73"/>
+      <c r="C42" s="77" t="s">
+        <v>831</v>
+      </c>
+      <c r="D42" s="73"/>
+      <c r="E42" s="73">
+        <v>-38.6</v>
+      </c>
+      <c r="F42" s="73">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="G42" s="73">
+        <v>1.48</v>
+      </c>
+      <c r="H42" s="73">
+        <v>167.9</v>
+      </c>
+      <c r="I42" s="73"/>
+      <c r="J42" s="73"/>
+      <c r="K42" s="73"/>
+      <c r="L42" s="84">
+        <v>-10.381277508814</v>
+      </c>
+      <c r="M42" s="77" t="str">
+        <f>VLOOKUP(A42,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.6.1.1</v>
+      </c>
+      <c r="N42" s="73"/>
+      <c r="O42" s="73"/>
+      <c r="P42" s="73"/>
+      <c r="Q42" s="73"/>
+      <c r="R42" s="73"/>
+      <c r="S42" s="73"/>
+      <c r="T42" s="73"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" s="77" t="s">
+        <v>178</v>
+      </c>
+      <c r="B43" s="73"/>
+      <c r="C43" s="77" t="s">
+        <v>177</v>
+      </c>
+      <c r="D43" s="73"/>
+      <c r="E43" s="73">
+        <v>-40.200000000000003</v>
+      </c>
+      <c r="F43" s="73">
+        <v>35.1</v>
+      </c>
+      <c r="G43" s="73">
+        <v>2.82</v>
+      </c>
+      <c r="H43" s="73">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="I43" s="73"/>
+      <c r="J43" s="73"/>
+      <c r="K43" s="73"/>
+      <c r="L43" s="84">
+        <v>0</v>
+      </c>
+      <c r="M43" s="77" t="str">
+        <f>VLOOKUP(A43,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.4.3</v>
+      </c>
+      <c r="N43" s="73"/>
+      <c r="O43" s="73"/>
+      <c r="P43" s="73"/>
+      <c r="Q43" s="73"/>
+      <c r="R43" s="73"/>
+      <c r="S43" s="73"/>
+      <c r="T43" s="73"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" s="77" t="s">
+        <v>171</v>
+      </c>
+      <c r="B44" s="73"/>
+      <c r="C44" s="77" t="s">
+        <v>172</v>
+      </c>
+      <c r="D44" s="73">
+        <f>VLOOKUP(A44,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-6.6</v>
+      </c>
+      <c r="E44" s="73"/>
+      <c r="F44" s="73"/>
+      <c r="G44" s="73"/>
+      <c r="H44" s="73">
+        <v>1</v>
+      </c>
+      <c r="I44" s="73">
+        <v>0</v>
+      </c>
+      <c r="J44" s="73"/>
+      <c r="K44" s="73"/>
+      <c r="L44" s="84">
+        <v>8.39</v>
+      </c>
+      <c r="M44" s="77">
+        <f>VLOOKUP(A44,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="N44" s="73"/>
+      <c r="O44" s="73"/>
+      <c r="P44" s="73"/>
+      <c r="Q44" s="73"/>
+      <c r="R44" s="73"/>
+      <c r="S44" s="73"/>
+      <c r="T44" s="73"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" s="77" t="s">
+        <v>173</v>
+      </c>
+      <c r="B45" s="73"/>
+      <c r="C45" s="77" t="s">
+        <v>207</v>
+      </c>
+      <c r="D45" s="73"/>
+      <c r="E45" s="73">
+        <v>-62.3</v>
+      </c>
+      <c r="F45" s="73">
+        <v>1.5</v>
+      </c>
+      <c r="G45" s="11">
+        <v>42000</v>
+      </c>
+      <c r="H45" s="73">
+        <v>3800</v>
+      </c>
+      <c r="I45" s="73">
+        <v>2200</v>
+      </c>
+      <c r="J45" s="73"/>
+      <c r="K45" s="73"/>
+      <c r="L45" s="84">
+        <v>-7.35555836532013</v>
+      </c>
+      <c r="M45" s="77" t="str">
+        <f>VLOOKUP(A45,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>3.6.3.14</v>
+      </c>
+      <c r="N45" s="73"/>
+      <c r="O45" s="73"/>
+      <c r="P45" s="73"/>
+      <c r="Q45" s="73"/>
+      <c r="R45" s="73"/>
+      <c r="S45" s="73"/>
+      <c r="T45" s="73"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" s="77" t="s">
+        <v>167</v>
+      </c>
+      <c r="B46" s="73"/>
+      <c r="C46" s="77" t="s">
+        <v>168</v>
+      </c>
+      <c r="D46" s="73">
+        <f>VLOOKUP(A46,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-37.200000000000003</v>
+      </c>
+      <c r="E46" s="73"/>
+      <c r="F46" s="73"/>
+      <c r="G46" s="73"/>
+      <c r="H46" s="73">
+        <v>341</v>
+      </c>
+      <c r="I46" s="73">
+        <v>0</v>
+      </c>
+      <c r="J46" s="73"/>
+      <c r="K46" s="73"/>
+      <c r="L46" s="84">
+        <v>20</v>
+      </c>
+      <c r="M46" s="77" t="s">
+        <v>810</v>
+      </c>
+      <c r="N46" s="73"/>
+      <c r="O46" s="73"/>
+      <c r="P46" s="73"/>
+      <c r="Q46" s="73"/>
+      <c r="R46" s="73"/>
+      <c r="S46" s="73"/>
+      <c r="T46" s="73"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" s="77" t="s">
+        <v>234</v>
+      </c>
+      <c r="B47" s="73"/>
+      <c r="C47" s="77" t="s">
+        <v>832</v>
+      </c>
+      <c r="D47" s="73">
+        <v>6.8</v>
+      </c>
+      <c r="E47" s="73">
+        <v>-7.1</v>
+      </c>
+      <c r="F47" s="73">
+        <v>55.6</v>
+      </c>
+      <c r="G47" s="73"/>
+      <c r="H47" s="73">
+        <v>13.74</v>
+      </c>
+      <c r="I47" s="73">
+        <v>540</v>
+      </c>
+      <c r="J47" s="73"/>
+      <c r="K47" s="73">
+        <v>18.2</v>
+      </c>
+      <c r="L47" s="84">
+        <v>0</v>
+      </c>
+      <c r="M47" s="77" t="str">
+        <f>VLOOKUP(A47,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.1.1.31</v>
+      </c>
+      <c r="N47" s="73"/>
+      <c r="O47" s="73"/>
+      <c r="P47" s="73"/>
+      <c r="Q47" s="73"/>
+      <c r="R47" s="73"/>
+      <c r="S47" s="73"/>
+      <c r="T47" s="73"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A48" s="77" t="s">
+        <v>237</v>
+      </c>
+      <c r="B48" s="73"/>
+      <c r="C48" s="77" t="s">
+        <v>236</v>
+      </c>
+      <c r="D48" s="73">
+        <f>VLOOKUP(A48,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0.2</v>
+      </c>
+      <c r="E48" s="73">
+        <v>-44.4</v>
+      </c>
+      <c r="F48" s="73">
+        <v>30.9</v>
+      </c>
+      <c r="G48" s="73"/>
+      <c r="H48" s="73">
+        <v>1</v>
+      </c>
+      <c r="I48" s="73"/>
+      <c r="J48" s="73"/>
+      <c r="K48" s="73">
+        <v>0</v>
+      </c>
+      <c r="L48" s="84">
+        <v>0</v>
+      </c>
+      <c r="M48" s="77" t="str">
+        <f>VLOOKUP(A48,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.1.1.49</v>
+      </c>
+      <c r="N48" s="73"/>
+      <c r="O48" s="73"/>
+      <c r="P48" s="73"/>
+      <c r="Q48" s="73"/>
+      <c r="R48" s="73"/>
+      <c r="S48" s="73"/>
+      <c r="T48" s="73"/>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A49" s="77" t="s">
+        <v>254</v>
+      </c>
+      <c r="B49" s="73"/>
+      <c r="C49" s="77" t="s">
+        <v>262</v>
+      </c>
+      <c r="D49" s="73">
+        <f>VLOOKUP(A49,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>1.3</v>
+      </c>
+      <c r="E49" s="73">
+        <v>-41.8</v>
+      </c>
+      <c r="F49" s="73">
+        <v>33.6</v>
+      </c>
+      <c r="G49" s="73"/>
+      <c r="H49" s="73">
+        <v>1</v>
+      </c>
+      <c r="I49" s="73"/>
+      <c r="J49" s="73"/>
+      <c r="K49" s="73">
+        <v>0</v>
+      </c>
+      <c r="L49" s="84">
+        <v>0</v>
+      </c>
+      <c r="M49" s="77" t="str">
+        <f>VLOOKUP(A49,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.1.1.38</v>
+      </c>
+      <c r="N49" s="73"/>
+      <c r="O49" s="73"/>
+      <c r="P49" s="73"/>
+      <c r="Q49" s="73"/>
+      <c r="R49" s="73"/>
+      <c r="S49" s="73"/>
+      <c r="T49" s="73"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A50" s="77" t="s">
+        <v>364</v>
+      </c>
+      <c r="B50" s="73"/>
+      <c r="C50" s="77" t="s">
+        <v>367</v>
+      </c>
+      <c r="D50" s="73">
+        <f>VLOOKUP(A50,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>1.6</v>
+      </c>
+      <c r="E50" s="73">
+        <v>-40.799999999999997</v>
+      </c>
+      <c r="F50" s="73">
+        <v>34.5</v>
+      </c>
+      <c r="G50" s="73"/>
+      <c r="H50" s="73">
+        <v>1</v>
+      </c>
+      <c r="I50" s="73"/>
+      <c r="J50" s="73"/>
+      <c r="K50" s="73">
+        <v>0</v>
+      </c>
+      <c r="L50" s="84">
+        <v>2.2628125829063799</v>
+      </c>
+      <c r="M50" s="77" t="str">
+        <f>VLOOKUP(A50,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.1.1.40</v>
+      </c>
+      <c r="N50" s="73"/>
+      <c r="O50" s="73"/>
+      <c r="P50" s="73"/>
+      <c r="Q50" s="73"/>
+      <c r="R50" s="73"/>
+      <c r="S50" s="73"/>
+      <c r="T50" s="73"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A51" s="77" t="s">
+        <v>663</v>
+      </c>
+      <c r="B51" s="73"/>
+      <c r="C51" s="77" t="s">
+        <v>665</v>
+      </c>
+      <c r="D51" s="73">
+        <f>VLOOKUP(A51,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E51" s="73"/>
+      <c r="F51" s="73"/>
+      <c r="G51" s="73"/>
+      <c r="H51" s="73">
+        <v>1</v>
+      </c>
+      <c r="I51" s="73">
+        <v>1</v>
+      </c>
+      <c r="J51" s="73"/>
+      <c r="K51" s="73"/>
+      <c r="L51" s="84">
+        <v>7.11118951189348</v>
+      </c>
+      <c r="M51" s="77"/>
+      <c r="N51" s="73"/>
+      <c r="O51" s="73"/>
+      <c r="P51" s="73"/>
+      <c r="Q51" s="73"/>
+      <c r="R51" s="73"/>
+      <c r="S51" s="73"/>
+      <c r="T51" s="73"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A52" s="77" t="s">
+        <v>463</v>
+      </c>
+      <c r="B52" s="73"/>
+      <c r="C52" s="77" t="s">
+        <v>166</v>
+      </c>
+      <c r="D52" s="73">
+        <f>VLOOKUP(A52,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E52" s="73"/>
+      <c r="F52" s="73"/>
+      <c r="G52" s="73"/>
+      <c r="H52" s="86">
+        <v>1.6670000000000001E-2</v>
+      </c>
+      <c r="I52" s="73">
+        <v>1.6670000000000001E-2</v>
+      </c>
+      <c r="J52" s="73"/>
+      <c r="K52" s="73"/>
+      <c r="L52" s="84">
+        <v>10</v>
+      </c>
+      <c r="M52" s="77"/>
+      <c r="N52" s="73"/>
+      <c r="O52" s="73"/>
+      <c r="P52" s="73"/>
+      <c r="Q52" s="73"/>
+      <c r="R52" s="73"/>
+      <c r="S52" s="73"/>
+      <c r="T52" s="73"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A53" s="77" t="s">
+        <v>456</v>
+      </c>
+      <c r="B53" s="73"/>
+      <c r="C53" s="77" t="s">
+        <v>458</v>
+      </c>
+      <c r="D53" s="73">
+        <f>VLOOKUP(A53,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E53" s="73"/>
+      <c r="F53" s="73"/>
+      <c r="G53" s="73"/>
+      <c r="H53" s="86">
+        <v>1</v>
+      </c>
+      <c r="I53" s="73">
+        <v>1</v>
+      </c>
+      <c r="J53" s="73"/>
+      <c r="K53" s="73"/>
+      <c r="L53" s="84">
+        <v>3.5703232462952501</v>
+      </c>
+      <c r="M53" s="77"/>
+      <c r="N53" s="73"/>
+      <c r="O53" s="73"/>
+      <c r="P53" s="73"/>
+      <c r="Q53" s="73"/>
+      <c r="R53" s="73"/>
+      <c r="S53" s="73"/>
+      <c r="T53" s="73"/>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A54" s="77" t="s">
+        <v>397</v>
+      </c>
+      <c r="B54" s="73"/>
+      <c r="C54" s="77" t="s">
+        <v>399</v>
+      </c>
+      <c r="D54" s="73">
+        <f>VLOOKUP(A54,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E54" s="73"/>
+      <c r="F54" s="73"/>
+      <c r="G54" s="73"/>
+      <c r="H54" s="86">
+        <v>1</v>
+      </c>
+      <c r="I54" s="73">
+        <v>1</v>
+      </c>
+      <c r="J54" s="73"/>
+      <c r="K54" s="73"/>
+      <c r="L54" s="84">
+        <v>-6.25968789018712</v>
+      </c>
+      <c r="M54" s="77"/>
+      <c r="N54" s="73"/>
+      <c r="O54" s="73"/>
+      <c r="P54" s="73"/>
+      <c r="Q54" s="73"/>
+      <c r="R54" s="73"/>
+      <c r="S54" s="73"/>
+      <c r="T54" s="73"/>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A55" s="77" t="s">
+        <v>343</v>
+      </c>
+      <c r="B55" s="73"/>
+      <c r="C55" s="77" t="s">
+        <v>345</v>
+      </c>
+      <c r="D55" s="73">
+        <v>0</v>
+      </c>
+      <c r="E55" s="73"/>
+      <c r="F55" s="73"/>
+      <c r="G55" s="73"/>
+      <c r="H55" s="86">
+        <v>1</v>
+      </c>
+      <c r="I55" s="73">
+        <v>1</v>
+      </c>
+      <c r="J55" s="73"/>
+      <c r="K55" s="73"/>
+      <c r="L55" s="84">
+        <v>0</v>
+      </c>
+      <c r="M55" s="77"/>
+      <c r="N55" s="73"/>
+      <c r="O55" s="73"/>
+      <c r="P55" s="73"/>
+      <c r="Q55" s="73"/>
+      <c r="R55" s="73"/>
+      <c r="S55" s="73"/>
+      <c r="T55" s="73"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A56" s="77" t="s">
+        <v>346</v>
+      </c>
+      <c r="B56" s="73"/>
+      <c r="C56" s="77" t="s">
+        <v>352</v>
+      </c>
+      <c r="D56" s="73">
+        <v>0</v>
+      </c>
+      <c r="E56" s="73"/>
+      <c r="F56" s="73"/>
+      <c r="G56" s="73"/>
+      <c r="H56" s="86">
+        <v>1</v>
+      </c>
+      <c r="I56" s="73">
+        <v>1</v>
+      </c>
+      <c r="J56" s="73"/>
+      <c r="K56" s="73"/>
+      <c r="L56" s="84">
+        <v>0</v>
+      </c>
+      <c r="M56" s="77"/>
+      <c r="N56" s="73"/>
+      <c r="O56" s="73"/>
+      <c r="P56" s="73"/>
+      <c r="Q56" s="73"/>
+      <c r="R56" s="73"/>
+      <c r="S56" s="73"/>
+      <c r="T56" s="73"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A57" s="77" t="s">
+        <v>349</v>
+      </c>
+      <c r="B57" s="73"/>
+      <c r="C57" s="77" t="s">
+        <v>351</v>
+      </c>
+      <c r="D57" s="73">
+        <v>0</v>
+      </c>
+      <c r="E57" s="73"/>
+      <c r="F57" s="73"/>
+      <c r="G57" s="73"/>
+      <c r="H57" s="86">
+        <v>1</v>
+      </c>
+      <c r="I57" s="73">
+        <v>1</v>
+      </c>
+      <c r="J57" s="73"/>
+      <c r="K57" s="73"/>
+      <c r="L57" s="84">
+        <v>0</v>
+      </c>
+      <c r="M57" s="77"/>
+      <c r="N57" s="73"/>
+      <c r="O57" s="73"/>
+      <c r="P57" s="73"/>
+      <c r="Q57" s="73"/>
+      <c r="R57" s="73"/>
+      <c r="S57" s="73"/>
+      <c r="T57" s="73"/>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A58" s="77" t="s">
+        <v>353</v>
+      </c>
+      <c r="B58" s="73"/>
+      <c r="C58" s="77" t="s">
+        <v>355</v>
+      </c>
+      <c r="D58" s="73">
+        <f>VLOOKUP(A58,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E58" s="73"/>
+      <c r="F58" s="73"/>
+      <c r="G58" s="73"/>
+      <c r="H58" s="86">
+        <v>1</v>
+      </c>
+      <c r="I58" s="73">
+        <v>1</v>
+      </c>
+      <c r="J58" s="73"/>
+      <c r="K58" s="73"/>
+      <c r="L58" s="84">
+        <v>0</v>
+      </c>
+      <c r="M58" s="77"/>
+      <c r="N58" s="73"/>
+      <c r="O58" s="73"/>
+      <c r="P58" s="73"/>
+      <c r="Q58" s="73"/>
+      <c r="R58" s="73"/>
+      <c r="S58" s="73"/>
+      <c r="T58" s="73"/>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A59" s="77" t="s">
+        <v>356</v>
+      </c>
+      <c r="B59" s="73"/>
+      <c r="C59" s="77" t="s">
+        <v>359</v>
+      </c>
+      <c r="D59" s="73">
+        <f>VLOOKUP(A59,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E59" s="73"/>
+      <c r="F59" s="73"/>
+      <c r="G59" s="73"/>
+      <c r="H59" s="86">
+        <v>1</v>
+      </c>
+      <c r="I59" s="73">
+        <v>0</v>
+      </c>
+      <c r="J59" s="73"/>
+      <c r="K59" s="73"/>
+      <c r="L59" s="84">
+        <v>0</v>
+      </c>
+      <c r="M59" s="77"/>
+      <c r="N59" s="73"/>
+      <c r="O59" s="73"/>
+      <c r="P59" s="73"/>
+      <c r="Q59" s="73"/>
+      <c r="R59" s="73"/>
+      <c r="S59" s="73"/>
+      <c r="T59" s="73"/>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A60" s="78" t="s">
+        <v>360</v>
+      </c>
+      <c r="B60" s="73"/>
+      <c r="C60" s="78" t="s">
+        <v>363</v>
+      </c>
+      <c r="D60" s="73">
+        <f>VLOOKUP(A60,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E60" s="73"/>
+      <c r="F60" s="73"/>
+      <c r="G60" s="73"/>
+      <c r="H60" s="86">
+        <v>1</v>
+      </c>
+      <c r="I60" s="73">
+        <v>0</v>
+      </c>
+      <c r="J60" s="73"/>
+      <c r="K60" s="73"/>
+      <c r="L60" s="84">
+        <v>0</v>
+      </c>
+      <c r="M60" s="77"/>
+      <c r="N60" s="73"/>
+      <c r="O60" s="73"/>
+      <c r="P60" s="73"/>
+      <c r="Q60" s="73"/>
+      <c r="R60" s="73"/>
+      <c r="S60" s="73"/>
+      <c r="T60" s="73"/>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A61" s="77" t="s">
+        <v>368</v>
+      </c>
+      <c r="B61" s="73"/>
+      <c r="C61" s="77" t="s">
+        <v>371</v>
+      </c>
+      <c r="D61" s="73">
+        <f>VLOOKUP(A61,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E61" s="73"/>
+      <c r="F61" s="73"/>
+      <c r="G61" s="73"/>
+      <c r="H61" s="86">
+        <v>1</v>
+      </c>
+      <c r="I61" s="73">
+        <v>1</v>
+      </c>
+      <c r="J61" s="73"/>
+      <c r="K61" s="73"/>
+      <c r="L61" s="84">
+        <v>0</v>
+      </c>
+      <c r="M61" s="77"/>
+      <c r="N61" s="73"/>
+      <c r="O61" s="73"/>
+      <c r="P61" s="73"/>
+      <c r="Q61" s="73"/>
+      <c r="R61" s="73"/>
+      <c r="S61" s="73"/>
+      <c r="T61" s="73"/>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A62" s="78" t="s">
+        <v>378</v>
+      </c>
+      <c r="B62" s="73"/>
+      <c r="C62" s="78" t="s">
+        <v>380</v>
+      </c>
+      <c r="D62" s="73">
+        <f>VLOOKUP(A62,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E62" s="73"/>
+      <c r="F62" s="73"/>
+      <c r="G62" s="73"/>
+      <c r="H62" s="86">
+        <v>1</v>
+      </c>
+      <c r="I62" s="73">
+        <v>0</v>
+      </c>
+      <c r="J62" s="73"/>
+      <c r="K62" s="73"/>
+      <c r="L62" s="84">
+        <v>0</v>
+      </c>
+      <c r="M62" s="77"/>
+      <c r="N62" s="73"/>
+      <c r="O62" s="73"/>
+      <c r="P62" s="73"/>
+      <c r="Q62" s="73"/>
+      <c r="R62" s="73"/>
+      <c r="S62" s="73"/>
+      <c r="T62" s="73"/>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A63" s="78" t="s">
+        <v>381</v>
+      </c>
+      <c r="B63" s="73"/>
+      <c r="C63" s="78" t="s">
+        <v>383</v>
+      </c>
+      <c r="D63" s="73">
+        <f>VLOOKUP(A63,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E63" s="73"/>
+      <c r="F63" s="73"/>
+      <c r="G63" s="73"/>
+      <c r="H63" s="86">
+        <v>1</v>
+      </c>
+      <c r="I63" s="73">
+        <v>0</v>
+      </c>
+      <c r="J63" s="73"/>
+      <c r="K63" s="73"/>
+      <c r="L63" s="84">
+        <v>34.977749829395002</v>
+      </c>
+      <c r="M63" s="77"/>
+      <c r="N63" s="73"/>
+      <c r="O63" s="73"/>
+      <c r="P63" s="73"/>
+      <c r="Q63" s="73"/>
+      <c r="R63" s="73"/>
+      <c r="S63" s="73"/>
+      <c r="T63" s="73"/>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A64" s="77" t="s">
+        <v>384</v>
+      </c>
+      <c r="B64" s="73"/>
+      <c r="C64" s="77" t="s">
+        <v>386</v>
+      </c>
+      <c r="D64" s="73">
+        <f>VLOOKUP(A64,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E64" s="73"/>
+      <c r="F64" s="73"/>
+      <c r="G64" s="73"/>
+      <c r="H64" s="86">
+        <v>1</v>
+      </c>
+      <c r="I64" s="73">
+        <v>1</v>
+      </c>
+      <c r="J64" s="73"/>
+      <c r="K64" s="73"/>
+      <c r="L64" s="84">
+        <v>-10.1045270920776</v>
+      </c>
+      <c r="M64" s="77"/>
+      <c r="N64" s="73"/>
+      <c r="O64" s="73"/>
+      <c r="P64" s="73"/>
+      <c r="Q64" s="73"/>
+      <c r="R64" s="73"/>
+      <c r="S64" s="73"/>
+      <c r="T64" s="73"/>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A65" s="77" t="s">
+        <v>387</v>
+      </c>
+      <c r="B65" s="73"/>
+      <c r="C65" s="77" t="s">
+        <v>389</v>
+      </c>
+      <c r="D65" s="73">
+        <f>VLOOKUP(A65,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E65" s="73"/>
+      <c r="F65" s="73"/>
+      <c r="G65" s="73"/>
+      <c r="H65" s="86">
+        <v>1</v>
+      </c>
+      <c r="I65" s="73">
+        <v>1</v>
+      </c>
+      <c r="J65" s="73"/>
+      <c r="K65" s="73"/>
+      <c r="L65" s="84">
+        <v>-21.2358352193176</v>
+      </c>
+      <c r="M65" s="77"/>
+      <c r="N65" s="73"/>
+      <c r="O65" s="73"/>
+      <c r="P65" s="73"/>
+      <c r="Q65" s="73"/>
+      <c r="R65" s="73"/>
+      <c r="S65" s="73"/>
+      <c r="T65" s="73"/>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A66" s="78" t="s">
+        <v>390</v>
+      </c>
+      <c r="B66" s="73"/>
+      <c r="C66" s="78" t="s">
+        <v>392</v>
+      </c>
+      <c r="D66" s="73">
+        <f>VLOOKUP(A66,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E66" s="73"/>
+      <c r="F66" s="73"/>
+      <c r="G66" s="73"/>
+      <c r="H66" s="86">
+        <v>1</v>
+      </c>
+      <c r="I66" s="73">
+        <v>1</v>
+      </c>
+      <c r="J66" s="73"/>
+      <c r="K66" s="73"/>
+      <c r="L66" s="84">
+        <v>0</v>
+      </c>
+      <c r="M66" s="77"/>
+      <c r="N66" s="73"/>
+      <c r="O66" s="73"/>
+      <c r="P66" s="73"/>
+      <c r="Q66" s="73"/>
+      <c r="R66" s="73"/>
+      <c r="S66" s="73"/>
+      <c r="T66" s="73"/>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A67" s="77" t="s">
+        <v>401</v>
+      </c>
+      <c r="B67" s="73"/>
+      <c r="C67" s="77" t="s">
+        <v>149</v>
+      </c>
+      <c r="D67" s="73">
+        <v>0</v>
+      </c>
+      <c r="E67" s="73"/>
+      <c r="F67" s="73"/>
+      <c r="G67" s="73"/>
+      <c r="H67" s="73"/>
+      <c r="I67" s="73"/>
+      <c r="J67" s="73"/>
+      <c r="K67" s="73"/>
+      <c r="L67" s="84">
+        <v>0</v>
+      </c>
+      <c r="M67" s="77"/>
+      <c r="N67" s="73"/>
+      <c r="O67" s="73"/>
+      <c r="P67" s="73"/>
+      <c r="Q67" s="73"/>
+      <c r="R67" s="73"/>
+      <c r="S67" s="73"/>
+      <c r="T67" s="73"/>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A68" s="77" t="s">
+        <v>402</v>
+      </c>
+      <c r="B68" s="73"/>
+      <c r="C68" s="77" t="s">
+        <v>258</v>
+      </c>
+      <c r="D68" s="73">
+        <v>0</v>
+      </c>
+      <c r="E68" s="73"/>
+      <c r="F68" s="73"/>
+      <c r="G68" s="73"/>
+      <c r="H68" s="73"/>
+      <c r="I68" s="73"/>
+      <c r="J68" s="73"/>
+      <c r="K68" s="73"/>
+      <c r="L68" s="84">
+        <v>0</v>
+      </c>
+      <c r="M68" s="77"/>
+      <c r="N68" s="73"/>
+      <c r="O68" s="73"/>
+      <c r="P68" s="73"/>
+      <c r="Q68" s="73"/>
+      <c r="R68" s="73"/>
+      <c r="S68" s="73"/>
+      <c r="T68" s="73"/>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A69" s="77" t="s">
+        <v>403</v>
+      </c>
+      <c r="B69" s="73"/>
+      <c r="C69" s="77" t="s">
+        <v>256</v>
+      </c>
+      <c r="D69" s="73">
+        <v>0</v>
+      </c>
+      <c r="E69" s="73"/>
+      <c r="F69" s="73"/>
+      <c r="G69" s="73"/>
+      <c r="H69" s="73"/>
+      <c r="I69" s="73"/>
+      <c r="J69" s="73"/>
+      <c r="K69" s="73"/>
+      <c r="L69" s="84">
+        <v>0</v>
+      </c>
+      <c r="M69" s="77"/>
+      <c r="N69" s="73"/>
+      <c r="O69" s="73"/>
+      <c r="P69" s="73"/>
+      <c r="Q69" s="73"/>
+      <c r="R69" s="73"/>
+      <c r="S69" s="73"/>
+      <c r="T69" s="73"/>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A70" s="77" t="s">
+        <v>404</v>
+      </c>
+      <c r="B70" s="73"/>
+      <c r="C70" s="77" t="s">
+        <v>260</v>
+      </c>
+      <c r="D70" s="73">
+        <v>0</v>
+      </c>
+      <c r="E70" s="73"/>
+      <c r="F70" s="73"/>
+      <c r="G70" s="73"/>
+      <c r="H70" s="73"/>
+      <c r="I70" s="73"/>
+      <c r="J70" s="73"/>
+      <c r="K70" s="73"/>
+      <c r="L70" s="84">
+        <v>0</v>
+      </c>
+      <c r="M70" s="77"/>
+      <c r="N70" s="73"/>
+      <c r="O70" s="73"/>
+      <c r="P70" s="73"/>
+      <c r="Q70" s="73"/>
+      <c r="R70" s="73"/>
+      <c r="S70" s="73"/>
+      <c r="T70" s="73"/>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A71" s="77" t="s">
+        <v>405</v>
+      </c>
+      <c r="B71" s="73"/>
+      <c r="C71" s="77" t="s">
+        <v>265</v>
+      </c>
+      <c r="D71" s="73">
+        <v>0</v>
+      </c>
+      <c r="E71" s="73"/>
+      <c r="F71" s="73"/>
+      <c r="G71" s="73"/>
+      <c r="H71" s="73"/>
+      <c r="I71" s="73"/>
+      <c r="J71" s="73"/>
+      <c r="K71" s="73"/>
+      <c r="L71" s="84">
+        <v>0</v>
+      </c>
+      <c r="M71" s="77"/>
+      <c r="N71" s="73"/>
+      <c r="O71" s="73"/>
+      <c r="P71" s="73"/>
+      <c r="Q71" s="73"/>
+      <c r="R71" s="73"/>
+      <c r="S71" s="73"/>
+      <c r="T71" s="73"/>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A72" s="77" t="s">
+        <v>406</v>
+      </c>
+      <c r="B72" s="73"/>
+      <c r="C72" s="77" t="s">
+        <v>152</v>
+      </c>
+      <c r="D72" s="73">
+        <v>0</v>
+      </c>
+      <c r="E72" s="73"/>
+      <c r="F72" s="73"/>
+      <c r="G72" s="73"/>
+      <c r="H72" s="73"/>
+      <c r="I72" s="73"/>
+      <c r="J72" s="73"/>
+      <c r="K72" s="73"/>
+      <c r="L72" s="84">
+        <v>0</v>
+      </c>
+      <c r="M72" s="77"/>
+      <c r="N72" s="73"/>
+      <c r="O72" s="73"/>
+      <c r="P72" s="73"/>
+      <c r="Q72" s="73"/>
+      <c r="R72" s="73"/>
+      <c r="S72" s="73"/>
+      <c r="T72" s="73"/>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A73" s="77" t="s">
+        <v>407</v>
+      </c>
+      <c r="B73" s="73"/>
+      <c r="C73" s="77" t="s">
+        <v>285</v>
+      </c>
+      <c r="D73" s="73">
+        <v>0</v>
+      </c>
+      <c r="E73" s="73"/>
+      <c r="F73" s="73"/>
+      <c r="G73" s="73"/>
+      <c r="H73" s="73"/>
+      <c r="I73" s="73"/>
+      <c r="J73" s="73"/>
+      <c r="K73" s="73"/>
+      <c r="L73" s="84">
+        <v>34.977749829395002</v>
+      </c>
+      <c r="M73" s="77"/>
+      <c r="N73" s="73"/>
+      <c r="O73" s="73"/>
+      <c r="P73" s="73"/>
+      <c r="Q73" s="73"/>
+      <c r="R73" s="73"/>
+      <c r="S73" s="73"/>
+      <c r="T73" s="73"/>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A74" s="77" t="s">
+        <v>408</v>
+      </c>
+      <c r="B74" s="73"/>
+      <c r="C74" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="D74" s="73">
+        <v>0</v>
+      </c>
+      <c r="E74" s="73"/>
+      <c r="F74" s="73"/>
+      <c r="G74" s="73"/>
+      <c r="H74" s="73"/>
+      <c r="I74" s="73"/>
+      <c r="J74" s="73"/>
+      <c r="K74" s="73"/>
+      <c r="L74" s="84">
+        <v>10.1045270920776</v>
+      </c>
+      <c r="M74" s="77"/>
+      <c r="N74" s="73"/>
+      <c r="O74" s="73"/>
+      <c r="P74" s="73"/>
+      <c r="Q74" s="73"/>
+      <c r="R74" s="73"/>
+      <c r="S74" s="73"/>
+      <c r="T74" s="73"/>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A75" s="77" t="s">
+        <v>409</v>
+      </c>
+      <c r="B75" s="73"/>
+      <c r="C75" s="77" t="s">
+        <v>216</v>
+      </c>
+      <c r="D75" s="73">
+        <v>0</v>
+      </c>
+      <c r="E75" s="73"/>
+      <c r="F75" s="73"/>
+      <c r="G75" s="73"/>
+      <c r="H75" s="73"/>
+      <c r="I75" s="73"/>
+      <c r="J75" s="73"/>
+      <c r="K75" s="73"/>
+      <c r="L75" s="84">
+        <v>21.2358352193176</v>
+      </c>
+      <c r="M75" s="77"/>
+      <c r="N75" s="73"/>
+      <c r="O75" s="73"/>
+      <c r="P75" s="73"/>
+      <c r="Q75" s="73"/>
+      <c r="R75" s="73"/>
+      <c r="S75" s="73"/>
+      <c r="T75" s="73"/>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A76" s="77" t="s">
+        <v>410</v>
+      </c>
+      <c r="B76" s="73"/>
+      <c r="C76" s="77" t="s">
+        <v>157</v>
+      </c>
+      <c r="D76" s="73">
+        <v>0</v>
+      </c>
+      <c r="E76" s="73"/>
+      <c r="F76" s="73"/>
+      <c r="G76" s="73"/>
+      <c r="H76" s="73"/>
+      <c r="I76" s="73"/>
+      <c r="J76" s="73"/>
+      <c r="K76" s="73"/>
+      <c r="L76" s="84">
+        <v>0</v>
+      </c>
+      <c r="M76" s="77"/>
+      <c r="N76" s="73"/>
+      <c r="O76" s="73"/>
+      <c r="P76" s="73"/>
+      <c r="Q76" s="73"/>
+      <c r="R76" s="73"/>
+      <c r="S76" s="73"/>
+      <c r="T76" s="73"/>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A77" s="77" t="s">
+        <v>411</v>
+      </c>
+      <c r="B77" s="73"/>
+      <c r="C77" s="77" t="s">
+        <v>794</v>
+      </c>
+      <c r="D77" s="73">
+        <v>0</v>
+      </c>
+      <c r="E77" s="73"/>
+      <c r="F77" s="73"/>
+      <c r="G77" s="73"/>
+      <c r="H77" s="73"/>
+      <c r="I77" s="73"/>
+      <c r="J77" s="73"/>
+      <c r="K77" s="73"/>
+      <c r="L77" s="84">
+        <v>-20</v>
+      </c>
+      <c r="M77" s="77"/>
+      <c r="N77" s="73"/>
+      <c r="O77" s="73"/>
+      <c r="P77" s="73"/>
+      <c r="Q77" s="73"/>
+      <c r="R77" s="73"/>
+      <c r="S77" s="73"/>
+      <c r="T77" s="73"/>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A78" s="77" t="s">
+        <v>412</v>
+      </c>
+      <c r="B78" s="73"/>
+      <c r="C78" s="77" t="s">
+        <v>400</v>
+      </c>
+      <c r="D78" s="73">
+        <v>0</v>
+      </c>
+      <c r="E78" s="73"/>
+      <c r="F78" s="73"/>
+      <c r="G78" s="73"/>
+      <c r="H78" s="73"/>
+      <c r="I78" s="73"/>
+      <c r="J78" s="73"/>
+      <c r="K78" s="73"/>
+      <c r="L78" s="84">
+        <v>6.25968789018712</v>
+      </c>
+      <c r="M78" s="77"/>
+      <c r="N78" s="73"/>
+      <c r="O78" s="73"/>
+      <c r="P78" s="73"/>
+      <c r="Q78" s="73"/>
+      <c r="R78" s="73"/>
+      <c r="S78" s="73"/>
+      <c r="T78" s="73"/>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A79" s="77" t="s">
+        <v>413</v>
+      </c>
+      <c r="B79" s="73"/>
+      <c r="C79" s="77" t="s">
+        <v>205</v>
+      </c>
+      <c r="D79" s="73">
+        <v>0</v>
+      </c>
+      <c r="E79" s="73"/>
+      <c r="F79" s="73"/>
+      <c r="G79" s="73"/>
+      <c r="H79" s="73"/>
+      <c r="I79" s="73"/>
+      <c r="J79" s="73"/>
+      <c r="K79" s="73"/>
+      <c r="L79" s="84">
+        <v>65.594624664349297</v>
+      </c>
+      <c r="M79" s="77"/>
+      <c r="N79" s="73"/>
+      <c r="O79" s="73"/>
+      <c r="P79" s="73"/>
+      <c r="Q79" s="73"/>
+      <c r="R79" s="73"/>
+      <c r="S79" s="73"/>
+      <c r="T79" s="73"/>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A80" s="77" t="s">
+        <v>414</v>
+      </c>
+      <c r="B80" s="73"/>
+      <c r="C80" s="77" t="s">
+        <v>206</v>
+      </c>
+      <c r="D80" s="73">
+        <v>0</v>
+      </c>
+      <c r="E80" s="73"/>
+      <c r="F80" s="73"/>
+      <c r="G80" s="73"/>
+      <c r="H80" s="73"/>
+      <c r="I80" s="73"/>
+      <c r="J80" s="73"/>
+      <c r="K80" s="73"/>
+      <c r="L80" s="84">
+        <v>-7.11118951189348</v>
+      </c>
+      <c r="M80" s="77"/>
+      <c r="N80" s="73"/>
+      <c r="O80" s="73"/>
+      <c r="P80" s="73"/>
+      <c r="Q80" s="73"/>
+      <c r="R80" s="73"/>
+      <c r="S80" s="73"/>
+      <c r="T80" s="73"/>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A81" s="77" t="s">
+        <v>460</v>
+      </c>
+      <c r="B81" s="73"/>
+      <c r="C81" s="77" t="s">
+        <v>209</v>
+      </c>
+      <c r="D81" s="73">
+        <v>0</v>
+      </c>
+      <c r="E81" s="73"/>
+      <c r="F81" s="73"/>
+      <c r="G81" s="73"/>
+      <c r="H81" s="73"/>
+      <c r="I81" s="73"/>
+      <c r="J81" s="73"/>
+      <c r="K81" s="73"/>
+      <c r="L81" s="84">
+        <v>-3.5703232462952501</v>
+      </c>
+      <c r="M81" s="77"/>
+      <c r="N81" s="73"/>
+      <c r="O81" s="73"/>
+      <c r="P81" s="73"/>
+      <c r="Q81" s="73"/>
+      <c r="R81" s="73"/>
+      <c r="S81" s="73"/>
+      <c r="T81" s="73"/>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A82" s="77" t="s">
+        <v>461</v>
+      </c>
+      <c r="B82" s="73"/>
+      <c r="C82" s="77" t="s">
+        <v>462</v>
+      </c>
+      <c r="D82" s="73">
+        <v>0</v>
+      </c>
+      <c r="E82" s="73"/>
+      <c r="F82" s="73"/>
+      <c r="G82" s="73"/>
+      <c r="H82" s="73"/>
+      <c r="I82" s="73"/>
+      <c r="J82" s="73"/>
+      <c r="K82" s="73"/>
+      <c r="L82" s="84">
+        <v>-10</v>
+      </c>
+      <c r="M82" s="77"/>
+      <c r="N82" s="73"/>
+      <c r="O82" s="73"/>
+      <c r="P82" s="73"/>
+      <c r="Q82" s="73"/>
+      <c r="R82" s="73"/>
+      <c r="S82" s="73"/>
+      <c r="T82" s="73"/>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A83" s="78" t="s">
+        <v>179</v>
+      </c>
+      <c r="B83" s="73"/>
+      <c r="C83" s="78" t="s">
+        <v>793</v>
+      </c>
+      <c r="D83" s="73">
+        <v>0</v>
+      </c>
+      <c r="E83" s="73"/>
+      <c r="F83" s="73"/>
+      <c r="G83" s="73"/>
+      <c r="H83" s="73"/>
+      <c r="I83" s="73"/>
+      <c r="J83" s="73"/>
+      <c r="K83" s="73"/>
+      <c r="L83" s="84">
+        <v>0.97053938790751804</v>
+      </c>
+      <c r="M83" s="73"/>
+      <c r="N83" s="73"/>
+      <c r="O83" s="73"/>
+      <c r="P83" s="73"/>
+      <c r="Q83" s="73"/>
+      <c r="R83" s="73"/>
+      <c r="S83" s="73"/>
+      <c r="T83" s="73"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
SS flux with pFBA
</commit_message>
<xml_diff>
--- a/KineticModel/ecoli_test.xlsx
+++ b/KineticModel/ecoli_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="840" windowWidth="18195" windowHeight="6765" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="480" yWindow="900" windowWidth="18195" windowHeight="6705" firstSheet="5" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="ecoliT1" sheetId="1" r:id="rId1"/>
@@ -21,16 +21,17 @@
     <sheet name="ecoliN2" sheetId="10" r:id="rId12"/>
     <sheet name="Sheet3" sheetId="12" r:id="rId13"/>
     <sheet name="Sheet4" sheetId="14" r:id="rId14"/>
+    <sheet name="Sheet5" sheetId="15" r:id="rId15"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId15"/>
+    <externalReference r:id="rId16"/>
   </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="834">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="977">
   <si>
     <t>Enzymes</t>
   </si>
@@ -2574,6 +2575,435 @@
   </si>
   <si>
     <t>0.28,0.147</t>
+  </si>
+  <si>
+    <t>'GLCpts'</t>
+  </si>
+  <si>
+    <t>'PGI_f'</t>
+  </si>
+  <si>
+    <t>'PGI_b'</t>
+  </si>
+  <si>
+    <t>'PFK'</t>
+  </si>
+  <si>
+    <t>'FBP'</t>
+  </si>
+  <si>
+    <t>'FBA_f'</t>
+  </si>
+  <si>
+    <t>'FBA_b'</t>
+  </si>
+  <si>
+    <t>'TPI_f'</t>
+  </si>
+  <si>
+    <t>'TPI_b'</t>
+  </si>
+  <si>
+    <t>'GAPD_f'</t>
+  </si>
+  <si>
+    <t>'GAPD_b'</t>
+  </si>
+  <si>
+    <t>'PGK_f'</t>
+  </si>
+  <si>
+    <t>'PGK_b'</t>
+  </si>
+  <si>
+    <t>'PGM_f'</t>
+  </si>
+  <si>
+    <t>'PGM_b'</t>
+  </si>
+  <si>
+    <t>'ENO_f'</t>
+  </si>
+  <si>
+    <t>'ENO_b'</t>
+  </si>
+  <si>
+    <t>'PYK_f'</t>
+  </si>
+  <si>
+    <t>'PYK_b'</t>
+  </si>
+  <si>
+    <t>'PPS'</t>
+  </si>
+  <si>
+    <t>'PDH'</t>
+  </si>
+  <si>
+    <t>'CS_f'</t>
+  </si>
+  <si>
+    <t>'CS_b'</t>
+  </si>
+  <si>
+    <t>'ACONTa_f'</t>
+  </si>
+  <si>
+    <t>'ACONTa_b'</t>
+  </si>
+  <si>
+    <t>'ICDHyr_f'</t>
+  </si>
+  <si>
+    <t>'ICDHyr_b'</t>
+  </si>
+  <si>
+    <t>'ICL'</t>
+  </si>
+  <si>
+    <t>'MALS_f'</t>
+  </si>
+  <si>
+    <t>'MALS_b'</t>
+  </si>
+  <si>
+    <t>'AKGDH'</t>
+  </si>
+  <si>
+    <t>'SUCOAS_f'</t>
+  </si>
+  <si>
+    <t>'SUCOAS_b'</t>
+  </si>
+  <si>
+    <t>'SUCDi'</t>
+  </si>
+  <si>
+    <t>'FRD7_f'</t>
+  </si>
+  <si>
+    <t>'FRD7_b'</t>
+  </si>
+  <si>
+    <t>'FUM_f'</t>
+  </si>
+  <si>
+    <t>'FUM_b'</t>
+  </si>
+  <si>
+    <t>'MDH_f'</t>
+  </si>
+  <si>
+    <t>'MDH_b'</t>
+  </si>
+  <si>
+    <t>'PFL_f'</t>
+  </si>
+  <si>
+    <t>'PFL_b'</t>
+  </si>
+  <si>
+    <t>'LDH_D_f'</t>
+  </si>
+  <si>
+    <t>'LDH_D_b'</t>
+  </si>
+  <si>
+    <t>'PTAr_f'</t>
+  </si>
+  <si>
+    <t>'PTAr_b'</t>
+  </si>
+  <si>
+    <t>'ACKr_f'</t>
+  </si>
+  <si>
+    <t>'ACKr_b'</t>
+  </si>
+  <si>
+    <t>'ACALD_f'</t>
+  </si>
+  <si>
+    <t>'ACALD_b'</t>
+  </si>
+  <si>
+    <t>'ALCD2x_f'</t>
+  </si>
+  <si>
+    <t>'ALCD2x_b'</t>
+  </si>
+  <si>
+    <t>'G6PDH2r_f'</t>
+  </si>
+  <si>
+    <t>'G6PDH2r_b'</t>
+  </si>
+  <si>
+    <t>'PGL'</t>
+  </si>
+  <si>
+    <t>'GND'</t>
+  </si>
+  <si>
+    <t>'RPE_f'</t>
+  </si>
+  <si>
+    <t>'RPE_b'</t>
+  </si>
+  <si>
+    <t>'RPI_f'</t>
+  </si>
+  <si>
+    <t>'RPI_b'</t>
+  </si>
+  <si>
+    <t>'TKT1_f'</t>
+  </si>
+  <si>
+    <t>'TKT1_b'</t>
+  </si>
+  <si>
+    <t>'TALA_f'</t>
+  </si>
+  <si>
+    <t>'TALA_b'</t>
+  </si>
+  <si>
+    <t>'TKT2_f'</t>
+  </si>
+  <si>
+    <t>'TKT2_b'</t>
+  </si>
+  <si>
+    <t>'NADH16_f'</t>
+  </si>
+  <si>
+    <t>'NADH16_b'</t>
+  </si>
+  <si>
+    <t>'NADTRHD_f'</t>
+  </si>
+  <si>
+    <t>'NADTRHD_b'</t>
+  </si>
+  <si>
+    <t>'THD2_f'</t>
+  </si>
+  <si>
+    <t>'THD2_b'</t>
+  </si>
+  <si>
+    <t>'ADK1_f'</t>
+  </si>
+  <si>
+    <t>'ADK1_b'</t>
+  </si>
+  <si>
+    <t>'ATPM'</t>
+  </si>
+  <si>
+    <t>'ATPS4r_f'</t>
+  </si>
+  <si>
+    <t>'ATPS4r_b'</t>
+  </si>
+  <si>
+    <t>'CYTBD'</t>
+  </si>
+  <si>
+    <t>'PPC_f'</t>
+  </si>
+  <si>
+    <t>'PPC_b'</t>
+  </si>
+  <si>
+    <t>'PPCK'</t>
+  </si>
+  <si>
+    <t>'ME1'</t>
+  </si>
+  <si>
+    <t>'ME2'</t>
+  </si>
+  <si>
+    <t>'H2Ot_f'</t>
+  </si>
+  <si>
+    <t>'H2Ot_b'</t>
+  </si>
+  <si>
+    <t>'O2t_f'</t>
+  </si>
+  <si>
+    <t>'O2t_b'</t>
+  </si>
+  <si>
+    <t>'PIt2r_f'</t>
+  </si>
+  <si>
+    <t>'PIt2r_b'</t>
+  </si>
+  <si>
+    <t>'CO2t_f'</t>
+  </si>
+  <si>
+    <t>'CO2t_b'</t>
+  </si>
+  <si>
+    <t>'PYRt2r_f'</t>
+  </si>
+  <si>
+    <t>'PYRt2r_b'</t>
+  </si>
+  <si>
+    <t>'SUCCt2_2'</t>
+  </si>
+  <si>
+    <t>'SUCCt3'</t>
+  </si>
+  <si>
+    <t>'AKGt2r_f'</t>
+  </si>
+  <si>
+    <t>'AKGt2r_b'</t>
+  </si>
+  <si>
+    <t>'FUMt2_2'</t>
+  </si>
+  <si>
+    <t>'MALt2_2'</t>
+  </si>
+  <si>
+    <t>'D_LACt2_f'</t>
+  </si>
+  <si>
+    <t>'D_LACt2_b'</t>
+  </si>
+  <si>
+    <t>'FORt2'</t>
+  </si>
+  <si>
+    <t>'FORti'</t>
+  </si>
+  <si>
+    <t>'ETOHt2r_f'</t>
+  </si>
+  <si>
+    <t>'ETOHt2r_b'</t>
+  </si>
+  <si>
+    <t>'ACt2r_f'</t>
+  </si>
+  <si>
+    <t>'ACt2r_b'</t>
+  </si>
+  <si>
+    <t>'ACALDt_f'</t>
+  </si>
+  <si>
+    <t>'ACALDt_b'</t>
+  </si>
+  <si>
+    <t>'exPYR_f'</t>
+  </si>
+  <si>
+    <t>'exPYR_b'</t>
+  </si>
+  <si>
+    <t>'exSUCC_f'</t>
+  </si>
+  <si>
+    <t>'exSUCC_b'</t>
+  </si>
+  <si>
+    <t>'exAKG_f'</t>
+  </si>
+  <si>
+    <t>'exAKG_b'</t>
+  </si>
+  <si>
+    <t>'exFUM_f'</t>
+  </si>
+  <si>
+    <t>'exFUM_b'</t>
+  </si>
+  <si>
+    <t>'exMAL_f'</t>
+  </si>
+  <si>
+    <t>'exMAL_b'</t>
+  </si>
+  <si>
+    <t>'exLAC_f'</t>
+  </si>
+  <si>
+    <t>'exLAC_b'</t>
+  </si>
+  <si>
+    <t>'exFOR_f'</t>
+  </si>
+  <si>
+    <t>'exFOR_b'</t>
+  </si>
+  <si>
+    <t>'exETOH_f'</t>
+  </si>
+  <si>
+    <t>'exETOH_b'</t>
+  </si>
+  <si>
+    <t>'exAC_f'</t>
+  </si>
+  <si>
+    <t>'exAC_b'</t>
+  </si>
+  <si>
+    <t>'exACALD_f'</t>
+  </si>
+  <si>
+    <t>'exACALD_b'</t>
+  </si>
+  <si>
+    <t>'exGLC_f'</t>
+  </si>
+  <si>
+    <t>'exGLC_b'</t>
+  </si>
+  <si>
+    <t>'exCO2_f'</t>
+  </si>
+  <si>
+    <t>'exCO2_b'</t>
+  </si>
+  <si>
+    <t>'exH_f'</t>
+  </si>
+  <si>
+    <t>'exH_b'</t>
+  </si>
+  <si>
+    <t>'exH2O_f'</t>
+  </si>
+  <si>
+    <t>'exH2O_b'</t>
+  </si>
+  <si>
+    <t>'exPI_f'</t>
+  </si>
+  <si>
+    <t>'exPI_b'</t>
+  </si>
+  <si>
+    <t>'exO2_f'</t>
+  </si>
+  <si>
+    <t>'exO2_b'</t>
+  </si>
+  <si>
+    <t>'EC_biomass'</t>
+  </si>
+  <si>
+    <t>'netFlux'</t>
   </si>
 </sst>
 </file>
@@ -6807,8 +7237,8 @@
   <dimension ref="A1:T83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8829,10 +9259,10 @@
         <v>0</v>
       </c>
       <c r="H52" s="86">
-        <v>1.6670000000000001E-2</v>
+        <v>1</v>
       </c>
       <c r="I52">
-        <v>1.6670000000000001E-2</v>
+        <v>1</v>
       </c>
       <c r="J52" s="73"/>
       <c r="K52" s="73"/>
@@ -10998,7 +11428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L96"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I83" sqref="I83"/>
     </sheetView>
   </sheetViews>
@@ -14331,11 +14761,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T83"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection sqref="A1:T83"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="44" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="73" t="s">
@@ -17576,6 +18009,1910 @@
       <c r="R83" s="73"/>
       <c r="S83" s="73"/>
       <c r="T83" s="73"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F143"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="73" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>834</v>
+      </c>
+      <c r="B1">
+        <v>20</v>
+      </c>
+      <c r="E1" s="79" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>835</v>
+      </c>
+      <c r="B2">
+        <v>19.487319257707199</v>
+      </c>
+      <c r="D2" s="77" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="84">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>836</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="77" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="84">
+        <v>19.641084088999801</v>
+      </c>
+      <c r="F3">
+        <v>19.641084088999801</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>837</v>
+      </c>
+      <c r="B4">
+        <v>17.512373003127401</v>
+      </c>
+      <c r="D4" s="77" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="84">
+        <v>18.2584699674542</v>
+      </c>
+      <c r="F4">
+        <v>18.2584699674542</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>838</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="77" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" s="84">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>839</v>
+      </c>
+      <c r="B6">
+        <v>17.512373003127401</v>
+      </c>
+      <c r="D6" s="77" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="84">
+        <v>18.2584699674542</v>
+      </c>
+      <c r="F6">
+        <v>18.2584699674542</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>840</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="77" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" s="85">
+        <v>-18.2584699674542</v>
+      </c>
+      <c r="F7">
+        <v>-18.2584699674542</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>841</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="D8" s="77" t="s">
+        <v>127</v>
+      </c>
+      <c r="E8" s="84">
+        <v>35.345823579454603</v>
+      </c>
+      <c r="F8">
+        <v>35.345823579454603</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>842</v>
+      </c>
+      <c r="B9">
+        <v>17.512373003127401</v>
+      </c>
+      <c r="D9" s="77" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" s="84">
+        <v>-35.345823579454603</v>
+      </c>
+      <c r="F9">
+        <v>-35.345823579454603</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>843</v>
+      </c>
+      <c r="B10">
+        <v>33.351906257377699</v>
+      </c>
+      <c r="D10" s="77" t="s">
+        <v>130</v>
+      </c>
+      <c r="E10" s="84">
+        <v>-32.726612833814102</v>
+      </c>
+      <c r="F10">
+        <v>-32.726612833814102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>844</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="D11" s="77" t="s">
+        <v>134</v>
+      </c>
+      <c r="E11" s="84">
+        <v>32.726612833814102</v>
+      </c>
+      <c r="F11">
+        <v>32.726612833814102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>845</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="84">
+        <v>-15.8997796489202</v>
+      </c>
+      <c r="F12">
+        <v>-15.8997796489202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>846</v>
+      </c>
+      <c r="B13">
+        <v>33.351906257377699</v>
+      </c>
+      <c r="D13" s="77" t="s">
+        <v>136</v>
+      </c>
+      <c r="E13" s="84">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>847</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="D14" s="77" t="s">
+        <v>140</v>
+      </c>
+      <c r="E14" s="84">
+        <v>8.4636074707051101</v>
+      </c>
+      <c r="F14">
+        <v>8.4636074707046305</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>848</v>
+      </c>
+      <c r="B15">
+        <v>29.6105872794733</v>
+      </c>
+      <c r="D15" s="77" t="s">
+        <v>239</v>
+      </c>
+      <c r="E15" s="84">
+        <v>7.2101829496634</v>
+      </c>
+      <c r="F15">
+        <v>7.2101829496634</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>849</v>
+      </c>
+      <c r="B16">
+        <v>29.6105872794733</v>
+      </c>
+      <c r="D16" s="78" t="s">
+        <v>317</v>
+      </c>
+      <c r="E16" s="84">
+        <v>-7.2101829496634</v>
+      </c>
+      <c r="F16">
+        <v>-7.2101829496634</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>850</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="D17" s="77" t="s">
+        <v>323</v>
+      </c>
+      <c r="E17" s="84">
+        <v>-7.2101829496634</v>
+      </c>
+      <c r="F17">
+        <v>-7.2101829496634</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>851</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="D18" s="77" t="s">
+        <v>325</v>
+      </c>
+      <c r="E18" s="84">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>852</v>
+      </c>
+      <c r="B19">
+        <v>14.1431852176778</v>
+      </c>
+      <c r="D19" s="77" t="s">
+        <v>328</v>
+      </c>
+      <c r="E19" s="84">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>853</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="D20" s="77" t="s">
+        <v>245</v>
+      </c>
+      <c r="E20" s="84">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>854</v>
+      </c>
+      <c r="B21">
+        <v>27.0586876236889</v>
+      </c>
+      <c r="D21" s="77" t="s">
+        <v>332</v>
+      </c>
+      <c r="E21" s="84">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>855</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="D22" s="78" t="s">
+        <v>334</v>
+      </c>
+      <c r="E22" s="84">
+        <v>100</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>856</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="D23" s="78" t="s">
+        <v>251</v>
+      </c>
+      <c r="E23" s="84">
+        <v>-100</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>857</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="D24" s="77" t="s">
+        <v>252</v>
+      </c>
+      <c r="E24" s="84">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>858</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="D25" s="77" t="s">
+        <v>253</v>
+      </c>
+      <c r="E25" s="84">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>859</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="D26" s="77" t="s">
+        <v>141</v>
+      </c>
+      <c r="E26" s="84">
+        <v>-22.476479530989</v>
+      </c>
+      <c r="F26">
+        <v>-22.476479530989501</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>860</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="D27" s="77" t="s">
+        <v>305</v>
+      </c>
+      <c r="E27" s="84">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>861</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="D28" s="77" t="s">
+        <v>212</v>
+      </c>
+      <c r="E28" s="85">
+        <v>31.588586774545199</v>
+      </c>
+      <c r="F28">
+        <v>31.588586774545501</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>862</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="D29" s="77" t="s">
+        <v>214</v>
+      </c>
+      <c r="E29" s="84">
+        <v>-31.588586774545199</v>
+      </c>
+      <c r="F29">
+        <v>-31.588586774545501</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>863</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="D30" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="E30" s="84">
+        <v>0</v>
+      </c>
+      <c r="F30" s="11">
+        <v>2.4868995751603501E-13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>864</v>
+      </c>
+      <c r="B31">
+        <v>10.299130892249799</v>
+      </c>
+      <c r="D31" s="78" t="s">
+        <v>145</v>
+      </c>
+      <c r="E31" s="84">
+        <v>0</v>
+      </c>
+      <c r="F31" s="11">
+        <v>2.4868995751603501E-13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>865</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="D32" s="77" t="s">
+        <v>415</v>
+      </c>
+      <c r="E32" s="84">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>866</v>
+      </c>
+      <c r="B33">
+        <v>10.299130892249799</v>
+      </c>
+      <c r="D33" s="77" t="s">
+        <v>419</v>
+      </c>
+      <c r="E33" s="84">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>867</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="D34" s="77" t="s">
+        <v>422</v>
+      </c>
+      <c r="E34" s="84">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>868</v>
+      </c>
+      <c r="B35">
+        <v>10.299130892249799</v>
+      </c>
+      <c r="D35" s="77" t="s">
+        <v>425</v>
+      </c>
+      <c r="E35" s="85">
+        <v>-1.2584817406192199</v>
+      </c>
+      <c r="F35">
+        <v>-1.2584817406192199</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>869</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="D36" s="77" t="s">
+        <v>428</v>
+      </c>
+      <c r="E36" s="85">
+        <v>-1.2584817406192199</v>
+      </c>
+      <c r="F36">
+        <v>-1.2584817406192199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>870</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="D37" s="77" t="s">
+        <v>431</v>
+      </c>
+      <c r="E37" s="84">
+        <v>0.31321978769724201</v>
+      </c>
+      <c r="F37">
+        <v>0.31321978769724201</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>871</v>
+      </c>
+      <c r="B38">
+        <v>10.299130892249799</v>
+      </c>
+      <c r="D38" s="77" t="s">
+        <v>436</v>
+      </c>
+      <c r="E38" s="84">
+        <v>-0.31321978769724201</v>
+      </c>
+      <c r="F38">
+        <v>-0.31321978769724201</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>872</v>
+      </c>
+      <c r="B39">
+        <v>10.299130892249799</v>
+      </c>
+      <c r="D39" s="77" t="s">
+        <v>434</v>
+      </c>
+      <c r="E39" s="84">
+        <v>0.94526195292197401</v>
+      </c>
+      <c r="F39">
+        <v>0.94526195292197401</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>873</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="D40" s="78" t="s">
+        <v>169</v>
+      </c>
+      <c r="E40" s="84">
+        <v>-20</v>
+      </c>
+      <c r="F40">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>874</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="D41" s="77" t="s">
+        <v>441</v>
+      </c>
+      <c r="E41" s="84">
+        <v>-100</v>
+      </c>
+      <c r="F41">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>875</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="D42" s="77" t="s">
+        <v>444</v>
+      </c>
+      <c r="E42" s="84">
+        <v>69.980448284876005</v>
+      </c>
+      <c r="F42">
+        <v>69.980448284876005</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>876</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="D43" s="77" t="s">
+        <v>178</v>
+      </c>
+      <c r="E43" s="84">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>877</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="D44" s="77" t="s">
+        <v>171</v>
+      </c>
+      <c r="E44" s="84">
+        <v>8.39</v>
+      </c>
+      <c r="F44">
+        <v>8.39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>878</v>
+      </c>
+      <c r="B45">
+        <v>17.685883301904202</v>
+      </c>
+      <c r="D45" s="77" t="s">
+        <v>173</v>
+      </c>
+      <c r="E45" s="84">
+        <v>-48.530185510493098</v>
+      </c>
+      <c r="F45">
+        <v>-48.530185510492899</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>879</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="D46" s="77" t="s">
+        <v>167</v>
+      </c>
+      <c r="E46" s="84">
+        <v>20</v>
+      </c>
+      <c r="F46">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>880</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="D47" s="77" t="s">
+        <v>234</v>
+      </c>
+      <c r="E47" s="84">
+        <v>4.0820119341314696</v>
+      </c>
+      <c r="F47">
+        <v>4.0820119341314696</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>881</v>
+      </c>
+      <c r="B48">
+        <v>17.685883301904202</v>
+      </c>
+      <c r="D48" s="77" t="s">
+        <v>237</v>
+      </c>
+      <c r="E48" s="84">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>882</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="D49" s="77" t="s">
+        <v>254</v>
+      </c>
+      <c r="E49" s="84">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>883</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="D50" s="77" t="s">
+        <v>364</v>
+      </c>
+      <c r="E50" s="84">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>884</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="D51" s="77" t="s">
+        <v>663</v>
+      </c>
+      <c r="E51" s="84">
+        <v>0.55691231785686302</v>
+      </c>
+      <c r="F51">
+        <v>0.55691231785706197</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>885</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="D52" s="77" t="s">
+        <v>463</v>
+      </c>
+      <c r="E52" s="84">
+        <v>10</v>
+      </c>
+      <c r="F52">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>886</v>
+      </c>
+      <c r="B53" s="11">
+        <v>-2.2382096176443199E-13</v>
+      </c>
+      <c r="D53" s="77" t="s">
+        <v>456</v>
+      </c>
+      <c r="E53" s="84">
+        <v>6.4407022526654396</v>
+      </c>
+      <c r="F53">
+        <v>6.4407022526654298</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>887</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="D54" s="77" t="s">
+        <v>397</v>
+      </c>
+      <c r="E54" s="84">
+        <v>-5.3354364551731797</v>
+      </c>
+      <c r="F54">
+        <v>-5.3354364551727</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>888</v>
+      </c>
+      <c r="B55" s="11">
+        <v>-2.2315482794965601E-13</v>
+      </c>
+      <c r="D55" s="77" t="s">
+        <v>343</v>
+      </c>
+      <c r="E55" s="84">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>889</v>
+      </c>
+      <c r="B56" s="11">
+        <v>-2.2315482794965601E-13</v>
+      </c>
+      <c r="D56" s="77" t="s">
+        <v>346</v>
+      </c>
+      <c r="E56" s="84">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>890</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="D57" s="77" t="s">
+        <v>349</v>
+      </c>
+      <c r="E57" s="84">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>891</v>
+      </c>
+      <c r="B58">
+        <v>1.7976337441964301</v>
+      </c>
+      <c r="D58" s="77" t="s">
+        <v>353</v>
+      </c>
+      <c r="E58" s="84">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>892</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="D59" s="77" t="s">
+        <v>356</v>
+      </c>
+      <c r="E59" s="84">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>893</v>
+      </c>
+      <c r="B60">
+        <v>1.79763374419621</v>
+      </c>
+      <c r="D60" s="78" t="s">
+        <v>360</v>
+      </c>
+      <c r="E60" s="84">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>894</v>
+      </c>
+      <c r="B61">
+        <v>0.44740773071336798</v>
+      </c>
+      <c r="D61" s="77" t="s">
+        <v>368</v>
+      </c>
+      <c r="E61" s="84">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>895</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="D62" s="78" t="s">
+        <v>378</v>
+      </c>
+      <c r="E62" s="84">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>896</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="D63" s="78" t="s">
+        <v>381</v>
+      </c>
+      <c r="E63" s="84">
+        <v>22.476479530989</v>
+      </c>
+      <c r="F63">
+        <v>22.476479530989501</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>897</v>
+      </c>
+      <c r="B64">
+        <v>0.44740773071336798</v>
+      </c>
+      <c r="D64" s="77" t="s">
+        <v>384</v>
+      </c>
+      <c r="E64" s="84">
+        <v>0</v>
+      </c>
+      <c r="F64" s="11">
+        <v>2.4868995751603501E-13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>898</v>
+      </c>
+      <c r="B65">
+        <v>1.3502260134830599</v>
+      </c>
+      <c r="D65" s="77" t="s">
+        <v>387</v>
+      </c>
+      <c r="E65" s="84">
+        <v>-31.588586774545199</v>
+      </c>
+      <c r="F65">
+        <v>-31.588586774545501</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>899</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="D66" s="78" t="s">
+        <v>390</v>
+      </c>
+      <c r="E66" s="84">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>900</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="D67" s="77" t="s">
+        <v>401</v>
+      </c>
+      <c r="E67" s="84">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>901</v>
+      </c>
+      <c r="B68">
+        <v>57.298246643096903</v>
+      </c>
+      <c r="D68" s="77" t="s">
+        <v>402</v>
+      </c>
+      <c r="E68" s="84">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>902</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="D69" s="77" t="s">
+        <v>403</v>
+      </c>
+      <c r="E69" s="84">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>903</v>
+      </c>
+      <c r="B70">
+        <v>95.722996525785405</v>
+      </c>
+      <c r="D70" s="77" t="s">
+        <v>404</v>
+      </c>
+      <c r="E70" s="84">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>904</v>
+      </c>
+      <c r="B71">
+        <v>63.141760220811697</v>
+      </c>
+      <c r="D71" s="77" t="s">
+        <v>405</v>
+      </c>
+      <c r="E71" s="84">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>905</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="D72" s="77" t="s">
+        <v>406</v>
+      </c>
+      <c r="E72" s="84">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>906</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="D73" s="77" t="s">
+        <v>407</v>
+      </c>
+      <c r="E73" s="84">
+        <v>22.476479530989</v>
+      </c>
+      <c r="F73">
+        <v>22.476479530989501</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>907</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="D74" s="77" t="s">
+        <v>408</v>
+      </c>
+      <c r="E74" s="84">
+        <v>0</v>
+      </c>
+      <c r="F74" s="11">
+        <v>-2.4868995751603501E-13</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>908</v>
+      </c>
+      <c r="B75">
+        <v>8.39</v>
+      </c>
+      <c r="D75" s="77" t="s">
+        <v>409</v>
+      </c>
+      <c r="E75" s="84">
+        <v>31.588586774545199</v>
+      </c>
+      <c r="F75">
+        <v>31.588586774545501</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>909</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="D76" s="77" t="s">
+        <v>410</v>
+      </c>
+      <c r="E76" s="84">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>910</v>
+      </c>
+      <c r="B77">
+        <v>100</v>
+      </c>
+      <c r="D77" s="77" t="s">
+        <v>411</v>
+      </c>
+      <c r="E77" s="84">
+        <v>-20</v>
+      </c>
+      <c r="F77">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>911</v>
+      </c>
+      <c r="B78">
+        <v>67.597377535346595</v>
+      </c>
+      <c r="D78" s="77" t="s">
+        <v>412</v>
+      </c>
+      <c r="E78" s="84">
+        <v>5.3354364551731797</v>
+      </c>
+      <c r="F78">
+        <v>5.3354364551727</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>912</v>
+      </c>
+      <c r="B79">
+        <v>5.8308056129572003</v>
+      </c>
+      <c r="D79" s="77" t="s">
+        <v>413</v>
+      </c>
+      <c r="E79" s="84">
+        <v>70.988039049659307</v>
+      </c>
+      <c r="F79">
+        <v>70.988039049660202</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>913</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="D80" s="77" t="s">
+        <v>414</v>
+      </c>
+      <c r="E80" s="84">
+        <v>-0.55691231785686302</v>
+      </c>
+      <c r="F80">
+        <v>-0.55691231785706197</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>914</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="D81" s="77" t="s">
+        <v>460</v>
+      </c>
+      <c r="E81" s="84">
+        <v>-6.4407022526654396</v>
+      </c>
+      <c r="F81">
+        <v>-6.4407022526654298</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>915</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="D82" s="77" t="s">
+        <v>461</v>
+      </c>
+      <c r="E82" s="84">
+        <v>-10</v>
+      </c>
+      <c r="F82">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>916</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="D83" s="78" t="s">
+        <v>179</v>
+      </c>
+      <c r="E83" s="84">
+        <v>1.7508093219521601</v>
+      </c>
+      <c r="F83">
+        <v>1.7508093219521601</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>917</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>918</v>
+      </c>
+      <c r="B85">
+        <v>34.771906869445701</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>919</v>
+      </c>
+      <c r="B86">
+        <v>33.798688767673298</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>920</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>921</v>
+      </c>
+      <c r="B88">
+        <v>9.1999933984068996</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>922</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>923</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>924</v>
+      </c>
+      <c r="B91">
+        <v>43.188624128895597</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>925</v>
+      </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>926</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>927</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>928</v>
+      </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>929</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>930</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>931</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>932</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>933</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>934</v>
+      </c>
+      <c r="B101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>935</v>
+      </c>
+      <c r="B102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>936</v>
+      </c>
+      <c r="B103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>937</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>938</v>
+      </c>
+      <c r="B105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>939</v>
+      </c>
+      <c r="B106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>940</v>
+      </c>
+      <c r="B107">
+        <v>17.685883301904202</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>941</v>
+      </c>
+      <c r="B108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>942</v>
+      </c>
+      <c r="B109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>943</v>
+      </c>
+      <c r="B110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>944</v>
+      </c>
+      <c r="B111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>945</v>
+      </c>
+      <c r="B112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>946</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>947</v>
+      </c>
+      <c r="B114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>948</v>
+      </c>
+      <c r="B115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>949</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>950</v>
+      </c>
+      <c r="B117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>951</v>
+      </c>
+      <c r="B118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>952</v>
+      </c>
+      <c r="B119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>953</v>
+      </c>
+      <c r="B120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>954</v>
+      </c>
+      <c r="B121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>955</v>
+      </c>
+      <c r="B122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>956</v>
+      </c>
+      <c r="B123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>957</v>
+      </c>
+      <c r="B124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>958</v>
+      </c>
+      <c r="B125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>959</v>
+      </c>
+      <c r="B126">
+        <v>17.685883301904202</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>960</v>
+      </c>
+      <c r="B127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>961</v>
+      </c>
+      <c r="B128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>962</v>
+      </c>
+      <c r="B129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>963</v>
+      </c>
+      <c r="B130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>964</v>
+      </c>
+      <c r="B131">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>965</v>
+      </c>
+      <c r="B132">
+        <v>43.188624128895597</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>966</v>
+      </c>
+      <c r="B133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>967</v>
+      </c>
+      <c r="B134">
+        <v>41.858905345104603</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>968</v>
+      </c>
+      <c r="B135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>969</v>
+      </c>
+      <c r="B136">
+        <v>34.771906869445701</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>970</v>
+      </c>
+      <c r="B137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>971</v>
+      </c>
+      <c r="B138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>972</v>
+      </c>
+      <c r="B139">
+        <v>9.1999933984068996</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>973</v>
+      </c>
+      <c r="B140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>974</v>
+      </c>
+      <c r="B141">
+        <v>33.798688767673298</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>975</v>
+      </c>
+      <c r="B142">
+        <v>2.5008816697221499</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>976</v>
+      </c>
+      <c r="B143">
+        <v>1091.4901946959901</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Working Version of initial sampler
</commit_message>
<xml_diff>
--- a/KineticModel/ecoli_test.xlsx
+++ b/KineticModel/ecoli_test.xlsx
@@ -7237,8 +7237,8 @@
   <dimension ref="A1:T83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14761,8 +14761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18019,8 +18019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F143"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18071,7 +18071,7 @@
         <v>19.641084088999801</v>
       </c>
       <c r="F3">
-        <v>19.641084088999801</v>
+        <v>19.487319257707</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -18088,7 +18088,7 @@
         <v>18.2584699674542</v>
       </c>
       <c r="F4">
-        <v>18.2584699674542</v>
+        <v>17.512373003127401</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -18122,7 +18122,7 @@
         <v>18.2584699674542</v>
       </c>
       <c r="F6">
-        <v>18.2584699674542</v>
+        <v>17.512373003127401</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -18139,7 +18139,7 @@
         <v>-18.2584699674542</v>
       </c>
       <c r="F7">
-        <v>-18.2584699674542</v>
+        <v>-17.512373003127401</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -18156,7 +18156,7 @@
         <v>35.345823579454603</v>
       </c>
       <c r="F8">
-        <v>35.345823579454603</v>
+        <v>33.3519062573776</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -18173,7 +18173,7 @@
         <v>-35.345823579454603</v>
       </c>
       <c r="F9">
-        <v>-35.345823579454603</v>
+        <v>-33.3519062573776</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -18190,7 +18190,7 @@
         <v>-32.726612833814102</v>
       </c>
       <c r="F10">
-        <v>-32.726612833814102</v>
+        <v>-29.6105872794733</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -18207,7 +18207,7 @@
         <v>32.726612833814102</v>
       </c>
       <c r="F11">
-        <v>32.726612833814102</v>
+        <v>29.6105872794733</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -18224,7 +18224,7 @@
         <v>-15.8997796489202</v>
       </c>
       <c r="F12">
-        <v>-15.8997796489202</v>
+        <v>-14.143185217677701</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -18258,7 +18258,7 @@
         <v>8.4636074707051101</v>
       </c>
       <c r="F14">
-        <v>8.4636074707046305</v>
+        <v>27.058687623688801</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -18275,7 +18275,7 @@
         <v>7.2101829496634</v>
       </c>
       <c r="F15">
-        <v>7.2101829496634</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -18292,7 +18292,7 @@
         <v>-7.2101829496634</v>
       </c>
       <c r="F16">
-        <v>-7.2101829496634</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -18309,7 +18309,7 @@
         <v>-7.2101829496634</v>
       </c>
       <c r="F17">
-        <v>-7.2101829496634</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -18360,7 +18360,7 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>10.2991308922496</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -18377,7 +18377,7 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>-10.2991308922496</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -18411,7 +18411,7 @@
         <v>-100</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>10.2991308922496</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -18428,7 +18428,7 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>-10.2991308922496</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -18445,7 +18445,7 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>10.2991308922496</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -18462,7 +18462,7 @@
         <v>-22.476479530989</v>
       </c>
       <c r="F26">
-        <v>-22.476479530989501</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -18496,7 +18496,7 @@
         <v>31.588586774545199</v>
       </c>
       <c r="F28">
-        <v>31.588586774545501</v>
+        <v>17.6858833019045</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -18513,7 +18513,7 @@
         <v>-31.588586774545199</v>
       </c>
       <c r="F29">
-        <v>-31.588586774545501</v>
+        <v>-17.6858833019045</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -18530,7 +18530,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="11">
-        <v>2.4868995751603501E-13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -18547,7 +18547,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="11">
-        <v>2.4868995751603501E-13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -18615,7 +18615,7 @@
         <v>-1.2584817406192199</v>
       </c>
       <c r="F35">
-        <v>-1.2584817406192199</v>
+        <v>-1.79763374419628</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -18632,7 +18632,7 @@
         <v>-1.2584817406192199</v>
       </c>
       <c r="F36">
-        <v>-1.2584817406192199</v>
+        <v>-1.79763374419628</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -18649,7 +18649,7 @@
         <v>0.31321978769724201</v>
       </c>
       <c r="F37">
-        <v>0.31321978769724201</v>
+        <v>0.44740773071329298</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -18666,7 +18666,7 @@
         <v>-0.31321978769724201</v>
       </c>
       <c r="F38">
-        <v>-0.31321978769724201</v>
+        <v>-0.44740773071329298</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -18683,7 +18683,7 @@
         <v>0.94526195292197401</v>
       </c>
       <c r="F39">
-        <v>0.94526195292197401</v>
+        <v>1.35022601348299</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -18700,7 +18700,7 @@
         <v>-20</v>
       </c>
       <c r="F40">
-        <v>-20</v>
+        <v>-57.298246643096498</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -18717,7 +18717,7 @@
         <v>-100</v>
       </c>
       <c r="F41">
-        <v>-100</v>
+        <v>-95.722996525786201</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -18734,7 +18734,7 @@
         <v>69.980448284876005</v>
       </c>
       <c r="F42">
-        <v>69.980448284876005</v>
+        <v>63.141760220812799</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -18785,7 +18785,7 @@
         <v>-48.530185510493098</v>
       </c>
       <c r="F45">
-        <v>-48.530185510492899</v>
+        <v>-100</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -18802,7 +18802,7 @@
         <v>20</v>
       </c>
       <c r="F46">
-        <v>20</v>
+        <v>67.597377535346098</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -18819,7 +18819,7 @@
         <v>4.0820119341314696</v>
       </c>
       <c r="F47">
-        <v>4.0820119341314696</v>
+        <v>5.8308056129572003</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -18887,7 +18887,7 @@
         <v>0.55691231785686302</v>
       </c>
       <c r="F51">
-        <v>0.55691231785706197</v>
+        <v>-34.771906869445303</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -18904,7 +18904,7 @@
         <v>10</v>
       </c>
       <c r="F52">
-        <v>10</v>
+        <v>33.798688767672999</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -18921,7 +18921,7 @@
         <v>6.4407022526654396</v>
       </c>
       <c r="F53">
-        <v>6.4407022526654298</v>
+        <v>9.19999339840688</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -18938,7 +18938,7 @@
         <v>-5.3354364551731797</v>
       </c>
       <c r="F54">
-        <v>-5.3354364551727</v>
+        <v>-43.188624128895299</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -19091,7 +19091,7 @@
         <v>22.476479530989</v>
       </c>
       <c r="F63">
-        <v>22.476479530989501</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -19108,7 +19108,7 @@
         <v>0</v>
       </c>
       <c r="F64" s="11">
-        <v>2.4868995751603501E-13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -19125,7 +19125,7 @@
         <v>-31.588586774545199</v>
       </c>
       <c r="F65">
-        <v>-31.588586774545501</v>
+        <v>-17.6858833019045</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -19261,7 +19261,7 @@
         <v>22.476479530989</v>
       </c>
       <c r="F73">
-        <v>22.476479530989501</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -19278,7 +19278,7 @@
         <v>0</v>
       </c>
       <c r="F74" s="11">
-        <v>-2.4868995751603501E-13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -19295,7 +19295,7 @@
         <v>31.588586774545199</v>
       </c>
       <c r="F75">
-        <v>31.588586774545501</v>
+        <v>17.6858833019045</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -19346,7 +19346,7 @@
         <v>5.3354364551731797</v>
       </c>
       <c r="F78">
-        <v>5.3354364551727</v>
+        <v>43.188624128895299</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -19363,7 +19363,7 @@
         <v>70.988039049659307</v>
       </c>
       <c r="F79">
-        <v>70.988039049660202</v>
+        <v>41.858905345104802</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -19380,7 +19380,7 @@
         <v>-0.55691231785686302</v>
       </c>
       <c r="F80">
-        <v>-0.55691231785706197</v>
+        <v>34.771906869445303</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -19397,7 +19397,7 @@
         <v>-6.4407022526654396</v>
       </c>
       <c r="F81">
-        <v>-6.4407022526654298</v>
+        <v>-9.19999339840688</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -19414,7 +19414,7 @@
         <v>-10</v>
       </c>
       <c r="F82">
-        <v>-10</v>
+        <v>-33.798688767672999</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -19431,7 +19431,7 @@
         <v>1.7508093219521601</v>
       </c>
       <c r="F83">
-        <v>1.7508093219521601</v>
+        <v>2.5008816697221499</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ACHR work in Progress
</commit_message>
<xml_diff>
--- a/KineticModel/ecoli_test.xlsx
+++ b/KineticModel/ecoli_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="900" windowWidth="18195" windowHeight="6705" firstSheet="5" activeTab="14"/>
+    <workbookView xWindow="480" yWindow="900" windowWidth="18195" windowHeight="6705" firstSheet="5" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="ecoliT1" sheetId="1" r:id="rId1"/>
@@ -7253,9 +7253,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18036,7 +18036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J83" sqref="J83"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Code corrections - Work in Progress
</commit_message>
<xml_diff>
--- a/KineticModel/ecoli_test.xlsx
+++ b/KineticModel/ecoli_test.xlsx
@@ -7254,8 +7254,8 @@
   <dimension ref="A1:T83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7263,7 +7263,7 @@
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" customWidth="1"/>
     <col min="3" max="3" width="50.140625" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
     <col min="5" max="5" width="6.85546875" customWidth="1"/>
     <col min="6" max="6" width="7" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" customWidth="1"/>
@@ -7387,8 +7387,7 @@
         <v>22</v>
       </c>
       <c r="D3" s="73">
-        <f>VLOOKUP(A3,Sheet3!$A$2:$I$84,6,FALSE)</f>
-        <v>-0.8</v>
+        <v>3.1320000000000001</v>
       </c>
       <c r="E3">
         <v>-17.100000000000001</v>
@@ -7397,7 +7396,7 @@
         <v>20.6</v>
       </c>
       <c r="H3" s="73">
-        <v>11.09</v>
+        <v>120</v>
       </c>
       <c r="J3" s="73"/>
       <c r="K3" s="73"/>
@@ -7528,6 +7527,9 @@
       <c r="H6" s="73">
         <v>8.5</v>
       </c>
+      <c r="I6">
+        <v>0.4</v>
+      </c>
       <c r="J6" s="73"/>
       <c r="K6" s="73"/>
       <c r="L6" s="84">
@@ -7557,17 +7559,14 @@
       <c r="C7" s="77" t="s">
         <v>818</v>
       </c>
-      <c r="D7" s="73">
-        <v>-1.4</v>
+      <c r="D7" s="86">
+        <v>7.5979999999999999</v>
       </c>
       <c r="E7">
         <v>-24.3</v>
       </c>
       <c r="F7">
         <v>13.4</v>
-      </c>
-      <c r="G7">
-        <v>9.1199999999999992</v>
       </c>
       <c r="H7" s="73"/>
       <c r="I7">
@@ -7613,7 +7612,7 @@
         <v>62.6</v>
       </c>
       <c r="H8" s="73">
-        <v>671.72</v>
+        <v>268</v>
       </c>
       <c r="J8" s="73"/>
       <c r="K8" s="73"/>
@@ -7645,7 +7644,7 @@
         <v>128</v>
       </c>
       <c r="D9" s="73">
-        <v>2.8</v>
+        <v>-10.51</v>
       </c>
       <c r="E9">
         <v>-19.2</v>
@@ -7655,7 +7654,7 @@
       </c>
       <c r="G9" s="11"/>
       <c r="I9" s="73">
-        <v>2225</v>
+        <v>654</v>
       </c>
       <c r="J9" s="73"/>
       <c r="K9" s="73"/>
@@ -7686,18 +7685,17 @@
       <c r="C10" s="77" t="s">
         <v>300</v>
       </c>
-      <c r="D10" s="73"/>
+      <c r="D10" s="73">
+        <v>6.2290000000000001</v>
+      </c>
       <c r="E10">
         <v>-23.1</v>
       </c>
       <c r="F10">
         <v>14.6</v>
       </c>
-      <c r="G10">
-        <v>5.49</v>
-      </c>
       <c r="I10" s="73">
-        <v>90.55</v>
+        <v>530</v>
       </c>
       <c r="J10" s="73"/>
       <c r="K10" s="73"/>
@@ -7770,16 +7768,16 @@
       <c r="C12" s="77" t="s">
         <v>819</v>
       </c>
-      <c r="D12" s="73"/>
+      <c r="D12" s="73">
+        <v>-31.12</v>
+      </c>
       <c r="E12">
         <v>-10.8</v>
       </c>
       <c r="F12">
         <v>65.3</v>
       </c>
-      <c r="G12" s="11">
-        <v>1.4E-5</v>
-      </c>
+      <c r="G12" s="11"/>
       <c r="I12" s="73">
         <v>10.17</v>
       </c>
@@ -8937,6 +8935,9 @@
       </c>
       <c r="H42" s="73">
         <v>167.9</v>
+      </c>
+      <c r="I42">
+        <v>100</v>
       </c>
       <c r="J42" s="73"/>
       <c r="K42" s="73"/>
@@ -9072,7 +9073,7 @@
         <v>341</v>
       </c>
       <c r="I46">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J46" s="73"/>
       <c r="K46" s="73"/>
@@ -11445,8 +11446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I83" sqref="I83"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14778,7 +14779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T83"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
@@ -18037,7 +18038,7 @@
   <dimension ref="A1:K143"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J83" sqref="J83"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Everything works-Requires dynamic growth rate evaluation
</commit_message>
<xml_diff>
--- a/KineticModel/ecoli_test.xlsx
+++ b/KineticModel/ecoli_test.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2383" uniqueCount="998">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2396" uniqueCount="1004">
   <si>
     <t>Enzymes</t>
   </si>
@@ -3063,13 +3063,31 @@
     <t>0.6,1,1,0.1,1,4.2</t>
   </si>
   <si>
-    <t>2.2e-5,1</t>
-  </si>
-  <si>
     <t>1,0.02,1,0.02</t>
   </si>
   <si>
-    <t>1,2.2e-5</t>
+    <t>2.2e-5,1e1</t>
+  </si>
+  <si>
+    <t>1e1,2.2e-5</t>
+  </si>
+  <si>
+    <t>1e1,1e-5</t>
+  </si>
+  <si>
+    <t>1,1e1,1,1e-5</t>
+  </si>
+  <si>
+    <t>1,1e-5,1,1e1</t>
+  </si>
+  <si>
+    <t>1e1,1,1e-5,1</t>
+  </si>
+  <si>
+    <t>1e-5,1e1</t>
+  </si>
+  <si>
+    <t>1e-3,1e-3</t>
   </si>
 </sst>
 </file>
@@ -7334,9 +7352,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7348,8 +7366,7 @@
     <col min="6" max="6" width="6.85546875" customWidth="1"/>
     <col min="7" max="7" width="7" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" customWidth="1"/>
-    <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="10" max="10" width="5.28515625" customWidth="1"/>
+    <col min="9" max="10" width="8" customWidth="1"/>
     <col min="12" max="12" width="6.5703125" customWidth="1"/>
     <col min="13" max="13" width="8.28515625" customWidth="1"/>
     <col min="14" max="14" width="11.85546875" customWidth="1"/>
@@ -9418,7 +9435,7 @@
         <v>1</v>
       </c>
       <c r="J51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K51" s="73"/>
       <c r="L51" s="73"/>
@@ -9426,7 +9443,9 @@
         <v>-13.3040694607334</v>
       </c>
       <c r="N51" s="77"/>
-      <c r="O51" s="73"/>
+      <c r="O51" s="73" t="s">
+        <v>1003</v>
+      </c>
       <c r="P51" s="73"/>
       <c r="R51" s="73"/>
       <c r="S51" s="73"/>
@@ -9448,7 +9467,7 @@
         <v>1</v>
       </c>
       <c r="J52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K52" s="73"/>
       <c r="L52" s="73"/>
@@ -9457,7 +9476,7 @@
       </c>
       <c r="N52" s="77"/>
       <c r="O52" s="73" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="P52" s="73"/>
       <c r="R52" s="73"/>
@@ -9477,10 +9496,10 @@
         <v>0</v>
       </c>
       <c r="I53" s="11">
-        <v>6.4800000000000004E-10</v>
+        <v>6.4799999999999998E-7</v>
       </c>
       <c r="J53" s="11">
-        <v>6.4800000000000004E-10</v>
+        <v>6.4799999999999998E-7</v>
       </c>
       <c r="K53" s="73"/>
       <c r="L53" s="73"/>
@@ -9489,7 +9508,7 @@
       </c>
       <c r="N53" s="77"/>
       <c r="O53" s="11" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="P53" s="73"/>
       <c r="R53" s="73"/>
@@ -9509,7 +9528,7 @@
         <v>0</v>
       </c>
       <c r="I54" s="86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J54">
         <v>1</v>
@@ -9554,7 +9573,9 @@
         <v>0</v>
       </c>
       <c r="N55" s="77"/>
-      <c r="O55" s="73"/>
+      <c r="O55" s="73" t="s">
+        <v>999</v>
+      </c>
       <c r="P55" s="73"/>
       <c r="R55" s="73"/>
       <c r="S55" s="73"/>
@@ -9586,7 +9607,9 @@
         <v>0</v>
       </c>
       <c r="N56" s="77"/>
-      <c r="O56" s="73"/>
+      <c r="O56" s="73" t="s">
+        <v>999</v>
+      </c>
       <c r="P56" s="73"/>
       <c r="R56" s="73"/>
       <c r="S56" s="73"/>
@@ -9618,7 +9641,9 @@
         <v>0</v>
       </c>
       <c r="N57" s="77"/>
-      <c r="O57" s="73"/>
+      <c r="O57" s="73" t="s">
+        <v>1000</v>
+      </c>
       <c r="P57" s="73"/>
       <c r="R57" s="73"/>
       <c r="S57" s="73"/>
@@ -9651,7 +9676,9 @@
         <v>0</v>
       </c>
       <c r="N58" s="77"/>
-      <c r="O58" s="73"/>
+      <c r="O58" s="73" t="s">
+        <v>1001</v>
+      </c>
       <c r="P58" s="73"/>
       <c r="R58" s="73"/>
       <c r="S58" s="73"/>
@@ -9684,7 +9711,9 @@
         <v>0</v>
       </c>
       <c r="N59" s="77"/>
-      <c r="O59" s="73"/>
+      <c r="O59" s="73" t="s">
+        <v>1001</v>
+      </c>
       <c r="P59" s="73"/>
       <c r="R59" s="73"/>
       <c r="S59" s="73"/>
@@ -9717,7 +9746,9 @@
         <v>0</v>
       </c>
       <c r="N60" s="77"/>
-      <c r="O60" s="73"/>
+      <c r="O60" s="73" t="s">
+        <v>999</v>
+      </c>
       <c r="P60" s="73"/>
       <c r="R60" s="73"/>
       <c r="S60" s="73"/>
@@ -9750,7 +9781,9 @@
         <v>0</v>
       </c>
       <c r="N61" s="77"/>
-      <c r="O61" s="73"/>
+      <c r="O61" s="73" t="s">
+        <v>999</v>
+      </c>
       <c r="P61" s="73"/>
       <c r="R61" s="73"/>
       <c r="S61" s="73"/>
@@ -9783,7 +9816,9 @@
         <v>0</v>
       </c>
       <c r="N62" s="77"/>
-      <c r="O62" s="73"/>
+      <c r="O62" s="73" t="s">
+        <v>1001</v>
+      </c>
       <c r="P62" s="73"/>
       <c r="R62" s="73"/>
       <c r="S62" s="73"/>
@@ -9813,7 +9848,9 @@
         <v>21.922606910894501</v>
       </c>
       <c r="N63" s="77"/>
-      <c r="O63" s="73"/>
+      <c r="O63" s="73" t="s">
+        <v>1002</v>
+      </c>
       <c r="P63" s="73"/>
       <c r="R63" s="73"/>
       <c r="S63" s="73"/>
@@ -9843,7 +9880,9 @@
         <v>0</v>
       </c>
       <c r="N64" s="77"/>
-      <c r="O64" s="73"/>
+      <c r="O64" s="73" t="s">
+        <v>1001</v>
+      </c>
       <c r="P64" s="73"/>
       <c r="R64" s="73"/>
       <c r="S64" s="73"/>
@@ -9876,7 +9915,9 @@
         <v>-19.215657194822899</v>
       </c>
       <c r="N65" s="77"/>
-      <c r="O65" s="73"/>
+      <c r="O65" s="73" t="s">
+        <v>1001</v>
+      </c>
       <c r="P65" s="73"/>
       <c r="R65" s="73"/>
       <c r="S65" s="73"/>
@@ -9906,7 +9947,9 @@
         <v>0</v>
       </c>
       <c r="N66" s="77"/>
-      <c r="O66" s="73"/>
+      <c r="O66" s="73" t="s">
+        <v>998</v>
+      </c>
       <c r="P66" s="73"/>
       <c r="R66" s="73"/>
       <c r="S66" s="73"/>

</xml_diff>

<commit_message>
Working Jacobian calculation using ADMAT
</commit_message>
<xml_diff>
--- a/KineticModel/ecoli_test.xlsx
+++ b/KineticModel/ecoli_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1140" windowWidth="18195" windowHeight="6465" firstSheet="6" activeTab="16"/>
+    <workbookView xWindow="480" yWindow="1140" windowWidth="18195" windowHeight="6465" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="ecoliT1" sheetId="1" r:id="rId1"/>
@@ -18,25 +18,25 @@
     <sheet name="Sheet2" sheetId="5" r:id="rId9"/>
     <sheet name="ecoliN1" sheetId="11" r:id="rId10"/>
     <sheet name="Sheet1" sheetId="13" r:id="rId11"/>
-    <sheet name="ecoliN2" sheetId="10" r:id="rId12"/>
-    <sheet name="Sheet3" sheetId="12" r:id="rId13"/>
-    <sheet name="Sheet4" sheetId="14" r:id="rId14"/>
-    <sheet name="Sheet5" sheetId="15" r:id="rId15"/>
-    <sheet name="Sheet6" sheetId="16" r:id="rId16"/>
-    <sheet name="Sheet7" sheetId="17" r:id="rId17"/>
+    <sheet name="Sheet8" sheetId="18" r:id="rId12"/>
+    <sheet name="ecoliN2" sheetId="10" r:id="rId13"/>
+    <sheet name="Sheet3" sheetId="12" r:id="rId14"/>
+    <sheet name="Sheet4" sheetId="14" r:id="rId15"/>
+    <sheet name="Sheet5" sheetId="15" r:id="rId16"/>
+    <sheet name="Sheet6" sheetId="16" r:id="rId17"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId18"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Sheet5!$A$1:$J$143</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">Sheet5!$A$1:$J$143</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2745" uniqueCount="1004">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2705" uniqueCount="1004">
   <si>
     <t>Enzymes</t>
   </si>
@@ -3327,7 +3327,7 @@
       <sheetName val="metabolites"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="1">
           <cell r="A1" t="str">
@@ -4815,8 +4815,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7355,8 +7355,8 @@
   <dimension ref="A1:U83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A83"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A83" sqref="A83:XFD83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10371,6 +10371,321 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="41.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="73" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="73" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="73" t="s">
+        <v>813</v>
+      </c>
+      <c r="C1" s="79" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="73" t="s">
+        <v>982</v>
+      </c>
+      <c r="E1" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="73" t="s">
+        <v>814</v>
+      </c>
+      <c r="G1" s="73" t="s">
+        <v>815</v>
+      </c>
+      <c r="H1" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="73" t="s">
+        <v>816</v>
+      </c>
+      <c r="J1" s="73" t="s">
+        <v>817</v>
+      </c>
+      <c r="K1" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="73" t="s">
+        <v>807</v>
+      </c>
+      <c r="O1" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="73" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="73" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" s="73" t="s">
+        <v>13</v>
+      </c>
+      <c r="T1" s="73" t="s">
+        <v>14</v>
+      </c>
+      <c r="U1" s="73" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="77" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="77" t="s">
+        <v>303</v>
+      </c>
+      <c r="E2" s="73">
+        <f>VLOOKUP(A2,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-9.1</v>
+      </c>
+      <c r="F2" s="73">
+        <v>-50.4</v>
+      </c>
+      <c r="G2" s="73">
+        <v>0.9</v>
+      </c>
+      <c r="I2" s="86">
+        <v>250</v>
+      </c>
+      <c r="M2" s="84">
+        <v>20</v>
+      </c>
+      <c r="N2" s="77">
+        <f>VLOOKUP(A2,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S2" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="73">
+        <v>5.5599999999999997E-2</v>
+      </c>
+      <c r="U2" s="73">
+        <v>5.5599999999999997E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="77" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="77" t="s">
+        <v>302</v>
+      </c>
+      <c r="E3" s="73">
+        <f>VLOOKUP(A3,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-0.9</v>
+      </c>
+      <c r="F3" s="73">
+        <v>-22.9</v>
+      </c>
+      <c r="G3" s="73">
+        <v>14.7</v>
+      </c>
+      <c r="I3" s="73">
+        <v>355.79</v>
+      </c>
+      <c r="M3" s="84">
+        <v>24.294625983764298</v>
+      </c>
+      <c r="N3" s="77" t="str">
+        <f>VLOOKUP(A3,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.2.1.11</v>
+      </c>
+      <c r="S3" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3" s="73">
+        <v>2.67</v>
+      </c>
+      <c r="U3" s="73">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="77" t="s">
+        <v>819</v>
+      </c>
+      <c r="E4" s="73">
+        <v>-31.12</v>
+      </c>
+      <c r="F4" s="73">
+        <v>-10.8</v>
+      </c>
+      <c r="G4" s="73">
+        <v>65.3</v>
+      </c>
+      <c r="H4" s="11"/>
+      <c r="J4" s="73">
+        <v>10.17</v>
+      </c>
+      <c r="L4" s="73">
+        <v>0.97</v>
+      </c>
+      <c r="M4" s="84">
+        <v>-8.5077261088811902</v>
+      </c>
+      <c r="N4" s="77" t="str">
+        <f>VLOOKUP(A4,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.1.40</v>
+      </c>
+      <c r="S4" s="73" t="s">
+        <v>797</v>
+      </c>
+      <c r="T4" s="73">
+        <v>0.111</v>
+      </c>
+      <c r="U4" s="73">
+        <v>0.111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="77" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="77" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="73" t="s">
+        <v>985</v>
+      </c>
+      <c r="E5" s="73">
+        <f>VLOOKUP(A5,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>-1.2</v>
+      </c>
+      <c r="F5" s="73">
+        <v>-50.9</v>
+      </c>
+      <c r="G5" s="73">
+        <v>24.4</v>
+      </c>
+      <c r="I5" s="73">
+        <v>1</v>
+      </c>
+      <c r="M5" s="84">
+        <v>0</v>
+      </c>
+      <c r="N5" s="77" t="str">
+        <f>VLOOKUP(A5,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.9.2</v>
+      </c>
+      <c r="S5" s="73" t="s">
+        <v>798</v>
+      </c>
+      <c r="T5" s="73">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="U5" s="73">
+        <v>0.13800000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="77" t="s">
+        <v>234</v>
+      </c>
+      <c r="C6" s="77" t="s">
+        <v>832</v>
+      </c>
+      <c r="D6" s="73" t="s">
+        <v>988</v>
+      </c>
+      <c r="E6" s="73">
+        <v>6.8</v>
+      </c>
+      <c r="F6" s="73">
+        <v>-7.1</v>
+      </c>
+      <c r="G6" s="73">
+        <v>55.6</v>
+      </c>
+      <c r="J6" s="73">
+        <v>540</v>
+      </c>
+      <c r="L6" s="73">
+        <v>18.2</v>
+      </c>
+      <c r="M6" s="84">
+        <v>5.4197985774166799</v>
+      </c>
+      <c r="N6" s="77" t="str">
+        <f>VLOOKUP(A6,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.1.1.31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="77" t="s">
+        <v>237</v>
+      </c>
+      <c r="C7" s="77" t="s">
+        <v>236</v>
+      </c>
+      <c r="D7" s="73" t="s">
+        <v>986</v>
+      </c>
+      <c r="E7" s="73">
+        <f>VLOOKUP(A7,Sheet3!$A$2:$I$84,6,FALSE)</f>
+        <v>0.2</v>
+      </c>
+      <c r="F7" s="73">
+        <v>-44.4</v>
+      </c>
+      <c r="G7" s="73">
+        <v>30.9</v>
+      </c>
+      <c r="I7" s="73">
+        <v>1</v>
+      </c>
+      <c r="M7" s="84">
+        <v>0</v>
+      </c>
+      <c r="N7" s="77" t="str">
+        <f>VLOOKUP(A7,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.1.1.49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="78" t="s">
+        <v>179</v>
+      </c>
+      <c r="C8" s="78" t="s">
+        <v>793</v>
+      </c>
+      <c r="E8" s="73">
+        <v>0</v>
+      </c>
+      <c r="M8" s="84">
+        <v>2.3245972881907302</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11685,7 +12000,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L96"/>
   <sheetViews>
@@ -15018,7 +15333,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T83"/>
   <sheetViews>
@@ -18276,7 +18591,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K143"/>
   <sheetViews>
@@ -21415,7 +21730,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U83"/>
   <sheetViews>
@@ -24819,923 +25134,6 @@
       <c r="S83" s="73"/>
       <c r="T83" s="73"/>
       <c r="U83" s="73"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C82"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="77" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2">
-        <v>-100</v>
-      </c>
-      <c r="C2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="77" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="77" t="s">
-        <v>124</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="77" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5">
-        <v>-100</v>
-      </c>
-      <c r="C5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="77" t="s">
-        <v>125</v>
-      </c>
-      <c r="B6">
-        <v>-100</v>
-      </c>
-      <c r="C6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="77" t="s">
-        <v>127</v>
-      </c>
-      <c r="B7">
-        <v>-100</v>
-      </c>
-      <c r="C7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="77" t="s">
-        <v>129</v>
-      </c>
-      <c r="B8">
-        <v>-100</v>
-      </c>
-      <c r="C8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="77" t="s">
-        <v>130</v>
-      </c>
-      <c r="B9">
-        <v>-100</v>
-      </c>
-      <c r="C9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="77" t="s">
-        <v>134</v>
-      </c>
-      <c r="B10">
-        <v>-100</v>
-      </c>
-      <c r="C10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="77" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11">
-        <v>-100</v>
-      </c>
-      <c r="C11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="77" t="s">
-        <v>136</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="77" t="s">
-        <v>140</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="77" t="s">
-        <v>239</v>
-      </c>
-      <c r="B14">
-        <v>-100</v>
-      </c>
-      <c r="C14">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="78" t="s">
-        <v>317</v>
-      </c>
-      <c r="B15">
-        <v>-100</v>
-      </c>
-      <c r="C15">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="77" t="s">
-        <v>323</v>
-      </c>
-      <c r="B16">
-        <v>-100</v>
-      </c>
-      <c r="C16">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="77" t="s">
-        <v>325</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="77" t="s">
-        <v>328</v>
-      </c>
-      <c r="B18">
-        <v>-100</v>
-      </c>
-      <c r="C18">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="77" t="s">
-        <v>245</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="77" t="s">
-        <v>332</v>
-      </c>
-      <c r="B20">
-        <v>-100</v>
-      </c>
-      <c r="C20">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="78" t="s">
-        <v>334</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="78" t="s">
-        <v>251</v>
-      </c>
-      <c r="B22">
-        <v>-100</v>
-      </c>
-      <c r="C22">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="77" t="s">
-        <v>252</v>
-      </c>
-      <c r="B23">
-        <v>-100</v>
-      </c>
-      <c r="C23">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="77" t="s">
-        <v>253</v>
-      </c>
-      <c r="B24">
-        <v>-100</v>
-      </c>
-      <c r="C24">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="77" t="s">
-        <v>141</v>
-      </c>
-      <c r="B25">
-        <v>-100</v>
-      </c>
-      <c r="C25">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="77" t="s">
-        <v>305</v>
-      </c>
-      <c r="B26">
-        <v>-100</v>
-      </c>
-      <c r="C26">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="77" t="s">
-        <v>212</v>
-      </c>
-      <c r="B27">
-        <v>-100</v>
-      </c>
-      <c r="C27">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="77" t="s">
-        <v>214</v>
-      </c>
-      <c r="B28">
-        <v>-100</v>
-      </c>
-      <c r="C28">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="78" t="s">
-        <v>144</v>
-      </c>
-      <c r="B29">
-        <v>-100</v>
-      </c>
-      <c r="C29">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="78" t="s">
-        <v>145</v>
-      </c>
-      <c r="B30">
-        <v>-100</v>
-      </c>
-      <c r="C30">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="77" t="s">
-        <v>415</v>
-      </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="77" t="s">
-        <v>419</v>
-      </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="77" t="s">
-        <v>422</v>
-      </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="77" t="s">
-        <v>425</v>
-      </c>
-      <c r="B34">
-        <v>-100</v>
-      </c>
-      <c r="C34">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="77" t="s">
-        <v>428</v>
-      </c>
-      <c r="B35">
-        <v>-100</v>
-      </c>
-      <c r="C35">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="77" t="s">
-        <v>431</v>
-      </c>
-      <c r="B36">
-        <v>-100</v>
-      </c>
-      <c r="C36">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="77" t="s">
-        <v>436</v>
-      </c>
-      <c r="B37">
-        <v>-100</v>
-      </c>
-      <c r="C37">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="77" t="s">
-        <v>434</v>
-      </c>
-      <c r="B38">
-        <v>-100</v>
-      </c>
-      <c r="C38">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="92" t="s">
-        <v>169</v>
-      </c>
-      <c r="B39">
-        <v>-100</v>
-      </c>
-      <c r="C39">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="94" t="s">
-        <v>441</v>
-      </c>
-      <c r="B40">
-        <v>0</v>
-      </c>
-      <c r="C40">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="94" t="s">
-        <v>444</v>
-      </c>
-      <c r="B41">
-        <v>0</v>
-      </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="77" t="s">
-        <v>178</v>
-      </c>
-      <c r="B42">
-        <v>-100</v>
-      </c>
-      <c r="C42">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="77" t="s">
-        <v>171</v>
-      </c>
-      <c r="B43">
-        <v>8.39</v>
-      </c>
-      <c r="C43">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="94" t="s">
-        <v>173</v>
-      </c>
-      <c r="B44">
-        <v>-100</v>
-      </c>
-      <c r="C44">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="94" t="s">
-        <v>167</v>
-      </c>
-      <c r="B45">
-        <v>0</v>
-      </c>
-      <c r="C45">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="77" t="s">
-        <v>234</v>
-      </c>
-      <c r="B46">
-        <v>-100</v>
-      </c>
-      <c r="C46">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="77" t="s">
-        <v>237</v>
-      </c>
-      <c r="B47">
-        <v>0</v>
-      </c>
-      <c r="C47">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="77" t="s">
-        <v>254</v>
-      </c>
-      <c r="B48">
-        <v>0</v>
-      </c>
-      <c r="C48">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="77" t="s">
-        <v>364</v>
-      </c>
-      <c r="B49">
-        <v>0</v>
-      </c>
-      <c r="C49">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="77" t="s">
-        <v>663</v>
-      </c>
-      <c r="B50">
-        <v>-100</v>
-      </c>
-      <c r="C50">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="77" t="s">
-        <v>463</v>
-      </c>
-      <c r="B51">
-        <v>-100</v>
-      </c>
-      <c r="C51">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="77" t="s">
-        <v>456</v>
-      </c>
-      <c r="B52">
-        <v>-100</v>
-      </c>
-      <c r="C52">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="77" t="s">
-        <v>397</v>
-      </c>
-      <c r="B53">
-        <v>-100</v>
-      </c>
-      <c r="C53">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="77" t="s">
-        <v>343</v>
-      </c>
-      <c r="B54">
-        <v>-100</v>
-      </c>
-      <c r="C54">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="77" t="s">
-        <v>346</v>
-      </c>
-      <c r="B55">
-        <v>0</v>
-      </c>
-      <c r="C55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="77" t="s">
-        <v>349</v>
-      </c>
-      <c r="B56">
-        <v>0</v>
-      </c>
-      <c r="C56">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="77" t="s">
-        <v>353</v>
-      </c>
-      <c r="B57">
-        <v>-100</v>
-      </c>
-      <c r="C57">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="77" t="s">
-        <v>356</v>
-      </c>
-      <c r="B58">
-        <v>0</v>
-      </c>
-      <c r="C58">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="78" t="s">
-        <v>360</v>
-      </c>
-      <c r="B59">
-        <v>0</v>
-      </c>
-      <c r="C59">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="77" t="s">
-        <v>368</v>
-      </c>
-      <c r="B60">
-        <v>-100</v>
-      </c>
-      <c r="C60">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="78" t="s">
-        <v>378</v>
-      </c>
-      <c r="B61">
-        <v>0</v>
-      </c>
-      <c r="C61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="78" t="s">
-        <v>381</v>
-      </c>
-      <c r="B62">
-        <v>0</v>
-      </c>
-      <c r="C62">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="77" t="s">
-        <v>384</v>
-      </c>
-      <c r="B63">
-        <v>-100</v>
-      </c>
-      <c r="C63">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="77" t="s">
-        <v>387</v>
-      </c>
-      <c r="B64">
-        <v>-100</v>
-      </c>
-      <c r="C64">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="78" t="s">
-        <v>390</v>
-      </c>
-      <c r="B65">
-        <v>-100</v>
-      </c>
-      <c r="C65">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="77" t="s">
-        <v>401</v>
-      </c>
-      <c r="B66">
-        <v>0</v>
-      </c>
-      <c r="C66">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="77" t="s">
-        <v>402</v>
-      </c>
-      <c r="B67">
-        <v>0</v>
-      </c>
-      <c r="C67">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="77" t="s">
-        <v>403</v>
-      </c>
-      <c r="B68">
-        <v>0</v>
-      </c>
-      <c r="C68">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="77" t="s">
-        <v>404</v>
-      </c>
-      <c r="B69">
-        <v>0</v>
-      </c>
-      <c r="C69">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="77" t="s">
-        <v>405</v>
-      </c>
-      <c r="B70">
-        <v>0</v>
-      </c>
-      <c r="C70">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="77" t="s">
-        <v>406</v>
-      </c>
-      <c r="B71">
-        <v>0</v>
-      </c>
-      <c r="C71">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="77" t="s">
-        <v>407</v>
-      </c>
-      <c r="B72">
-        <v>0</v>
-      </c>
-      <c r="C72">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="77" t="s">
-        <v>408</v>
-      </c>
-      <c r="B73">
-        <v>0</v>
-      </c>
-      <c r="C73">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="77" t="s">
-        <v>409</v>
-      </c>
-      <c r="B74">
-        <v>0</v>
-      </c>
-      <c r="C74">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="77" t="s">
-        <v>410</v>
-      </c>
-      <c r="B75">
-        <v>0</v>
-      </c>
-      <c r="C75">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="77" t="s">
-        <v>411</v>
-      </c>
-      <c r="B76">
-        <v>20</v>
-      </c>
-      <c r="C76">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="77" t="s">
-        <v>412</v>
-      </c>
-      <c r="B77">
-        <v>-100</v>
-      </c>
-      <c r="C77">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="77" t="s">
-        <v>413</v>
-      </c>
-      <c r="B78">
-        <v>-100</v>
-      </c>
-      <c r="C78">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="77" t="s">
-        <v>414</v>
-      </c>
-      <c r="B79">
-        <v>-100</v>
-      </c>
-      <c r="C79">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="77" t="s">
-        <v>460</v>
-      </c>
-      <c r="B80">
-        <v>-100</v>
-      </c>
-      <c r="C80">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="77" t="s">
-        <v>461</v>
-      </c>
-      <c r="B81">
-        <v>1000</v>
-      </c>
-      <c r="C81">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="78" t="s">
-        <v>179</v>
-      </c>
-      <c r="B82">
-        <v>0</v>
-      </c>
-      <c r="C82">
-        <v>100</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ensemble construction does not work
</commit_message>
<xml_diff>
--- a/KineticModel/ecoli_test.xlsx
+++ b/KineticModel/ecoli_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1140" windowWidth="18195" windowHeight="6465" firstSheet="7" activeTab="11"/>
+    <workbookView xWindow="480" yWindow="1140" windowWidth="18195" windowHeight="6465" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="ecoliT1" sheetId="1" r:id="rId1"/>
@@ -18,25 +18,24 @@
     <sheet name="Sheet2" sheetId="5" r:id="rId9"/>
     <sheet name="ecoliN1" sheetId="11" r:id="rId10"/>
     <sheet name="Sheet1" sheetId="13" r:id="rId11"/>
-    <sheet name="Sheet8" sheetId="18" r:id="rId12"/>
-    <sheet name="ecoliN2" sheetId="10" r:id="rId13"/>
-    <sheet name="Sheet3" sheetId="12" r:id="rId14"/>
-    <sheet name="Sheet4" sheetId="14" r:id="rId15"/>
-    <sheet name="Sheet5" sheetId="15" r:id="rId16"/>
-    <sheet name="Sheet6" sheetId="16" r:id="rId17"/>
+    <sheet name="ecoliN2" sheetId="10" r:id="rId12"/>
+    <sheet name="Sheet3" sheetId="12" r:id="rId13"/>
+    <sheet name="Sheet4" sheetId="14" r:id="rId14"/>
+    <sheet name="Sheet5" sheetId="15" r:id="rId15"/>
+    <sheet name="Sheet6" sheetId="16" r:id="rId16"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId18"/>
+    <externalReference r:id="rId17"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">Sheet5!$A$1:$J$143</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Sheet5!$A$1:$J$143</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2705" uniqueCount="1004">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2663" uniqueCount="1004">
   <si>
     <t>Enzymes</t>
   </si>
@@ -7354,9 +7353,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A83" sqref="A83:XFD83"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10371,321 +10370,6 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="41.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" s="73" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="73" t="s">
-        <v>813</v>
-      </c>
-      <c r="C1" s="79" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="73" t="s">
-        <v>982</v>
-      </c>
-      <c r="E1" s="74" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="73" t="s">
-        <v>814</v>
-      </c>
-      <c r="G1" s="73" t="s">
-        <v>815</v>
-      </c>
-      <c r="H1" s="73" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="73" t="s">
-        <v>816</v>
-      </c>
-      <c r="J1" s="73" t="s">
-        <v>817</v>
-      </c>
-      <c r="K1" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="73" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="73" t="s">
-        <v>807</v>
-      </c>
-      <c r="O1" s="73" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="73" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q1" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" s="73" t="s">
-        <v>12</v>
-      </c>
-      <c r="S1" s="73" t="s">
-        <v>13</v>
-      </c>
-      <c r="T1" s="73" t="s">
-        <v>14</v>
-      </c>
-      <c r="U1" s="73" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="77" t="s">
-        <v>303</v>
-      </c>
-      <c r="E2" s="73">
-        <f>VLOOKUP(A2,Sheet3!$A$2:$I$84,6,FALSE)</f>
-        <v>-9.1</v>
-      </c>
-      <c r="F2" s="73">
-        <v>-50.4</v>
-      </c>
-      <c r="G2" s="73">
-        <v>0.9</v>
-      </c>
-      <c r="I2" s="86">
-        <v>250</v>
-      </c>
-      <c r="M2" s="84">
-        <v>20</v>
-      </c>
-      <c r="N2" s="77">
-        <f>VLOOKUP(A2,[1]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="S2" s="73" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="73">
-        <v>5.5599999999999997E-2</v>
-      </c>
-      <c r="U2" s="73">
-        <v>5.5599999999999997E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="77" t="s">
-        <v>134</v>
-      </c>
-      <c r="C3" s="77" t="s">
-        <v>302</v>
-      </c>
-      <c r="E3" s="73">
-        <f>VLOOKUP(A3,Sheet3!$A$2:$I$84,6,FALSE)</f>
-        <v>-0.9</v>
-      </c>
-      <c r="F3" s="73">
-        <v>-22.9</v>
-      </c>
-      <c r="G3" s="73">
-        <v>14.7</v>
-      </c>
-      <c r="I3" s="73">
-        <v>355.79</v>
-      </c>
-      <c r="M3" s="84">
-        <v>24.294625983764298</v>
-      </c>
-      <c r="N3" s="77" t="str">
-        <f>VLOOKUP(A3,[1]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>4.2.1.11</v>
-      </c>
-      <c r="S3" s="73" t="s">
-        <v>26</v>
-      </c>
-      <c r="T3" s="73">
-        <v>2.67</v>
-      </c>
-      <c r="U3" s="73">
-        <v>2.67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="77" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="77" t="s">
-        <v>819</v>
-      </c>
-      <c r="E4" s="73">
-        <v>-31.12</v>
-      </c>
-      <c r="F4" s="73">
-        <v>-10.8</v>
-      </c>
-      <c r="G4" s="73">
-        <v>65.3</v>
-      </c>
-      <c r="H4" s="11"/>
-      <c r="J4" s="73">
-        <v>10.17</v>
-      </c>
-      <c r="L4" s="73">
-        <v>0.97</v>
-      </c>
-      <c r="M4" s="84">
-        <v>-8.5077261088811902</v>
-      </c>
-      <c r="N4" s="77" t="str">
-        <f>VLOOKUP(A4,[1]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>2.7.1.40</v>
-      </c>
-      <c r="S4" s="73" t="s">
-        <v>797</v>
-      </c>
-      <c r="T4" s="73">
-        <v>0.111</v>
-      </c>
-      <c r="U4" s="73">
-        <v>0.111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="77" t="s">
-        <v>136</v>
-      </c>
-      <c r="C5" s="77" t="s">
-        <v>135</v>
-      </c>
-      <c r="D5" s="73" t="s">
-        <v>985</v>
-      </c>
-      <c r="E5" s="73">
-        <f>VLOOKUP(A5,Sheet3!$A$2:$I$84,6,FALSE)</f>
-        <v>-1.2</v>
-      </c>
-      <c r="F5" s="73">
-        <v>-50.9</v>
-      </c>
-      <c r="G5" s="73">
-        <v>24.4</v>
-      </c>
-      <c r="I5" s="73">
-        <v>1</v>
-      </c>
-      <c r="M5" s="84">
-        <v>0</v>
-      </c>
-      <c r="N5" s="77" t="str">
-        <f>VLOOKUP(A5,[1]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>2.7.9.2</v>
-      </c>
-      <c r="S5" s="73" t="s">
-        <v>798</v>
-      </c>
-      <c r="T5" s="73">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="U5" s="73">
-        <v>0.13800000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="77" t="s">
-        <v>234</v>
-      </c>
-      <c r="C6" s="77" t="s">
-        <v>832</v>
-      </c>
-      <c r="D6" s="73" t="s">
-        <v>988</v>
-      </c>
-      <c r="E6" s="73">
-        <v>6.8</v>
-      </c>
-      <c r="F6" s="73">
-        <v>-7.1</v>
-      </c>
-      <c r="G6" s="73">
-        <v>55.6</v>
-      </c>
-      <c r="J6" s="73">
-        <v>540</v>
-      </c>
-      <c r="L6" s="73">
-        <v>18.2</v>
-      </c>
-      <c r="M6" s="84">
-        <v>5.4197985774166799</v>
-      </c>
-      <c r="N6" s="77" t="str">
-        <f>VLOOKUP(A6,[1]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>4.1.1.31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="77" t="s">
-        <v>237</v>
-      </c>
-      <c r="C7" s="77" t="s">
-        <v>236</v>
-      </c>
-      <c r="D7" s="73" t="s">
-        <v>986</v>
-      </c>
-      <c r="E7" s="73">
-        <f>VLOOKUP(A7,Sheet3!$A$2:$I$84,6,FALSE)</f>
-        <v>0.2</v>
-      </c>
-      <c r="F7" s="73">
-        <v>-44.4</v>
-      </c>
-      <c r="G7" s="73">
-        <v>30.9</v>
-      </c>
-      <c r="I7" s="73">
-        <v>1</v>
-      </c>
-      <c r="M7" s="84">
-        <v>0</v>
-      </c>
-      <c r="N7" s="77" t="str">
-        <f>VLOOKUP(A7,[1]reactions!$A$1:$E$96,5,FALSE)</f>
-        <v>4.1.1.49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="78" t="s">
-        <v>179</v>
-      </c>
-      <c r="C8" s="78" t="s">
-        <v>793</v>
-      </c>
-      <c r="E8" s="73">
-        <v>0</v>
-      </c>
-      <c r="M8" s="84">
-        <v>2.3245972881907302</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12000,7 +11684,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L96"/>
   <sheetViews>
@@ -15333,7 +15017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T83"/>
   <sheetViews>
@@ -18591,7 +18275,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K143"/>
   <sheetViews>
@@ -21730,7 +21414,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U83"/>
   <sheetViews>

</xml_diff>

<commit_message>
Changes to Mathematica files
</commit_message>
<xml_diff>
--- a/KineticModel/ecoli_test.xlsx
+++ b/KineticModel/ecoli_test.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="1140" windowWidth="18195" windowHeight="6465" firstSheet="7" activeTab="10"/>
   </bookViews>
@@ -30,7 +35,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Sheet5!$A$1:$J$143</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -4864,7 +4869,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4899,7 +4904,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7354,8 +7359,8 @@
   <dimension ref="A1:U83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changes to model analysi files
</commit_message>
<xml_diff>
--- a/KineticModel/ecoli_test.xlsx
+++ b/KineticModel/ecoli_test.xlsx
@@ -31,11 +31,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Sheet5!$A$1:$J$143</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2252" uniqueCount="904">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2275" uniqueCount="909">
   <si>
     <t>Enzymes</t>
   </si>
@@ -2790,6 +2791,21 @@
   <si>
     <t>[c] : q8h2 --&gt; q8</t>
   </si>
+  <si>
+    <t>6e-2,1.25e-2,2e-1,1.25e-2,1</t>
+  </si>
+  <si>
+    <t>Mc (mM)</t>
+  </si>
+  <si>
+    <t>h2o[c]</t>
+  </si>
+  <si>
+    <t>[c] : 1.496 3pg + 59.8100 atp + 0.0709 f6p + 0.1290 g3p + 0.2050 g6p + 59.8100 h2o + 3.5470 nad + 0.5191 pep + 2.8328 pyr --&gt; 59.8100 adp + 59.8100 h + 3.5470 nadh + 59.8100 pi</t>
+  </si>
+  <si>
+    <t>h2o[e]</t>
+  </si>
 </sst>
 </file>
 
@@ -2799,7 +2815,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000E+00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2850,6 +2866,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -2902,7 +2926,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -2935,6 +2959,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -2945,9 +2970,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -5130,8 +5152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U83"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:XFD46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17971,16 +17993,16 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U16"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="48.140625" customWidth="1"/>
-    <col min="15" max="15" width="17.7109375" customWidth="1"/>
+    <col min="15" max="15" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.35">
@@ -18111,7 +18133,7 @@
         <v>120</v>
       </c>
       <c r="M3" s="21">
-        <v>1.37855905020609</v>
+        <v>11.639423575531699</v>
       </c>
       <c r="N3" s="14" t="str">
         <f>VLOOKUP(A3,[1]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -18160,6 +18182,9 @@
         <f>VLOOKUP(A4,[1]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>2.7.1.11</v>
       </c>
+      <c r="O4" s="10" t="s">
+        <v>904</v>
+      </c>
       <c r="S4" s="10" t="s">
         <v>29</v>
       </c>
@@ -18252,7 +18277,7 @@
         <v>196</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>876</v>
+        <v>882</v>
       </c>
       <c r="E7" s="10">
         <f>VLOOKUP(A7,ecoli_core!$A$2:$I$84,6,FALSE)</f>
@@ -18551,6 +18576,115 @@
       </c>
       <c r="O16" s="10" t="s">
         <v>898</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>354</v>
+      </c>
+      <c r="E17" s="10">
+        <f>VLOOKUP(A17,ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="9">
+        <v>6.4799999999999998E-7</v>
+      </c>
+      <c r="J17" s="9">
+        <v>6.4799999999999998E-7</v>
+      </c>
+      <c r="M17" s="21">
+        <v>8.5514960440672301</v>
+      </c>
+      <c r="N17" s="14"/>
+      <c r="O17" s="9" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0</v>
+      </c>
+      <c r="M18" s="21">
+        <v>-8.5514960440672301</v>
+      </c>
+      <c r="N18" s="14"/>
+    </row>
+    <row r="19" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="E19" s="10">
+        <v>0</v>
+      </c>
+      <c r="M19" s="21">
+        <v>63.607356573910501</v>
+      </c>
+      <c r="N19" s="14"/>
+    </row>
+    <row r="20" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>559</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>561</v>
+      </c>
+      <c r="E20" s="10">
+        <f>VLOOKUP(A20,ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="10">
+        <v>1</v>
+      </c>
+      <c r="J20" s="10">
+        <v>2</v>
+      </c>
+      <c r="M20" s="21">
+        <v>-13.3040694607334</v>
+      </c>
+      <c r="N20" s="14"/>
+      <c r="O20" s="10" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="E21" s="10">
+        <v>0</v>
+      </c>
+      <c r="M21" s="21">
+        <v>13.304069460733899</v>
+      </c>
+      <c r="N21" s="14"/>
+    </row>
+    <row r="22" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>907</v>
+      </c>
+      <c r="E22" s="10">
+        <v>0</v>
+      </c>
+      <c r="M22" s="21">
+        <v>2.3245972881907302</v>
       </c>
     </row>
   </sheetData>
@@ -18560,12 +18694,123 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="10">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>906</v>
+      </c>
+      <c r="B4" s="9">
+        <v>55000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="B5" s="9">
+        <v>55000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="9">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="9"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="9"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Need to check solution
</commit_message>
<xml_diff>
--- a/KineticModel/ecoli_test.xlsx
+++ b/KineticModel/ecoli_test.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2275" uniqueCount="909">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2273" uniqueCount="908">
   <si>
     <t>Enzymes</t>
   </si>
@@ -2799,9 +2799,6 @@
   </si>
   <si>
     <t>h2o[c]</t>
-  </si>
-  <si>
-    <t>[c] : 1.496 3pg + 59.8100 atp + 0.0709 f6p + 0.1290 g3p + 0.2050 g6p + 59.8100 h2o + 3.5470 nad + 0.5191 pep + 2.8328 pyr --&gt; 59.8100 adp + 59.8100 h + 3.5470 nadh + 59.8100 pi</t>
   </si>
   <si>
     <t>h2o[e]</t>
@@ -5152,8 +5149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C66" sqref="C51:C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17995,8 +17992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18674,18 +18671,9 @@
       <c r="N21" s="14"/>
     </row>
     <row r="22" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>907</v>
-      </c>
-      <c r="E22" s="10">
-        <v>0</v>
-      </c>
-      <c r="M22" s="21">
-        <v>2.3245972881907302</v>
-      </c>
+      <c r="A22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="M22" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18736,7 +18724,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="B5" s="9">
         <v>55000</v>

</xml_diff>

<commit_message>
Non-working changes to enable ETC flux
</commit_message>
<xml_diff>
--- a/KineticModel/ecoli_test.xlsx
+++ b/KineticModel/ecoli_test.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1260" windowWidth="18195" windowHeight="6345" firstSheet="10" activeTab="19"/>
+    <workbookView xWindow="480" yWindow="1260" windowWidth="18195" windowHeight="6345" firstSheet="9" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="ecoliT1" sheetId="1" r:id="rId1"/>
@@ -34,12 +39,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Sheet5!$A$1:$J$143</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2580" uniqueCount="926">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2582" uniqueCount="926">
   <si>
     <t>Enzymes</t>
   </si>
@@ -4582,7 +4587,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4617,7 +4622,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5211,8 +5216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20795,10 +20800,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B7"/>
+      <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20857,6 +20862,22 @@
       </c>
       <c r="B7" s="9">
         <v>0.27300000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="9">
+        <v>9.9999999999999995E-8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="9">
+        <v>7.9999999999999996E-7</v>
       </c>
     </row>
   </sheetData>
@@ -21184,13 +21205,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="48.42578125" customWidth="1"/>
+    <col min="3" max="3" width="70.5703125" customWidth="1"/>
     <col min="15" max="15" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
ETCflux requires completion and testing
</commit_message>
<xml_diff>
--- a/KineticModel/ecoli_test.xlsx
+++ b/KineticModel/ecoli_test.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="1260" windowWidth="18195" windowHeight="6345" firstSheet="9" activeTab="19"/>
   </bookViews>
@@ -39,12 +34,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Sheet5!$A$1:$J$143</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2582" uniqueCount="926">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2581" uniqueCount="928">
   <si>
     <t>Enzymes</t>
   </si>
@@ -2864,6 +2859,12 @@
   </si>
   <si>
     <t>1,42e-3,1,42e-3</t>
+  </si>
+  <si>
+    <t>5 h[c] + nadh[c] + q8[c] &lt;==&gt; 4 h[e] + nad[c] + q8h2[c]</t>
+  </si>
+  <si>
+    <t>adp[c] + 4 h[e] + pi[c] &lt;==&gt; atp[c] + 3 h[c]</t>
   </si>
 </sst>
 </file>
@@ -4587,7 +4588,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4622,7 +4623,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5216,8 +5217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U83"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6999,7 +7000,7 @@
       </c>
       <c r="B40" s="30"/>
       <c r="C40" s="29" t="s">
-        <v>871</v>
+        <v>926</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>884</v>
@@ -7011,7 +7012,7 @@
         <v>122.4</v>
       </c>
       <c r="H40" s="9">
-        <v>1.4000000000000001E-15</v>
+        <v>714300000000000</v>
       </c>
       <c r="J40" s="10">
         <v>26</v>
@@ -7195,7 +7196,7 @@
       </c>
       <c r="B45" s="30"/>
       <c r="C45" s="31" t="s">
-        <v>917</v>
+        <v>927</v>
       </c>
       <c r="D45" s="10" t="s">
         <v>886</v>
@@ -7207,7 +7208,7 @@
         <v>1.5</v>
       </c>
       <c r="H45" s="9">
-        <v>42000</v>
+        <v>2.3810000000000001E-5</v>
       </c>
       <c r="J45" s="10">
         <v>2200</v>
@@ -21205,8 +21206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21672,7 +21673,7 @@
       </c>
       <c r="B12" s="30"/>
       <c r="C12" s="29" t="s">
-        <v>871</v>
+        <v>926</v>
       </c>
       <c r="F12" s="10">
         <v>24.2</v>
@@ -21681,7 +21682,7 @@
         <v>122.4</v>
       </c>
       <c r="H12" s="9">
-        <v>1.4000000000000001E-15</v>
+        <v>714300000000000</v>
       </c>
       <c r="J12" s="10">
         <v>200</v>
@@ -21731,10 +21732,7 @@
       </c>
       <c r="B14" s="30"/>
       <c r="C14" s="31" t="s">
-        <v>917</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>884</v>
+        <v>927</v>
       </c>
       <c r="F14" s="10">
         <v>-62.3</v>
@@ -21743,7 +21741,7 @@
         <v>1.5</v>
       </c>
       <c r="H14" s="9">
-        <v>42000</v>
+        <v>2.3810000000000001E-5</v>
       </c>
       <c r="I14" s="9">
         <v>2160</v>

</xml_diff>

<commit_message>
Changes to setupMetLP_red to accomodate pmf in ETC
</commit_message>
<xml_diff>
--- a/KineticModel/ecoli_test.xlsx
+++ b/KineticModel/ecoli_test.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1260" windowWidth="18195" windowHeight="6345" firstSheet="10" activeTab="17"/>
+    <workbookView xWindow="480" yWindow="1260" windowWidth="18195" windowHeight="6345" firstSheet="10" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="ecoliT1" sheetId="1" r:id="rId1"/>
@@ -31,19 +26,20 @@
     <sheet name="gly_testC" sheetId="23" r:id="rId17"/>
     <sheet name="red_test" sheetId="24" r:id="rId18"/>
     <sheet name="red_testC" sheetId="25" r:id="rId19"/>
+    <sheet name="red_test2" sheetId="26" r:id="rId20"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId20"/>
+    <externalReference r:id="rId21"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Sheet5!$A$1:$J$143</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2486" uniqueCount="921">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2580" uniqueCount="923">
   <si>
     <t>Enzymes</t>
   </si>
@@ -2848,6 +2844,12 @@
   </si>
   <si>
     <t>1,3.4e-6,42e-3,1,1,42e-3</t>
+  </si>
+  <si>
+    <t>adp[c] + 4 h[e] + pi[c] &lt;==&gt; atp[c] + 3 h[c]</t>
+  </si>
+  <si>
+    <t>5 h[c] + nadh[c] + q8[c] &lt;==&gt; 4 h[e] + nad[c] + q8h2[c]</t>
   </si>
 </sst>
 </file>
@@ -4571,7 +4573,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4606,7 +4608,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -19706,8 +19708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C12:C15"/>
+    <sheetView topLeftCell="D3" workbookViewId="0">
+      <selection sqref="A1:U25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21138,6 +21140,1071 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:U25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="49.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>706</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>875</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>707</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>708</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>709</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>710</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>700</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10">
+        <f>VLOOKUP(A2,ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-9.1</v>
+      </c>
+      <c r="F2" s="10">
+        <v>-50.4</v>
+      </c>
+      <c r="G2" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="23">
+        <v>250</v>
+      </c>
+      <c r="J2" s="23">
+        <v>0</v>
+      </c>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="21">
+        <v>20</v>
+      </c>
+      <c r="N2" s="14">
+        <f>VLOOKUP(A2,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>902</v>
+      </c>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="10">
+        <v>5.5599999999999997E-2</v>
+      </c>
+      <c r="U2" s="10">
+        <v>5.5599999999999997E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10">
+        <v>3.1320000000000001</v>
+      </c>
+      <c r="F3" s="10">
+        <v>-17.100000000000001</v>
+      </c>
+      <c r="G3" s="10">
+        <v>20.6</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10">
+        <v>120</v>
+      </c>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="21">
+        <v>11.639423575531699</v>
+      </c>
+      <c r="N3" s="14" t="str">
+        <f>VLOOKUP(A3,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.3.1.9</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>726</v>
+      </c>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="T3" s="10">
+        <v>3.48</v>
+      </c>
+      <c r="U3" s="10">
+        <v>3.48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10">
+        <f>VLOOKUP(A4,ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-3.8</v>
+      </c>
+      <c r="F4" s="10">
+        <v>-53.9</v>
+      </c>
+      <c r="G4" s="10">
+        <v>21.4</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10">
+        <v>49</v>
+      </c>
+      <c r="J4" s="10">
+        <v>0</v>
+      </c>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="21">
+        <v>11.639423575531699</v>
+      </c>
+      <c r="N4" s="14" t="str">
+        <f>VLOOKUP(A4,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.1.11</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>904</v>
+      </c>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="T4" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="U4" s="10">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10">
+        <f>VLOOKUP(A5,ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>4.2</v>
+      </c>
+      <c r="F5" s="10">
+        <v>-29.4</v>
+      </c>
+      <c r="G5" s="10">
+        <v>27.1</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="10">
+        <v>8.5</v>
+      </c>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="21">
+        <v>11.639423575531699</v>
+      </c>
+      <c r="N5" s="14" t="str">
+        <f>VLOOKUP(A5,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.1.2.13</v>
+      </c>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10" t="s">
+        <v>691</v>
+      </c>
+      <c r="T5" s="10">
+        <v>0.218</v>
+      </c>
+      <c r="U5" s="10">
+        <v>0.218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="14" t="s">
+        <v>711</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="23">
+        <v>7.5979999999999999</v>
+      </c>
+      <c r="F6" s="10">
+        <v>-24.3</v>
+      </c>
+      <c r="G6" s="10">
+        <v>13.4</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10">
+        <v>9000</v>
+      </c>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="22">
+        <v>-11.639423575531699</v>
+      </c>
+      <c r="N6" s="14" t="str">
+        <f>VLOOKUP(A6,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.3.1.1</v>
+      </c>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="T6" s="10">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="U6" s="10">
+        <v>0.16700000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10">
+        <f>VLOOKUP(A7,ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="F7" s="10">
+        <v>-12.8</v>
+      </c>
+      <c r="G7" s="10">
+        <v>62.6</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10">
+        <v>268</v>
+      </c>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="21">
+        <v>27.772223526897601</v>
+      </c>
+      <c r="N7" s="14" t="str">
+        <f>VLOOKUP(A7,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.2.1.12</v>
+      </c>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="T7" s="10">
+        <v>2.13</v>
+      </c>
+      <c r="U7" s="10">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10">
+        <v>-10.51</v>
+      </c>
+      <c r="F8" s="10">
+        <v>-19.2</v>
+      </c>
+      <c r="G8" s="10">
+        <v>56.1</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10">
+        <v>654</v>
+      </c>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="21">
+        <v>-27.772223526897601</v>
+      </c>
+      <c r="N8" s="14" t="str">
+        <f>VLOOKUP(A8,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.2.3</v>
+      </c>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="T8" s="10">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="U8" s="10">
+        <v>0.39900000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10">
+        <v>6.2290000000000001</v>
+      </c>
+      <c r="F9" s="10">
+        <v>-23.1</v>
+      </c>
+      <c r="G9" s="10">
+        <v>14.6</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10">
+        <v>530</v>
+      </c>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="21">
+        <v>-24.294625983764298</v>
+      </c>
+      <c r="N9" s="14" t="str">
+        <f>VLOOKUP(A9,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>5.4.2.1</v>
+      </c>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="T9" s="10">
+        <v>2.67</v>
+      </c>
+      <c r="U9" s="10">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10">
+        <f>VLOOKUP(A10,ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-0.9</v>
+      </c>
+      <c r="F10" s="10">
+        <v>-22.9</v>
+      </c>
+      <c r="G10" s="10">
+        <v>14.7</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10">
+        <v>355.79</v>
+      </c>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="21">
+        <v>24.294625983764298</v>
+      </c>
+      <c r="N10" s="14" t="str">
+        <f>VLOOKUP(A10,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>4.2.1.11</v>
+      </c>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="T10" s="10">
+        <v>2.67</v>
+      </c>
+      <c r="U10" s="10">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="14" t="s">
+        <v>909</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10">
+        <v>-31.12</v>
+      </c>
+      <c r="F11" s="10">
+        <v>-10.8</v>
+      </c>
+      <c r="G11" s="10">
+        <v>65.3</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="10">
+        <v>2540</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="21">
+        <v>-8.5077261088811902</v>
+      </c>
+      <c r="N11" s="14" t="str">
+        <f>VLOOKUP(A11,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>2.7.1.40</v>
+      </c>
+      <c r="O11" s="10" t="s">
+        <v>910</v>
+      </c>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10" t="s">
+        <v>692</v>
+      </c>
+      <c r="T11" s="10">
+        <v>0.111</v>
+      </c>
+      <c r="U11" s="10">
+        <v>0.111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" s="30"/>
+      <c r="C12" s="29" t="s">
+        <v>922</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10">
+        <v>24.2</v>
+      </c>
+      <c r="G12" s="10">
+        <v>122.4</v>
+      </c>
+      <c r="H12" s="9">
+        <v>714300000000000</v>
+      </c>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10">
+        <v>200</v>
+      </c>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="21">
+        <v>-43.153531211344998</v>
+      </c>
+      <c r="N12" s="14" t="str">
+        <f>VLOOKUP(A12,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>1.6.5.3</v>
+      </c>
+      <c r="O12" s="10" t="s">
+        <v>900</v>
+      </c>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>885</v>
+      </c>
+      <c r="E13" s="10">
+        <f>VLOOKUP(A13,ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-6.6</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10">
+        <v>1</v>
+      </c>
+      <c r="J13" s="10">
+        <v>0</v>
+      </c>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="21">
+        <v>8.39</v>
+      </c>
+      <c r="N13" s="14"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" s="30"/>
+      <c r="C14" s="31" t="s">
+        <v>921</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>884</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10">
+        <v>-62.3</v>
+      </c>
+      <c r="G14" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="H14" s="9">
+        <v>2.3810000000000001E-5</v>
+      </c>
+      <c r="I14" s="9">
+        <v>2160</v>
+      </c>
+      <c r="J14" s="9">
+        <v>5130</v>
+      </c>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="21">
+        <v>-100</v>
+      </c>
+      <c r="N14" s="14" t="str">
+        <f>VLOOKUP(A14,[1]reactions!$A$1:$E$96,5,FALSE)</f>
+        <v>3.6.3.14</v>
+      </c>
+      <c r="O14" s="10" t="s">
+        <v>918</v>
+      </c>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" s="30"/>
+      <c r="C15" s="31" t="s">
+        <v>870</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10">
+        <f>VLOOKUP(A15,ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>-37.200000000000003</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10">
+        <v>469</v>
+      </c>
+      <c r="J15" s="10">
+        <v>0</v>
+      </c>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="21">
+        <v>46.7215117629625</v>
+      </c>
+      <c r="N15" s="14" t="s">
+        <v>703</v>
+      </c>
+      <c r="O15" s="10" t="s">
+        <v>920</v>
+      </c>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>559</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="26" t="s">
+        <v>561</v>
+      </c>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10">
+        <f>VLOOKUP(A16,ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10">
+        <v>1</v>
+      </c>
+      <c r="J16" s="10">
+        <v>2</v>
+      </c>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="21">
+        <v>-13.3040694607334</v>
+      </c>
+      <c r="N16" s="14"/>
+      <c r="O16" s="10" t="s">
+        <v>896</v>
+      </c>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10">
+        <f>VLOOKUP(A17,ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="23">
+        <v>1</v>
+      </c>
+      <c r="J17" s="10">
+        <v>0</v>
+      </c>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="21">
+        <v>23.3607558814812</v>
+      </c>
+      <c r="N17" s="14"/>
+      <c r="O17" s="10" t="s">
+        <v>889</v>
+      </c>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
+        <v>352</v>
+      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="26" t="s">
+        <v>354</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10">
+        <f>VLOOKUP(A18,ecoli_core!$A$2:$I$84,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="9">
+        <v>100</v>
+      </c>
+      <c r="J18" s="9">
+        <v>100</v>
+      </c>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="21">
+        <v>8.5514960440672301</v>
+      </c>
+      <c r="N18" s="14"/>
+      <c r="O18" s="9" t="s">
+        <v>888</v>
+      </c>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
+        <v>241</v>
+      </c>
+      <c r="B19" s="33"/>
+      <c r="C19" s="26" t="s">
+        <v>243</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>884</v>
+      </c>
+      <c r="E19" s="10">
+        <v>0</v>
+      </c>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="23">
+        <v>2540</v>
+      </c>
+      <c r="J19" s="10">
+        <v>2540</v>
+      </c>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="21">
+        <v>-8.5077261088811902</v>
+      </c>
+      <c r="N19" s="14"/>
+      <c r="O19" s="10" t="s">
+        <v>899</v>
+      </c>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10">
+        <v>0</v>
+      </c>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="21">
+        <v>0</v>
+      </c>
+      <c r="N20" s="14"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="28" t="s">
+        <v>690</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10">
+        <v>0</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="21">
+        <v>-20</v>
+      </c>
+      <c r="N21" s="14"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10">
+        <v>0</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="21">
+        <v>63.607356573910501</v>
+      </c>
+      <c r="N22" s="14"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10">
+        <v>0</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="21">
+        <v>13.304069460733899</v>
+      </c>
+      <c r="N23" s="14"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10">
+        <v>0</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="21">
+        <v>-8.5514960440672301</v>
+      </c>
+      <c r="N24" s="14"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="28" t="s">
+        <v>358</v>
+      </c>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10">
+        <v>0</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="21">
+        <v>-23.3607558814812</v>
+      </c>
+      <c r="N25" s="14"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>